<commit_message>
v.0.6.0 Almost all instructions working
</commit_message>
<xml_diff>
--- a/2nd gen - 8 bit cpu/Instruction control lines.xlsx
+++ b/2nd gen - 8 bit cpu/Instruction control lines.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Control Lines" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="75">
   <si>
     <t>LD R1, data</t>
   </si>
@@ -231,6 +231,15 @@
   </si>
   <si>
     <t>0c</t>
+  </si>
+  <si>
+    <t>001011</t>
+  </si>
+  <si>
+    <t>2c</t>
+  </si>
+  <si>
+    <t>0[addr]</t>
   </si>
 </sst>
 </file>
@@ -388,7 +397,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -423,7 +432,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -634,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W31"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="X6" sqref="X6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1946,85 +1955,102 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="9.140625" style="11"/>
+    <col min="2" max="5" width="9.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="C1" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="11" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="C2" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="D2" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="E2" s="11" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="C3" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="D3" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="E3" s="11" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="C4" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="D4" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="E4" s="11" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="C5" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>60</v>
-      </c>
       <c r="D5" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" s="11" t="s">
         <v>70</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Small improvements in Assembler program / Binary test progarm to Logisim CPU
</commit_message>
<xml_diff>
--- a/2nd gen - 8 bit cpu/Instruction control lines.xlsx
+++ b/2nd gen - 8 bit cpu/Instruction control lines.xlsx
@@ -9,14 +9,14 @@
   <sheets>
     <sheet name="Control Lines" sheetId="1" r:id="rId1"/>
     <sheet name="Some instructions for test" sheetId="2" r:id="rId2"/>
-    <sheet name="TestProgram_Counter" sheetId="3" r:id="rId3"/>
+    <sheet name="Test Programs" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="117">
   <si>
     <t>LD R1, data</t>
   </si>
@@ -307,13 +307,73 @@
   </si>
   <si>
     <t>2c 00 06</t>
+  </si>
+  <si>
+    <t>LD E, 0x0</t>
+  </si>
+  <si>
+    <t>LD F, 0xff</t>
+  </si>
+  <si>
+    <t>LD A, E</t>
+  </si>
+  <si>
+    <t>LD E, A</t>
+  </si>
+  <si>
+    <t>LD A, F</t>
+  </si>
+  <si>
+    <t>LD F, A</t>
+  </si>
+  <si>
+    <t>JP [0x009]</t>
+  </si>
+  <si>
+    <t>Equiv to ADD E, B</t>
+  </si>
+  <si>
+    <t>06 00 00</t>
+  </si>
+  <si>
+    <t>06 80 ff</t>
+  </si>
+  <si>
+    <t>08 40 00</t>
+  </si>
+  <si>
+    <t>08 50 00</t>
+  </si>
+  <si>
+    <t>0a 80 00</t>
+  </si>
+  <si>
+    <t>0a 00 00</t>
+  </si>
+  <si>
+    <t>2c 00 09</t>
+  </si>
+  <si>
+    <t>// Increments E, decrements F</t>
+  </si>
+  <si>
+    <t>Equiv to SUB F, B</t>
+  </si>
+  <si>
+    <t>// Increments A</t>
+  </si>
+  <si>
+    <t>Dec</t>
+  </si>
+  <si>
+    <t>Hexa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -352,6 +412,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -379,7 +446,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -404,6 +471,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2182,74 +2253,279 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20:E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="11"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="13" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B6" si="0">DEC2HEX(A3,3)</f>
+        <v>000</v>
+      </c>
+      <c r="C3" t="s">
         <v>87</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D3" s="11" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>003</v>
+      </c>
+      <c r="C4" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="D4" s="11" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>006</v>
+      </c>
+      <c r="C5" t="s">
         <v>89</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="D5" s="11" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>009</v>
+      </c>
+      <c r="C6" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="D6" s="11" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" t="str">
+        <f t="shared" ref="B9" si="1">DEC2HEX(A9,3)</f>
+        <v>006</v>
+      </c>
+      <c r="C9" t="s">
         <v>90</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="D9" s="11" t="s">
         <v>91</v>
       </c>
     </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C16" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" ref="B17:B22" si="2">DEC2HEX(A17,3)</f>
+        <v>000</v>
+      </c>
+      <c r="C17" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="2"/>
+        <v>003</v>
+      </c>
+      <c r="C18" t="s">
+        <v>97</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>6</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="2"/>
+        <v>006</v>
+      </c>
+      <c r="C19" t="s">
+        <v>98</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>9</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="2"/>
+        <v>009</v>
+      </c>
+      <c r="C20" t="s">
+        <v>99</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>12</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" si="2"/>
+        <v>00C</v>
+      </c>
+      <c r="C21" t="s">
+        <v>89</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E21" s="12"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>15</v>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" si="2"/>
+        <v>00F</v>
+      </c>
+      <c r="C22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="E22" s="12"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>18</v>
+      </c>
+      <c r="B23" t="str">
+        <f>DEC2HEX(A23,3)</f>
+        <v>012</v>
+      </c>
+      <c r="C23" t="s">
+        <v>101</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>21</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" ref="B24:B26" si="3">DEC2HEX(A24,3)</f>
+        <v>015</v>
+      </c>
+      <c r="C24" t="s">
+        <v>90</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="E24" s="12"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="3"/>
+        <v>018</v>
+      </c>
+      <c r="C25" t="s">
+        <v>102</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="E25" s="12"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>27</v>
+      </c>
+      <c r="B26" t="str">
+        <f t="shared" si="3"/>
+        <v>01B</v>
+      </c>
+      <c r="C26" t="s">
+        <v>103</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>111</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="E23:E25"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
v.0.8.1 Almost all instructions implemented
</commit_message>
<xml_diff>
--- a/2nd gen - 8 bit cpu/Instruction control lines.xlsx
+++ b/2nd gen - 8 bit cpu/Instruction control lines.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Control Lines" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="126">
   <si>
     <t>LD R1, data</t>
   </si>
@@ -367,6 +367,33 @@
   </si>
   <si>
     <t>Hexa</t>
+  </si>
+  <si>
+    <t>// Increments A, stops at 0</t>
+  </si>
+  <si>
+    <t>JP [0x00f]</t>
+  </si>
+  <si>
+    <t>JP Z, [0x00f]</t>
+  </si>
+  <si>
+    <t>2c 00 0f</t>
+  </si>
+  <si>
+    <t>30 00 0f</t>
+  </si>
+  <si>
+    <t>// Load value from memory, puts it in A</t>
+  </si>
+  <si>
+    <t>LD A, [0x003]</t>
+  </si>
+  <si>
+    <t>a0</t>
+  </si>
+  <si>
+    <t>0c 00 03</t>
   </si>
 </sst>
 </file>
@@ -471,10 +498,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -781,8 +808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X31"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="X8" sqref="X8"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2253,10 +2280,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20:E22"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2277,7 +2304,7 @@
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>114</v>
       </c>
     </row>
@@ -2357,7 +2384,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="12" t="s">
         <v>112</v>
       </c>
     </row>
@@ -2420,7 +2447,7 @@
       <c r="D20" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E20" s="13" t="s">
         <v>104</v>
       </c>
     </row>
@@ -2438,7 +2465,7 @@
       <c r="D21" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="E21" s="12"/>
+      <c r="E21" s="13"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
@@ -2454,7 +2481,7 @@
       <c r="D22" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="E22" s="12"/>
+      <c r="E22" s="13"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
@@ -2470,7 +2497,7 @@
       <c r="D23" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="E23" s="13" t="s">
         <v>113</v>
       </c>
     </row>
@@ -2488,7 +2515,7 @@
       <c r="D24" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="E24" s="12"/>
+      <c r="E24" s="13"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
@@ -2504,7 +2531,7 @@
       <c r="D25" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="E25" s="12"/>
+      <c r="E25" s="13"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
@@ -2519,6 +2546,135 @@
       </c>
       <c r="D26" s="11" t="s">
         <v>111</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>0</v>
+      </c>
+      <c r="B32" t="str">
+        <f t="shared" ref="B32:B35" si="4">DEC2HEX(A32,3)</f>
+        <v>000</v>
+      </c>
+      <c r="C32" t="s">
+        <v>87</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>3</v>
+      </c>
+      <c r="B33" t="str">
+        <f t="shared" si="4"/>
+        <v>003</v>
+      </c>
+      <c r="C33" t="s">
+        <v>88</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>6</v>
+      </c>
+      <c r="B34" t="str">
+        <f t="shared" si="4"/>
+        <v>006</v>
+      </c>
+      <c r="C34" t="s">
+        <v>89</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>9</v>
+      </c>
+      <c r="B35" t="str">
+        <f t="shared" si="4"/>
+        <v>009</v>
+      </c>
+      <c r="C35" t="s">
+        <v>119</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>12</v>
+      </c>
+      <c r="B36" t="str">
+        <f t="shared" ref="B36:B37" si="5">DEC2HEX(A36,3)</f>
+        <v>00C</v>
+      </c>
+      <c r="C36" t="s">
+        <v>95</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>15</v>
+      </c>
+      <c r="B37" t="str">
+        <f t="shared" si="5"/>
+        <v>00F</v>
+      </c>
+      <c r="C37" t="s">
+        <v>118</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C41" s="12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>0</v>
+      </c>
+      <c r="B42" t="str">
+        <f t="shared" ref="B42:B47" si="6">DEC2HEX(A42,3)</f>
+        <v>000</v>
+      </c>
+      <c r="C42" t="s">
+        <v>123</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>3</v>
+      </c>
+      <c r="B43" t="str">
+        <f t="shared" si="6"/>
+        <v>003</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v.0.9.0 instruction ST [addr], R2 working fine
</commit_message>
<xml_diff>
--- a/2nd gen - 8 bit cpu/Instruction control lines.xlsx
+++ b/2nd gen - 8 bit cpu/Instruction control lines.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Control Lines" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="129">
   <si>
     <t>LD R1, data</t>
   </si>
@@ -384,16 +384,25 @@
     <t>30 00 0f</t>
   </si>
   <si>
-    <t>// Load value from memory, puts it in A</t>
-  </si>
-  <si>
-    <t>LD A, [0x003]</t>
-  </si>
-  <si>
-    <t>a0</t>
-  </si>
-  <si>
-    <t>0c 00 03</t>
+    <t>LD A, [0x010]</t>
+  </si>
+  <si>
+    <t>ST [0x011], A</t>
+  </si>
+  <si>
+    <t>34 00 11</t>
+  </si>
+  <si>
+    <t>0c 00 10</t>
+  </si>
+  <si>
+    <t>// Load value from memory, copies it to next address</t>
+  </si>
+  <si>
+    <t>R1 to MEM_DATA, provisorily using R2</t>
+  </si>
+  <si>
+    <t>f0</t>
   </si>
 </sst>
 </file>
@@ -447,7 +456,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -457,6 +466,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -473,7 +488,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -501,6 +516,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -808,8 +826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="X23" sqref="X23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,7 +876,7 @@
       <c r="M1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="14" t="s">
         <v>53</v>
       </c>
       <c r="O1" s="7" t="s">
@@ -1822,7 +1840,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:22" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="4" t="s">
         <v>19</v>
@@ -1861,7 +1879,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>41</v>
       </c>
@@ -1923,7 +1941,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>42</v>
       </c>
@@ -1985,7 +2003,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
         <v>43</v>
       </c>
@@ -2007,7 +2025,7 @@
       <c r="U20" s="3"/>
       <c r="V20" s="3"/>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>44</v>
       </c>
@@ -2029,7 +2047,7 @@
       <c r="U21" s="3"/>
       <c r="V21" s="3"/>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>45</v>
       </c>
@@ -2050,8 +2068,11 @@
       <c r="T22" s="3"/>
       <c r="U22" s="3"/>
       <c r="V22" s="3"/>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="X22" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
         <v>46</v>
       </c>
@@ -2073,17 +2094,17 @@
       <c r="U23" s="3"/>
       <c r="V23" s="3"/>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
         <v>22</v>
       </c>
@@ -2091,7 +2112,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B28" s="8" t="s">
         <v>30</v>
       </c>
@@ -2099,7 +2120,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>49</v>
       </c>
@@ -2107,7 +2128,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>56</v>
       </c>
@@ -2280,10 +2301,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2647,7 +2668,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C41" s="12" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -2655,11 +2676,11 @@
         <v>0</v>
       </c>
       <c r="B42" t="str">
-        <f t="shared" ref="B42:B47" si="6">DEC2HEX(A42,3)</f>
+        <f t="shared" ref="B42:B45" si="6">DEC2HEX(A42,3)</f>
         <v>000</v>
       </c>
       <c r="C42" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D42" s="11" t="s">
         <v>125</v>
@@ -2673,8 +2694,38 @@
         <f t="shared" si="6"/>
         <v>003</v>
       </c>
+      <c r="C43" t="s">
+        <v>123</v>
+      </c>
       <c r="D43" s="11" t="s">
         <v>124</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>6</v>
+      </c>
+      <c r="B44" t="str">
+        <f t="shared" si="6"/>
+        <v>006</v>
+      </c>
+      <c r="C44" t="s">
+        <v>95</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>16</v>
+      </c>
+      <c r="B45" t="str">
+        <f t="shared" si="6"/>
+        <v>010</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Instruction to write to LCD output still not working; first draft to change the instruction decoder ICs to a microcoded ROM
</commit_message>
<xml_diff>
--- a/2nd gen - 8 bit cpu/Instruction control lines.xlsx
+++ b/2nd gen - 8 bit cpu/Instruction control lines.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Control Lines" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="143">
   <si>
     <t>LD R1, data</t>
   </si>
@@ -159,21 +159,12 @@
     <t>JP STE R1, R2</t>
   </si>
   <si>
-    <t>IN R1</t>
-  </si>
-  <si>
-    <t>OUT R1</t>
-  </si>
-  <si>
     <t>R1, R2</t>
   </si>
   <si>
     <t>general use 8-bit registers</t>
   </si>
   <si>
-    <t>pair of 8-bit registers (as addressing is 12-bit, only half of the High register will be used)</t>
-  </si>
-  <si>
     <t>ST [addr], R1</t>
   </si>
   <si>
@@ -366,9 +357,6 @@
     <t>Dec</t>
   </si>
   <si>
-    <t>Hexa</t>
-  </si>
-  <si>
     <t>// Increments A, stops at 0</t>
   </si>
   <si>
@@ -403,6 +391,60 @@
   </si>
   <si>
     <t>f0</t>
+  </si>
+  <si>
+    <t>pair of 8-bit registers (as addressing is 12-bit, only lower half of the High register will be used)</t>
+  </si>
+  <si>
+    <t>IN R1, R2</t>
+  </si>
+  <si>
+    <t>OUT R1. R2</t>
+  </si>
+  <si>
+    <t>Read byte from input selected by R2, and writes it to R1</t>
+  </si>
+  <si>
+    <t>Write byte value of R1 in output selected in R2</t>
+  </si>
+  <si>
+    <t>R1 to OUT</t>
+  </si>
+  <si>
+    <t>// Write letter A to LCD output</t>
+  </si>
+  <si>
+    <t>LD A, 0x0</t>
+  </si>
+  <si>
+    <t>LD B, 0x41</t>
+  </si>
+  <si>
+    <t>04 80 41</t>
+  </si>
+  <si>
+    <t>OUT A, B</t>
+  </si>
+  <si>
+    <t>04 00 00</t>
+  </si>
+  <si>
+    <t>// ASCII code for letter A</t>
+  </si>
+  <si>
+    <t>44 10 00</t>
+  </si>
+  <si>
+    <t>Hex</t>
+  </si>
+  <si>
+    <t>Mnemonic</t>
+  </si>
+  <si>
+    <t>Opcode (Hex)</t>
+  </si>
+  <si>
+    <t>ROM Output in Hex</t>
   </si>
 </sst>
 </file>
@@ -488,7 +530,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -514,11 +556,14 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment textRotation="90"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -824,25 +869,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X31"/>
+  <dimension ref="A1:AE31"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="X23" sqref="X23"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AE2" sqref="AE2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="1" max="1" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="10" width="3" customWidth="1"/>
     <col min="11" max="14" width="2.85546875" customWidth="1"/>
     <col min="15" max="15" width="2.85546875" style="6" customWidth="1"/>
     <col min="16" max="16" width="3.140625" style="6" customWidth="1"/>
-    <col min="17" max="22" width="2.85546875" customWidth="1"/>
+    <col min="17" max="17" width="2.85546875" customWidth="1"/>
+    <col min="18" max="18" width="3.140625" style="6" customWidth="1"/>
+    <col min="19" max="25" width="2.85546875" customWidth="1"/>
+    <col min="26" max="26" width="5.42578125" customWidth="1"/>
+    <col min="27" max="27" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="1" customFormat="1" ht="130.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="10"/>
+    <row r="1" spans="1:31" s="1" customFormat="1" ht="130.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>140</v>
+      </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
@@ -865,7 +920,7 @@
         <v>15</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>11</v>
@@ -876,8 +931,8 @@
       <c r="M1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="14" t="s">
-        <v>53</v>
+      <c r="N1" s="13" t="s">
+        <v>50</v>
       </c>
       <c r="O1" s="7" t="s">
         <v>20</v>
@@ -886,26 +941,35 @@
         <v>21</v>
       </c>
       <c r="Q1" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="R1" s="7"/>
+      <c r="S1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="W1" s="2"/>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="AA1" s="15"/>
+      <c r="AB1" s="15"/>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -948,11 +1012,8 @@
       <c r="N2" s="3">
         <v>0</v>
       </c>
-      <c r="Q2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>14</v>
+      <c r="Q2" s="3">
+        <v>0</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>14</v>
@@ -966,8 +1027,31 @@
       <c r="V2" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="W2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y2" s="3"/>
+      <c r="Z2" t="str">
+        <f>BIN2HEX(C2 &amp; D2 &amp; E2 &amp; F2 &amp; G2 &amp; H2 &amp; I2 &amp; J2, 2)</f>
+        <v>00</v>
+      </c>
+      <c r="AA2" t="e">
+        <f>BIN2HEX(K2 &amp; L2 &amp; M2 &amp; N2 &amp; S2 &amp; T2 &amp; U2 &amp; V2, 2)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AB2" t="e">
+        <f>BIN2HEX(W2 &amp; X2, 1)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="AE2" t="str">
+        <f>IF(S2="x", 0, S2) &amp; IF(T2="x", 0, T2)</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -1010,11 +1094,8 @@
       <c r="N3" s="3">
         <v>0</v>
       </c>
-      <c r="Q3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>14</v>
+      <c r="Q3" s="3">
+        <v>0</v>
       </c>
       <c r="S3" s="3" t="s">
         <v>14</v>
@@ -1028,8 +1109,15 @@
       <c r="V3" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="W3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y3" s="3"/>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1072,11 +1160,8 @@
       <c r="N4" s="3">
         <v>0</v>
       </c>
-      <c r="Q4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>14</v>
+      <c r="Q4" s="3">
+        <v>0</v>
       </c>
       <c r="S4" s="3" t="s">
         <v>14</v>
@@ -1090,8 +1175,15 @@
       <c r="V4" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="W4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y4" s="3"/>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -1134,11 +1226,8 @@
       <c r="N5" s="3">
         <v>0</v>
       </c>
-      <c r="Q5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="R5" s="3" t="s">
-        <v>14</v>
+      <c r="Q5" s="3">
+        <v>0</v>
       </c>
       <c r="S5" s="3" t="s">
         <v>14</v>
@@ -1152,13 +1241,20 @@
       <c r="V5" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="W5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y5" s="3"/>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C6" s="3">
         <v>0</v>
@@ -1196,11 +1292,8 @@
       <c r="N6" s="3">
         <v>0</v>
       </c>
-      <c r="Q6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>14</v>
+      <c r="Q6" s="3">
+        <v>0</v>
       </c>
       <c r="S6" s="3" t="s">
         <v>14</v>
@@ -1214,8 +1307,15 @@
       <c r="V6" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="W6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="X6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y6" s="3"/>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -1259,16 +1359,13 @@
         <v>0</v>
       </c>
       <c r="Q7" s="3">
-        <v>1</v>
-      </c>
-      <c r="R7" s="3">
         <v>0</v>
       </c>
       <c r="S7" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T7" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U7" s="3">
         <v>0</v>
@@ -1276,11 +1373,18 @@
       <c r="V7" s="3">
         <v>1</v>
       </c>
-      <c r="X7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="W7" s="3">
+        <v>0</v>
+      </c>
+      <c r="X7" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="3"/>
+      <c r="AD7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -1326,23 +1430,27 @@
       <c r="Q8" s="3">
         <v>0</v>
       </c>
-      <c r="R8" s="3">
-        <v>1</v>
-      </c>
       <c r="S8" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T8" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U8" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V8" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="W8" s="3">
+        <v>0</v>
+      </c>
+      <c r="X8" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="3"/>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -1388,9 +1496,6 @@
       <c r="Q9" s="3">
         <v>0</v>
       </c>
-      <c r="R9" s="3">
-        <v>0</v>
-      </c>
       <c r="S9" s="3">
         <v>0</v>
       </c>
@@ -1398,13 +1503,20 @@
         <v>0</v>
       </c>
       <c r="U9" s="3">
-        <v>1</v>
-      </c>
-      <c r="V9" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="V9" s="3">
+        <v>0</v>
+      </c>
+      <c r="W9" s="3">
+        <v>1</v>
+      </c>
+      <c r="X9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y9" s="3"/>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -1448,25 +1560,29 @@
         <v>0</v>
       </c>
       <c r="Q10" s="3">
-        <v>1</v>
-      </c>
-      <c r="R10" s="3">
         <v>0</v>
       </c>
       <c r="S10" s="3">
         <v>1</v>
       </c>
       <c r="T10" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U10" s="3">
         <v>1</v>
       </c>
-      <c r="V10" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="V10" s="3">
+        <v>1</v>
+      </c>
+      <c r="W10" s="3">
+        <v>1</v>
+      </c>
+      <c r="X10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y10" s="3"/>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -1510,25 +1626,29 @@
         <v>0</v>
       </c>
       <c r="Q11" s="3">
-        <v>1</v>
-      </c>
-      <c r="R11" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S11" s="3">
         <v>1</v>
       </c>
       <c r="T11" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U11" s="3">
         <v>1</v>
       </c>
-      <c r="V11" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="V11" s="3">
+        <v>0</v>
+      </c>
+      <c r="W11" s="3">
+        <v>1</v>
+      </c>
+      <c r="X11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y11" s="3"/>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>38</v>
       </c>
@@ -1574,23 +1694,27 @@
       <c r="Q12" s="3">
         <v>0</v>
       </c>
-      <c r="R12" s="3">
-        <v>1</v>
-      </c>
       <c r="S12" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T12" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U12" s="3">
         <v>1</v>
       </c>
-      <c r="V12" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="V12" s="3">
+        <v>0</v>
+      </c>
+      <c r="W12" s="3">
+        <v>1</v>
+      </c>
+      <c r="X12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y12" s="3"/>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>39</v>
       </c>
@@ -1633,11 +1757,8 @@
       <c r="N13" s="3">
         <v>0</v>
       </c>
-      <c r="Q13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="R13" s="3" t="s">
-        <v>14</v>
+      <c r="Q13" s="3">
+        <v>0</v>
       </c>
       <c r="S13" s="3" t="s">
         <v>14</v>
@@ -1651,8 +1772,15 @@
       <c r="V13" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="W13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="X13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y13" s="3"/>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>40</v>
       </c>
@@ -1695,11 +1823,8 @@
       <c r="N14" s="3">
         <v>0</v>
       </c>
-      <c r="Q14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="R14" s="3" t="s">
-        <v>14</v>
+      <c r="Q14" s="3">
+        <v>0</v>
       </c>
       <c r="S14" s="3" t="s">
         <v>14</v>
@@ -1713,8 +1838,15 @@
       <c r="V14" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:24" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="W14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="X14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y14" s="3"/>
+    </row>
+    <row r="15" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="4" t="s">
         <v>17</v>
@@ -1758,11 +1890,8 @@
       <c r="O15" s="5">
         <v>1</v>
       </c>
-      <c r="Q15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="R15" s="3" t="s">
-        <v>14</v>
+      <c r="Q15" s="3">
+        <v>0</v>
       </c>
       <c r="S15" s="3" t="s">
         <v>14</v>
@@ -1776,8 +1905,15 @@
       <c r="V15" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:24" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="W15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="X15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y15" s="3"/>
+    </row>
+    <row r="16" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="4" t="s">
         <v>18</v>
@@ -1821,11 +1957,8 @@
       <c r="O16" s="5">
         <v>1</v>
       </c>
-      <c r="Q16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="R16" s="3" t="s">
-        <v>14</v>
+      <c r="Q16" s="3">
+        <v>0</v>
       </c>
       <c r="S16" s="3" t="s">
         <v>14</v>
@@ -1839,8 +1972,15 @@
       <c r="V16" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:24" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="W16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="X16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y16" s="3"/>
+    </row>
+    <row r="17" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="4" t="s">
         <v>19</v>
@@ -1857,14 +1997,8 @@
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
-      <c r="P17" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q17" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="R17" s="3" t="s">
-        <v>14</v>
+      <c r="Q17" s="3">
+        <v>1</v>
       </c>
       <c r="S17" s="3" t="s">
         <v>14</v>
@@ -1878,13 +2012,20 @@
       <c r="V17" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="W17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="X17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y17" s="3"/>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C18" s="3">
         <v>0</v>
@@ -1922,11 +2063,8 @@
       <c r="N18">
         <v>1</v>
       </c>
-      <c r="Q18" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="R18" s="3" t="s">
-        <v>14</v>
+      <c r="Q18" s="3">
+        <v>0</v>
       </c>
       <c r="S18" s="3" t="s">
         <v>14</v>
@@ -1940,13 +2078,20 @@
       <c r="V18" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="W18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="X18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y18" s="3"/>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C19" s="3">
         <v>0</v>
@@ -1984,11 +2129,8 @@
       <c r="N19">
         <v>1</v>
       </c>
-      <c r="Q19" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="R19" s="3" t="s">
-        <v>14</v>
+      <c r="Q19" s="3">
+        <v>0</v>
       </c>
       <c r="S19" s="3" t="s">
         <v>14</v>
@@ -2002,8 +2144,15 @@
       <c r="V19" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="W19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="X19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y19" s="3"/>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
         <v>43</v>
       </c>
@@ -2019,13 +2168,15 @@
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
       <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
       <c r="S20" s="3"/>
       <c r="T20" s="3"/>
       <c r="U20" s="3"/>
       <c r="V20" s="3"/>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="W20" s="3"/>
+      <c r="X20" s="3"/>
+      <c r="Y20" s="3"/>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>44</v>
       </c>
@@ -2041,13 +2192,15 @@
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
       <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
       <c r="S21" s="3"/>
       <c r="T21" s="3"/>
       <c r="U21" s="3"/>
       <c r="V21" s="3"/>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="W21" s="3"/>
+      <c r="X21" s="3"/>
+      <c r="Y21" s="3"/>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>45</v>
       </c>
@@ -2063,16 +2216,18 @@
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
       <c r="Q22" s="3"/>
-      <c r="R22" s="3"/>
       <c r="S22" s="3"/>
       <c r="T22" s="3"/>
       <c r="U22" s="3"/>
       <c r="V22" s="3"/>
-      <c r="X22" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="W22" s="3"/>
+      <c r="X22" s="3"/>
+      <c r="Y22" s="3"/>
+      <c r="AB22" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
         <v>46</v>
       </c>
@@ -2088,23 +2243,37 @@
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
       <c r="Q23" s="3"/>
-      <c r="R23" s="3"/>
       <c r="S23" s="3"/>
       <c r="T23" s="3"/>
       <c r="U23" s="3"/>
       <c r="V23" s="3"/>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="W23" s="3"/>
+      <c r="X23" s="3"/>
+      <c r="Y23" s="3"/>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>10</v>
+      </c>
       <c r="B24" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>11</v>
+      </c>
       <c r="B25" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
         <v>22</v>
       </c>
@@ -2112,7 +2281,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B28" s="8" t="s">
         <v>30</v>
       </c>
@@ -2120,23 +2289,26 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C30" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C31" t="s">
-        <v>51</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="Z1:AB1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2158,72 +2330,72 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>58</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C3" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>66</v>
-      </c>
       <c r="E3" s="11" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D4" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>64</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C5" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>74</v>
-      </c>
       <c r="E5" s="11" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2231,67 +2403,67 @@
         <v>4</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>78</v>
-      </c>
       <c r="E7" s="11" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D8" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" t="s">
         <v>78</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="F8" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C9" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="11" t="s">
-        <v>86</v>
-      </c>
       <c r="E9" s="11" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -2301,10 +2473,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2316,17 +2488,17 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="12" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2334,14 +2506,14 @@
         <v>0</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" ref="B3:B6" si="0">DEC2HEX(A3,3)</f>
-        <v>000</v>
+        <f>"0x" &amp; DEC2HEX(A3,3)</f>
+        <v>0x000</v>
       </c>
       <c r="C3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2349,14 +2521,14 @@
         <v>3</v>
       </c>
       <c r="B4" t="str">
-        <f t="shared" si="0"/>
-        <v>003</v>
+        <f t="shared" ref="B4:B6" si="0">"0x" &amp; DEC2HEX(A4,3)</f>
+        <v>0x003</v>
       </c>
       <c r="C4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2365,13 +2537,13 @@
       </c>
       <c r="B5" t="str">
         <f t="shared" si="0"/>
-        <v>006</v>
+        <v>0x006</v>
       </c>
       <c r="C5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>89</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2380,13 +2552,13 @@
       </c>
       <c r="B6" t="str">
         <f t="shared" si="0"/>
-        <v>009</v>
+        <v>0x009</v>
       </c>
       <c r="C6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2394,19 +2566,19 @@
         <v>6</v>
       </c>
       <c r="B9" t="str">
-        <f t="shared" ref="B9" si="1">DEC2HEX(A9,3)</f>
-        <v>006</v>
+        <f>"0x" &amp; DEC2HEX(A9,3)</f>
+        <v>0x006</v>
       </c>
       <c r="C9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C16" s="12" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2414,14 +2586,14 @@
         <v>0</v>
       </c>
       <c r="B17" t="str">
-        <f t="shared" ref="B17:B22" si="2">DEC2HEX(A17,3)</f>
-        <v>000</v>
+        <f t="shared" ref="B17:B26" si="1">"0x" &amp; DEC2HEX(A17,3)</f>
+        <v>0x000</v>
       </c>
       <c r="C17" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2429,14 +2601,14 @@
         <v>3</v>
       </c>
       <c r="B18" t="str">
-        <f t="shared" si="2"/>
-        <v>003</v>
+        <f t="shared" si="1"/>
+        <v>0x003</v>
       </c>
       <c r="C18" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2444,14 +2616,14 @@
         <v>6</v>
       </c>
       <c r="B19" t="str">
-        <f t="shared" si="2"/>
-        <v>006</v>
+        <f t="shared" si="1"/>
+        <v>0x006</v>
       </c>
       <c r="C19" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -2459,17 +2631,17 @@
         <v>9</v>
       </c>
       <c r="B20" t="str">
-        <f t="shared" si="2"/>
-        <v>009</v>
+        <f t="shared" si="1"/>
+        <v>0x009</v>
       </c>
       <c r="C20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="E20" s="13" t="s">
         <v>104</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2477,49 +2649,49 @@
         <v>12</v>
       </c>
       <c r="B21" t="str">
-        <f t="shared" si="2"/>
-        <v>00C</v>
+        <f t="shared" si="1"/>
+        <v>0x00C</v>
       </c>
       <c r="C21" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="D21" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="E21" s="13"/>
+      <c r="E21" s="14"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>15</v>
       </c>
       <c r="B22" t="str">
-        <f t="shared" si="2"/>
-        <v>00F</v>
+        <f t="shared" si="1"/>
+        <v>0x00F</v>
       </c>
       <c r="C22" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="E22" s="13"/>
+        <v>107</v>
+      </c>
+      <c r="E22" s="14"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>18</v>
       </c>
       <c r="B23" t="str">
-        <f>DEC2HEX(A23,3)</f>
-        <v>012</v>
+        <f t="shared" si="1"/>
+        <v>0x012</v>
       </c>
       <c r="C23" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>113</v>
+        <v>105</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2527,53 +2699,53 @@
         <v>21</v>
       </c>
       <c r="B24" t="str">
-        <f t="shared" ref="B24:B26" si="3">DEC2HEX(A24,3)</f>
-        <v>015</v>
+        <f t="shared" si="1"/>
+        <v>0x015</v>
       </c>
       <c r="C24" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="E24" s="13"/>
+        <v>88</v>
+      </c>
+      <c r="E24" s="14"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="str">
-        <f t="shared" si="3"/>
-        <v>018</v>
+        <f t="shared" si="1"/>
+        <v>0x018</v>
       </c>
       <c r="C25" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="E25" s="13"/>
+        <v>106</v>
+      </c>
+      <c r="E25" s="14"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>27</v>
       </c>
       <c r="B26" t="str">
-        <f t="shared" si="3"/>
-        <v>01B</v>
+        <f t="shared" si="1"/>
+        <v>0x01B</v>
       </c>
       <c r="C26" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="12" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -2581,14 +2753,14 @@
         <v>0</v>
       </c>
       <c r="B32" t="str">
-        <f t="shared" ref="B32:B35" si="4">DEC2HEX(A32,3)</f>
-        <v>000</v>
+        <f t="shared" ref="B32:B37" si="2">"0x" &amp; DEC2HEX(A32,3)</f>
+        <v>0x000</v>
       </c>
       <c r="C32" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -2596,14 +2768,14 @@
         <v>3</v>
       </c>
       <c r="B33" t="str">
-        <f t="shared" si="4"/>
-        <v>003</v>
+        <f t="shared" si="2"/>
+        <v>0x003</v>
       </c>
       <c r="C33" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -2611,14 +2783,14 @@
         <v>6</v>
       </c>
       <c r="B34" t="str">
-        <f t="shared" si="4"/>
-        <v>006</v>
+        <f t="shared" si="2"/>
+        <v>0x006</v>
       </c>
       <c r="C34" t="s">
+        <v>86</v>
+      </c>
+      <c r="D34" s="11" t="s">
         <v>89</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -2626,14 +2798,14 @@
         <v>9</v>
       </c>
       <c r="B35" t="str">
-        <f t="shared" si="4"/>
-        <v>009</v>
+        <f t="shared" si="2"/>
+        <v>0x009</v>
       </c>
       <c r="C35" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -2641,14 +2813,14 @@
         <v>12</v>
       </c>
       <c r="B36" t="str">
-        <f t="shared" ref="B36:B37" si="5">DEC2HEX(A36,3)</f>
-        <v>00C</v>
+        <f t="shared" si="2"/>
+        <v>0x00C</v>
       </c>
       <c r="C36" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -2656,19 +2828,19 @@
         <v>15</v>
       </c>
       <c r="B37" t="str">
-        <f t="shared" si="5"/>
-        <v>00F</v>
+        <f t="shared" si="2"/>
+        <v>0x00F</v>
       </c>
       <c r="C37" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C41" s="12" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -2676,14 +2848,14 @@
         <v>0</v>
       </c>
       <c r="B42" t="str">
-        <f t="shared" ref="B42:B45" si="6">DEC2HEX(A42,3)</f>
-        <v>000</v>
+        <f t="shared" ref="B42:B45" si="3">"0x" &amp; DEC2HEX(A42,3)</f>
+        <v>0x000</v>
       </c>
       <c r="C42" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -2691,14 +2863,14 @@
         <v>3</v>
       </c>
       <c r="B43" t="str">
-        <f t="shared" si="6"/>
-        <v>003</v>
+        <f t="shared" si="3"/>
+        <v>0x003</v>
       </c>
       <c r="C43" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -2706,14 +2878,14 @@
         <v>6</v>
       </c>
       <c r="B44" t="str">
-        <f t="shared" si="6"/>
-        <v>006</v>
+        <f t="shared" si="3"/>
+        <v>0x006</v>
       </c>
       <c r="C44" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -2721,11 +2893,64 @@
         <v>16</v>
       </c>
       <c r="B45" t="str">
-        <f t="shared" si="6"/>
-        <v>010</v>
+        <f t="shared" si="3"/>
+        <v>0x010</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>128</v>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C48" s="12" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>0</v>
+      </c>
+      <c r="B49" t="str">
+        <f t="shared" ref="B49:B51" si="4">"0x" &amp; DEC2HEX(A49,3)</f>
+        <v>0x000</v>
+      </c>
+      <c r="C49" t="s">
+        <v>132</v>
+      </c>
+      <c r="D49" s="11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>3</v>
+      </c>
+      <c r="B50" t="str">
+        <f t="shared" si="4"/>
+        <v>0x003</v>
+      </c>
+      <c r="C50" t="s">
+        <v>133</v>
+      </c>
+      <c r="D50" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="E50" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>6</v>
+      </c>
+      <c r="B51" t="str">
+        <f t="shared" si="4"/>
+        <v>0x006</v>
+      </c>
+      <c r="C51" t="s">
+        <v>135</v>
+      </c>
+      <c r="D51" s="11" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented microcoded ROM. All working. Writing to LCD output
</commit_message>
<xml_diff>
--- a/2nd gen - 8 bit cpu/Instruction control lines.xlsx
+++ b/2nd gen - 8 bit cpu/Instruction control lines.xlsx
@@ -15,8 +15,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Autor</author>
+  </authors>
+  <commentList>
+    <comment ref="AB2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Warning : caution with this byte (look the rom output in circuit)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="143">
   <si>
     <t>LD R1, data</t>
   </si>
@@ -444,14 +478,14 @@
     <t>Opcode (Hex)</t>
   </si>
   <si>
-    <t>ROM Output in Hex</t>
+    <t>ROM DATA in Hex</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -496,6 +530,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -559,11 +606,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -868,11 +915,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AE2" sqref="AE2"/>
+      <selection activeCell="AA29" sqref="AA29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -886,8 +933,7 @@
     <col min="17" max="17" width="2.85546875" customWidth="1"/>
     <col min="18" max="18" width="3.140625" style="6" customWidth="1"/>
     <col min="19" max="25" width="2.85546875" customWidth="1"/>
-    <col min="26" max="26" width="5.42578125" customWidth="1"/>
-    <col min="27" max="27" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="28" width="5.85546875" customWidth="1"/>
     <col min="29" max="29" width="2" customWidth="1"/>
   </cols>
   <sheetData>
@@ -963,11 +1009,11 @@
         <v>37</v>
       </c>
       <c r="Y1" s="2"/>
-      <c r="Z1" s="15" t="s">
+      <c r="Z1" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="AA1" s="15"/>
-      <c r="AB1" s="15"/>
+      <c r="AA1" s="14"/>
+      <c r="AB1" s="14"/>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
@@ -1035,16 +1081,16 @@
       </c>
       <c r="Y2" s="3"/>
       <c r="Z2" t="str">
-        <f>BIN2HEX(C2 &amp; D2 &amp; E2 &amp; F2 &amp; G2 &amp; H2 &amp; I2 &amp; J2, 2)</f>
+        <f>BIN2HEX(IF(C2="x", 0, C2) &amp; IF(D2="x", 0, D2) &amp; IF(E2="x", 0, E2) &amp; IF(F2="x", 0, F2) &amp; IF(G2="x", 0, G2) &amp; IF(H2="x", 0, H2) &amp; IF(I2="x", 0, I2) &amp; IF(J2="x", 0, J2), 2)</f>
         <v>00</v>
       </c>
-      <c r="AA2" t="e">
-        <f>BIN2HEX(K2 &amp; L2 &amp; M2 &amp; N2 &amp; S2 &amp; T2 &amp; U2 &amp; V2, 2)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="AB2" t="e">
-        <f>BIN2HEX(W2 &amp; X2, 1)</f>
-        <v>#NUM!</v>
+      <c r="AA2" t="str">
+        <f>BIN2HEX(IF(K2="x", 0, K2) &amp; IF(L2="x", 0, L2) &amp; IF(M2="x", 0, M2) &amp; IF(N2="x", 0, N2) &amp;  IF(Q2="x", 0, Q2) &amp; IF(S2="x", 0, S2) &amp; IF(T2="x", 0, T2) &amp; IF(U2="x", 0, U2), 2)</f>
+        <v>00</v>
+      </c>
+      <c r="AB2" t="str">
+        <f>BIN2HEX(IF(V2="x", 0, V2) &amp; IF(W2="x", 0, W2) &amp; IF(X2="x", 0, X2), 2)</f>
+        <v>00</v>
       </c>
       <c r="AE2" t="str">
         <f>IF(S2="x", 0, S2) &amp; IF(T2="x", 0, T2)</f>
@@ -1116,6 +1162,18 @@
         <v>14</v>
       </c>
       <c r="Y3" s="3"/>
+      <c r="Z3" t="str">
+        <f>BIN2HEX(IF(C3="x", 0, C3) &amp; IF(D3="x", 0, D3) &amp; IF(E3="x", 0, E3) &amp; IF(F3="x", 0, F3) &amp; IF(G3="x", 0, G3) &amp; IF(H3="x", 0, H3) &amp; IF(I3="x", 0, I3) &amp; IF(J3="x", 0, J3), 2)</f>
+        <v>C0</v>
+      </c>
+      <c r="AA3" t="str">
+        <f t="shared" ref="AA3:AA19" si="0">BIN2HEX(IF(K3="x", 0, K3) &amp; IF(L3="x", 0, L3) &amp; IF(M3="x", 0, M3) &amp; IF(N3="x", 0, N3) &amp;  IF(Q3="x", 0, Q3) &amp; IF(S3="x", 0, S3) &amp; IF(T3="x", 0, T3) &amp; IF(U3="x", 0, U3), 2)</f>
+        <v>00</v>
+      </c>
+      <c r="AB3" t="str">
+        <f t="shared" ref="AB3:AB16" si="1">BIN2HEX(IF(V3="x", 0, V3) &amp; IF(W3="x", 0, W3) &amp; IF(X3="x", 0, X3), 2)</f>
+        <v>00</v>
+      </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
@@ -1182,6 +1240,18 @@
         <v>14</v>
       </c>
       <c r="Y4" s="3"/>
+      <c r="Z4" t="str">
+        <f t="shared" ref="Z4:Z19" si="2">BIN2HEX(IF(C4="x", 0, C4) &amp; IF(D4="x", 0, D4) &amp; IF(E4="x", 0, E4) &amp; IF(F4="x", 0, F4) &amp; IF(G4="x", 0, G4) &amp; IF(H4="x", 0, H4) &amp; IF(I4="x", 0, I4) &amp; IF(J4="x", 0, J4), 2)</f>
+        <v>60</v>
+      </c>
+      <c r="AA4" t="str">
+        <f t="shared" si="0"/>
+        <v>00</v>
+      </c>
+      <c r="AB4" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
@@ -1248,6 +1318,18 @@
         <v>14</v>
       </c>
       <c r="Y5" s="3"/>
+      <c r="Z5" t="str">
+        <f t="shared" si="2"/>
+        <v>5E</v>
+      </c>
+      <c r="AA5" t="str">
+        <f t="shared" si="0"/>
+        <v>00</v>
+      </c>
+      <c r="AB5" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
@@ -1314,6 +1396,18 @@
         <v>14</v>
       </c>
       <c r="Y6" s="3"/>
+      <c r="Z6" t="str">
+        <f t="shared" si="2"/>
+        <v>4F</v>
+      </c>
+      <c r="AA6" t="str">
+        <f t="shared" si="0"/>
+        <v>00</v>
+      </c>
+      <c r="AB6" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
@@ -1380,6 +1474,18 @@
         <v>1</v>
       </c>
       <c r="Y7" s="3"/>
+      <c r="Z7" t="str">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="AA7" t="str">
+        <f t="shared" si="0"/>
+        <v>84</v>
+      </c>
+      <c r="AB7" t="str">
+        <f>BIN2HEX(IF(V7="x", 0, V7) &amp; IF(W7="x", 0, W7) &amp; IF(X7="x", 0, X7), 2)</f>
+        <v>05</v>
+      </c>
       <c r="AD7" t="s">
         <v>79</v>
       </c>
@@ -1449,6 +1555,18 @@
         <v>0</v>
       </c>
       <c r="Y8" s="3"/>
+      <c r="Z8" t="str">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="AA8" t="str">
+        <f t="shared" si="0"/>
+        <v>83</v>
+      </c>
+      <c r="AB8" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
@@ -1515,6 +1633,18 @@
         <v>14</v>
       </c>
       <c r="Y9" s="3"/>
+      <c r="Z9" t="str">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="AA9" t="str">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="AB9" t="str">
+        <f t="shared" si="1"/>
+        <v>02</v>
+      </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -1581,6 +1711,18 @@
         <v>14</v>
       </c>
       <c r="Y10" s="3"/>
+      <c r="Z10" t="str">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="AA10" t="str">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+      <c r="AB10" t="str">
+        <f t="shared" si="1"/>
+        <v>06</v>
+      </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
@@ -1647,6 +1789,18 @@
         <v>14</v>
       </c>
       <c r="Y11" s="3"/>
+      <c r="Z11" t="str">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="AA11" t="str">
+        <f t="shared" si="0"/>
+        <v>87</v>
+      </c>
+      <c r="AB11" t="str">
+        <f t="shared" si="1"/>
+        <v>02</v>
+      </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -1713,6 +1867,18 @@
         <v>14</v>
       </c>
       <c r="Y12" s="3"/>
+      <c r="Z12" t="str">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="AA12" t="str">
+        <f t="shared" si="0"/>
+        <v>83</v>
+      </c>
+      <c r="AB12" t="str">
+        <f t="shared" si="1"/>
+        <v>02</v>
+      </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -1779,6 +1945,18 @@
         <v>14</v>
       </c>
       <c r="Y13" s="3"/>
+      <c r="Z13" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="AA13" t="str">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="AB13" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
@@ -1845,6 +2023,18 @@
         <v>14</v>
       </c>
       <c r="Y14" s="3"/>
+      <c r="Z14" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="AA14" t="str">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="AB14" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
     </row>
     <row r="15" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
@@ -1912,6 +2102,18 @@
         <v>14</v>
       </c>
       <c r="Y15" s="3"/>
+      <c r="Z15" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="AA15" t="str">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="AB15" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
     </row>
     <row r="16" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
@@ -1979,8 +2181,20 @@
         <v>14</v>
       </c>
       <c r="Y16" s="3"/>
-    </row>
-    <row r="17" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z16" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="AA16" t="str">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="AB16" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="4" t="s">
         <v>19</v>
@@ -1997,9 +2211,7 @@
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
-      <c r="Q17" s="3">
-        <v>1</v>
-      </c>
+      <c r="Q17" s="3"/>
       <c r="S17" s="3" t="s">
         <v>14</v>
       </c>
@@ -2019,8 +2231,10 @@
         <v>14</v>
       </c>
       <c r="Y17" s="3"/>
-    </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="Z17"/>
+      <c r="AA17"/>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>41</v>
       </c>
@@ -2085,8 +2299,20 @@
         <v>14</v>
       </c>
       <c r="Y18" s="3"/>
-    </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="Z18" t="str">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="AA18" t="str">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="AB18" t="str">
+        <f t="shared" ref="AB18:AB19" si="3">BIN2HEX(IF(V18="x", 0, V18) &amp; IF(W18="x", 0, W18) &amp; IF(X18="x", 0, X18), 2)</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>42</v>
       </c>
@@ -2151,8 +2377,20 @@
         <v>14</v>
       </c>
       <c r="Y19" s="3"/>
-    </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="Z19" t="str">
+        <f t="shared" si="2"/>
+        <v>09</v>
+      </c>
+      <c r="AA19" t="str">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="AB19" t="str">
+        <f t="shared" si="3"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
         <v>43</v>
       </c>
@@ -2167,7 +2405,9 @@
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
-      <c r="Q20" s="3"/>
+      <c r="Q20" s="3">
+        <v>0</v>
+      </c>
       <c r="S20" s="3"/>
       <c r="T20" s="3"/>
       <c r="U20" s="3"/>
@@ -2176,7 +2416,7 @@
       <c r="X20" s="3"/>
       <c r="Y20" s="3"/>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>44</v>
       </c>
@@ -2191,7 +2431,9 @@
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
-      <c r="Q21" s="3"/>
+      <c r="Q21" s="3">
+        <v>0</v>
+      </c>
       <c r="S21" s="3"/>
       <c r="T21" s="3"/>
       <c r="U21" s="3"/>
@@ -2200,7 +2442,7 @@
       <c r="X21" s="3"/>
       <c r="Y21" s="3"/>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>45</v>
       </c>
@@ -2215,7 +2457,9 @@
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
-      <c r="Q22" s="3"/>
+      <c r="Q22" s="3">
+        <v>0</v>
+      </c>
       <c r="S22" s="3"/>
       <c r="T22" s="3"/>
       <c r="U22" s="3"/>
@@ -2223,11 +2467,11 @@
       <c r="W22" s="3"/>
       <c r="X22" s="3"/>
       <c r="Y22" s="3"/>
-      <c r="AB22" t="s">
+      <c r="AD22" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
         <v>46</v>
       </c>
@@ -2242,7 +2486,9 @@
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
-      <c r="Q23" s="3"/>
+      <c r="Q23" s="3">
+        <v>0</v>
+      </c>
       <c r="S23" s="3"/>
       <c r="T23" s="3"/>
       <c r="U23" s="3"/>
@@ -2251,29 +2497,101 @@
       <c r="X23" s="3"/>
       <c r="Y23" s="3"/>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>10</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="AB24" t="s">
+      <c r="Q24">
+        <v>0</v>
+      </c>
+      <c r="AD24" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>11</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="AB25" t="s">
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <v>1</v>
+      </c>
+      <c r="S25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="T25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="U25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="V25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="W25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="X25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z25" t="str">
+        <f t="shared" ref="Z24:Z25" si="4">BIN2HEX(IF(C25="x", 0, C25) &amp; IF(D25="x", 0, D25) &amp; IF(E25="x", 0, E25) &amp; IF(F25="x", 0, F25) &amp; IF(G25="x", 0, G25) &amp; IF(H25="x", 0, H25) &amp; IF(I25="x", 0, I25) &amp; IF(J25="x", 0, J25), 2)</f>
+        <v>00</v>
+      </c>
+      <c r="AA25" t="str">
+        <f t="shared" ref="AA24:AA25" si="5">BIN2HEX(IF(K25="x", 0, K25) &amp; IF(L25="x", 0, L25) &amp; IF(M25="x", 0, M25) &amp; IF(N25="x", 0, N25) &amp;  IF(Q25="x", 0, Q25) &amp; IF(S25="x", 0, S25) &amp; IF(T25="x", 0, T25) &amp; IF(U25="x", 0, U25), 2)</f>
+        <v>08</v>
+      </c>
+      <c r="AB25" t="str">
+        <f t="shared" ref="AB24:AB25" si="6">BIN2HEX(IF(V25="x", 0, V25) &amp; IF(W25="x", 0, W25) &amp; IF(X25="x", 0, X25), 2)</f>
+        <v>00</v>
+      </c>
+      <c r="AD25" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
         <v>22</v>
       </c>
@@ -2281,7 +2599,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B28" s="8" t="s">
         <v>30</v>
       </c>
@@ -2289,7 +2607,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>47</v>
       </c>
@@ -2297,7 +2615,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>53</v>
       </c>
@@ -2311,6 +2629,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2475,8 +2794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2640,7 +2959,7 @@
       <c r="D20" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="15" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2658,7 +2977,7 @@
       <c r="D21" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="E21" s="14"/>
+      <c r="E21" s="15"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
@@ -2674,7 +2993,7 @@
       <c r="D22" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="E22" s="14"/>
+      <c r="E22" s="15"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
@@ -2690,7 +3009,7 @@
       <c r="D23" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="E23" s="14" t="s">
+      <c r="E23" s="15" t="s">
         <v>110</v>
       </c>
     </row>
@@ -2708,7 +3027,7 @@
       <c r="D24" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="E24" s="14"/>
+      <c r="E24" s="15"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
@@ -2724,7 +3043,7 @@
       <c r="D25" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="E25" s="14"/>
+      <c r="E25" s="15"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">

</xml_diff>

<commit_message>
v.0.11.1 - small improvements in OUT instr
</commit_message>
<xml_diff>
--- a/2nd gen - 8 bit cpu/Instruction control lines.xlsx
+++ b/2nd gen - 8 bit cpu/Instruction control lines.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Control Lines" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="178">
   <si>
     <t>LD R1, data</t>
   </si>
@@ -202,9 +202,6 @@
     <t>ST [addr], R1</t>
   </si>
   <si>
-    <t>R1 to MEM_DATA</t>
-  </si>
-  <si>
     <t>LD R1, [RR3]</t>
   </si>
   <si>
@@ -421,30 +418,18 @@
     <t>// Load value from memory, copies it to next address</t>
   </si>
   <si>
-    <t>R1 to MEM_DATA, provisorily using R2</t>
-  </si>
-  <si>
     <t>f0</t>
   </si>
   <si>
     <t>pair of 8-bit registers (as addressing is 12-bit, only lower half of the High register will be used)</t>
   </si>
   <si>
-    <t>IN R1, R2</t>
-  </si>
-  <si>
-    <t>OUT R1. R2</t>
-  </si>
-  <si>
     <t>Read byte from input selected by R2, and writes it to R1</t>
   </si>
   <si>
     <t>Write byte value of R1 in output selected in R2</t>
   </si>
   <si>
-    <t>R1 to OUT</t>
-  </si>
-  <si>
     <t>// Write letter A to LCD output</t>
   </si>
   <si>
@@ -568,7 +553,37 @@
     <t>LD B, 0x21</t>
   </si>
   <si>
-    <t>040000</t>
+    <t>output device address (0 - LCD Display; 1 - Led matrix)</t>
+  </si>
+  <si>
+    <t>input device address (0 - Keyboard)</t>
+  </si>
+  <si>
+    <t>R2 to MEM_DATA</t>
+  </si>
+  <si>
+    <t>OUT 0, B</t>
+  </si>
+  <si>
+    <t>[OD_addr]</t>
+  </si>
+  <si>
+    <t>[ID_addr]</t>
+  </si>
+  <si>
+    <t>OUT [OD_addr]. R2</t>
+  </si>
+  <si>
+    <t>IN [ID_addr], R2</t>
+  </si>
+  <si>
+    <t>literal byte value</t>
+  </si>
+  <si>
+    <t>memory address with 12 bits</t>
+  </si>
+  <si>
+    <t>R2 to OUT</t>
   </si>
 </sst>
 </file>
@@ -1006,16 +1021,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE31"/>
+  <dimension ref="A1:AE35"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AA29" sqref="AA29"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="10" width="3" customWidth="1"/>
     <col min="11" max="14" width="2.85546875" customWidth="1"/>
     <col min="15" max="15" width="2.85546875" style="6" customWidth="1"/>
@@ -1029,10 +1044,10 @@
   <sheetData>
     <row r="1" spans="1:31" s="1" customFormat="1" ht="130.5" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -1056,7 +1071,7 @@
         <v>15</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>11</v>
@@ -1068,7 +1083,7 @@
         <v>13</v>
       </c>
       <c r="N1" s="13" t="s">
-        <v>50</v>
+        <v>169</v>
       </c>
       <c r="O1" s="7" t="s">
         <v>20</v>
@@ -1077,7 +1092,7 @@
         <v>21</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>130</v>
+        <v>177</v>
       </c>
       <c r="R1" s="7"/>
       <c r="S1" s="2" t="s">
@@ -1100,7 +1115,7 @@
       </c>
       <c r="Y1" s="2"/>
       <c r="Z1" s="14" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="AA1" s="14"/>
       <c r="AB1" s="14"/>
@@ -1426,7 +1441,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C6" s="3">
         <v>0</v>
@@ -1577,7 +1592,7 @@
         <v>05</v>
       </c>
       <c r="AD7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
@@ -2407,7 +2422,7 @@
         <v>42</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C19" s="3">
         <v>0</v>
@@ -2557,9 +2572,6 @@
       <c r="W22" s="3"/>
       <c r="X22" s="3"/>
       <c r="Y22" s="3"/>
-      <c r="AD22" t="s">
-        <v>123</v>
-      </c>
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
@@ -2592,13 +2604,13 @@
         <v>10</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>126</v>
+        <v>174</v>
       </c>
       <c r="Q24">
         <v>0</v>
       </c>
       <c r="AD24" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.25">
@@ -2606,7 +2618,7 @@
         <v>11</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>127</v>
+        <v>173</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -2678,7 +2690,7 @@
         <v>00</v>
       </c>
       <c r="AD25" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.25">
@@ -2699,18 +2711,50 @@
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C30" t="s">
-        <v>48</v>
+        <v>175</v>
       </c>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="C31" t="s">
-        <v>125</v>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C34" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C35" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -2739,72 +2783,72 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="11" t="s">
         <v>57</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D3" s="11" t="s">
+      <c r="E3" s="11" t="s">
         <v>63</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C4" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="11" t="s">
-        <v>61</v>
-      </c>
       <c r="E4" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>66</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2812,67 +2856,67 @@
         <v>4</v>
       </c>
       <c r="B6" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="D6" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>71</v>
-      </c>
       <c r="E6" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" t="s">
         <v>72</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="F7" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" t="s">
         <v>77</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="F8" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" t="s">
         <v>81</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="F9" t="s">
-        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -2882,10 +2926,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E93"/>
+  <dimension ref="A1:E92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D80" sqref="D57:D80"/>
+    <sheetView topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56:XFD56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2897,17 +2941,17 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2919,10 +2963,10 @@
         <v>0x000</v>
       </c>
       <c r="C3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2934,10 +2978,10 @@
         <v>0x003</v>
       </c>
       <c r="C4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2949,10 +2993,10 @@
         <v>0x006</v>
       </c>
       <c r="C5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2964,10 +3008,10 @@
         <v>0x009</v>
       </c>
       <c r="C6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>92</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2979,15 +3023,15 @@
         <v>0x006</v>
       </c>
       <c r="C9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>87</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C16" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2999,10 +3043,10 @@
         <v>0x000</v>
       </c>
       <c r="C17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -3014,10 +3058,10 @@
         <v>0x003</v>
       </c>
       <c r="C18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -3029,10 +3073,10 @@
         <v>0x006</v>
       </c>
       <c r="C19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -3044,13 +3088,13 @@
         <v>0x009</v>
       </c>
       <c r="C20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -3062,10 +3106,10 @@
         <v>0x00C</v>
       </c>
       <c r="C21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E21" s="15"/>
     </row>
@@ -3078,10 +3122,10 @@
         <v>0x00F</v>
       </c>
       <c r="C22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E22" s="15"/>
     </row>
@@ -3094,13 +3138,13 @@
         <v>0x012</v>
       </c>
       <c r="C23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -3112,10 +3156,10 @@
         <v>0x015</v>
       </c>
       <c r="C24" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" s="11" t="s">
         <v>87</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>88</v>
       </c>
       <c r="E24" s="15"/>
     </row>
@@ -3128,10 +3172,10 @@
         <v>0x018</v>
       </c>
       <c r="C25" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E25" s="15"/>
     </row>
@@ -3144,17 +3188,17 @@
         <v>0x01B</v>
       </c>
       <c r="C26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -3166,10 +3210,10 @@
         <v>0x000</v>
       </c>
       <c r="C31" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -3181,10 +3225,10 @@
         <v>0x003</v>
       </c>
       <c r="C32" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -3196,10 +3240,10 @@
         <v>0x006</v>
       </c>
       <c r="C33" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3211,10 +3255,10 @@
         <v>0x009</v>
       </c>
       <c r="C34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -3226,10 +3270,10 @@
         <v>0x00C</v>
       </c>
       <c r="C35" t="s">
+        <v>91</v>
+      </c>
+      <c r="D35" s="11" t="s">
         <v>92</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -3241,15 +3285,15 @@
         <v>0x00F</v>
       </c>
       <c r="C36" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C40" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -3261,10 +3305,10 @@
         <v>0x000</v>
       </c>
       <c r="C41" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -3276,10 +3320,10 @@
         <v>0x003</v>
       </c>
       <c r="C42" t="s">
+        <v>118</v>
+      </c>
+      <c r="D42" s="11" t="s">
         <v>119</v>
-      </c>
-      <c r="D42" s="11" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -3291,10 +3335,10 @@
         <v>0x006</v>
       </c>
       <c r="C43" t="s">
+        <v>91</v>
+      </c>
+      <c r="D43" s="11" t="s">
         <v>92</v>
-      </c>
-      <c r="D43" s="11" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -3306,12 +3350,12 @@
         <v>0x010</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C48" s="12" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -3323,13 +3367,13 @@
         <v>0x000</v>
       </c>
       <c r="C49" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -3341,13 +3385,13 @@
         <v>0x003</v>
       </c>
       <c r="C50" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -3359,15 +3403,15 @@
         <v>0x006</v>
       </c>
       <c r="C51" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C55" s="12" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -3375,17 +3419,17 @@
         <v>0</v>
       </c>
       <c r="B56" t="str">
-        <f t="shared" ref="B56:B80" si="5">"0x" &amp; DEC2HEX(A56,3)</f>
+        <f t="shared" ref="B56:B79" si="5">"0x" &amp; DEC2HEX(A56,3)</f>
         <v>0x000</v>
       </c>
       <c r="C56" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="D56" s="11" t="s">
-        <v>172</v>
+        <v>141</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -3397,14 +3441,12 @@
         <v>0x003</v>
       </c>
       <c r="C57" t="s">
-        <v>145</v>
+        <v>170</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="E57" s="12" t="s">
-        <v>147</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="E57" s="12"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
@@ -3415,12 +3457,14 @@
         <v>0x006</v>
       </c>
       <c r="C58" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="E58" s="12"/>
+        <v>146</v>
+      </c>
+      <c r="E58" s="12" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
@@ -3431,14 +3475,12 @@
         <v>0x009</v>
       </c>
       <c r="C59" t="s">
-        <v>150</v>
+        <v>170</v>
       </c>
       <c r="D59" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="E59" s="12" t="s">
-        <v>148</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="E59" s="12"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
@@ -3449,12 +3491,14 @@
         <v>0x00C</v>
       </c>
       <c r="C60" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="D60" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="E60" s="12"/>
+        <v>148</v>
+      </c>
+      <c r="E60" s="12" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
@@ -3465,14 +3509,12 @@
         <v>0x00F</v>
       </c>
       <c r="C61" t="s">
-        <v>152</v>
+        <v>170</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E61" s="12" t="s">
-        <v>149</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="E61" s="12"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
@@ -3483,12 +3525,14 @@
         <v>0x012</v>
       </c>
       <c r="C62" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="E62" s="12"/>
+        <v>148</v>
+      </c>
+      <c r="E62" s="12" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
@@ -3499,14 +3543,12 @@
         <v>0x015</v>
       </c>
       <c r="C63" t="s">
-        <v>152</v>
+        <v>170</v>
       </c>
       <c r="D63" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E63" s="12" t="s">
-        <v>149</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="E63" s="12"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
@@ -3517,12 +3559,14 @@
         <v>0x018</v>
       </c>
       <c r="C64" t="s">
-        <v>135</v>
+        <v>151</v>
       </c>
       <c r="D64" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="E64" s="12"/>
+        <v>150</v>
+      </c>
+      <c r="E64" s="12" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
@@ -3533,14 +3577,12 @@
         <v>0x01B</v>
       </c>
       <c r="C65" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="E65" s="12" t="s">
-        <v>154</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="E65" s="12"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
@@ -3551,12 +3593,14 @@
         <v>0x01E</v>
       </c>
       <c r="C66" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
       <c r="D66" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="E66" s="12"/>
+        <v>153</v>
+      </c>
+      <c r="E66" s="12" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
@@ -3567,14 +3611,12 @@
         <v>0x021</v>
       </c>
       <c r="C67" t="s">
-        <v>157</v>
+        <v>170</v>
       </c>
       <c r="D67" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="E67" s="12" t="s">
-        <v>159</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="E67" s="12"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
@@ -3585,12 +3627,14 @@
         <v>0x024</v>
       </c>
       <c r="C68" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
       <c r="D68" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="E68" s="12"/>
+        <v>156</v>
+      </c>
+      <c r="E68" s="12" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
@@ -3601,14 +3645,12 @@
         <v>0x027</v>
       </c>
       <c r="C69" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="D69" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="E69" s="12" t="s">
-        <v>162</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="E69" s="12"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
@@ -3619,12 +3661,14 @@
         <v>0x02A</v>
       </c>
       <c r="C70" t="s">
-        <v>135</v>
+        <v>151</v>
       </c>
       <c r="D70" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="E70" s="12"/>
+        <v>150</v>
+      </c>
+      <c r="E70" s="12" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
@@ -3635,14 +3679,12 @@
         <v>0x02D</v>
       </c>
       <c r="C71" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
       <c r="D71" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="E71" s="12" t="s">
-        <v>154</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="E71" s="12"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
@@ -3653,12 +3695,14 @@
         <v>0x030</v>
       </c>
       <c r="C72" t="s">
-        <v>135</v>
+        <v>160</v>
       </c>
       <c r="D72" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="E72" s="12"/>
+        <v>159</v>
+      </c>
+      <c r="E72" s="12" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
@@ -3669,14 +3713,12 @@
         <v>0x033</v>
       </c>
       <c r="C73" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="D73" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="E73" s="12" t="s">
-        <v>163</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="E73" s="12"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
@@ -3687,12 +3729,14 @@
         <v>0x036</v>
       </c>
       <c r="C74" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="D74" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="E74" s="12"/>
+        <v>148</v>
+      </c>
+      <c r="E74" s="12" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
@@ -3703,14 +3747,12 @@
         <v>0x039</v>
       </c>
       <c r="C75" t="s">
-        <v>152</v>
+        <v>170</v>
       </c>
       <c r="D75" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E75" s="12" t="s">
-        <v>149</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="E75" s="12"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
@@ -3721,12 +3763,14 @@
         <v>0x03C</v>
       </c>
       <c r="C76" t="s">
-        <v>135</v>
+        <v>163</v>
       </c>
       <c r="D76" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="E76" s="12"/>
+        <v>162</v>
+      </c>
+      <c r="E76" s="12" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
@@ -3737,14 +3781,12 @@
         <v>0x03F</v>
       </c>
       <c r="C77" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D77" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="E77" s="12" t="s">
-        <v>166</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="E77" s="12"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78">
@@ -3755,12 +3797,14 @@
         <v>0x042</v>
       </c>
       <c r="C78" t="s">
-        <v>135</v>
+        <v>166</v>
       </c>
       <c r="D78" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="E78" s="12"/>
+        <v>165</v>
+      </c>
+      <c r="E78" s="12" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79">
@@ -3771,69 +3815,51 @@
         <v>0x045</v>
       </c>
       <c r="C79" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D79" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="E79" s="12" t="s">
-        <v>169</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="E79" s="12"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80">
-        <v>72</v>
-      </c>
-      <c r="B80" t="str">
-        <f t="shared" si="5"/>
-        <v>0x048</v>
-      </c>
-      <c r="C80" t="s">
-        <v>135</v>
-      </c>
-      <c r="D80" s="11" t="s">
-        <v>138</v>
-      </c>
       <c r="E80" s="12"/>
     </row>
-    <row r="81" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="5:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E81" s="12"/>
     </row>
-    <row r="82" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="5:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E82" s="12"/>
     </row>
-    <row r="83" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="5:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E83" s="12"/>
     </row>
-    <row r="84" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="5:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E84" s="12"/>
     </row>
-    <row r="85" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="5:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E85" s="12"/>
     </row>
-    <row r="86" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="5:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E86" s="12"/>
     </row>
-    <row r="87" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="5:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E87" s="12"/>
     </row>
-    <row r="88" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="5:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E88" s="12"/>
     </row>
-    <row r="89" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="5:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E89" s="12"/>
     </row>
-    <row r="90" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="5:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E90" s="12"/>
     </row>
-    <row r="91" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="5:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E91" s="12"/>
     </row>
-    <row r="92" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="5:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E92" s="12"/>
-    </row>
-    <row r="93" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E93" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Improvements in test programs
</commit_message>
<xml_diff>
--- a/2nd gen - 8 bit cpu/Instruction control lines.xlsx
+++ b/2nd gen - 8 bit cpu/Instruction control lines.xlsx
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="232">
   <si>
     <t>LD R1, data</t>
   </si>
@@ -595,9 +595,6 @@
     <t>R2 to OUT</t>
   </si>
   <si>
-    <t>OUT [OD_addr]. R1, R2</t>
-  </si>
-  <si>
     <t>// Write 'Hello World!' to LCD output</t>
   </si>
   <si>
@@ -607,12 +604,6 @@
     <t>//Counting in LCD output</t>
   </si>
   <si>
-    <t>JP [0x003]</t>
-  </si>
-  <si>
-    <t>2c 00 03</t>
-  </si>
-  <si>
     <t>LD A, 0x30</t>
   </si>
   <si>
@@ -622,27 +613,12 @@
     <t>// ASCII char '0'</t>
   </si>
   <si>
-    <t>// ASCII char '9'</t>
-  </si>
-  <si>
     <t>OUT 0, A</t>
   </si>
   <si>
     <t>44 00 00</t>
   </si>
   <si>
-    <t>LD B, 0x39</t>
-  </si>
-  <si>
-    <t>04 80 39</t>
-  </si>
-  <si>
-    <t>JP Z, [0x015]</t>
-  </si>
-  <si>
-    <t>30 00 15</t>
-  </si>
-  <si>
     <t>LD C, A</t>
   </si>
   <si>
@@ -652,9 +628,6 @@
     <t>// Saves the value of A register in C</t>
   </si>
   <si>
-    <t>// Restores valu of A register</t>
-  </si>
-  <si>
     <t>04 20 00</t>
   </si>
   <si>
@@ -665,6 +638,132 @@
   </si>
   <si>
     <t>// Not working. Reason: there is no C register implemented...</t>
+  </si>
+  <si>
+    <t>OUT [OD_addr], R1, R2</t>
+  </si>
+  <si>
+    <t>04 10 00</t>
+  </si>
+  <si>
+    <t>LD E, 0x1</t>
+  </si>
+  <si>
+    <t>06 00 01</t>
+  </si>
+  <si>
+    <t>ADD A, E</t>
+  </si>
+  <si>
+    <t>14 40 00</t>
+  </si>
+  <si>
+    <t>08 80 00</t>
+  </si>
+  <si>
+    <t>// Addr of first char</t>
+  </si>
+  <si>
+    <t>// Constant to use in increment</t>
+  </si>
+  <si>
+    <t>// Reads char from memory</t>
+  </si>
+  <si>
+    <t>// Print out char to LCD</t>
+  </si>
+  <si>
+    <t>// Restores value of A register</t>
+  </si>
+  <si>
+    <t>SUB A, F</t>
+  </si>
+  <si>
+    <t>// Addr of last char</t>
+  </si>
+  <si>
+    <t>LD B, 0x30</t>
+  </si>
+  <si>
+    <t>LD F, 0x3b</t>
+  </si>
+  <si>
+    <t>04 80 30</t>
+  </si>
+  <si>
+    <t>06 80 3b</t>
+  </si>
+  <si>
+    <t>// Data</t>
+  </si>
+  <si>
+    <t>48 65 6c</t>
+  </si>
+  <si>
+    <t>6c 6f 20</t>
+  </si>
+  <si>
+    <t>57 6f 72</t>
+  </si>
+  <si>
+    <t>6c 64 21</t>
+  </si>
+  <si>
+    <t>// Hel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">// lo </t>
+  </si>
+  <si>
+    <t>// Wor</t>
+  </si>
+  <si>
+    <t>// ld!</t>
+  </si>
+  <si>
+    <t>// Tests whether is the last char</t>
+  </si>
+  <si>
+    <t>LD A, [CB]</t>
+  </si>
+  <si>
+    <t>LD C, 0x00</t>
+  </si>
+  <si>
+    <t>JP Z, [0x01e]</t>
+  </si>
+  <si>
+    <t>30 00 1e</t>
+  </si>
+  <si>
+    <t>LD B, 0x40</t>
+  </si>
+  <si>
+    <t>04 80 40</t>
+  </si>
+  <si>
+    <t>// ASCII char '9' + 1</t>
+  </si>
+  <si>
+    <t>OUT 0, F</t>
+  </si>
+  <si>
+    <t>// Clear Display</t>
+  </si>
+  <si>
+    <t>// Code to clear display</t>
+  </si>
+  <si>
+    <t>30 00 18</t>
+  </si>
+  <si>
+    <t>JP Z, [0x018]</t>
+  </si>
+  <si>
+    <t>// Stops if is the last char</t>
+  </si>
+  <si>
+    <t>// next iteration of loop</t>
   </si>
 </sst>
 </file>
@@ -763,7 +862,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -798,6 +897,7 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1104,8 +1204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE35"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+    <sheetView topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AF12" sqref="AF12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1521,7 +1621,7 @@
       <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="4" t="s">
         <v>50</v>
       </c>
       <c r="C6" s="3">
@@ -2702,7 +2802,7 @@
         <v>11</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -3010,17 +3110,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E96"/>
+  <dimension ref="A1:E116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E96" sqref="E96"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E115" sqref="E115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3315,7 +3415,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>6</v>
       </c>
@@ -3330,7 +3430,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>9</v>
       </c>
@@ -3345,7 +3445,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>12</v>
       </c>
@@ -3360,7 +3460,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>15</v>
       </c>
@@ -3375,12 +3475,12 @@
         <v>115</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C40" s="12" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>0</v>
       </c>
@@ -3395,7 +3495,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>3</v>
       </c>
@@ -3410,7 +3510,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>6</v>
       </c>
@@ -3425,7 +3525,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>16</v>
       </c>
@@ -3436,8 +3536,11 @@
       <c r="D44" s="11" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44" s="12" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C48" s="12" t="s">
         <v>126</v>
       </c>
@@ -3495,7 +3598,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C55" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -3915,193 +4018,497 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C82" s="12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D82"/>
       <c r="E82" s="12"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D83"/>
+      <c r="A83">
+        <v>0</v>
+      </c>
+      <c r="B83" t="str">
+        <f>"0x" &amp; DEC2HEX(A83,3)</f>
+        <v>0x000</v>
+      </c>
+      <c r="C83" t="s">
+        <v>219</v>
+      </c>
       <c r="E83" s="12"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C84" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="D84"/>
-      <c r="E84" s="12"/>
+      <c r="A84">
+        <v>3</v>
+      </c>
+      <c r="B84" t="str">
+        <f>"0x" &amp; DEC2HEX(A84,3)</f>
+        <v>0x003</v>
+      </c>
+      <c r="C84" t="s">
+        <v>204</v>
+      </c>
+      <c r="D84" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="E84" s="12" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B85" t="str">
-        <f t="shared" ref="B85:B94" si="6">"0x" &amp; DEC2HEX(A85,3)</f>
-        <v>0x000</v>
+        <f>"0x" &amp; DEC2HEX(A85,3)</f>
+        <v>0x006</v>
       </c>
       <c r="C85" t="s">
-        <v>181</v>
+        <v>205</v>
       </c>
       <c r="D85" s="11" t="s">
-        <v>182</v>
+        <v>207</v>
       </c>
       <c r="E85" s="12" t="s">
-        <v>183</v>
+        <v>203</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B86" t="str">
-        <f t="shared" si="6"/>
-        <v>0x003</v>
+        <f>"0x" &amp; DEC2HEX(A86,3)</f>
+        <v>0x009</v>
       </c>
       <c r="C86" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="D86" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="E86" s="12"/>
+        <v>193</v>
+      </c>
+      <c r="E86" s="12" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B87" t="str">
-        <f t="shared" si="6"/>
-        <v>0x006</v>
+        <f>"0x" &amp; DEC2HEX(A87,3)</f>
+        <v>0x00C</v>
       </c>
       <c r="C87" t="s">
-        <v>83</v>
-      </c>
-      <c r="D87" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="E87" s="12"/>
+        <v>218</v>
+      </c>
+      <c r="D87"/>
+      <c r="E87" s="12" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B88" t="str">
-        <f t="shared" si="6"/>
-        <v>0x009</v>
+        <f>"0x" &amp; DEC2HEX(A88,3)</f>
+        <v>0x00F</v>
       </c>
       <c r="C88" t="s">
-        <v>85</v>
-      </c>
-      <c r="D88" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="E88" s="12"/>
+        <v>181</v>
+      </c>
+      <c r="D88" t="s">
+        <v>182</v>
+      </c>
+      <c r="E88" s="12" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B89" t="str">
-        <f t="shared" si="6"/>
-        <v>0x00C</v>
+        <f>"0x" &amp; DEC2HEX(A89,3)</f>
+        <v>0x012</v>
       </c>
       <c r="C89" t="s">
+        <v>61</v>
+      </c>
+      <c r="D89" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="D89" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="E89" s="12" t="s">
-        <v>193</v>
-      </c>
+      <c r="E89" s="12"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B90" t="str">
-        <f t="shared" si="6"/>
-        <v>0x00F</v>
+        <f>"0x" &amp; DEC2HEX(A90,3)</f>
+        <v>0x015</v>
       </c>
       <c r="C90" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="D90" s="11" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="E90" s="12" t="s">
-        <v>184</v>
+        <v>110</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B91" t="str">
-        <f t="shared" si="6"/>
-        <v>0x012</v>
+        <f>"0x" &amp; DEC2HEX(A91,3)</f>
+        <v>0x018</v>
       </c>
       <c r="C91" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="D91" s="11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E91" s="12"/>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B92" t="str">
-        <f t="shared" si="6"/>
-        <v>0x015</v>
+        <f>"0x" &amp; DEC2HEX(A92,3)</f>
+        <v>0x01B</v>
       </c>
       <c r="C92" t="s">
-        <v>189</v>
-      </c>
-      <c r="D92" s="11" t="s">
-        <v>190</v>
-      </c>
-      <c r="E92" s="12"/>
+        <v>202</v>
+      </c>
+      <c r="D92"/>
+      <c r="E92" s="12" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B93" t="str">
-        <f t="shared" si="6"/>
-        <v>0x018</v>
+        <f>"0x" &amp; DEC2HEX(A93,3)</f>
+        <v>0x01E</v>
       </c>
       <c r="C93" t="s">
-        <v>192</v>
+        <v>220</v>
       </c>
       <c r="D93" s="11" t="s">
-        <v>195</v>
-      </c>
-      <c r="E93" s="12" t="s">
-        <v>194</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="E93" s="12"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94">
+        <v>33</v>
+      </c>
+      <c r="B94" t="str">
+        <f>"0x" &amp; DEC2HEX(A94,3)</f>
+        <v>0x021</v>
+      </c>
+      <c r="C94" t="s">
+        <v>99</v>
+      </c>
+      <c r="D94" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="E94" s="12"/>
+    </row>
+    <row r="95" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E95" s="12" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>48</v>
+      </c>
+      <c r="B96" t="str">
+        <f t="shared" ref="B84:B99" si="6">"0x" &amp; DEC2HEX(A96,3)</f>
+        <v>0x030</v>
+      </c>
+      <c r="D96" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="E96" s="12" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>51</v>
+      </c>
+      <c r="B97" t="str">
+        <f t="shared" si="6"/>
+        <v>0x033</v>
+      </c>
+      <c r="D97" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="E97" s="16" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>54</v>
+      </c>
+      <c r="B98" t="str">
+        <f t="shared" si="6"/>
+        <v>0x036</v>
+      </c>
+      <c r="D98" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="E98" s="12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>57</v>
+      </c>
+      <c r="B99" t="str">
+        <f t="shared" si="6"/>
+        <v>0x039</v>
+      </c>
+      <c r="D99" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="E99" s="12" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E100" s="12"/>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D101"/>
+      <c r="E101" s="12"/>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C102" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="D102"/>
+      <c r="E102" s="12"/>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>0</v>
+      </c>
+      <c r="B103" t="str">
+        <f t="shared" ref="B103:B114" si="7">"0x" &amp; DEC2HEX(A103,3)</f>
+        <v>0x000</v>
+      </c>
+      <c r="C103" t="s">
+        <v>178</v>
+      </c>
+      <c r="D103" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="E103" s="12" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>3</v>
+      </c>
+      <c r="B104" t="str">
+        <f>"0x" &amp; DEC2HEX(A104,3)</f>
+        <v>0x003</v>
+      </c>
+      <c r="C104" t="s">
+        <v>94</v>
+      </c>
+      <c r="D104" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="E104" s="12" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>6</v>
+      </c>
+      <c r="B105" t="str">
+        <f>"0x" &amp; DEC2HEX(A105,3)</f>
+        <v>0x006</v>
+      </c>
+      <c r="C105" t="s">
+        <v>181</v>
+      </c>
+      <c r="D105" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="E105" s="12"/>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>9</v>
+      </c>
+      <c r="B106" t="str">
+        <f>"0x" &amp; DEC2HEX(A106,3)</f>
+        <v>0x009</v>
+      </c>
+      <c r="C106" t="s">
+        <v>83</v>
+      </c>
+      <c r="D106" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="E106" s="12"/>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>12</v>
+      </c>
+      <c r="B107" t="str">
+        <f>"0x" &amp; DEC2HEX(A107,3)</f>
+        <v>0x00C</v>
+      </c>
+      <c r="C107" t="s">
+        <v>85</v>
+      </c>
+      <c r="D107" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="E107" s="12"/>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>15</v>
+      </c>
+      <c r="B108" t="str">
+        <f>"0x" &amp; DEC2HEX(A108,3)</f>
+        <v>0x00F</v>
+      </c>
+      <c r="C108" t="s">
+        <v>183</v>
+      </c>
+      <c r="D108" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="E108" s="12" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>18</v>
+      </c>
+      <c r="B109" t="str">
+        <f>"0x" &amp; DEC2HEX(A109,3)</f>
+        <v>0x012</v>
+      </c>
+      <c r="C109" t="s">
+        <v>222</v>
+      </c>
+      <c r="D109" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="E109" s="12" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>21</v>
+      </c>
+      <c r="B110" t="str">
+        <f>"0x" &amp; DEC2HEX(A110,3)</f>
+        <v>0x015</v>
+      </c>
+      <c r="C110" t="s">
+        <v>86</v>
+      </c>
+      <c r="D110" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="E110" s="12"/>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>24</v>
+      </c>
+      <c r="B111" t="str">
+        <f>"0x" &amp; DEC2HEX(A111,3)</f>
+        <v>0x018</v>
+      </c>
+      <c r="C111" t="s">
+        <v>229</v>
+      </c>
+      <c r="D111" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="E111" s="12" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112">
         <v>27</v>
       </c>
-      <c r="B94" t="str">
-        <f t="shared" si="6"/>
+      <c r="B112" t="str">
+        <f>"0x" &amp; DEC2HEX(A112,3)</f>
         <v>0x01B</v>
       </c>
-      <c r="C94" t="s">
-        <v>179</v>
-      </c>
-      <c r="D94" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="E94" s="12"/>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E96" t="s">
-        <v>198</v>
+      <c r="C112" t="s">
+        <v>184</v>
+      </c>
+      <c r="D112" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="E112" s="12" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>30</v>
+      </c>
+      <c r="B113" t="str">
+        <f>"0x" &amp; DEC2HEX(A113,3)</f>
+        <v>0x01E</v>
+      </c>
+      <c r="C113" t="s">
+        <v>225</v>
+      </c>
+      <c r="E113" s="12" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>33</v>
+      </c>
+      <c r="B114" t="str">
+        <f>"0x" &amp; DEC2HEX(A114,3)</f>
+        <v>0x021</v>
+      </c>
+      <c r="C114" t="s">
+        <v>91</v>
+      </c>
+      <c r="D114" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E114" s="12" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E116" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
File accidentally left out last checkin
</commit_message>
<xml_diff>
--- a/2nd gen - 8 bit cpu/Instruction control lines.xlsx
+++ b/2nd gen - 8 bit cpu/Instruction control lines.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="Control Lines" sheetId="1" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="235">
   <si>
     <t>LD R1, data</t>
   </si>
@@ -643,9 +643,6 @@
     <t>OUT [OD_addr], R1, R2</t>
   </si>
   <si>
-    <t>04 10 00</t>
-  </si>
-  <si>
     <t>LD E, 0x1</t>
   </si>
   <si>
@@ -679,21 +676,12 @@
     <t>SUB A, F</t>
   </si>
   <si>
-    <t>// Addr of last char</t>
-  </si>
-  <si>
     <t>LD B, 0x30</t>
   </si>
   <si>
-    <t>LD F, 0x3b</t>
-  </si>
-  <si>
     <t>04 80 30</t>
   </si>
   <si>
-    <t>06 80 3b</t>
-  </si>
-  <si>
     <t>// Data</t>
   </si>
   <si>
@@ -724,18 +712,6 @@
     <t>// Tests whether is the last char</t>
   </si>
   <si>
-    <t>LD A, [CB]</t>
-  </si>
-  <si>
-    <t>LD C, 0x00</t>
-  </si>
-  <si>
-    <t>JP Z, [0x01e]</t>
-  </si>
-  <si>
-    <t>30 00 1e</t>
-  </si>
-  <si>
     <t>LD B, 0x40</t>
   </si>
   <si>
@@ -764,6 +740,39 @@
   </si>
   <si>
     <t>// next iteration of loop</t>
+  </si>
+  <si>
+    <t>LD A, [?B]</t>
+  </si>
+  <si>
+    <t>10 10 00</t>
+  </si>
+  <si>
+    <t>18 50 00</t>
+  </si>
+  <si>
+    <t>JP Z, [0x01b]</t>
+  </si>
+  <si>
+    <t>30 00 1b</t>
+  </si>
+  <si>
+    <t>// If true, stops here</t>
+  </si>
+  <si>
+    <t>// If false, next loop iteration</t>
+  </si>
+  <si>
+    <t>08 10 00</t>
+  </si>
+  <si>
+    <t>06 80 3c</t>
+  </si>
+  <si>
+    <t>LD F, 0x3c</t>
+  </si>
+  <si>
+    <t>// Addr of last char + 1</t>
   </si>
 </sst>
 </file>
@@ -891,13 +900,13 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1204,8 +1213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE35"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AF12" sqref="AF12"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1295,11 +1304,11 @@
         <v>37</v>
       </c>
       <c r="Y1" s="2"/>
-      <c r="Z1" s="14" t="s">
+      <c r="Z1" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="AA1" s="14"/>
-      <c r="AB1" s="14"/>
+      <c r="AA1" s="15"/>
+      <c r="AB1" s="15"/>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
@@ -3110,10 +3119,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E116"/>
+  <dimension ref="A1:E115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E115" sqref="E115"/>
+    <sheetView topLeftCell="A73" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E84" sqref="E84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3277,7 +3286,7 @@
       <c r="D20" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="E20" s="15" t="s">
+      <c r="E20" s="16" t="s">
         <v>100</v>
       </c>
     </row>
@@ -3295,7 +3304,7 @@
       <c r="D21" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="E21" s="15"/>
+      <c r="E21" s="16"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
@@ -3311,7 +3320,7 @@
       <c r="D22" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="E22" s="15"/>
+      <c r="E22" s="16"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
@@ -3327,7 +3336,7 @@
       <c r="D23" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="E23" s="15" t="s">
+      <c r="E23" s="16" t="s">
         <v>109</v>
       </c>
     </row>
@@ -3345,7 +3354,7 @@
       <c r="D24" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="E24" s="15"/>
+      <c r="E24" s="16"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
@@ -3361,7 +3370,7 @@
       <c r="D25" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="E25" s="15"/>
+      <c r="E25" s="16"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
@@ -3537,7 +3546,7 @@
         <v>122</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -4028,30 +4037,35 @@
         <v>0</v>
       </c>
       <c r="B83" t="str">
-        <f>"0x" &amp; DEC2HEX(A83,3)</f>
+        <f t="shared" ref="B83:B93" si="6">"0x" &amp; DEC2HEX(A83,3)</f>
         <v>0x000</v>
       </c>
       <c r="C83" t="s">
-        <v>219</v>
-      </c>
-      <c r="E83" s="12"/>
+        <v>202</v>
+      </c>
+      <c r="D83" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="E83" s="12" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>3</v>
       </c>
       <c r="B84" t="str">
-        <f>"0x" &amp; DEC2HEX(A84,3)</f>
+        <f t="shared" si="6"/>
         <v>0x003</v>
       </c>
       <c r="C84" t="s">
-        <v>204</v>
+        <v>233</v>
       </c>
       <c r="D84" s="11" t="s">
-        <v>206</v>
+        <v>232</v>
       </c>
       <c r="E84" s="12" t="s">
-        <v>197</v>
+        <v>234</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -4059,17 +4073,17 @@
         <v>6</v>
       </c>
       <c r="B85" t="str">
-        <f>"0x" &amp; DEC2HEX(A85,3)</f>
+        <f t="shared" si="6"/>
         <v>0x006</v>
       </c>
       <c r="C85" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="D85" s="11" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="E85" s="12" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -4077,14 +4091,14 @@
         <v>9</v>
       </c>
       <c r="B86" t="str">
-        <f>"0x" &amp; DEC2HEX(A86,3)</f>
+        <f t="shared" si="6"/>
         <v>0x009</v>
       </c>
       <c r="C86" t="s">
-        <v>192</v>
+        <v>224</v>
       </c>
       <c r="D86" s="11" t="s">
-        <v>193</v>
+        <v>225</v>
       </c>
       <c r="E86" s="12" t="s">
         <v>198</v>
@@ -4095,13 +4109,15 @@
         <v>12</v>
       </c>
       <c r="B87" t="str">
-        <f>"0x" &amp; DEC2HEX(A87,3)</f>
+        <f t="shared" si="6"/>
         <v>0x00C</v>
       </c>
       <c r="C87" t="s">
-        <v>218</v>
-      </c>
-      <c r="D87"/>
+        <v>181</v>
+      </c>
+      <c r="D87" t="s">
+        <v>182</v>
+      </c>
       <c r="E87" s="12" t="s">
         <v>199</v>
       </c>
@@ -4111,83 +4127,85 @@
         <v>15</v>
       </c>
       <c r="B88" t="str">
-        <f>"0x" &amp; DEC2HEX(A88,3)</f>
+        <f t="shared" si="6"/>
         <v>0x00F</v>
       </c>
       <c r="C88" t="s">
-        <v>181</v>
-      </c>
-      <c r="D88" t="s">
-        <v>182</v>
-      </c>
-      <c r="E88" s="12" t="s">
-        <v>200</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="D88" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="E88" s="12"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>18</v>
       </c>
       <c r="B89" t="str">
-        <f>"0x" &amp; DEC2HEX(A89,3)</f>
+        <f t="shared" si="6"/>
         <v>0x012</v>
       </c>
       <c r="C89" t="s">
-        <v>61</v>
+        <v>193</v>
       </c>
       <c r="D89" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="E89" s="12"/>
+        <v>194</v>
+      </c>
+      <c r="E89" s="12" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>21</v>
       </c>
       <c r="B90" t="str">
-        <f>"0x" &amp; DEC2HEX(A90,3)</f>
+        <f t="shared" si="6"/>
         <v>0x015</v>
       </c>
       <c r="C90" t="s">
-        <v>194</v>
+        <v>64</v>
       </c>
       <c r="D90" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="E90" s="12" t="s">
-        <v>110</v>
-      </c>
+      <c r="E90" s="12"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>24</v>
       </c>
       <c r="B91" t="str">
-        <f>"0x" &amp; DEC2HEX(A91,3)</f>
+        <f t="shared" si="6"/>
         <v>0x018</v>
       </c>
       <c r="C91" t="s">
-        <v>64</v>
+        <v>201</v>
       </c>
       <c r="D91" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="E91" s="12"/>
+        <v>226</v>
+      </c>
+      <c r="E91" s="12" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>27</v>
       </c>
       <c r="B92" t="str">
-        <f>"0x" &amp; DEC2HEX(A92,3)</f>
+        <f t="shared" si="6"/>
         <v>0x01B</v>
       </c>
       <c r="C92" t="s">
-        <v>202</v>
-      </c>
-      <c r="D92"/>
+        <v>227</v>
+      </c>
+      <c r="D92" s="11" t="s">
+        <v>228</v>
+      </c>
       <c r="E92" s="12" t="s">
-        <v>217</v>
+        <v>229</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -4195,319 +4213,305 @@
         <v>30</v>
       </c>
       <c r="B93" t="str">
-        <f>"0x" &amp; DEC2HEX(A93,3)</f>
+        <f t="shared" si="6"/>
         <v>0x01E</v>
       </c>
       <c r="C93" t="s">
-        <v>220</v>
+        <v>99</v>
       </c>
       <c r="D93" s="11" t="s">
-        <v>221</v>
-      </c>
-      <c r="E93" s="12"/>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94">
-        <v>33</v>
-      </c>
-      <c r="B94" t="str">
-        <f>"0x" &amp; DEC2HEX(A94,3)</f>
-        <v>0x021</v>
-      </c>
-      <c r="C94" t="s">
-        <v>99</v>
-      </c>
-      <c r="D94" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="E94" s="12"/>
-    </row>
-    <row r="95" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E93" s="12" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E94" s="12" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>48</v>
+      </c>
+      <c r="B95" t="str">
+        <f t="shared" ref="B95:B98" si="7">"0x" &amp; DEC2HEX(A95,3)</f>
+        <v>0x030</v>
+      </c>
+      <c r="D95" s="11" t="s">
+        <v>205</v>
+      </c>
       <c r="E95" s="12" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B96" t="str">
-        <f t="shared" ref="B84:B99" si="6">"0x" &amp; DEC2HEX(A96,3)</f>
-        <v>0x030</v>
+        <f t="shared" si="7"/>
+        <v>0x033</v>
       </c>
       <c r="D96" s="11" t="s">
-        <v>209</v>
-      </c>
-      <c r="E96" s="12" t="s">
-        <v>213</v>
+        <v>206</v>
+      </c>
+      <c r="E96" s="14" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B97" t="str">
-        <f t="shared" si="6"/>
-        <v>0x033</v>
+        <f t="shared" si="7"/>
+        <v>0x036</v>
       </c>
       <c r="D97" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="E97" s="16" t="s">
-        <v>214</v>
+        <v>207</v>
+      </c>
+      <c r="E97" s="12" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B98" t="str">
-        <f t="shared" si="6"/>
-        <v>0x036</v>
+        <f t="shared" si="7"/>
+        <v>0x039</v>
       </c>
       <c r="D98" s="11" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E98" s="12" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99">
-        <v>57</v>
-      </c>
-      <c r="B99" t="str">
-        <f t="shared" si="6"/>
-        <v>0x039</v>
-      </c>
-      <c r="D99" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="E99" s="12" t="s">
-        <v>216</v>
-      </c>
+      <c r="E99" s="12"/>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D100"/>
       <c r="E100" s="12"/>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C101" s="12" t="s">
+        <v>177</v>
+      </c>
       <c r="D101"/>
       <c r="E101" s="12"/>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C102" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="D102"/>
-      <c r="E102" s="12"/>
+      <c r="A102">
+        <v>0</v>
+      </c>
+      <c r="B102" t="str">
+        <f t="shared" ref="B102" si="8">"0x" &amp; DEC2HEX(A102,3)</f>
+        <v>0x000</v>
+      </c>
+      <c r="C102" t="s">
+        <v>178</v>
+      </c>
+      <c r="D102" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="E102" s="12" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B103" t="str">
-        <f t="shared" ref="B103:B114" si="7">"0x" &amp; DEC2HEX(A103,3)</f>
-        <v>0x000</v>
+        <f t="shared" ref="B103:B113" si="9">"0x" &amp; DEC2HEX(A103,3)</f>
+        <v>0x003</v>
       </c>
       <c r="C103" t="s">
-        <v>178</v>
+        <v>94</v>
       </c>
       <c r="D103" s="11" t="s">
-        <v>179</v>
+        <v>102</v>
       </c>
       <c r="E103" s="12" t="s">
-        <v>180</v>
+        <v>219</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B104" t="str">
-        <f>"0x" &amp; DEC2HEX(A104,3)</f>
-        <v>0x003</v>
+        <f t="shared" si="9"/>
+        <v>0x006</v>
       </c>
       <c r="C104" t="s">
-        <v>94</v>
+        <v>181</v>
       </c>
       <c r="D104" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="E104" s="12" t="s">
-        <v>227</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="E104" s="12"/>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B105" t="str">
-        <f>"0x" &amp; DEC2HEX(A105,3)</f>
-        <v>0x006</v>
+        <f t="shared" si="9"/>
+        <v>0x009</v>
       </c>
       <c r="C105" t="s">
-        <v>181</v>
+        <v>83</v>
       </c>
       <c r="D105" s="11" t="s">
-        <v>182</v>
+        <v>90</v>
       </c>
       <c r="E105" s="12"/>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B106" t="str">
-        <f>"0x" &amp; DEC2HEX(A106,3)</f>
-        <v>0x009</v>
+        <f t="shared" si="9"/>
+        <v>0x00C</v>
       </c>
       <c r="C106" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D106" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E106" s="12"/>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B107" t="str">
-        <f>"0x" &amp; DEC2HEX(A107,3)</f>
-        <v>0x00C</v>
+        <f t="shared" si="9"/>
+        <v>0x00F</v>
       </c>
       <c r="C107" t="s">
-        <v>85</v>
+        <v>183</v>
       </c>
       <c r="D107" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="E107" s="12"/>
+        <v>187</v>
+      </c>
+      <c r="E107" s="12" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B108" t="str">
-        <f>"0x" &amp; DEC2HEX(A108,3)</f>
-        <v>0x00F</v>
+        <f t="shared" si="9"/>
+        <v>0x012</v>
       </c>
       <c r="C108" t="s">
-        <v>183</v>
+        <v>214</v>
       </c>
       <c r="D108" s="11" t="s">
-        <v>187</v>
+        <v>215</v>
       </c>
       <c r="E108" s="12" t="s">
-        <v>185</v>
+        <v>216</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B109" t="str">
-        <f>"0x" &amp; DEC2HEX(A109,3)</f>
-        <v>0x012</v>
+        <f t="shared" si="9"/>
+        <v>0x015</v>
       </c>
       <c r="C109" t="s">
-        <v>222</v>
+        <v>86</v>
       </c>
       <c r="D109" s="11" t="s">
-        <v>223</v>
-      </c>
-      <c r="E109" s="12" t="s">
-        <v>224</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="E109" s="12"/>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B110" t="str">
-        <f>"0x" &amp; DEC2HEX(A110,3)</f>
-        <v>0x015</v>
+        <f t="shared" si="9"/>
+        <v>0x018</v>
       </c>
       <c r="C110" t="s">
-        <v>86</v>
+        <v>221</v>
       </c>
       <c r="D110" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="E110" s="12"/>
+        <v>220</v>
+      </c>
+      <c r="E110" s="12" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B111" t="str">
-        <f>"0x" &amp; DEC2HEX(A111,3)</f>
-        <v>0x018</v>
+        <f t="shared" si="9"/>
+        <v>0x01B</v>
       </c>
       <c r="C111" t="s">
-        <v>229</v>
+        <v>184</v>
       </c>
       <c r="D111" s="11" t="s">
-        <v>228</v>
+        <v>186</v>
       </c>
       <c r="E111" s="12" t="s">
-        <v>230</v>
+        <v>200</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B112" t="str">
-        <f>"0x" &amp; DEC2HEX(A112,3)</f>
-        <v>0x01B</v>
+        <f t="shared" si="9"/>
+        <v>0x01E</v>
       </c>
       <c r="C112" t="s">
-        <v>184</v>
-      </c>
-      <c r="D112" s="11" t="s">
-        <v>186</v>
+        <v>217</v>
       </c>
       <c r="E112" s="12" t="s">
-        <v>201</v>
+        <v>218</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B113" t="str">
-        <f>"0x" &amp; DEC2HEX(A113,3)</f>
-        <v>0x01E</v>
+        <f t="shared" si="9"/>
+        <v>0x021</v>
       </c>
       <c r="C113" t="s">
-        <v>225</v>
+        <v>91</v>
+      </c>
+      <c r="D113" s="11" t="s">
+        <v>92</v>
       </c>
       <c r="E113" s="12" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114">
-        <v>33</v>
-      </c>
-      <c r="B114" t="str">
-        <f>"0x" &amp; DEC2HEX(A114,3)</f>
-        <v>0x021</v>
-      </c>
-      <c r="C114" t="s">
-        <v>91</v>
-      </c>
-      <c r="D114" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="E114" s="12" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E116" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E115" t="s">
         <v>189</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v.0.12.1 Cosmetic changes; Program to count on LCD display
</commit_message>
<xml_diff>
--- a/2nd gen - 8 bit cpu/Instruction control lines.xlsx
+++ b/2nd gen - 8 bit cpu/Instruction control lines.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Control Lines" sheetId="1" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="230">
   <si>
     <t>LD R1, data</t>
   </si>
@@ -619,27 +619,9 @@
     <t>44 00 00</t>
   </si>
   <si>
-    <t>LD C, A</t>
-  </si>
-  <si>
-    <t>LD A, C</t>
-  </si>
-  <si>
     <t>// Saves the value of A register in C</t>
   </si>
   <si>
-    <t>04 20 00</t>
-  </si>
-  <si>
-    <t>05 00 00</t>
-  </si>
-  <si>
-    <t>18 20 00</t>
-  </si>
-  <si>
-    <t>// Not working. Reason: there is no C register implemented...</t>
-  </si>
-  <si>
     <t>OUT [OD_addr], R1, R2</t>
   </si>
   <si>
@@ -712,12 +694,6 @@
     <t>// Tests whether is the last char</t>
   </si>
   <si>
-    <t>LD B, 0x40</t>
-  </si>
-  <si>
-    <t>04 80 40</t>
-  </si>
-  <si>
     <t>// ASCII char '9' + 1</t>
   </si>
   <si>
@@ -773,6 +749,15 @@
   </si>
   <si>
     <t>// Addr of last char + 1</t>
+  </si>
+  <si>
+    <t>LD B, 0x3a</t>
+  </si>
+  <si>
+    <t>04 80 3a</t>
+  </si>
+  <si>
+    <t>44 50 00</t>
   </si>
 </sst>
 </file>
@@ -1213,8 +1198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2811,7 +2796,7 @@
         <v>11</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -3119,10 +3104,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E115"/>
+  <dimension ref="A1:E113"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E84" sqref="E84"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3546,7 +3531,7 @@
         <v>122</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -4041,13 +4026,13 @@
         <v>0x000</v>
       </c>
       <c r="C83" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="D83" s="11" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="E83" s="12" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -4059,13 +4044,13 @@
         <v>0x003</v>
       </c>
       <c r="C84" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="D84" s="11" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="E84" s="12" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -4077,13 +4062,13 @@
         <v>0x006</v>
       </c>
       <c r="C85" t="s">
+        <v>185</v>
+      </c>
+      <c r="D85" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="E85" s="12" t="s">
         <v>191</v>
-      </c>
-      <c r="D85" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="E85" s="12" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -4095,13 +4080,13 @@
         <v>0x009</v>
       </c>
       <c r="C86" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="D86" s="11" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="E86" s="12" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -4119,7 +4104,7 @@
         <v>182</v>
       </c>
       <c r="E87" s="12" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -4134,7 +4119,7 @@
         <v>61</v>
       </c>
       <c r="D88" s="11" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="E88" s="12"/>
     </row>
@@ -4147,10 +4132,10 @@
         <v>0x012</v>
       </c>
       <c r="C89" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="D89" s="11" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="E89" s="12" t="s">
         <v>110</v>
@@ -4168,7 +4153,7 @@
         <v>64</v>
       </c>
       <c r="D90" s="11" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="E90" s="12"/>
     </row>
@@ -4181,13 +4166,13 @@
         <v>0x018</v>
       </c>
       <c r="C91" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="D91" s="11" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="E91" s="12" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -4199,13 +4184,13 @@
         <v>0x01B</v>
       </c>
       <c r="C92" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="D92" s="11" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="E92" s="12" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -4223,12 +4208,12 @@
         <v>107</v>
       </c>
       <c r="E93" s="12" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E94" s="12" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -4240,10 +4225,10 @@
         <v>0x030</v>
       </c>
       <c r="D95" s="11" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="E95" s="12" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -4255,10 +4240,10 @@
         <v>0x033</v>
       </c>
       <c r="D96" s="11" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="E96" s="14" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -4270,10 +4255,10 @@
         <v>0x036</v>
       </c>
       <c r="D97" s="11" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="E97" s="12" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -4285,10 +4270,10 @@
         <v>0x039</v>
       </c>
       <c r="D98" s="11" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="E98" s="12" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -4338,7 +4323,7 @@
         <v>102</v>
       </c>
       <c r="E103" s="12" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -4398,13 +4383,13 @@
         <v>0x00F</v>
       </c>
       <c r="C107" t="s">
+        <v>96</v>
+      </c>
+      <c r="D107" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="E107" s="12" t="s">
         <v>183</v>
-      </c>
-      <c r="D107" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="E107" s="12" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -4416,13 +4401,13 @@
         <v>0x012</v>
       </c>
       <c r="C108" t="s">
-        <v>214</v>
+        <v>227</v>
       </c>
       <c r="D108" s="11" t="s">
-        <v>215</v>
+        <v>228</v>
       </c>
       <c r="E108" s="12" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -4437,7 +4422,7 @@
         <v>86</v>
       </c>
       <c r="D109" s="11" t="s">
-        <v>188</v>
+        <v>87</v>
       </c>
       <c r="E109" s="12"/>
     </row>
@@ -4450,13 +4435,13 @@
         <v>0x018</v>
       </c>
       <c r="C110" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="D110" s="11" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="E110" s="12" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -4468,13 +4453,13 @@
         <v>0x01B</v>
       </c>
       <c r="C111" t="s">
-        <v>184</v>
+        <v>95</v>
       </c>
       <c r="D111" s="11" t="s">
-        <v>186</v>
+        <v>103</v>
       </c>
       <c r="E111" s="12" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -4486,10 +4471,13 @@
         <v>0x01E</v>
       </c>
       <c r="C112" t="s">
-        <v>217</v>
+        <v>209</v>
+      </c>
+      <c r="D112" t="s">
+        <v>229</v>
       </c>
       <c r="E112" s="12" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -4507,12 +4495,7 @@
         <v>92</v>
       </c>
       <c r="E113" s="12" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E115" t="s">
-        <v>189</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New test program in xlsx file / Breadboard pictures
</commit_message>
<xml_diff>
--- a/2nd gen - 8 bit cpu/Instruction control lines.xlsx
+++ b/2nd gen - 8 bit cpu/Instruction control lines.xlsx
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="246">
   <si>
     <t>LD R1, data</t>
   </si>
@@ -761,6 +761,51 @@
   </si>
   <si>
     <t>// Copy a block of memory from one place to another</t>
+  </si>
+  <si>
+    <t>// Source addr of first byte</t>
+  </si>
+  <si>
+    <t>// Source addr of last byte + 1</t>
+  </si>
+  <si>
+    <t>LD C, 0x60</t>
+  </si>
+  <si>
+    <t>// Destitation addr of first byte</t>
+  </si>
+  <si>
+    <t>ST [?C], A</t>
+  </si>
+  <si>
+    <t>// Store byte in destiny addr</t>
+  </si>
+  <si>
+    <t>// Reads byte from memory</t>
+  </si>
+  <si>
+    <t>// Increments B</t>
+  </si>
+  <si>
+    <t>JP [0x00c]</t>
+  </si>
+  <si>
+    <t>2c 00 0c</t>
+  </si>
+  <si>
+    <t>// Increments C</t>
+  </si>
+  <si>
+    <t>LD A, C</t>
+  </si>
+  <si>
+    <t>LD C, A</t>
+  </si>
+  <si>
+    <t>JP Z, [0x01e]</t>
+  </si>
+  <si>
+    <t>30 00 1e</t>
   </si>
 </sst>
 </file>
@@ -859,7 +904,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -894,6 +939,9 @@
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3107,10 +3155,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E117"/>
+  <dimension ref="A1:E132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C118" sqref="C118"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E129" sqref="E129:E131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4124,7 +4172,9 @@
       <c r="D88" s="11" t="s">
         <v>223</v>
       </c>
-      <c r="E88" s="12"/>
+      <c r="E88" s="17" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89">
@@ -4140,9 +4190,7 @@
       <c r="D89" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="E89" s="12" t="s">
-        <v>110</v>
-      </c>
+      <c r="E89" s="17"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90">
@@ -4158,7 +4206,7 @@
       <c r="D90" s="11" t="s">
         <v>189</v>
       </c>
-      <c r="E90" s="12"/>
+      <c r="E90" s="17"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91">
@@ -4506,10 +4554,263 @@
         <v>230</v>
       </c>
     </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>0</v>
+      </c>
+      <c r="B118" t="str">
+        <f t="shared" ref="B118:B123" si="10">"0x" &amp; DEC2HEX(A118,3)</f>
+        <v>0x000</v>
+      </c>
+      <c r="C118" t="s">
+        <v>196</v>
+      </c>
+      <c r="D118" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="E118" s="12" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>3</v>
+      </c>
+      <c r="B119" t="str">
+        <f t="shared" si="10"/>
+        <v>0x003</v>
+      </c>
+      <c r="C119" t="s">
+        <v>225</v>
+      </c>
+      <c r="D119" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="E119" s="12" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>6</v>
+      </c>
+      <c r="B120" t="str">
+        <f t="shared" si="10"/>
+        <v>0x006</v>
+      </c>
+      <c r="C120" t="s">
+        <v>233</v>
+      </c>
+      <c r="E120" s="12" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>9</v>
+      </c>
+      <c r="B121" t="str">
+        <f t="shared" si="10"/>
+        <v>0x009</v>
+      </c>
+      <c r="C121" t="s">
+        <v>185</v>
+      </c>
+      <c r="D121" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="E121" s="12" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>12</v>
+      </c>
+      <c r="B122" t="str">
+        <f t="shared" si="10"/>
+        <v>0x00C</v>
+      </c>
+      <c r="C122" t="s">
+        <v>216</v>
+      </c>
+      <c r="D122" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="E122" s="12" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>15</v>
+      </c>
+      <c r="B123" t="str">
+        <f t="shared" ref="B123:B132" si="11">"0x" &amp; DEC2HEX(A123,3)</f>
+        <v>0x00F</v>
+      </c>
+      <c r="C123" t="s">
+        <v>235</v>
+      </c>
+      <c r="E123" s="12" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>18</v>
+      </c>
+      <c r="B124" t="str">
+        <f t="shared" si="11"/>
+        <v>0x012</v>
+      </c>
+      <c r="C124" t="s">
+        <v>61</v>
+      </c>
+      <c r="D124" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="E124" s="17" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>21</v>
+      </c>
+      <c r="B125" t="str">
+        <f t="shared" si="11"/>
+        <v>0x015</v>
+      </c>
+      <c r="C125" t="s">
+        <v>187</v>
+      </c>
+      <c r="D125" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="E125" s="17"/>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>24</v>
+      </c>
+      <c r="B126" t="str">
+        <f t="shared" si="11"/>
+        <v>0x018</v>
+      </c>
+      <c r="C126" t="s">
+        <v>64</v>
+      </c>
+      <c r="D126" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="E126" s="17"/>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>27</v>
+      </c>
+      <c r="B127" t="str">
+        <f t="shared" si="11"/>
+        <v>0x01B</v>
+      </c>
+      <c r="C127" t="s">
+        <v>195</v>
+      </c>
+      <c r="D127" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="E127" s="12" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>30</v>
+      </c>
+      <c r="B128" t="str">
+        <f t="shared" si="11"/>
+        <v>0x01E</v>
+      </c>
+      <c r="C128" t="s">
+        <v>244</v>
+      </c>
+      <c r="D128" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="E128" s="12" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>33</v>
+      </c>
+      <c r="B129" t="str">
+        <f t="shared" si="11"/>
+        <v>0x021</v>
+      </c>
+      <c r="C129" t="s">
+        <v>242</v>
+      </c>
+      <c r="E129" s="17" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>36</v>
+      </c>
+      <c r="B130" t="str">
+        <f t="shared" si="11"/>
+        <v>0x024</v>
+      </c>
+      <c r="C130" t="s">
+        <v>187</v>
+      </c>
+      <c r="D130" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="E130" s="17"/>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>39</v>
+      </c>
+      <c r="B131" t="str">
+        <f t="shared" si="11"/>
+        <v>0x027</v>
+      </c>
+      <c r="C131" t="s">
+        <v>243</v>
+      </c>
+      <c r="E131" s="17"/>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>42</v>
+      </c>
+      <c r="B132" t="str">
+        <f t="shared" si="11"/>
+        <v>0x02A</v>
+      </c>
+      <c r="C132" t="s">
+        <v>239</v>
+      </c>
+      <c r="D132" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="E132" s="12" t="s">
+        <v>222</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
     <mergeCell ref="E20:E22"/>
     <mergeCell ref="E23:E25"/>
+    <mergeCell ref="E88:E90"/>
+    <mergeCell ref="E124:E126"/>
+    <mergeCell ref="E129:E131"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Small changes in docs
</commit_message>
<xml_diff>
--- a/2nd gen - 8 bit cpu/Instruction control lines.xlsx
+++ b/2nd gen - 8 bit cpu/Instruction control lines.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="Control Lines" sheetId="1" r:id="rId1"/>
@@ -442,9 +442,6 @@
     <t>pair of 8-bit registers (as addressing is 12-bit, only lower half of the High register will be used)</t>
   </si>
   <si>
-    <t>Read byte from input selected by R2, and writes it to R1</t>
-  </si>
-  <si>
     <t>Write byte value of R1 in output selected in R2</t>
   </si>
   <si>
@@ -806,6 +803,9 @@
   </si>
   <si>
     <t>30 00 1e</t>
+  </si>
+  <si>
+    <t>Read byte from input selected by R2, and write it to R1</t>
   </si>
 </sst>
 </file>
@@ -1249,8 +1249,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE35"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AD25" sqref="AD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1270,10 +1270,10 @@
   <sheetData>
     <row r="1" spans="1:31" s="1" customFormat="1" ht="130.5" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -1309,7 +1309,7 @@
         <v>13</v>
       </c>
       <c r="N1" s="13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O1" s="7" t="s">
         <v>20</v>
@@ -1318,7 +1318,7 @@
         <v>21</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="R1" s="7"/>
       <c r="S1" s="2" t="s">
@@ -1341,7 +1341,7 @@
       </c>
       <c r="Y1" s="2"/>
       <c r="Z1" s="15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AA1" s="15"/>
       <c r="AB1" s="15"/>
@@ -2833,13 +2833,13 @@
         <v>10</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="Q24">
         <v>0</v>
       </c>
       <c r="AD24" t="s">
-        <v>124</v>
+        <v>245</v>
       </c>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.25">
@@ -2847,7 +2847,7 @@
         <v>11</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -2919,7 +2919,7 @@
         <v>00</v>
       </c>
       <c r="AD25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.25">
@@ -2943,7 +2943,7 @@
         <v>57</v>
       </c>
       <c r="C30" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.25">
@@ -2951,7 +2951,7 @@
         <v>66</v>
       </c>
       <c r="C31" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.25">
@@ -2972,18 +2972,18 @@
     </row>
     <row r="34" spans="2:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C34" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="35" spans="2:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C35" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -3157,7 +3157,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A85" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="E129" sqref="E129:E131"/>
     </sheetView>
   </sheetViews>
@@ -3173,7 +3173,7 @@
         <v>111</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3582,12 +3582,12 @@
         <v>122</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C48" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -3599,13 +3599,13 @@
         <v>0x000</v>
       </c>
       <c r="C49" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -3617,13 +3617,13 @@
         <v>0x003</v>
       </c>
       <c r="C50" t="s">
+        <v>127</v>
+      </c>
+      <c r="D50" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="D50" s="11" t="s">
-        <v>129</v>
-      </c>
       <c r="E50" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -3635,15 +3635,15 @@
         <v>0x006</v>
       </c>
       <c r="C51" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C55" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -3655,13 +3655,13 @@
         <v>0x000</v>
       </c>
       <c r="C56" t="s">
+        <v>137</v>
+      </c>
+      <c r="D56" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="D56" s="11" t="s">
+      <c r="E56" s="12" t="s">
         <v>139</v>
-      </c>
-      <c r="E56" s="12" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -3673,10 +3673,10 @@
         <v>0x003</v>
       </c>
       <c r="C57" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E57" s="12"/>
     </row>
@@ -3689,13 +3689,13 @@
         <v>0x006</v>
       </c>
       <c r="C58" t="s">
+        <v>142</v>
+      </c>
+      <c r="D58" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="D58" s="11" t="s">
-        <v>144</v>
-      </c>
       <c r="E58" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -3707,10 +3707,10 @@
         <v>0x009</v>
       </c>
       <c r="C59" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D59" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E59" s="12"/>
     </row>
@@ -3723,13 +3723,13 @@
         <v>0x00C</v>
       </c>
       <c r="C60" t="s">
+        <v>144</v>
+      </c>
+      <c r="D60" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="D60" s="11" t="s">
-        <v>146</v>
-      </c>
       <c r="E60" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -3741,10 +3741,10 @@
         <v>0x00F</v>
       </c>
       <c r="C61" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E61" s="12"/>
     </row>
@@ -3757,13 +3757,13 @@
         <v>0x012</v>
       </c>
       <c r="C62" t="s">
+        <v>144</v>
+      </c>
+      <c r="D62" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="D62" s="11" t="s">
-        <v>146</v>
-      </c>
       <c r="E62" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -3775,10 +3775,10 @@
         <v>0x015</v>
       </c>
       <c r="C63" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D63" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E63" s="12"/>
     </row>
@@ -3791,13 +3791,13 @@
         <v>0x018</v>
       </c>
       <c r="C64" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D64" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E64" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -3809,10 +3809,10 @@
         <v>0x01B</v>
       </c>
       <c r="C65" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E65" s="12"/>
     </row>
@@ -3825,13 +3825,13 @@
         <v>0x01E</v>
       </c>
       <c r="C66" t="s">
+        <v>149</v>
+      </c>
+      <c r="D66" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="D66" s="11" t="s">
+      <c r="E66" s="12" t="s">
         <v>151</v>
-      </c>
-      <c r="E66" s="12" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -3843,10 +3843,10 @@
         <v>0x021</v>
       </c>
       <c r="C67" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D67" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E67" s="12"/>
     </row>
@@ -3859,13 +3859,13 @@
         <v>0x024</v>
       </c>
       <c r="C68" t="s">
+        <v>152</v>
+      </c>
+      <c r="D68" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="D68" s="11" t="s">
+      <c r="E68" s="12" t="s">
         <v>154</v>
-      </c>
-      <c r="E68" s="12" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -3877,10 +3877,10 @@
         <v>0x027</v>
       </c>
       <c r="C69" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D69" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E69" s="12"/>
     </row>
@@ -3893,13 +3893,13 @@
         <v>0x02A</v>
       </c>
       <c r="C70" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D70" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E70" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -3911,10 +3911,10 @@
         <v>0x02D</v>
       </c>
       <c r="C71" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D71" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E71" s="12"/>
     </row>
@@ -3927,13 +3927,13 @@
         <v>0x030</v>
       </c>
       <c r="C72" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D72" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E72" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -3945,10 +3945,10 @@
         <v>0x033</v>
       </c>
       <c r="C73" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D73" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E73" s="12"/>
     </row>
@@ -3961,13 +3961,13 @@
         <v>0x036</v>
       </c>
       <c r="C74" t="s">
+        <v>144</v>
+      </c>
+      <c r="D74" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="D74" s="11" t="s">
-        <v>146</v>
-      </c>
       <c r="E74" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -3979,10 +3979,10 @@
         <v>0x039</v>
       </c>
       <c r="C75" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D75" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E75" s="12"/>
     </row>
@@ -3995,13 +3995,13 @@
         <v>0x03C</v>
       </c>
       <c r="C76" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D76" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E76" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -4013,10 +4013,10 @@
         <v>0x03F</v>
       </c>
       <c r="C77" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D77" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E77" s="12"/>
     </row>
@@ -4029,13 +4029,13 @@
         <v>0x042</v>
       </c>
       <c r="C78" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D78" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E78" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -4047,10 +4047,10 @@
         <v>0x045</v>
       </c>
       <c r="C79" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D79" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E79" s="12"/>
     </row>
@@ -4063,7 +4063,7 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C82" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D82"/>
       <c r="E82" s="12"/>
@@ -4077,13 +4077,13 @@
         <v>0x000</v>
       </c>
       <c r="C83" t="s">
+        <v>195</v>
+      </c>
+      <c r="D83" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="D83" s="11" t="s">
-        <v>197</v>
-      </c>
       <c r="E83" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -4095,13 +4095,13 @@
         <v>0x003</v>
       </c>
       <c r="C84" t="s">
+        <v>224</v>
+      </c>
+      <c r="D84" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="E84" s="12" t="s">
         <v>225</v>
-      </c>
-      <c r="D84" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="E84" s="12" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -4113,13 +4113,13 @@
         <v>0x006</v>
       </c>
       <c r="C85" t="s">
+        <v>184</v>
+      </c>
+      <c r="D85" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="D85" s="11" t="s">
-        <v>186</v>
-      </c>
       <c r="E85" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -4131,13 +4131,13 @@
         <v>0x009</v>
       </c>
       <c r="C86" t="s">
+        <v>215</v>
+      </c>
+      <c r="D86" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="D86" s="11" t="s">
-        <v>217</v>
-      </c>
       <c r="E86" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -4149,13 +4149,13 @@
         <v>0x00C</v>
       </c>
       <c r="C87" t="s">
+        <v>180</v>
+      </c>
+      <c r="D87" t="s">
         <v>181</v>
       </c>
-      <c r="D87" t="s">
-        <v>182</v>
-      </c>
       <c r="E87" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -4170,10 +4170,10 @@
         <v>61</v>
       </c>
       <c r="D88" s="11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E88" s="17" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -4185,10 +4185,10 @@
         <v>0x012</v>
       </c>
       <c r="C89" t="s">
+        <v>186</v>
+      </c>
+      <c r="D89" s="11" t="s">
         <v>187</v>
-      </c>
-      <c r="D89" s="11" t="s">
-        <v>188</v>
       </c>
       <c r="E89" s="17"/>
     </row>
@@ -4204,7 +4204,7 @@
         <v>64</v>
       </c>
       <c r="D90" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E90" s="17"/>
     </row>
@@ -4217,13 +4217,13 @@
         <v>0x018</v>
       </c>
       <c r="C91" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D91" s="11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E91" s="12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -4235,13 +4235,13 @@
         <v>0x01B</v>
       </c>
       <c r="C92" t="s">
+        <v>218</v>
+      </c>
+      <c r="D92" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="D92" s="11" t="s">
+      <c r="E92" s="12" t="s">
         <v>220</v>
-      </c>
-      <c r="E92" s="12" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -4259,12 +4259,12 @@
         <v>107</v>
       </c>
       <c r="E93" s="12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E94" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -4276,10 +4276,10 @@
         <v>0x030</v>
       </c>
       <c r="D95" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E95" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -4291,10 +4291,10 @@
         <v>0x033</v>
       </c>
       <c r="D96" s="11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E96" s="14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -4306,10 +4306,10 @@
         <v>0x036</v>
       </c>
       <c r="D97" s="11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E97" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -4321,10 +4321,10 @@
         <v>0x039</v>
       </c>
       <c r="D98" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E98" s="12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -4336,7 +4336,7 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C101" s="12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D101"/>
       <c r="E101" s="12"/>
@@ -4350,13 +4350,13 @@
         <v>0x000</v>
       </c>
       <c r="C102" t="s">
+        <v>177</v>
+      </c>
+      <c r="D102" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="D102" s="11" t="s">
+      <c r="E102" s="12" t="s">
         <v>179</v>
-      </c>
-      <c r="E102" s="12" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -4374,7 +4374,7 @@
         <v>102</v>
       </c>
       <c r="E103" s="12" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -4386,10 +4386,10 @@
         <v>0x006</v>
       </c>
       <c r="C104" t="s">
+        <v>180</v>
+      </c>
+      <c r="D104" s="11" t="s">
         <v>181</v>
-      </c>
-      <c r="D104" s="11" t="s">
-        <v>182</v>
       </c>
       <c r="E104" s="12"/>
     </row>
@@ -4440,7 +4440,7 @@
         <v>106</v>
       </c>
       <c r="E107" s="12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -4452,13 +4452,13 @@
         <v>0x012</v>
       </c>
       <c r="C108" t="s">
+        <v>226</v>
+      </c>
+      <c r="D108" s="11" t="s">
         <v>227</v>
       </c>
-      <c r="D108" s="11" t="s">
-        <v>228</v>
-      </c>
       <c r="E108" s="12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -4486,13 +4486,13 @@
         <v>0x018</v>
       </c>
       <c r="C110" t="s">
+        <v>212</v>
+      </c>
+      <c r="D110" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="E110" s="12" t="s">
         <v>213</v>
-      </c>
-      <c r="D110" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="E110" s="12" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -4510,7 +4510,7 @@
         <v>103</v>
       </c>
       <c r="E111" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -4522,13 +4522,13 @@
         <v>0x01E</v>
       </c>
       <c r="C112" t="s">
+        <v>208</v>
+      </c>
+      <c r="D112" t="s">
+        <v>228</v>
+      </c>
+      <c r="E112" s="12" t="s">
         <v>209</v>
-      </c>
-      <c r="D112" t="s">
-        <v>229</v>
-      </c>
-      <c r="E112" s="12" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -4546,12 +4546,12 @@
         <v>92</v>
       </c>
       <c r="E113" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C117" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -4559,17 +4559,17 @@
         <v>0</v>
       </c>
       <c r="B118" t="str">
-        <f t="shared" ref="B118:B123" si="10">"0x" &amp; DEC2HEX(A118,3)</f>
+        <f t="shared" ref="B118:B122" si="10">"0x" &amp; DEC2HEX(A118,3)</f>
         <v>0x000</v>
       </c>
       <c r="C118" t="s">
+        <v>195</v>
+      </c>
+      <c r="D118" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="D118" s="11" t="s">
-        <v>197</v>
-      </c>
       <c r="E118" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -4581,13 +4581,13 @@
         <v>0x003</v>
       </c>
       <c r="C119" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D119" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E119" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -4599,10 +4599,10 @@
         <v>0x006</v>
       </c>
       <c r="C120" t="s">
+        <v>232</v>
+      </c>
+      <c r="E120" s="12" t="s">
         <v>233</v>
-      </c>
-      <c r="E120" s="12" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -4614,13 +4614,13 @@
         <v>0x009</v>
       </c>
       <c r="C121" t="s">
+        <v>184</v>
+      </c>
+      <c r="D121" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="D121" s="11" t="s">
-        <v>186</v>
-      </c>
       <c r="E121" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -4632,13 +4632,13 @@
         <v>0x00C</v>
       </c>
       <c r="C122" t="s">
+        <v>215</v>
+      </c>
+      <c r="D122" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="D122" s="11" t="s">
-        <v>217</v>
-      </c>
       <c r="E122" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
@@ -4650,10 +4650,10 @@
         <v>0x00F</v>
       </c>
       <c r="C123" t="s">
+        <v>234</v>
+      </c>
+      <c r="E123" s="12" t="s">
         <v>235</v>
-      </c>
-      <c r="E123" s="12" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
@@ -4668,10 +4668,10 @@
         <v>61</v>
       </c>
       <c r="D124" s="11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E124" s="17" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
@@ -4683,10 +4683,10 @@
         <v>0x015</v>
       </c>
       <c r="C125" t="s">
+        <v>186</v>
+      </c>
+      <c r="D125" s="11" t="s">
         <v>187</v>
-      </c>
-      <c r="D125" s="11" t="s">
-        <v>188</v>
       </c>
       <c r="E125" s="17"/>
     </row>
@@ -4702,7 +4702,7 @@
         <v>64</v>
       </c>
       <c r="D126" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E126" s="17"/>
     </row>
@@ -4715,13 +4715,13 @@
         <v>0x01B</v>
       </c>
       <c r="C127" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D127" s="11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E127" s="12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -4733,13 +4733,13 @@
         <v>0x01E</v>
       </c>
       <c r="C128" t="s">
+        <v>243</v>
+      </c>
+      <c r="D128" s="11" t="s">
         <v>244</v>
       </c>
-      <c r="D128" s="11" t="s">
-        <v>245</v>
-      </c>
       <c r="E128" s="12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -4751,10 +4751,10 @@
         <v>0x021</v>
       </c>
       <c r="C129" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E129" s="17" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
@@ -4766,10 +4766,10 @@
         <v>0x024</v>
       </c>
       <c r="C130" t="s">
+        <v>186</v>
+      </c>
+      <c r="D130" s="11" t="s">
         <v>187</v>
-      </c>
-      <c r="D130" s="11" t="s">
-        <v>188</v>
       </c>
       <c r="E130" s="17"/>
     </row>
@@ -4782,7 +4782,7 @@
         <v>0x027</v>
       </c>
       <c r="C131" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E131" s="17"/>
     </row>
@@ -4795,13 +4795,13 @@
         <v>0x02A</v>
       </c>
       <c r="C132" t="s">
+        <v>238</v>
+      </c>
+      <c r="D132" s="11" t="s">
         <v>239</v>
       </c>
-      <c r="D132" s="11" t="s">
-        <v>240</v>
-      </c>
       <c r="E132" s="12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v.0.13.0 Big changes (not working yet)
</commit_message>
<xml_diff>
--- a/2nd gen - 8 bit cpu/Instruction control lines.xlsx
+++ b/2nd gen - 8 bit cpu/Instruction control lines.xlsx
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="275">
   <si>
     <t>LD R1, data</t>
   </si>
@@ -931,6 +931,9 @@
   </si>
   <si>
     <t>38 20 00</t>
+  </si>
+  <si>
+    <t>SUB A, E</t>
   </si>
 </sst>
 </file>
@@ -1077,29 +1080,11 @@
       <alignment textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1118,6 +1103,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1426,7 +1429,7 @@
   <dimension ref="A1:AE35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="V8" sqref="V8"/>
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1516,11 +1519,11 @@
         <v>37</v>
       </c>
       <c r="Y1" s="2"/>
-      <c r="Z1" s="15" t="s">
+      <c r="Z1" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="AA1" s="15"/>
-      <c r="AB1" s="15"/>
+      <c r="AA1" s="27"/>
+      <c r="AB1" s="27"/>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
@@ -3334,8 +3337,8 @@
   <dimension ref="A1:X136"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D132" sqref="D118:D132"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q3" sqref="Q3:S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3343,16 +3346,16 @@
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" style="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3" style="17" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.42578125" style="27" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" style="21" customWidth="1"/>
     <col min="13" max="14" width="9.140625" style="3"/>
     <col min="15" max="15" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.85546875" style="29" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.85546875" style="23" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="3.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3.42578125" style="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
@@ -3362,10 +3365,10 @@
       <c r="B1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="19" t="s">
         <v>252</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="20" t="s">
         <v>242</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -3380,27 +3383,27 @@
       <c r="K1" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="L1" s="30" t="s">
+      <c r="L1" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="M1" s="31" t="s">
+      <c r="M1" s="25" t="s">
         <v>245</v>
       </c>
-      <c r="N1" s="31" t="s">
+      <c r="N1" s="25" t="s">
         <v>246</v>
       </c>
-      <c r="O1" s="31" t="s">
+      <c r="O1" s="25" t="s">
         <v>248</v>
       </c>
-      <c r="P1" s="32" t="s">
+      <c r="P1" s="26" t="s">
         <v>247</v>
       </c>
-      <c r="Q1" s="23" t="s">
+      <c r="Q1" s="28" t="s">
         <v>250</v>
       </c>
-      <c r="R1" s="24"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="18"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -3408,9 +3411,9 @@
       <c r="C2" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
       <c r="U2" t="s">
         <v>257</v>
       </c>
@@ -3424,55 +3427,55 @@
         <v>0x000</v>
       </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>184</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>90</v>
       </c>
       <c r="E3" s="12"/>
-      <c r="F3" s="19">
-        <v>1</v>
-      </c>
-      <c r="G3" s="20" t="s">
-        <v>39</v>
+      <c r="F3" s="16">
+        <v>1</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>42</v>
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H5" si="0">IF(G3="", "", VLOOKUP(G3, $U$3:$V$10, 2))</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K3">
         <v>1</v>
       </c>
-      <c r="L3" s="27" t="str">
+      <c r="L3" s="21" t="str">
         <f>IF(F3="", "", TEXT(DEC2BIN(F3), "000000"))</f>
         <v>000001</v>
       </c>
-      <c r="M3" s="28" t="str">
-        <f>IF(H3="", "", TEXT(DEC2BIN(H3), "000"))</f>
-        <v>001</v>
-      </c>
-      <c r="N3" s="28" t="str">
-        <f>IF(I3="", "", TEXT(DEC2BIN(I3), "000"))</f>
+      <c r="M3" s="22" t="str">
+        <f t="shared" ref="M3:N6" si="1">IF(H3="", "", TEXT(DEC2BIN(H3), "000"))</f>
+        <v>100</v>
+      </c>
+      <c r="N3" s="22" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="O3" s="28" t="str">
-        <f>IF(J3="", "", TEXT(DEC2BIN(J3), "00000000"))</f>
+      <c r="O3" s="22" t="str">
+        <f t="shared" ref="O3:P6" si="2">IF(J3="", "", TEXT(DEC2BIN(J3), "00000000"))</f>
         <v/>
       </c>
-      <c r="P3" s="29" t="str">
-        <f>IF(K3="", "", TEXT(DEC2BIN(K3), "00000000"))</f>
+      <c r="P3" s="23" t="str">
+        <f t="shared" si="2"/>
         <v>00000001</v>
       </c>
       <c r="Q3" t="str">
-        <f t="shared" ref="Q3:Q5" si="1">BIN2HEX(LEFT(CONCATENATE(L3,IF(M3="", "000", M3)), 8), 2)</f>
-        <v>04</v>
+        <f t="shared" ref="Q3:Q5" si="3">BIN2HEX(LEFT(CONCATENATE(L3,IF(M3="", "000", M3)), 8), 2)</f>
+        <v>06</v>
       </c>
       <c r="R3" t="str">
         <f>BIN2HEX(CONCATENATE(RIGHT(M3, 1), IF(N3 = "", "000", N3), "0000"), 2)</f>
-        <v>80</v>
-      </c>
-      <c r="S3" s="21" t="str">
-        <f t="shared" ref="S3:S5" si="2">IF(O3="", BIN2HEX(P3, 2), BIN2HEX(O3,2))</f>
+        <v>00</v>
+      </c>
+      <c r="S3" s="18" t="str">
+        <f t="shared" ref="S3:S5" si="4">IF(O3="", BIN2HEX(P3, 2), BIN2HEX(O3,2))</f>
         <v>01</v>
       </c>
       <c r="U3" t="s">
@@ -3487,7 +3490,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="str">
-        <f t="shared" ref="B4:B6" si="3">"0x" &amp; DEC2HEX(A4,3)</f>
+        <f t="shared" ref="B4:B6" si="5">"0x" &amp; DEC2HEX(A4,3)</f>
         <v>0x003</v>
       </c>
       <c r="C4" t="s">
@@ -3499,10 +3502,10 @@
       <c r="E4" s="12" t="s">
         <v>249</v>
       </c>
-      <c r="F4" s="19">
-        <v>1</v>
-      </c>
-      <c r="G4" s="20" t="s">
+      <c r="F4" s="16">
+        <v>1</v>
+      </c>
+      <c r="G4" s="17" t="s">
         <v>38</v>
       </c>
       <c r="H4">
@@ -3512,36 +3515,36 @@
       <c r="K4">
         <v>32</v>
       </c>
-      <c r="L4" s="27" t="str">
+      <c r="L4" s="21" t="str">
         <f>IF(F4="", "", TEXT(DEC2BIN(F4), "000000"))</f>
         <v>000001</v>
       </c>
-      <c r="M4" s="28" t="str">
-        <f>IF(H4="", "", TEXT(DEC2BIN(H4), "000"))</f>
+      <c r="M4" s="22" t="str">
+        <f t="shared" si="1"/>
         <v>000</v>
       </c>
-      <c r="N4" s="28" t="str">
-        <f>IF(I4="", "", TEXT(DEC2BIN(I4), "000"))</f>
+      <c r="N4" s="22" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="O4" s="28" t="str">
-        <f>IF(J4="", "", TEXT(DEC2BIN(J4), "00000000"))</f>
+      <c r="O4" s="22" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="P4" s="29" t="str">
-        <f>IF(K4="", "", TEXT(DEC2BIN(K4), "00000000"))</f>
+      <c r="P4" s="23" t="str">
+        <f t="shared" si="2"/>
         <v>00100000</v>
       </c>
       <c r="Q4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>04</v>
       </c>
       <c r="R4" t="str">
         <f>BIN2HEX(CONCATENATE(RIGHT(M4, 1), IF(N4 = "", "000", N4), "0000"), 2)</f>
         <v>00</v>
       </c>
-      <c r="S4" s="21" t="str">
-        <f t="shared" si="2"/>
+      <c r="S4" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="U4" t="s">
@@ -3556,20 +3559,20 @@
         <v>6</v>
       </c>
       <c r="B5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0x006</v>
       </c>
       <c r="C5" t="s">
-        <v>85</v>
+        <v>186</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>88</v>
       </c>
       <c r="E5" s="12"/>
-      <c r="F5" s="19">
+      <c r="F5" s="16">
         <v>5</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="17" t="s">
         <v>38</v>
       </c>
       <c r="H5">
@@ -3577,38 +3580,38 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="L5" s="27" t="str">
+        <v>4</v>
+      </c>
+      <c r="L5" s="21" t="str">
         <f>IF(F5="", "", TEXT(DEC2BIN(F5), "000000"))</f>
         <v>000101</v>
       </c>
-      <c r="M5" s="28" t="str">
-        <f>IF(H5="", "", TEXT(DEC2BIN(H5), "000"))</f>
+      <c r="M5" s="22" t="str">
+        <f t="shared" si="1"/>
         <v>000</v>
       </c>
-      <c r="N5" s="28" t="str">
-        <f>IF(I5="", "", TEXT(DEC2BIN(I5), "000"))</f>
-        <v>001</v>
-      </c>
-      <c r="O5" s="28" t="str">
-        <f>IF(J5="", "", TEXT(DEC2BIN(J5), "00000000"))</f>
+      <c r="N5" s="22" t="str">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="O5" s="22" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="P5" s="29" t="str">
-        <f>IF(K5="", "", TEXT(DEC2BIN(K5), "00000000"))</f>
+      <c r="P5" s="23" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="Q5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="R5" t="str">
         <f>BIN2HEX(CONCATENATE(RIGHT(M5, 1), IF(N5 = "", "000", N5), "0000"), 2)</f>
-        <v>10</v>
-      </c>
-      <c r="S5" s="21" t="str">
-        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="S5" s="18" t="str">
+        <f t="shared" si="4"/>
         <v>00</v>
       </c>
       <c r="U5" t="s">
@@ -3623,7 +3626,7 @@
         <v>9</v>
       </c>
       <c r="B6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0x009</v>
       </c>
       <c r="C6" t="s">
@@ -3633,7 +3636,7 @@
         <v>92</v>
       </c>
       <c r="E6" s="12"/>
-      <c r="F6" s="19">
+      <c r="F6" s="16">
         <v>11</v>
       </c>
       <c r="H6" t="str">
@@ -3643,24 +3646,24 @@
       <c r="J6">
         <v>6</v>
       </c>
-      <c r="L6" s="27" t="str">
+      <c r="L6" s="21" t="str">
         <f>IF(F6="", "", TEXT(DEC2BIN(F6), "000000"))</f>
         <v>001011</v>
       </c>
-      <c r="M6" s="28" t="str">
-        <f>IF(H6="", "", TEXT(DEC2BIN(H6), "000"))</f>
+      <c r="M6" s="22" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="N6" s="28" t="str">
-        <f>IF(I6="", "", TEXT(DEC2BIN(I6), "000"))</f>
+      <c r="N6" s="22" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="O6" s="28" t="str">
-        <f>IF(J6="", "", TEXT(DEC2BIN(J6), "00000000"))</f>
+      <c r="O6" s="22" t="str">
+        <f t="shared" si="2"/>
         <v>00000110</v>
       </c>
-      <c r="P6" s="29" t="str">
-        <f>IF(K6="", "", TEXT(DEC2BIN(K6), "00000000"))</f>
+      <c r="P6" s="23" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="Q6" t="str">
@@ -3671,7 +3674,7 @@
         <f>BIN2HEX(CONCATENATE(RIGHT(M6, 1), IF(N6 = "", "000", N6), "0000"), 2)</f>
         <v>00</v>
       </c>
-      <c r="S6" s="21" t="str">
+      <c r="S6" s="18" t="str">
         <f>IF(O6="", BIN2HEX(P6, 2), BIN2HEX(O6,2))</f>
         <v>06</v>
       </c>
@@ -3684,9 +3687,9 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="E7" s="12"/>
-      <c r="M7" s="28"/>
-      <c r="N7" s="28"/>
-      <c r="O7" s="28"/>
+      <c r="M7" s="22"/>
+      <c r="N7" s="22"/>
+      <c r="O7" s="22"/>
       <c r="U7" t="s">
         <v>42</v>
       </c>
@@ -3712,38 +3715,38 @@
         <v>0x006</v>
       </c>
       <c r="C9" t="s">
-        <v>86</v>
+        <v>274</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>87</v>
       </c>
       <c r="E9" s="12"/>
-      <c r="F9" s="19">
+      <c r="F9" s="16">
         <v>6</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="L9" s="27" t="str">
+        <v>4</v>
+      </c>
+      <c r="L9" s="21" t="str">
         <f>IF(F9="", "", TEXT(DEC2BIN(F9), "000000"))</f>
         <v>000110</v>
       </c>
-      <c r="M9" s="28" t="str">
+      <c r="M9" s="22" t="str">
         <f>IF(H9="", "", TEXT(DEC2BIN(H9), "000"))</f>
         <v>000</v>
       </c>
-      <c r="N9" s="28" t="str">
+      <c r="N9" s="22" t="str">
         <f>IF(I9="", "", TEXT(DEC2BIN(I9), "000"))</f>
-        <v>001</v>
-      </c>
-      <c r="O9" s="28" t="str">
+        <v>100</v>
+      </c>
+      <c r="O9" s="22" t="str">
         <f>IF(J9="", "", TEXT(DEC2BIN(J9), "00000000"))</f>
         <v/>
       </c>
-      <c r="P9" s="29" t="str">
+      <c r="P9" s="23" t="str">
         <f>IF(K9="", "", TEXT(DEC2BIN(K9), "00000000"))</f>
         <v/>
       </c>
@@ -3753,9 +3756,9 @@
       </c>
       <c r="R9" t="str">
         <f>BIN2HEX(CONCATENATE(RIGHT(M9, 1), IF(N9 = "", "000", N9), "0000"), 2)</f>
-        <v>10</v>
-      </c>
-      <c r="S9" s="21" t="str">
+        <v>40</v>
+      </c>
+      <c r="S9" s="18" t="str">
         <f>IF(O9="", BIN2HEX(P9, 2), BIN2HEX(O9,2))</f>
         <v>00</v>
       </c>
@@ -3790,7 +3793,7 @@
         <v>0</v>
       </c>
       <c r="B17" t="str">
-        <f t="shared" ref="B17:B26" si="4">"0x" &amp; DEC2HEX(A17,3)</f>
+        <f t="shared" ref="B17:B26" si="6">"0x" &amp; DEC2HEX(A17,3)</f>
         <v>0x000</v>
       </c>
       <c r="C17" t="s">
@@ -3799,7 +3802,7 @@
       <c r="D17" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="F17" s="19">
+      <c r="F17" s="16">
         <v>1</v>
       </c>
       <c r="H17">
@@ -3808,24 +3811,24 @@
       <c r="K17">
         <v>1</v>
       </c>
-      <c r="L17" s="27" t="str">
+      <c r="L17" s="21" t="str">
         <f>IF(F17="", "", TEXT(DEC2BIN(F17), "000000"))</f>
         <v>000001</v>
       </c>
-      <c r="M17" s="28" t="str">
-        <f>IF(H17="", "", TEXT(DEC2BIN(H17), "000"))</f>
+      <c r="M17" s="22" t="str">
+        <f t="shared" ref="M17:N19" si="7">IF(H17="", "", TEXT(DEC2BIN(H17), "000"))</f>
         <v>001</v>
       </c>
-      <c r="N17" s="28" t="str">
-        <f>IF(I17="", "", TEXT(DEC2BIN(I17), "000"))</f>
+      <c r="N17" s="22" t="str">
+        <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="O17" s="28" t="str">
-        <f>IF(J17="", "", TEXT(DEC2BIN(J17), "00000000"))</f>
+      <c r="O17" s="22" t="str">
+        <f t="shared" ref="O17:P19" si="8">IF(J17="", "", TEXT(DEC2BIN(J17), "00000000"))</f>
         <v/>
       </c>
-      <c r="P17" s="29" t="str">
-        <f>IF(K17="", "", TEXT(DEC2BIN(K17), "00000000"))</f>
+      <c r="P17" s="23" t="str">
+        <f t="shared" si="8"/>
         <v>00000001</v>
       </c>
       <c r="Q17" t="str">
@@ -3836,7 +3839,7 @@
         <f>BIN2HEX(CONCATENATE(RIGHT(M17, 1), IF(N17 = "", "000", N17), "0000"), 2)</f>
         <v>80</v>
       </c>
-      <c r="S17" s="21" t="str">
+      <c r="S17" s="18" t="str">
         <f>IF(O17="", BIN2HEX(P17, 2), BIN2HEX(O17,2))</f>
         <v>01</v>
       </c>
@@ -3859,7 +3862,7 @@
         <v>3</v>
       </c>
       <c r="B18" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0x003</v>
       </c>
       <c r="C18" t="s">
@@ -3868,7 +3871,7 @@
       <c r="D18" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="F18" s="19">
+      <c r="F18" s="16">
         <v>1</v>
       </c>
       <c r="H18">
@@ -3877,24 +3880,24 @@
       <c r="K18">
         <v>0</v>
       </c>
-      <c r="L18" s="27" t="str">
+      <c r="L18" s="21" t="str">
         <f>IF(F18="", "", TEXT(DEC2BIN(F18), "000000"))</f>
         <v>000001</v>
       </c>
-      <c r="M18" s="28" t="str">
-        <f>IF(H18="", "", TEXT(DEC2BIN(H18), "000"))</f>
+      <c r="M18" s="22" t="str">
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
-      <c r="N18" s="28" t="str">
-        <f>IF(I18="", "", TEXT(DEC2BIN(I18), "000"))</f>
+      <c r="N18" s="22" t="str">
+        <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="O18" s="28" t="str">
-        <f>IF(J18="", "", TEXT(DEC2BIN(J18), "00000000"))</f>
+      <c r="O18" s="22" t="str">
+        <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="P18" s="29" t="str">
-        <f>IF(K18="", "", TEXT(DEC2BIN(K18), "00000000"))</f>
+      <c r="P18" s="23" t="str">
+        <f t="shared" si="8"/>
         <v>00000000</v>
       </c>
       <c r="Q18" t="str">
@@ -3905,7 +3908,7 @@
         <f>BIN2HEX(CONCATENATE(RIGHT(M18, 1), IF(N18 = "", "000", N18), "0000"), 2)</f>
         <v>00</v>
       </c>
-      <c r="S18" s="21" t="str">
+      <c r="S18" s="18" t="str">
         <f>IF(O18="", BIN2HEX(P18, 2), BIN2HEX(O18,2))</f>
         <v>00</v>
       </c>
@@ -3921,7 +3924,7 @@
         <v>6</v>
       </c>
       <c r="B19" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0x006</v>
       </c>
       <c r="C19" t="s">
@@ -3930,7 +3933,7 @@
       <c r="D19" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="F19" s="19">
+      <c r="F19" s="16">
         <v>1</v>
       </c>
       <c r="H19">
@@ -3939,24 +3942,24 @@
       <c r="K19">
         <v>255</v>
       </c>
-      <c r="L19" s="27" t="str">
+      <c r="L19" s="21" t="str">
         <f>IF(F19="", "", TEXT(DEC2BIN(F19), "000000"))</f>
         <v>000001</v>
       </c>
-      <c r="M19" s="28" t="str">
-        <f>IF(H19="", "", TEXT(DEC2BIN(H19), "000"))</f>
+      <c r="M19" s="22" t="str">
+        <f t="shared" si="7"/>
         <v>101</v>
       </c>
-      <c r="N19" s="28" t="str">
-        <f>IF(I19="", "", TEXT(DEC2BIN(I19), "000"))</f>
+      <c r="N19" s="22" t="str">
+        <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="O19" s="28" t="str">
-        <f>IF(J19="", "", TEXT(DEC2BIN(J19), "00000000"))</f>
+      <c r="O19" s="22" t="str">
+        <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="P19" s="29" t="str">
-        <f>IF(K19="", "", TEXT(DEC2BIN(K19), "00000000"))</f>
+      <c r="P19" s="23" t="str">
+        <f t="shared" si="8"/>
         <v>11111111</v>
       </c>
       <c r="Q19" t="str">
@@ -3967,7 +3970,7 @@
         <f>BIN2HEX(CONCATENATE(RIGHT(M19, 1), IF(N19 = "", "000", N19), "0000"), 2)</f>
         <v>80</v>
       </c>
-      <c r="S19" s="21" t="str">
+      <c r="S19" s="18" t="str">
         <f>IF(O19="", BIN2HEX(P19, 2), BIN2HEX(O19,2))</f>
         <v>FF</v>
       </c>
@@ -3977,7 +3980,7 @@
         <v>9</v>
       </c>
       <c r="B20" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0x009</v>
       </c>
       <c r="C20" t="s">
@@ -3986,7 +3989,7 @@
       <c r="D20" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="31" t="s">
         <v>100</v>
       </c>
     </row>
@@ -3995,7 +3998,7 @@
         <v>12</v>
       </c>
       <c r="B21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0x00C</v>
       </c>
       <c r="C21" t="s">
@@ -4004,14 +4007,14 @@
       <c r="D21" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="E21" s="16"/>
+      <c r="E21" s="31"/>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>15</v>
       </c>
       <c r="B22" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0x00F</v>
       </c>
       <c r="C22" t="s">
@@ -4020,14 +4023,14 @@
       <c r="D22" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="E22" s="16"/>
+      <c r="E22" s="31"/>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>18</v>
       </c>
       <c r="B23" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0x012</v>
       </c>
       <c r="C23" t="s">
@@ -4036,7 +4039,7 @@
       <c r="D23" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="E23" s="16" t="s">
+      <c r="E23" s="31" t="s">
         <v>109</v>
       </c>
     </row>
@@ -4045,7 +4048,7 @@
         <v>21</v>
       </c>
       <c r="B24" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0x015</v>
       </c>
       <c r="C24" t="s">
@@ -4054,14 +4057,14 @@
       <c r="D24" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="E24" s="16"/>
+      <c r="E24" s="31"/>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0x018</v>
       </c>
       <c r="C25" t="s">
@@ -4070,14 +4073,14 @@
       <c r="D25" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="E25" s="16"/>
+      <c r="E25" s="31"/>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>27</v>
       </c>
       <c r="B26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0x01B</v>
       </c>
       <c r="C26" t="s">
@@ -4099,7 +4102,7 @@
         <v>0</v>
       </c>
       <c r="B31" t="str">
-        <f t="shared" ref="B31:B36" si="5">"0x" &amp; DEC2HEX(A31,3)</f>
+        <f t="shared" ref="B31:B36" si="9">"0x" &amp; DEC2HEX(A31,3)</f>
         <v>0x000</v>
       </c>
       <c r="C31" t="s">
@@ -4114,7 +4117,7 @@
         <v>3</v>
       </c>
       <c r="B32" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0x003</v>
       </c>
       <c r="C32" t="s">
@@ -4129,7 +4132,7 @@
         <v>6</v>
       </c>
       <c r="B33" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0x006</v>
       </c>
       <c r="C33" t="s">
@@ -4144,7 +4147,7 @@
         <v>9</v>
       </c>
       <c r="B34" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0x009</v>
       </c>
       <c r="C34" t="s">
@@ -4153,29 +4156,29 @@
       <c r="D34" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="F34" s="19">
+      <c r="F34" s="16">
         <v>12</v>
       </c>
       <c r="J34">
         <v>15</v>
       </c>
-      <c r="L34" s="27" t="str">
+      <c r="L34" s="21" t="str">
         <f>IF(F34="", "", TEXT(DEC2BIN(F34), "000000"))</f>
         <v>001100</v>
       </c>
-      <c r="M34" s="28" t="str">
+      <c r="M34" s="22" t="str">
         <f>IF(H34="", "", TEXT(DEC2BIN(H34), "000"))</f>
         <v/>
       </c>
-      <c r="N34" s="28" t="str">
+      <c r="N34" s="22" t="str">
         <f>IF(I34="", "", TEXT(DEC2BIN(I34), "000"))</f>
         <v/>
       </c>
-      <c r="O34" s="28" t="str">
+      <c r="O34" s="22" t="str">
         <f>IF(J34="", "", TEXT(DEC2BIN(J34), "00000000"))</f>
         <v>00001111</v>
       </c>
-      <c r="P34" s="29" t="str">
+      <c r="P34" s="23" t="str">
         <f>IF(K34="", "", TEXT(DEC2BIN(K34), "00000000"))</f>
         <v/>
       </c>
@@ -4187,7 +4190,7 @@
         <f>BIN2HEX(CONCATENATE(RIGHT(M34, 1), IF(N34 = "", "000", N34), "0000"), 2)</f>
         <v>00</v>
       </c>
-      <c r="S34" s="21" t="str">
+      <c r="S34" s="18" t="str">
         <f>IF(O34="", BIN2HEX(P34, 2), BIN2HEX(O34,2))</f>
         <v>0F</v>
       </c>
@@ -4197,7 +4200,7 @@
         <v>12</v>
       </c>
       <c r="B35" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0x00C</v>
       </c>
       <c r="C35" t="s">
@@ -4206,16 +4209,16 @@
       <c r="D35" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="M35" s="28"/>
-      <c r="N35" s="28"/>
-      <c r="O35" s="28"/>
+      <c r="M35" s="22"/>
+      <c r="N35" s="22"/>
+      <c r="O35" s="22"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>15</v>
       </c>
       <c r="B36" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0x00F</v>
       </c>
       <c r="C36" t="s">
@@ -4235,7 +4238,7 @@
         <v>0</v>
       </c>
       <c r="B41" t="str">
-        <f t="shared" ref="B41:B44" si="6">"0x" &amp; DEC2HEX(A41,3)</f>
+        <f t="shared" ref="B41:B44" si="10">"0x" &amp; DEC2HEX(A41,3)</f>
         <v>0x000</v>
       </c>
       <c r="C41" t="s">
@@ -4244,42 +4247,42 @@
       <c r="D41" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="F41" s="19">
+      <c r="F41" s="16">
         <v>3</v>
       </c>
       <c r="K41">
         <v>16</v>
       </c>
-      <c r="L41" s="27" t="str">
-        <f t="shared" ref="L41:L42" si="7">IF(F41="", "", TEXT(DEC2BIN(F41), "000000"))</f>
+      <c r="L41" s="21" t="str">
+        <f t="shared" ref="L41:L42" si="11">IF(F41="", "", TEXT(DEC2BIN(F41), "000000"))</f>
         <v>000011</v>
       </c>
-      <c r="M41" s="28" t="str">
-        <f t="shared" ref="M41:M42" si="8">IF(H41="", "", TEXT(DEC2BIN(H41), "000"))</f>
+      <c r="M41" s="22" t="str">
+        <f t="shared" ref="M41:M42" si="12">IF(H41="", "", TEXT(DEC2BIN(H41), "000"))</f>
         <v/>
       </c>
-      <c r="N41" s="28" t="str">
-        <f t="shared" ref="N41:N42" si="9">IF(I41="", "", TEXT(DEC2BIN(I41), "000"))</f>
+      <c r="N41" s="22" t="str">
+        <f t="shared" ref="N41:N42" si="13">IF(I41="", "", TEXT(DEC2BIN(I41), "000"))</f>
         <v/>
       </c>
-      <c r="O41" s="28" t="str">
-        <f t="shared" ref="O41:O42" si="10">IF(J41="", "", TEXT(DEC2BIN(J41), "00000000"))</f>
+      <c r="O41" s="22" t="str">
+        <f t="shared" ref="O41:O42" si="14">IF(J41="", "", TEXT(DEC2BIN(J41), "00000000"))</f>
         <v/>
       </c>
-      <c r="P41" s="29" t="str">
-        <f t="shared" ref="P41:P42" si="11">IF(K41="", "", TEXT(DEC2BIN(K41), "00000000"))</f>
+      <c r="P41" s="23" t="str">
+        <f t="shared" ref="P41:P42" si="15">IF(K41="", "", TEXT(DEC2BIN(K41), "00000000"))</f>
         <v>00010000</v>
       </c>
       <c r="Q41" t="str">
-        <f t="shared" ref="Q41:Q42" si="12">BIN2HEX(LEFT(CONCATENATE(L41,IF(M41="", "000", M41)), 8), 2)</f>
+        <f t="shared" ref="Q41:Q42" si="16">BIN2HEX(LEFT(CONCATENATE(L41,IF(M41="", "000", M41)), 8), 2)</f>
         <v>0C</v>
       </c>
       <c r="R41" t="str">
-        <f t="shared" ref="R41:R42" si="13">BIN2HEX(CONCATENATE(RIGHT(M41, 1), IF(N41 = "", "000", N41), "0000"), 2)</f>
+        <f t="shared" ref="R41:R42" si="17">BIN2HEX(CONCATENATE(RIGHT(M41, 1), IF(N41 = "", "000", N41), "0000"), 2)</f>
         <v>00</v>
       </c>
-      <c r="S41" s="21" t="str">
-        <f t="shared" ref="S41:S42" si="14">IF(O41="", BIN2HEX(P41, 2), BIN2HEX(O41,2))</f>
+      <c r="S41" s="18" t="str">
+        <f t="shared" ref="S41:S42" si="18">IF(O41="", BIN2HEX(P41, 2), BIN2HEX(O41,2))</f>
         <v>10</v>
       </c>
     </row>
@@ -4288,7 +4291,7 @@
         <v>3</v>
       </c>
       <c r="B42" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0x003</v>
       </c>
       <c r="C42" t="s">
@@ -4297,7 +4300,7 @@
       <c r="D42" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="F42" s="19">
+      <c r="F42" s="16">
         <v>13</v>
       </c>
       <c r="H42">
@@ -4306,36 +4309,36 @@
       <c r="J42">
         <v>17</v>
       </c>
-      <c r="L42" s="27" t="str">
-        <f t="shared" si="7"/>
+      <c r="L42" s="21" t="str">
+        <f t="shared" si="11"/>
         <v>001101</v>
       </c>
-      <c r="M42" s="28" t="str">
-        <f t="shared" si="8"/>
+      <c r="M42" s="22" t="str">
+        <f t="shared" si="12"/>
         <v>000</v>
       </c>
-      <c r="N42" s="28" t="str">
-        <f t="shared" si="9"/>
+      <c r="N42" s="22" t="str">
+        <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="O42" s="28" t="str">
-        <f t="shared" si="10"/>
+      <c r="O42" s="22" t="str">
+        <f t="shared" si="14"/>
         <v>00010001</v>
       </c>
-      <c r="P42" s="29" t="str">
-        <f t="shared" si="11"/>
+      <c r="P42" s="23" t="str">
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="Q42" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>34</v>
       </c>
       <c r="R42" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>00</v>
       </c>
-      <c r="S42" s="21" t="str">
-        <f t="shared" si="14"/>
+      <c r="S42" s="18" t="str">
+        <f t="shared" si="18"/>
         <v>11</v>
       </c>
     </row>
@@ -4344,7 +4347,7 @@
         <v>6</v>
       </c>
       <c r="B43" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0x006</v>
       </c>
       <c r="C43" t="s">
@@ -4359,7 +4362,7 @@
         <v>16</v>
       </c>
       <c r="B44" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0x010</v>
       </c>
       <c r="D44" s="11" t="s">
@@ -4379,7 +4382,7 @@
         <v>0</v>
       </c>
       <c r="B49" t="str">
-        <f t="shared" ref="B49:B51" si="15">"0x" &amp; DEC2HEX(A49,3)</f>
+        <f t="shared" ref="B49:B51" si="19">"0x" &amp; DEC2HEX(A49,3)</f>
         <v>0x000</v>
       </c>
       <c r="C49" t="s">
@@ -4397,7 +4400,7 @@
         <v>3</v>
       </c>
       <c r="B50" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0x003</v>
       </c>
       <c r="C50" t="s">
@@ -4415,7 +4418,7 @@
         <v>6</v>
       </c>
       <c r="B51" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0x006</v>
       </c>
       <c r="C51" t="s">
@@ -4424,7 +4427,7 @@
       <c r="D51" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="F51" s="19">
+      <c r="F51" s="16">
         <v>17</v>
       </c>
       <c r="H51">
@@ -4433,36 +4436,36 @@
       <c r="I51">
         <v>1</v>
       </c>
-      <c r="L51" s="27" t="str">
-        <f t="shared" ref="L51" si="16">IF(F51="", "", TEXT(DEC2BIN(F51), "000000"))</f>
+      <c r="L51" s="21" t="str">
+        <f t="shared" ref="L51" si="20">IF(F51="", "", TEXT(DEC2BIN(F51), "000000"))</f>
         <v>010001</v>
       </c>
-      <c r="M51" s="28" t="str">
-        <f t="shared" ref="M51" si="17">IF(H51="", "", TEXT(DEC2BIN(H51), "000"))</f>
+      <c r="M51" s="22" t="str">
+        <f t="shared" ref="M51" si="21">IF(H51="", "", TEXT(DEC2BIN(H51), "000"))</f>
         <v>000</v>
       </c>
-      <c r="N51" s="28" t="str">
-        <f t="shared" ref="N51" si="18">IF(I51="", "", TEXT(DEC2BIN(I51), "000"))</f>
+      <c r="N51" s="22" t="str">
+        <f t="shared" ref="N51" si="22">IF(I51="", "", TEXT(DEC2BIN(I51), "000"))</f>
         <v>001</v>
       </c>
-      <c r="O51" s="28" t="str">
-        <f t="shared" ref="O51" si="19">IF(J51="", "", TEXT(DEC2BIN(J51), "00000000"))</f>
+      <c r="O51" s="22" t="str">
+        <f t="shared" ref="O51" si="23">IF(J51="", "", TEXT(DEC2BIN(J51), "00000000"))</f>
         <v/>
       </c>
-      <c r="P51" s="29" t="str">
-        <f t="shared" ref="P51" si="20">IF(K51="", "", TEXT(DEC2BIN(K51), "00000000"))</f>
+      <c r="P51" s="23" t="str">
+        <f t="shared" ref="P51" si="24">IF(K51="", "", TEXT(DEC2BIN(K51), "00000000"))</f>
         <v/>
       </c>
       <c r="Q51" t="str">
-        <f t="shared" ref="Q51" si="21">BIN2HEX(LEFT(CONCATENATE(L51,IF(M51="", "000", M51)), 8), 2)</f>
+        <f t="shared" ref="Q51" si="25">BIN2HEX(LEFT(CONCATENATE(L51,IF(M51="", "000", M51)), 8), 2)</f>
         <v>44</v>
       </c>
       <c r="R51" t="str">
-        <f t="shared" ref="R51" si="22">BIN2HEX(CONCATENATE(RIGHT(M51, 1), IF(N51 = "", "000", N51), "0000"), 2)</f>
+        <f t="shared" ref="R51" si="26">BIN2HEX(CONCATENATE(RIGHT(M51, 1), IF(N51 = "", "000", N51), "0000"), 2)</f>
         <v>10</v>
       </c>
-      <c r="S51" s="21" t="str">
-        <f t="shared" ref="S51" si="23">IF(O51="", BIN2HEX(P51, 2), BIN2HEX(O51,2))</f>
+      <c r="S51" s="18" t="str">
+        <f t="shared" ref="S51" si="27">IF(O51="", BIN2HEX(P51, 2), BIN2HEX(O51,2))</f>
         <v>00</v>
       </c>
     </row>
@@ -4476,7 +4479,7 @@
         <v>0</v>
       </c>
       <c r="B56" t="str">
-        <f t="shared" ref="B56:B79" si="24">"0x" &amp; DEC2HEX(A56,3)</f>
+        <f t="shared" ref="B56:B79" si="28">"0x" &amp; DEC2HEX(A56,3)</f>
         <v>0x000</v>
       </c>
       <c r="C56" t="s">
@@ -4494,7 +4497,7 @@
         <v>3</v>
       </c>
       <c r="B57" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0x003</v>
       </c>
       <c r="C57" t="s">
@@ -4510,7 +4513,7 @@
         <v>6</v>
       </c>
       <c r="B58" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0x006</v>
       </c>
       <c r="C58" t="s">
@@ -4528,7 +4531,7 @@
         <v>9</v>
       </c>
       <c r="B59" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0x009</v>
       </c>
       <c r="C59" t="s">
@@ -4544,7 +4547,7 @@
         <v>12</v>
       </c>
       <c r="B60" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0x00C</v>
       </c>
       <c r="C60" t="s">
@@ -4562,7 +4565,7 @@
         <v>15</v>
       </c>
       <c r="B61" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0x00F</v>
       </c>
       <c r="C61" t="s">
@@ -4578,7 +4581,7 @@
         <v>18</v>
       </c>
       <c r="B62" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0x012</v>
       </c>
       <c r="C62" t="s">
@@ -4596,7 +4599,7 @@
         <v>21</v>
       </c>
       <c r="B63" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0x015</v>
       </c>
       <c r="C63" t="s">
@@ -4612,7 +4615,7 @@
         <v>24</v>
       </c>
       <c r="B64" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0x018</v>
       </c>
       <c r="C64" t="s">
@@ -4630,7 +4633,7 @@
         <v>27</v>
       </c>
       <c r="B65" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0x01B</v>
       </c>
       <c r="C65" t="s">
@@ -4646,7 +4649,7 @@
         <v>30</v>
       </c>
       <c r="B66" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0x01E</v>
       </c>
       <c r="C66" t="s">
@@ -4664,7 +4667,7 @@
         <v>33</v>
       </c>
       <c r="B67" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0x021</v>
       </c>
       <c r="C67" t="s">
@@ -4680,7 +4683,7 @@
         <v>36</v>
       </c>
       <c r="B68" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0x024</v>
       </c>
       <c r="C68" t="s">
@@ -4698,7 +4701,7 @@
         <v>39</v>
       </c>
       <c r="B69" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0x027</v>
       </c>
       <c r="C69" t="s">
@@ -4714,7 +4717,7 @@
         <v>42</v>
       </c>
       <c r="B70" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0x02A</v>
       </c>
       <c r="C70" t="s">
@@ -4732,7 +4735,7 @@
         <v>45</v>
       </c>
       <c r="B71" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0x02D</v>
       </c>
       <c r="C71" t="s">
@@ -4748,7 +4751,7 @@
         <v>48</v>
       </c>
       <c r="B72" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0x030</v>
       </c>
       <c r="C72" t="s">
@@ -4766,7 +4769,7 @@
         <v>51</v>
       </c>
       <c r="B73" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0x033</v>
       </c>
       <c r="C73" t="s">
@@ -4782,7 +4785,7 @@
         <v>54</v>
       </c>
       <c r="B74" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0x036</v>
       </c>
       <c r="C74" t="s">
@@ -4800,7 +4803,7 @@
         <v>57</v>
       </c>
       <c r="B75" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0x039</v>
       </c>
       <c r="C75" t="s">
@@ -4816,7 +4819,7 @@
         <v>60</v>
       </c>
       <c r="B76" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0x03C</v>
       </c>
       <c r="C76" t="s">
@@ -4834,7 +4837,7 @@
         <v>63</v>
       </c>
       <c r="B77" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0x03F</v>
       </c>
       <c r="C77" t="s">
@@ -4850,7 +4853,7 @@
         <v>66</v>
       </c>
       <c r="B78" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0x042</v>
       </c>
       <c r="C78" t="s">
@@ -4868,7 +4871,7 @@
         <v>69</v>
       </c>
       <c r="B79" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0x045</v>
       </c>
       <c r="C79" t="s">
@@ -4898,7 +4901,7 @@
         <v>0</v>
       </c>
       <c r="B83" t="str">
-        <f t="shared" ref="B83:B93" si="25">"0x" &amp; DEC2HEX(A83,3)</f>
+        <f t="shared" ref="B83:B93" si="29">"0x" &amp; DEC2HEX(A83,3)</f>
         <v>0x000</v>
       </c>
       <c r="C83" t="s">
@@ -4916,7 +4919,7 @@
         <v>3</v>
       </c>
       <c r="B84" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0x003</v>
       </c>
       <c r="C84" t="s">
@@ -4934,7 +4937,7 @@
         <v>6</v>
       </c>
       <c r="B85" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0x006</v>
       </c>
       <c r="C85" t="s">
@@ -4952,7 +4955,7 @@
         <v>9</v>
       </c>
       <c r="B86" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0x009</v>
       </c>
       <c r="C86" t="s">
@@ -4970,7 +4973,7 @@
         <v>12</v>
       </c>
       <c r="B87" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0x00C</v>
       </c>
       <c r="C87" t="s">
@@ -4988,7 +4991,7 @@
         <v>15</v>
       </c>
       <c r="B88" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0x00F</v>
       </c>
       <c r="C88" t="s">
@@ -4997,7 +5000,7 @@
       <c r="D88" s="11" t="s">
         <v>218</v>
       </c>
-      <c r="E88" s="17" t="s">
+      <c r="E88" s="32" t="s">
         <v>232</v>
       </c>
     </row>
@@ -5006,7 +5009,7 @@
         <v>18</v>
       </c>
       <c r="B89" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0x012</v>
       </c>
       <c r="C89" t="s">
@@ -5015,14 +5018,14 @@
       <c r="D89" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="E89" s="17"/>
+      <c r="E89" s="32"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>21</v>
       </c>
       <c r="B90" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0x015</v>
       </c>
       <c r="C90" t="s">
@@ -5031,14 +5034,14 @@
       <c r="D90" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="E90" s="17"/>
+      <c r="E90" s="32"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>24</v>
       </c>
       <c r="B91" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0x018</v>
       </c>
       <c r="C91" t="s">
@@ -5056,7 +5059,7 @@
         <v>27</v>
       </c>
       <c r="B92" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0x01B</v>
       </c>
       <c r="C92" t="s">
@@ -5074,7 +5077,7 @@
         <v>30</v>
       </c>
       <c r="B93" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0x01E</v>
       </c>
       <c r="C93" t="s">
@@ -5097,7 +5100,7 @@
         <v>48</v>
       </c>
       <c r="B95" t="str">
-        <f t="shared" ref="B95:B98" si="26">"0x" &amp; DEC2HEX(A95,3)</f>
+        <f t="shared" ref="B95:B98" si="30">"0x" &amp; DEC2HEX(A95,3)</f>
         <v>0x030</v>
       </c>
       <c r="D95" s="11" t="s">
@@ -5112,7 +5115,7 @@
         <v>51</v>
       </c>
       <c r="B96" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>0x033</v>
       </c>
       <c r="D96" s="11" t="s">
@@ -5127,7 +5130,7 @@
         <v>54</v>
       </c>
       <c r="B97" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>0x036</v>
       </c>
       <c r="D97" s="11" t="s">
@@ -5142,7 +5145,7 @@
         <v>57</v>
       </c>
       <c r="B98" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>0x039</v>
       </c>
       <c r="D98" s="11" t="s">
@@ -5171,7 +5174,7 @@
         <v>0</v>
       </c>
       <c r="B102" t="str">
-        <f t="shared" ref="B102" si="27">"0x" &amp; DEC2HEX(A102,3)</f>
+        <f t="shared" ref="B102" si="31">"0x" &amp; DEC2HEX(A102,3)</f>
         <v>0x000</v>
       </c>
       <c r="C102" t="s">
@@ -5189,7 +5192,7 @@
         <v>3</v>
       </c>
       <c r="B103" t="str">
-        <f t="shared" ref="B103:B113" si="28">"0x" &amp; DEC2HEX(A103,3)</f>
+        <f t="shared" ref="B103:B113" si="32">"0x" &amp; DEC2HEX(A103,3)</f>
         <v>0x003</v>
       </c>
       <c r="C103" t="s">
@@ -5207,7 +5210,7 @@
         <v>6</v>
       </c>
       <c r="B104" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>0x006</v>
       </c>
       <c r="C104" t="s">
@@ -5225,7 +5228,7 @@
         <v>9</v>
       </c>
       <c r="B105" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>0x009</v>
       </c>
       <c r="C105" t="s">
@@ -5241,7 +5244,7 @@
         <v>12</v>
       </c>
       <c r="B106" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>0x00C</v>
       </c>
       <c r="C106" t="s">
@@ -5257,7 +5260,7 @@
         <v>15</v>
       </c>
       <c r="B107" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>0x00F</v>
       </c>
       <c r="C107" t="s">
@@ -5273,7 +5276,7 @@
         <v>18</v>
       </c>
       <c r="B108" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>0x012</v>
       </c>
       <c r="C108" t="s">
@@ -5291,7 +5294,7 @@
         <v>21</v>
       </c>
       <c r="B109" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>0x015</v>
       </c>
       <c r="C109" t="s">
@@ -5309,7 +5312,7 @@
         <v>24</v>
       </c>
       <c r="B110" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>0x018</v>
       </c>
       <c r="C110" t="s">
@@ -5325,7 +5328,7 @@
         <v>27</v>
       </c>
       <c r="B111" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>0x01B</v>
       </c>
       <c r="C111" t="s">
@@ -5343,7 +5346,7 @@
         <v>30</v>
       </c>
       <c r="B112" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>0x01E</v>
       </c>
       <c r="C112" t="s">
@@ -5361,7 +5364,7 @@
         <v>33</v>
       </c>
       <c r="B113" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>0x021</v>
       </c>
       <c r="C113" t="s">
@@ -5384,7 +5387,7 @@
         <v>0</v>
       </c>
       <c r="B118" t="str">
-        <f t="shared" ref="B118:B122" si="29">"0x" &amp; DEC2HEX(A118,3)</f>
+        <f t="shared" ref="B118:B122" si="33">"0x" &amp; DEC2HEX(A118,3)</f>
         <v>0x000</v>
       </c>
       <c r="C118" t="s">
@@ -5402,7 +5405,7 @@
         <v>3</v>
       </c>
       <c r="B119" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0x003</v>
       </c>
       <c r="C119" t="s">
@@ -5420,7 +5423,7 @@
         <v>6</v>
       </c>
       <c r="B120" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0x006</v>
       </c>
       <c r="C120" t="s">
@@ -5432,49 +5435,49 @@
       <c r="E120" s="12" t="s">
         <v>241</v>
       </c>
-      <c r="F120" s="19">
-        <v>1</v>
-      </c>
-      <c r="G120" s="20" t="s">
+      <c r="F120" s="16">
+        <v>1</v>
+      </c>
+      <c r="G120" s="17" t="s">
         <v>40</v>
       </c>
       <c r="H120">
-        <f t="shared" ref="H120:H121" si="30">IF(G120="", "", VLOOKUP(G120, $U$3:$V$10, 2))</f>
+        <f t="shared" ref="H120" si="34">IF(G120="", "", VLOOKUP(G120, $U$3:$V$10, 2))</f>
         <v>2</v>
       </c>
       <c r="K120">
         <v>96</v>
       </c>
-      <c r="L120" s="27" t="str">
+      <c r="L120" s="21" t="str">
         <f>IF(F120="", "", TEXT(DEC2BIN(F120), "000000"))</f>
         <v>000001</v>
       </c>
-      <c r="M120" s="28" t="str">
+      <c r="M120" s="22" t="str">
         <f>IF(H120="", "", TEXT(DEC2BIN(H120), "000"))</f>
         <v>010</v>
       </c>
-      <c r="N120" s="28" t="str">
+      <c r="N120" s="22" t="str">
         <f>IF(I120="", "", TEXT(DEC2BIN(I120), "000"))</f>
         <v/>
       </c>
-      <c r="O120" s="28" t="str">
+      <c r="O120" s="22" t="str">
         <f>IF(J120="", "", TEXT(DEC2BIN(J120), "00000000"))</f>
         <v/>
       </c>
-      <c r="P120" s="29" t="str">
+      <c r="P120" s="23" t="str">
         <f>IF(K120="", "", TEXT(DEC2BIN(K120), "00000000"))</f>
         <v>01100000</v>
       </c>
       <c r="Q120" t="str">
-        <f t="shared" ref="Q120" si="31">BIN2HEX(LEFT(CONCATENATE(L120,IF(M120="", "000", M120)), 8), 2)</f>
+        <f t="shared" ref="Q120" si="35">BIN2HEX(LEFT(CONCATENATE(L120,IF(M120="", "000", M120)), 8), 2)</f>
         <v>05</v>
       </c>
       <c r="R120" t="str">
         <f>BIN2HEX(CONCATENATE(RIGHT(M120, 1), IF(N120 = "", "000", N120), "0000"), 2)</f>
         <v>00</v>
       </c>
-      <c r="S120" s="21" t="str">
-        <f t="shared" ref="S120" si="32">IF(O120="", BIN2HEX(P120, 2), BIN2HEX(O120,2))</f>
+      <c r="S120" s="18" t="str">
+        <f t="shared" ref="S120" si="36">IF(O120="", BIN2HEX(P120, 2), BIN2HEX(O120,2))</f>
         <v>60</v>
       </c>
     </row>
@@ -5483,7 +5486,7 @@
         <v>9</v>
       </c>
       <c r="B121" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0x009</v>
       </c>
       <c r="C121" t="s">
@@ -5501,7 +5504,7 @@
         <v>12</v>
       </c>
       <c r="B122" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0x00C</v>
       </c>
       <c r="C122" t="s">
@@ -5519,7 +5522,7 @@
         <v>15</v>
       </c>
       <c r="B123" t="str">
-        <f t="shared" ref="B123:B136" si="33">"0x" &amp; DEC2HEX(A123,3)</f>
+        <f t="shared" ref="B123:B136" si="37">"0x" &amp; DEC2HEX(A123,3)</f>
         <v>0x00F</v>
       </c>
       <c r="C123" t="s">
@@ -5531,10 +5534,10 @@
       <c r="E123" s="12" t="s">
         <v>230</v>
       </c>
-      <c r="F123" s="19">
-        <v>14</v>
-      </c>
-      <c r="G123" s="20" t="s">
+      <c r="F123" s="16">
+        <v>14</v>
+      </c>
+      <c r="G123" s="17" t="s">
         <v>38</v>
       </c>
       <c r="H123">
@@ -5544,36 +5547,36 @@
       <c r="I123">
         <v>2</v>
       </c>
-      <c r="L123" s="27" t="str">
+      <c r="L123" s="21" t="str">
         <f>IF(F123="", "", TEXT(DEC2BIN(F123), "000000"))</f>
         <v>001110</v>
       </c>
-      <c r="M123" s="28" t="str">
+      <c r="M123" s="22" t="str">
         <f>IF(H123="", "", TEXT(DEC2BIN(H123), "000"))</f>
         <v>000</v>
       </c>
-      <c r="N123" s="28" t="str">
+      <c r="N123" s="22" t="str">
         <f>IF(I123="", "", TEXT(DEC2BIN(I123), "000"))</f>
         <v>010</v>
       </c>
-      <c r="O123" s="28" t="str">
+      <c r="O123" s="22" t="str">
         <f>IF(J123="", "", TEXT(DEC2BIN(J123), "00000000"))</f>
         <v/>
       </c>
-      <c r="P123" s="29" t="str">
+      <c r="P123" s="23" t="str">
         <f>IF(K123="", "", TEXT(DEC2BIN(K123), "00000000"))</f>
         <v/>
       </c>
       <c r="Q123" t="str">
-        <f t="shared" ref="Q123" si="34">BIN2HEX(LEFT(CONCATENATE(L123,IF(M123="", "000", M123)), 8), 2)</f>
+        <f t="shared" ref="Q123" si="38">BIN2HEX(LEFT(CONCATENATE(L123,IF(M123="", "000", M123)), 8), 2)</f>
         <v>38</v>
       </c>
       <c r="R123" t="str">
         <f>BIN2HEX(CONCATENATE(RIGHT(M123, 1), IF(N123 = "", "000", N123), "0000"), 2)</f>
         <v>20</v>
       </c>
-      <c r="S123" s="21" t="str">
-        <f t="shared" ref="S123" si="35">IF(O123="", BIN2HEX(P123, 2), BIN2HEX(O123,2))</f>
+      <c r="S123" s="18" t="str">
+        <f t="shared" ref="S123" si="39">IF(O123="", BIN2HEX(P123, 2), BIN2HEX(O123,2))</f>
         <v>00</v>
       </c>
     </row>
@@ -5582,7 +5585,7 @@
         <v>18</v>
       </c>
       <c r="B124" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0x012</v>
       </c>
       <c r="C124" t="s">
@@ -5591,7 +5594,7 @@
       <c r="D124" s="11" t="s">
         <v>218</v>
       </c>
-      <c r="E124" s="17" t="s">
+      <c r="E124" s="32" t="s">
         <v>232</v>
       </c>
     </row>
@@ -5600,7 +5603,7 @@
         <v>21</v>
       </c>
       <c r="B125" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0x015</v>
       </c>
       <c r="C125" t="s">
@@ -5609,14 +5612,14 @@
       <c r="D125" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="E125" s="17"/>
+      <c r="E125" s="32"/>
     </row>
     <row r="126" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>24</v>
       </c>
       <c r="B126" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0x018</v>
       </c>
       <c r="C126" t="s">
@@ -5625,14 +5628,14 @@
       <c r="D126" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="E126" s="17"/>
+      <c r="E126" s="32"/>
     </row>
     <row r="127" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>27</v>
       </c>
       <c r="B127" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0x01B</v>
       </c>
       <c r="C127" t="s">
@@ -5650,7 +5653,7 @@
         <v>30</v>
       </c>
       <c r="B128" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0x01E</v>
       </c>
       <c r="C128" t="s">
@@ -5668,7 +5671,7 @@
         <v>33</v>
       </c>
       <c r="B129" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0x021</v>
       </c>
       <c r="C129" t="s">
@@ -5677,52 +5680,52 @@
       <c r="D129" s="11" t="s">
         <v>271</v>
       </c>
-      <c r="E129" s="17" t="s">
+      <c r="E129" s="32" t="s">
         <v>235</v>
       </c>
-      <c r="F129" s="19">
+      <c r="F129" s="16">
         <v>2</v>
       </c>
-      <c r="G129" s="20" t="s">
+      <c r="G129" s="17" t="s">
         <v>38</v>
       </c>
       <c r="H129">
-        <f t="shared" ref="H129:H131" si="36">IF(G129="", "", VLOOKUP(G129, $U$3:$V$10, 2))</f>
+        <f t="shared" ref="H129:H131" si="40">IF(G129="", "", VLOOKUP(G129, $U$3:$V$10, 2))</f>
         <v>0</v>
       </c>
       <c r="I129">
         <v>2</v>
       </c>
-      <c r="L129" s="27" t="str">
+      <c r="L129" s="21" t="str">
         <f>IF(F129="", "", TEXT(DEC2BIN(F129), "000000"))</f>
         <v>000010</v>
       </c>
-      <c r="M129" s="28" t="str">
+      <c r="M129" s="22" t="str">
         <f>IF(H129="", "", TEXT(DEC2BIN(H129), "000"))</f>
         <v>000</v>
       </c>
-      <c r="N129" s="28" t="str">
+      <c r="N129" s="22" t="str">
         <f>IF(I129="", "", TEXT(DEC2BIN(I129), "000"))</f>
         <v>010</v>
       </c>
-      <c r="O129" s="28" t="str">
+      <c r="O129" s="22" t="str">
         <f>IF(J129="", "", TEXT(DEC2BIN(J129), "00000000"))</f>
         <v/>
       </c>
-      <c r="P129" s="29" t="str">
+      <c r="P129" s="23" t="str">
         <f>IF(K129="", "", TEXT(DEC2BIN(K129), "00000000"))</f>
         <v/>
       </c>
       <c r="Q129" t="str">
-        <f t="shared" ref="Q129" si="37">BIN2HEX(LEFT(CONCATENATE(L129,IF(M129="", "000", M129)), 8), 2)</f>
+        <f t="shared" ref="Q129" si="41">BIN2HEX(LEFT(CONCATENATE(L129,IF(M129="", "000", M129)), 8), 2)</f>
         <v>08</v>
       </c>
       <c r="R129" t="str">
         <f>BIN2HEX(CONCATENATE(RIGHT(M129, 1), IF(N129 = "", "000", N129), "0000"), 2)</f>
         <v>20</v>
       </c>
-      <c r="S129" s="21" t="str">
-        <f t="shared" ref="S129" si="38">IF(O129="", BIN2HEX(P129, 2), BIN2HEX(O129,2))</f>
+      <c r="S129" s="18" t="str">
+        <f t="shared" ref="S129" si="42">IF(O129="", BIN2HEX(P129, 2), BIN2HEX(O129,2))</f>
         <v>00</v>
       </c>
     </row>
@@ -5731,7 +5734,7 @@
         <v>36</v>
       </c>
       <c r="B130" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0x024</v>
       </c>
       <c r="C130" t="s">
@@ -5740,14 +5743,14 @@
       <c r="D130" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="E130" s="17"/>
+      <c r="E130" s="32"/>
     </row>
     <row r="131" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>39</v>
       </c>
       <c r="B131" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0x027</v>
       </c>
       <c r="C131" t="s">
@@ -5756,50 +5759,50 @@
       <c r="D131" s="11" t="s">
         <v>272</v>
       </c>
-      <c r="E131" s="17"/>
-      <c r="F131" s="19">
+      <c r="E131" s="32"/>
+      <c r="F131" s="16">
         <v>2</v>
       </c>
-      <c r="G131" s="20" t="s">
+      <c r="G131" s="17" t="s">
         <v>40</v>
       </c>
       <c r="H131">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>2</v>
       </c>
       <c r="I131">
         <v>0</v>
       </c>
-      <c r="L131" s="27" t="str">
+      <c r="L131" s="21" t="str">
         <f>IF(F131="", "", TEXT(DEC2BIN(F131), "000000"))</f>
         <v>000010</v>
       </c>
-      <c r="M131" s="28" t="str">
+      <c r="M131" s="22" t="str">
         <f>IF(H131="", "", TEXT(DEC2BIN(H131), "000"))</f>
         <v>010</v>
       </c>
-      <c r="N131" s="28" t="str">
+      <c r="N131" s="22" t="str">
         <f>IF(I131="", "", TEXT(DEC2BIN(I131), "000"))</f>
         <v>000</v>
       </c>
-      <c r="O131" s="28" t="str">
+      <c r="O131" s="22" t="str">
         <f>IF(J131="", "", TEXT(DEC2BIN(J131), "00000000"))</f>
         <v/>
       </c>
-      <c r="P131" s="29" t="str">
+      <c r="P131" s="23" t="str">
         <f>IF(K131="", "", TEXT(DEC2BIN(K131), "00000000"))</f>
         <v/>
       </c>
       <c r="Q131" t="str">
-        <f t="shared" ref="Q131" si="39">BIN2HEX(LEFT(CONCATENATE(L131,IF(M131="", "000", M131)), 8), 2)</f>
+        <f t="shared" ref="Q131" si="43">BIN2HEX(LEFT(CONCATENATE(L131,IF(M131="", "000", M131)), 8), 2)</f>
         <v>09</v>
       </c>
       <c r="R131" t="str">
         <f>BIN2HEX(CONCATENATE(RIGHT(M131, 1), IF(N131 = "", "000", N131), "0000"), 2)</f>
         <v>00</v>
       </c>
-      <c r="S131" s="21" t="str">
-        <f t="shared" ref="S131" si="40">IF(O131="", BIN2HEX(P131, 2), BIN2HEX(O131,2))</f>
+      <c r="S131" s="18" t="str">
+        <f t="shared" ref="S131" si="44">IF(O131="", BIN2HEX(P131, 2), BIN2HEX(O131,2))</f>
         <v>00</v>
       </c>
     </row>
@@ -5808,7 +5811,7 @@
         <v>42</v>
       </c>
       <c r="B132" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0x02A</v>
       </c>
       <c r="C132" t="s">
@@ -5831,7 +5834,7 @@
         <v>48</v>
       </c>
       <c r="B134" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0x030</v>
       </c>
       <c r="D134" s="11" t="s">
@@ -5843,7 +5846,7 @@
         <v>51</v>
       </c>
       <c r="B135" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0x033</v>
       </c>
       <c r="D135" s="11" t="s">
@@ -5855,7 +5858,7 @@
         <v>54</v>
       </c>
       <c r="B136" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0x036</v>
       </c>
       <c r="D136" s="11" t="s">
@@ -5867,12 +5870,12 @@
     <sortCondition ref="U13"/>
   </sortState>
   <mergeCells count="6">
+    <mergeCell ref="E129:E131"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="E20:E22"/>
     <mergeCell ref="E23:E25"/>
     <mergeCell ref="E88:E90"/>
     <mergeCell ref="E124:E126"/>
-    <mergeCell ref="E129:E131"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W17">

</xml_diff>

<commit_message>
Changed more 3 test programs to work with the new opcodes. Not tested yet
</commit_message>
<xml_diff>
--- a/2nd gen - 8 bit cpu/Instruction control lines.xlsx
+++ b/2nd gen - 8 bit cpu/Instruction control lines.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="288" windowWidth="14808" windowHeight="7836"/>
+    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="7830" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Control Lines" sheetId="1" r:id="rId1"/>
     <sheet name="Some instructions for test" sheetId="2" r:id="rId2"/>
     <sheet name="Test Programs" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
@@ -22,7 +22,7 @@
     <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="B20" authorId="0" shapeId="0">
+    <comment ref="B20" authorId="0">
       <text>
         <r>
           <rPr>
@@ -50,7 +50,7 @@
     <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="269">
   <si>
     <t>LD R1, data</t>
   </si>
@@ -328,33 +328,15 @@
     <t>0x</t>
   </si>
   <si>
-    <t>LD B, 0x1</t>
-  </si>
-  <si>
     <t>LD A, 0x20</t>
   </si>
   <si>
-    <t>ADD A, B</t>
-  </si>
-  <si>
     <t>SUB A, B</t>
   </si>
   <si>
-    <t>18 10 00</t>
-  </si>
-  <si>
-    <t>14 10 00</t>
-  </si>
-  <si>
-    <t>04 80 01</t>
-  </si>
-  <si>
     <t>JP [0x006]</t>
   </si>
   <si>
-    <t>2c 00 06</t>
-  </si>
-  <si>
     <t>LD F, 0xff</t>
   </si>
   <si>
@@ -370,18 +352,6 @@
     <t>Equiv to ADD E, B</t>
   </si>
   <si>
-    <t>06 80 ff</t>
-  </si>
-  <si>
-    <t>08 40 00</t>
-  </si>
-  <si>
-    <t>0a 00 00</t>
-  </si>
-  <si>
-    <t>2c 00 09</t>
-  </si>
-  <si>
     <t>Dec</t>
   </si>
   <si>
@@ -421,12 +391,6 @@
     <t>LD B, 0x41</t>
   </si>
   <si>
-    <t>04 80 41</t>
-  </si>
-  <si>
-    <t>04 00 00</t>
-  </si>
-  <si>
     <t>// ASCII code for letter A</t>
   </si>
   <si>
@@ -442,9 +406,6 @@
     <t>ROM DATA in Hex</t>
   </si>
   <si>
-    <t>// Addr of the LCD display</t>
-  </si>
-  <si>
     <t>LD B, 0x48</t>
   </si>
   <si>
@@ -568,21 +529,12 @@
     <t>LD A, 0x30</t>
   </si>
   <si>
-    <t>04 00 30</t>
-  </si>
-  <si>
     <t>// ASCII char '0'</t>
   </si>
   <si>
     <t>OUT 0, A</t>
   </si>
   <si>
-    <t>44 00 00</t>
-  </si>
-  <si>
-    <t>// Saves the value of A register in C</t>
-  </si>
-  <si>
     <t>OUT [OD_addr], R1, R2</t>
   </si>
   <si>
@@ -601,9 +553,6 @@
     <t>08 80 00</t>
   </si>
   <si>
-    <t>// Addr of first char</t>
-  </si>
-  <si>
     <t>// Constant to use in increment</t>
   </si>
   <si>
@@ -676,12 +625,6 @@
     <t>18 50 00</t>
   </si>
   <si>
-    <t>JP Z, [0x01b]</t>
-  </si>
-  <si>
-    <t>30 00 1b</t>
-  </si>
-  <si>
     <t>// If true, stops here</t>
   </si>
   <si>
@@ -691,9 +634,6 @@
     <t>08 10 00</t>
   </si>
   <si>
-    <t>06 80 3c</t>
-  </si>
-  <si>
     <t>LD F, 0x3c</t>
   </si>
   <si>
@@ -703,12 +643,6 @@
     <t>LD B, 0x3a</t>
   </si>
   <si>
-    <t>04 80 3a</t>
-  </si>
-  <si>
-    <t>44 50 00</t>
-  </si>
-  <si>
     <t>// Copy a block of memory from one place to another</t>
   </si>
   <si>
@@ -817,9 +751,6 @@
     <t>JP Z, [0x000]</t>
   </si>
   <si>
-    <t>30 00 00</t>
-  </si>
-  <si>
     <t>// Restart if is the last char</t>
   </si>
   <si>
@@ -917,12 +848,57 @@
   </si>
   <si>
     <t>ST [HL], R1</t>
+  </si>
+  <si>
+    <t>These machine codes doesn't changed</t>
+  </si>
+  <si>
+    <t>LD A, [HL]</t>
+  </si>
+  <si>
+    <t>// Addr of first char (low)</t>
+  </si>
+  <si>
+    <t>// Addr of first char (hi)</t>
+  </si>
+  <si>
+    <t>LD H, 0x0</t>
+  </si>
+  <si>
+    <t>LD L, 0x30</t>
+  </si>
+  <si>
+    <t>INC L</t>
+  </si>
+  <si>
+    <t>SUB L, F</t>
+  </si>
+  <si>
+    <t>JP Z, [0x018]</t>
+  </si>
+  <si>
+    <t>// Saves the value of A register in E</t>
+  </si>
+  <si>
+    <t>LD B, L</t>
+  </si>
+  <si>
+    <t>// Saves the value of L register in B</t>
+  </si>
+  <si>
+    <t>LD L, B</t>
+  </si>
+  <si>
+    <t>// Restores value of L register</t>
+  </si>
+  <si>
+    <t>Test these 3 programs above in v.0.14.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1122,7 +1098,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1198,6 +1174,10 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1213,10 +1193,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1237,7 +1218,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1275,9 +1256,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1310,26 +1291,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1362,26 +1326,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1557,25 +1504,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AL18" sqref="AL18"/>
+      <selection pane="bottomLeft" activeCell="P42" sqref="P42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16" width="3.33203125" customWidth="1"/>
-    <col min="17" max="18" width="3.33203125" style="4" customWidth="1"/>
-    <col min="19" max="19" width="3.33203125" customWidth="1"/>
-    <col min="20" max="20" width="3.33203125" style="46" customWidth="1"/>
-    <col min="21" max="26" width="3.33203125" customWidth="1"/>
-    <col min="27" max="29" width="5.88671875" customWidth="1"/>
+    <col min="3" max="16" width="3.28515625" customWidth="1"/>
+    <col min="17" max="18" width="3.28515625" style="4" customWidth="1"/>
+    <col min="19" max="19" width="3.28515625" customWidth="1"/>
+    <col min="20" max="20" width="3.28515625" style="41" customWidth="1"/>
+    <col min="21" max="26" width="3.28515625" customWidth="1"/>
+    <col min="27" max="29" width="5.85546875" customWidth="1"/>
     <col min="30" max="30" width="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C1">
         <v>23</v>
       </c>
@@ -1627,7 +1574,7 @@
       <c r="S1">
         <v>7</v>
       </c>
-      <c r="T1" s="46">
+      <c r="T1" s="41">
         <v>6</v>
       </c>
       <c r="U1">
@@ -1649,12 +1596,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:38" s="1" customFormat="1" ht="130.19999999999999" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:38" s="1" customFormat="1" ht="130.15" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
-        <v>259</v>
+        <v>236</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="C2" s="29" t="s">
         <v>1</v>
@@ -1690,13 +1637,13 @@
         <v>13</v>
       </c>
       <c r="N2" s="24" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="O2" s="23" t="s">
-        <v>256</v>
+        <v>233</v>
       </c>
       <c r="P2" s="23" t="s">
-        <v>255</v>
+        <v>232</v>
       </c>
       <c r="Q2" s="25" t="s">
         <v>20</v>
@@ -1705,10 +1652,10 @@
         <v>21</v>
       </c>
       <c r="S2" s="23" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="T2" s="40" t="s">
-        <v>264</v>
+        <v>241</v>
       </c>
       <c r="U2" s="23" t="s">
         <v>32</v>
@@ -1728,13 +1675,13 @@
       <c r="Z2" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="AA2" s="41" t="s">
-        <v>117</v>
-      </c>
-      <c r="AB2" s="41"/>
-      <c r="AC2" s="41"/>
-    </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AA2" s="43" t="s">
+        <v>105</v>
+      </c>
+      <c r="AB2" s="43"/>
+      <c r="AC2" s="43"/>
+    </row>
+    <row r="3" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>0</v>
       </c>
@@ -1792,7 +1739,7 @@
       <c r="S3" s="2">
         <v>0</v>
       </c>
-      <c r="T3" s="47">
+      <c r="T3" s="42">
         <v>0</v>
       </c>
       <c r="U3" s="2" t="s">
@@ -1834,7 +1781,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -1892,7 +1839,7 @@
       <c r="S4" s="2">
         <v>0</v>
       </c>
-      <c r="T4" s="47">
+      <c r="T4" s="42">
         <v>0</v>
       </c>
       <c r="U4" s="2" t="s">
@@ -1930,7 +1877,7 @@
         <v>C00000</v>
       </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -1988,7 +1935,7 @@
       <c r="S5" s="2">
         <v>0</v>
       </c>
-      <c r="T5" s="47">
+      <c r="T5" s="42">
         <v>0</v>
       </c>
       <c r="U5" s="2" t="s">
@@ -2026,7 +1973,7 @@
         <v>600400</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -2084,7 +2031,7 @@
       <c r="S6" s="2">
         <v>0</v>
       </c>
-      <c r="T6" s="47">
+      <c r="T6" s="42">
         <v>0</v>
       </c>
       <c r="U6" s="2" t="s">
@@ -2122,12 +2069,12 @@
         <v>5E0000</v>
       </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>4</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>269</v>
+        <v>246</v>
       </c>
       <c r="C7" s="2">
         <v>0</v>
@@ -2180,7 +2127,7 @@
       <c r="S7" s="2">
         <v>0</v>
       </c>
-      <c r="T7" s="47">
+      <c r="T7" s="42">
         <v>0</v>
       </c>
       <c r="U7" s="2" t="s">
@@ -2218,7 +2165,7 @@
         <v>4F0000</v>
       </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>5</v>
       </c>
@@ -2276,7 +2223,7 @@
       <c r="S8" s="2">
         <v>0</v>
       </c>
-      <c r="T8" s="47">
+      <c r="T8" s="42">
         <v>0</v>
       </c>
       <c r="U8" s="2" t="s">
@@ -2314,7 +2261,7 @@
         <v>004000</v>
       </c>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>6</v>
       </c>
@@ -2372,7 +2319,7 @@
       <c r="S9" s="2">
         <v>0</v>
       </c>
-      <c r="T9" s="47">
+      <c r="T9" s="42">
         <v>0</v>
       </c>
       <c r="U9" s="2" t="s">
@@ -2410,7 +2357,7 @@
         <v>006000</v>
       </c>
     </row>
-    <row r="10" spans="1:38" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:38" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="33">
         <v>7</v>
       </c>
@@ -2468,7 +2415,7 @@
       <c r="S10" s="33">
         <v>0</v>
       </c>
-      <c r="T10" s="47">
+      <c r="T10" s="42">
         <v>0</v>
       </c>
       <c r="U10" s="33" t="s">
@@ -2506,7 +2453,7 @@
         <v>004200</v>
       </c>
     </row>
-    <row r="11" spans="1:38" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:38" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="33">
         <v>8</v>
       </c>
@@ -2564,7 +2511,7 @@
       <c r="S11" s="33">
         <v>0</v>
       </c>
-      <c r="T11" s="47">
+      <c r="T11" s="42">
         <v>0</v>
       </c>
       <c r="U11" s="33" t="s">
@@ -2602,7 +2549,7 @@
         <v>006200</v>
       </c>
     </row>
-    <row r="12" spans="1:38" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:38" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="33">
         <v>9</v>
       </c>
@@ -2632,7 +2579,7 @@
       <c r="S12" s="33">
         <v>0</v>
       </c>
-      <c r="T12" s="47">
+      <c r="T12" s="42">
         <v>0</v>
       </c>
       <c r="U12" s="33" t="s">
@@ -2670,7 +2617,7 @@
         <v>000100</v>
       </c>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>10</v>
       </c>
@@ -2728,7 +2675,7 @@
       <c r="S13" s="2">
         <v>0</v>
       </c>
-      <c r="T13" s="47">
+      <c r="T13" s="42">
         <v>0</v>
       </c>
       <c r="U13" s="2" t="s">
@@ -2762,19 +2709,19 @@
         <v>00</v>
       </c>
       <c r="AE13" s="5" t="s">
-        <v>274</v>
+        <v>251</v>
       </c>
       <c r="AL13" s="8" t="str">
         <f t="shared" ref="AL13:AL44" si="4">AA13 &amp; AB13 &amp; AC13</f>
         <v>181800</v>
       </c>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>11</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>276</v>
+        <v>253</v>
       </c>
       <c r="C14" s="2">
         <v>0</v>
@@ -2827,7 +2774,7 @@
       <c r="S14" s="2">
         <v>0</v>
       </c>
-      <c r="T14" s="47">
+      <c r="T14" s="42">
         <v>0</v>
       </c>
       <c r="U14" s="2" t="s">
@@ -2865,7 +2812,7 @@
         <v>091000</v>
       </c>
     </row>
-    <row r="15" spans="1:38" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:38" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="33">
         <v>12</v>
       </c>
@@ -2886,7 +2833,7 @@
       <c r="S15" s="33">
         <v>0</v>
       </c>
-      <c r="T15" s="47">
+      <c r="T15" s="42">
         <v>0</v>
       </c>
       <c r="U15" s="33"/>
@@ -2912,7 +2859,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="16" spans="1:38" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:38" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="33">
         <v>13</v>
       </c>
@@ -2933,7 +2880,7 @@
       <c r="S16" s="33">
         <v>0</v>
       </c>
-      <c r="T16" s="47">
+      <c r="T16" s="42">
         <v>0</v>
       </c>
       <c r="U16" s="33"/>
@@ -2959,7 +2906,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="17" spans="1:38" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:38" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="33">
         <v>14</v>
       </c>
@@ -2980,7 +2927,7 @@
       <c r="S17" s="33">
         <v>0</v>
       </c>
-      <c r="T17" s="47">
+      <c r="T17" s="42">
         <v>0</v>
       </c>
       <c r="U17" s="33"/>
@@ -3006,7 +2953,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="18" spans="1:38" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:38" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="33">
         <v>15</v>
       </c>
@@ -3027,7 +2974,7 @@
       <c r="S18" s="33">
         <v>0</v>
       </c>
-      <c r="T18" s="47">
+      <c r="T18" s="42">
         <v>0</v>
       </c>
       <c r="U18" s="33"/>
@@ -3053,12 +3000,12 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="19" spans="1:38" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:38" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="33">
         <v>16</v>
       </c>
       <c r="B19" s="34" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="O19" s="8">
         <v>0</v>
@@ -3069,7 +3016,7 @@
       <c r="S19" s="8">
         <v>0</v>
       </c>
-      <c r="T19" s="47">
+      <c r="T19" s="42">
         <v>0</v>
       </c>
       <c r="AA19" s="35" t="str">
@@ -3085,19 +3032,19 @@
         <v>00</v>
       </c>
       <c r="AE19" s="8" t="s">
-        <v>222</v>
+        <v>200</v>
       </c>
       <c r="AL19" s="8" t="str">
         <f t="shared" si="4"/>
         <v>000000</v>
       </c>
     </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>17</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -3150,7 +3097,7 @@
       <c r="S20">
         <v>1</v>
       </c>
-      <c r="T20" s="47">
+      <c r="T20" s="42">
         <v>0</v>
       </c>
       <c r="U20" s="2" t="s">
@@ -3184,19 +3131,19 @@
         <v>80</v>
       </c>
       <c r="AE20" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="AL20" s="8" t="str">
         <f t="shared" si="4"/>
         <v>000080</v>
       </c>
     </row>
-    <row r="21" spans="1:38" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:38" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>18</v>
       </c>
       <c r="B21" s="31"/>
-      <c r="T21" s="47"/>
+      <c r="T21" s="42"/>
       <c r="U21" s="2"/>
       <c r="V21" s="2"/>
       <c r="W21" s="2"/>
@@ -3220,12 +3167,12 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="22" spans="1:38" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:38" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>19</v>
       </c>
       <c r="B22" s="31"/>
-      <c r="T22" s="47"/>
+      <c r="T22" s="42"/>
       <c r="U22" s="2"/>
       <c r="V22" s="2"/>
       <c r="W22" s="2"/>
@@ -3249,12 +3196,12 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="23" spans="1:38" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:38" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>20</v>
       </c>
       <c r="B23" s="31"/>
-      <c r="T23" s="47"/>
+      <c r="T23" s="42"/>
       <c r="U23" s="2"/>
       <c r="V23" s="2"/>
       <c r="W23" s="2"/>
@@ -3278,12 +3225,12 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="24" spans="1:38" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:38" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>21</v>
       </c>
       <c r="B24" s="31"/>
-      <c r="T24" s="47"/>
+      <c r="T24" s="42"/>
       <c r="U24" s="2"/>
       <c r="V24" s="2"/>
       <c r="W24" s="2"/>
@@ -3307,12 +3254,12 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="25" spans="1:38" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:38" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>22</v>
       </c>
       <c r="B25" s="31"/>
-      <c r="T25" s="47"/>
+      <c r="T25" s="42"/>
       <c r="U25" s="2"/>
       <c r="V25" s="2"/>
       <c r="W25" s="2"/>
@@ -3336,12 +3283,12 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="26" spans="1:38" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:38" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>23</v>
       </c>
       <c r="B26" s="31"/>
-      <c r="T26" s="47"/>
+      <c r="T26" s="42"/>
       <c r="U26" s="2"/>
       <c r="V26" s="2"/>
       <c r="W26" s="2"/>
@@ -3365,12 +3312,12 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="27" spans="1:38" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:38" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>24</v>
       </c>
       <c r="B27" s="31"/>
-      <c r="T27" s="47"/>
+      <c r="T27" s="42"/>
       <c r="U27" s="2"/>
       <c r="V27" s="2"/>
       <c r="W27" s="2"/>
@@ -3394,12 +3341,12 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="28" spans="1:38" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:38" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>25</v>
       </c>
       <c r="B28" s="31"/>
-      <c r="T28" s="47"/>
+      <c r="T28" s="42"/>
       <c r="U28" s="2"/>
       <c r="V28" s="2"/>
       <c r="W28" s="2"/>
@@ -3423,12 +3370,12 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="29" spans="1:38" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:38" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>26</v>
       </c>
       <c r="B29" s="31"/>
-      <c r="T29" s="47"/>
+      <c r="T29" s="42"/>
       <c r="U29" s="2"/>
       <c r="V29" s="2"/>
       <c r="W29" s="2"/>
@@ -3452,12 +3399,12 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="30" spans="1:38" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:38" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>27</v>
       </c>
       <c r="B30" s="31"/>
-      <c r="T30" s="47"/>
+      <c r="T30" s="42"/>
       <c r="U30" s="2"/>
       <c r="V30" s="2"/>
       <c r="W30" s="2"/>
@@ -3481,12 +3428,12 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="31" spans="1:38" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:38" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>28</v>
       </c>
       <c r="B31" s="31"/>
-      <c r="T31" s="47"/>
+      <c r="T31" s="42"/>
       <c r="U31" s="2"/>
       <c r="V31" s="2"/>
       <c r="W31" s="2"/>
@@ -3510,12 +3457,12 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="32" spans="1:38" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:38" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>29</v>
       </c>
       <c r="B32" s="31"/>
-      <c r="T32" s="47"/>
+      <c r="T32" s="42"/>
       <c r="U32" s="2"/>
       <c r="V32" s="2"/>
       <c r="W32" s="2"/>
@@ -3539,12 +3486,12 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="33" spans="1:38" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:38" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>30</v>
       </c>
       <c r="B33" s="31"/>
-      <c r="T33" s="47"/>
+      <c r="T33" s="42"/>
       <c r="U33" s="2"/>
       <c r="V33" s="2"/>
       <c r="W33" s="2"/>
@@ -3568,12 +3515,12 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="34" spans="1:38" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:38" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>31</v>
       </c>
       <c r="B34" s="31"/>
-      <c r="T34" s="47"/>
+      <c r="T34" s="42"/>
       <c r="U34" s="2"/>
       <c r="V34" s="2"/>
       <c r="W34" s="2"/>
@@ -3597,7 +3544,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="35" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>32</v>
       </c>
@@ -3655,7 +3602,7 @@
       <c r="S35" s="2">
         <v>0</v>
       </c>
-      <c r="T35" s="47">
+      <c r="T35" s="42">
         <v>0</v>
       </c>
       <c r="U35" s="2">
@@ -3689,14 +3636,14 @@
         <v>25</v>
       </c>
       <c r="AE35" t="s">
-        <v>257</v>
+        <v>234</v>
       </c>
       <c r="AL35" s="8" t="str">
         <f t="shared" si="4"/>
         <v>408825</v>
       </c>
     </row>
-    <row r="36" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>33</v>
       </c>
@@ -3754,7 +3701,7 @@
       <c r="S36" s="2">
         <v>0</v>
       </c>
-      <c r="T36" s="47">
+      <c r="T36" s="42">
         <v>0</v>
       </c>
       <c r="U36" s="2">
@@ -3788,14 +3735,14 @@
         <v>18</v>
       </c>
       <c r="AE36" t="s">
-        <v>258</v>
+        <v>235</v>
       </c>
       <c r="AL36" s="8" t="str">
         <f t="shared" si="4"/>
         <v>408818</v>
       </c>
     </row>
-    <row r="37" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>34</v>
       </c>
@@ -3853,7 +3800,7 @@
       <c r="S37" s="2">
         <v>0</v>
       </c>
-      <c r="T37" s="47">
+      <c r="T37" s="42">
         <v>0</v>
       </c>
       <c r="U37" s="2">
@@ -3891,7 +3838,7 @@
         <v>408802</v>
       </c>
     </row>
-    <row r="38" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>35</v>
       </c>
@@ -3949,7 +3896,7 @@
       <c r="S38" s="2">
         <v>0</v>
       </c>
-      <c r="T38" s="47">
+      <c r="T38" s="42">
         <v>0</v>
       </c>
       <c r="U38" s="2">
@@ -3987,7 +3934,7 @@
         <v>40882E</v>
       </c>
     </row>
-    <row r="39" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>36</v>
       </c>
@@ -4045,7 +3992,7 @@
       <c r="S39" s="2">
         <v>0</v>
       </c>
-      <c r="T39" s="47">
+      <c r="T39" s="42">
         <v>0</v>
       </c>
       <c r="U39" s="2">
@@ -4083,7 +4030,7 @@
         <v>40883A</v>
       </c>
     </row>
-    <row r="40" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>37</v>
       </c>
@@ -4141,7 +4088,7 @@
       <c r="S40" s="2">
         <v>0</v>
       </c>
-      <c r="T40" s="47">
+      <c r="T40" s="42">
         <v>0</v>
       </c>
       <c r="U40" s="2">
@@ -4179,12 +4126,12 @@
         <v>40881A</v>
       </c>
     </row>
-    <row r="41" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>38</v>
       </c>
       <c r="B41" s="30" t="s">
-        <v>260</v>
+        <v>237</v>
       </c>
       <c r="C41" s="6">
         <v>0</v>
@@ -4237,7 +4184,7 @@
       <c r="S41" s="2">
         <v>0</v>
       </c>
-      <c r="T41" s="47">
+      <c r="T41" s="42">
         <v>0</v>
       </c>
       <c r="U41" s="2">
@@ -4275,12 +4222,12 @@
         <v>408806</v>
       </c>
     </row>
-    <row r="42" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>39</v>
       </c>
       <c r="B42" s="30" t="s">
-        <v>261</v>
+        <v>238</v>
       </c>
       <c r="C42" s="6">
         <v>0</v>
@@ -4333,7 +4280,7 @@
       <c r="S42" s="2">
         <v>0</v>
       </c>
-      <c r="T42" s="47">
+      <c r="T42" s="42">
         <v>0</v>
       </c>
       <c r="U42" s="2">
@@ -4371,12 +4318,12 @@
         <v>408826</v>
       </c>
     </row>
-    <row r="43" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>40</v>
       </c>
       <c r="B43" s="30" t="s">
-        <v>262</v>
+        <v>239</v>
       </c>
       <c r="C43" s="6">
         <v>0</v>
@@ -4429,7 +4376,7 @@
       <c r="S43" s="2">
         <v>0</v>
       </c>
-      <c r="T43" s="47">
+      <c r="T43" s="42">
         <v>0</v>
       </c>
       <c r="U43" s="2">
@@ -4467,12 +4414,12 @@
         <v>408800</v>
       </c>
     </row>
-    <row r="44" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>41</v>
       </c>
       <c r="B44" s="30" t="s">
-        <v>263</v>
+        <v>240</v>
       </c>
       <c r="C44" s="6">
         <v>0</v>
@@ -4525,7 +4472,7 @@
       <c r="S44" s="2">
         <v>0</v>
       </c>
-      <c r="T44" s="47">
+      <c r="T44" s="42">
         <v>0</v>
       </c>
       <c r="U44" s="2">
@@ -4563,7 +4510,7 @@
         <v>40883D</v>
       </c>
     </row>
-    <row r="46" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B46" s="3" t="s">
         <v>22</v>
       </c>
@@ -4571,7 +4518,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B47" s="5" t="s">
         <v>30</v>
       </c>
@@ -4579,23 +4526,23 @@
         <v>31</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C49" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
         <v>64</v>
       </c>
       <c r="C50" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
         <v>47</v>
       </c>
@@ -4603,35 +4550,35 @@
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52"/>
       <c r="B52" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C52" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="Q52"/>
       <c r="R52"/>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53"/>
       <c r="B53" s="1" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="C53" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="Q53"/>
       <c r="R53"/>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54"/>
       <c r="B54" s="1" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="C54" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="Q54"/>
       <c r="R54"/>
@@ -4654,10 +4601,10 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="9.109375" style="7"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="9.140625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -4805,91 +4752,91 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X136"/>
+  <dimension ref="A1:X135"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G61" sqref="G61"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J93" sqref="J93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" style="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="3" style="12" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.44140625" style="16" customWidth="1"/>
-    <col min="13" max="14" width="9.109375" style="2"/>
-    <col min="15" max="15" width="10.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.88671875" style="18" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="3.44140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" style="16" customWidth="1"/>
+    <col min="13" max="14" width="9.140625" style="2"/>
+    <col min="15" max="15" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3.42578125" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>234</v>
+        <v>212</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>224</v>
+        <v>202</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>224</v>
+        <v>202</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>225</v>
+        <v>203</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>235</v>
+        <v>213</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>233</v>
+        <v>211</v>
       </c>
       <c r="L1" s="19" t="s">
-        <v>226</v>
+        <v>204</v>
       </c>
       <c r="M1" s="20" t="s">
-        <v>227</v>
+        <v>205</v>
       </c>
       <c r="N1" s="20" t="s">
-        <v>228</v>
+        <v>206</v>
       </c>
       <c r="O1" s="20" t="s">
-        <v>230</v>
+        <v>208</v>
       </c>
       <c r="P1" s="21" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q1" s="43" t="s">
-        <v>232</v>
-      </c>
-      <c r="R1" s="44"/>
-      <c r="S1" s="45"/>
+        <v>207</v>
+      </c>
+      <c r="Q1" s="45" t="s">
+        <v>210</v>
+      </c>
+      <c r="R1" s="46"/>
+      <c r="S1" s="47"/>
       <c r="T1" s="10"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="8" t="s">
-        <v>265</v>
+        <v>242</v>
       </c>
       <c r="M2" s="17"/>
       <c r="N2" s="17"/>
       <c r="O2" s="17"/>
       <c r="U2" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
@@ -4898,7 +4845,7 @@
         <v>0x000</v>
       </c>
       <c r="C3" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="11">
@@ -4953,7 +4900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4962,10 +4909,10 @@
         <v>0x003</v>
       </c>
       <c r="C4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>231</v>
+        <v>209</v>
       </c>
       <c r="F4" s="11">
         <v>1</v>
@@ -5019,7 +4966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>6</v>
       </c>
@@ -5028,7 +4975,7 @@
         <v>0x006</v>
       </c>
       <c r="C5" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="11">
@@ -5083,7 +5030,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>9</v>
       </c>
@@ -5092,7 +5039,7 @@
         <v>0x009</v>
       </c>
       <c r="C6" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="11">
@@ -5144,7 +5091,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E7" s="8"/>
       <c r="M7" s="17"/>
       <c r="N7" s="17"/>
@@ -5156,19 +5103,19 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C8" s="8" t="s">
-        <v>268</v>
+        <v>245</v>
       </c>
       <c r="E8" s="8"/>
       <c r="U8" t="s">
-        <v>240</v>
+        <v>218</v>
       </c>
       <c r="V8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0</v>
       </c>
@@ -5177,7 +5124,7 @@
         <v>0x000</v>
       </c>
       <c r="C9" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="11">
@@ -5226,13 +5173,13 @@
         <v>00</v>
       </c>
       <c r="U9" s="38" t="s">
-        <v>241</v>
+        <v>219</v>
       </c>
       <c r="V9" s="38">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3</v>
       </c>
@@ -5241,7 +5188,7 @@
         <v>0x003</v>
       </c>
       <c r="C10" t="s">
-        <v>266</v>
+        <v>243</v>
       </c>
       <c r="F10" s="11">
         <v>40</v>
@@ -5286,13 +5233,13 @@
         <v>00</v>
       </c>
       <c r="U10" s="38" t="s">
-        <v>270</v>
+        <v>247</v>
       </c>
       <c r="V10" s="38">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>6</v>
       </c>
@@ -5301,7 +5248,7 @@
         <v>0x006</v>
       </c>
       <c r="C11" t="s">
-        <v>267</v>
+        <v>244</v>
       </c>
       <c r="F11" s="11">
         <v>5</v>
@@ -5346,18 +5293,18 @@
         <v>03</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C16" s="8" t="s">
-        <v>271</v>
+        <v>248</v>
       </c>
       <c r="U16" t="s">
-        <v>238</v>
+        <v>216</v>
       </c>
       <c r="V16">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>0</v>
       </c>
@@ -5366,7 +5313,7 @@
         <v>0x000</v>
       </c>
       <c r="C17" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="F17" s="11">
         <v>1</v>
@@ -5414,20 +5361,20 @@
         <v>00</v>
       </c>
       <c r="U17" t="s">
-        <v>236</v>
+        <v>214</v>
       </c>
       <c r="V17">
         <v>1</v>
       </c>
       <c r="W17" t="s">
-        <v>237</v>
+        <v>215</v>
       </c>
       <c r="X17">
         <f>VLOOKUP(W17,U16:V18,2)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>3</v>
       </c>
@@ -5436,7 +5383,7 @@
         <v>0x003</v>
       </c>
       <c r="C18" t="s">
-        <v>272</v>
+        <v>249</v>
       </c>
       <c r="F18" s="11">
         <v>1</v>
@@ -5484,13 +5431,13 @@
         <v>FF</v>
       </c>
       <c r="U18" t="s">
-        <v>237</v>
+        <v>215</v>
       </c>
       <c r="V18">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>6</v>
       </c>
@@ -5499,7 +5446,7 @@
         <v>0x006</v>
       </c>
       <c r="C19" t="s">
-        <v>266</v>
+        <v>243</v>
       </c>
       <c r="F19" s="11">
         <v>40</v>
@@ -5544,7 +5491,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>9</v>
       </c>
@@ -5553,10 +5500,10 @@
         <v>0x009</v>
       </c>
       <c r="C20" t="s">
-        <v>273</v>
+        <v>250</v>
       </c>
       <c r="E20" s="39" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F20" s="11">
         <v>41</v>
@@ -5601,7 +5548,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>12</v>
       </c>
@@ -5610,7 +5557,7 @@
         <v>0x00C</v>
       </c>
       <c r="C21" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E21" s="39"/>
       <c r="F21" s="11">
@@ -5656,43 +5603,43 @@
         <v>06</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E22" s="39"/>
       <c r="M22" s="17"/>
       <c r="N22" s="17"/>
       <c r="O22" s="17"/>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E23" s="39"/>
       <c r="M23" s="17"/>
       <c r="N23" s="17"/>
       <c r="O23" s="17"/>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E24" s="39"/>
       <c r="M24" s="17"/>
       <c r="N24" s="17"/>
       <c r="O24" s="17"/>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E25" s="39"/>
       <c r="M25" s="17"/>
       <c r="N25" s="17"/>
       <c r="O25" s="17"/>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
       <c r="M26" s="17"/>
       <c r="N26" s="17"/>
       <c r="O26" s="17"/>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="8" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>0</v>
       </c>
@@ -5701,7 +5648,7 @@
         <v>0x000</v>
       </c>
       <c r="C31" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="F31" s="11">
         <v>1</v>
@@ -5749,7 +5696,7 @@
         <v>01</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>3</v>
       </c>
@@ -5758,7 +5705,7 @@
         <v>0x003</v>
       </c>
       <c r="C32" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F32" s="11">
         <v>1</v>
@@ -5806,7 +5753,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>6</v>
       </c>
@@ -5815,7 +5762,7 @@
         <v>0x006</v>
       </c>
       <c r="C33" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="F33" s="11">
         <v>32</v>
@@ -5863,7 +5810,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>9</v>
       </c>
@@ -5872,7 +5819,7 @@
         <v>0x009</v>
       </c>
       <c r="C34" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="F34" s="11">
         <v>6</v>
@@ -5913,7 +5860,7 @@
         <v>0F</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>12</v>
       </c>
@@ -5922,7 +5869,7 @@
         <v>0x00C</v>
       </c>
       <c r="C35" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F35" s="11">
         <v>5</v>
@@ -5963,7 +5910,7 @@
         <v>06</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>15</v>
       </c>
@@ -5972,7 +5919,7 @@
         <v>0x00F</v>
       </c>
       <c r="C36" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="F36" s="11">
         <v>5</v>
@@ -6013,12 +5960,12 @@
         <v>0F</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C40" s="8" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>0</v>
       </c>
@@ -6027,7 +5974,7 @@
         <v>0x000</v>
       </c>
       <c r="C41" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="F41" s="11">
         <v>3</v>
@@ -6075,7 +6022,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>3</v>
       </c>
@@ -6084,7 +6031,7 @@
         <v>0x003</v>
       </c>
       <c r="C42" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="F42" s="11">
         <v>10</v>
@@ -6132,7 +6079,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>6</v>
       </c>
@@ -6141,7 +6088,7 @@
         <v>0x006</v>
       </c>
       <c r="C43" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F43" s="11">
         <v>5</v>
@@ -6182,7 +6129,7 @@
         <v>06</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>16</v>
       </c>
@@ -6191,41 +6138,83 @@
         <v>0x010</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C46" s="38" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C48" s="8" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>0</v>
       </c>
       <c r="B49" t="str">
-        <f t="shared" ref="B49:B51" si="65">"0x" &amp; DEC2HEX(A49,3)</f>
+        <f t="shared" ref="B49:B50" si="65">"0x" &amp; DEC2HEX(A49,3)</f>
         <v>0x000</v>
       </c>
       <c r="C49" t="s">
-        <v>109</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+      <c r="F49" s="11">
+        <v>1</v>
+      </c>
+      <c r="G49" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="H49">
+        <f t="shared" ref="H49" si="66">IF(G49="", "", VLOOKUP(G49, $U$3:$V$10, 2))</f>
+        <v>1</v>
+      </c>
+      <c r="K49">
+        <v>65</v>
+      </c>
+      <c r="L49" s="16" t="str">
+        <f t="shared" ref="L49" si="67">IF(F49="", "", TEXT(DEC2BIN(F49), "000000"))</f>
+        <v>000001</v>
+      </c>
+      <c r="M49" s="17" t="str">
+        <f t="shared" ref="M49" si="68">IF(H49="", "", TEXT(DEC2BIN(H49), "000"))</f>
+        <v>001</v>
+      </c>
+      <c r="N49" s="17" t="str">
+        <f t="shared" ref="N49" si="69">IF(I49="", "", TEXT(DEC2BIN(I49), "000"))</f>
+        <v/>
+      </c>
+      <c r="O49" s="17" t="str">
+        <f t="shared" ref="O49" si="70">IF(J49="", "", TEXT(DEC2BIN(J49), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="P49" s="18" t="str">
+        <f t="shared" ref="P49" si="71">IF(K49="", "", TEXT(DEC2BIN(K49), "00000000"))</f>
+        <v>01000001</v>
+      </c>
+      <c r="Q49" t="str">
+        <f t="shared" ref="Q49" si="72">BIN2HEX(LEFT(CONCATENATE(L49,IF(M49="", "000", M49)), 8), 2)</f>
+        <v>04</v>
+      </c>
+      <c r="R49" t="str">
+        <f t="shared" ref="R49" si="73">BIN2HEX(CONCATENATE(RIGHT(M49, 1), IF(N49 = "", "000", N49), "0000"), 2)</f>
+        <v>80</v>
+      </c>
+      <c r="S49" s="13" t="str">
+        <f t="shared" ref="S49" si="74">IF(O49="", BIN2HEX(P49, 2), BIN2HEX(O49,2))</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>3</v>
       </c>
@@ -6234,1482 +6223,1838 @@
         <v>0x003</v>
       </c>
       <c r="C50" t="s">
-        <v>110</v>
-      </c>
-      <c r="D50" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="E50" s="8" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A51">
-        <v>6</v>
-      </c>
-      <c r="B51" t="str">
-        <f t="shared" si="65"/>
-        <v>0x006</v>
-      </c>
-      <c r="C51" t="s">
-        <v>149</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="F51" s="11">
+        <v>136</v>
+      </c>
+      <c r="F50" s="11">
         <v>17</v>
       </c>
-      <c r="H51">
-        <v>0</v>
-      </c>
-      <c r="I51">
-        <v>1</v>
-      </c>
-      <c r="L51" s="16" t="str">
-        <f t="shared" ref="L51" si="66">IF(F51="", "", TEXT(DEC2BIN(F51), "000000"))</f>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <v>1</v>
+      </c>
+      <c r="L50" s="16" t="str">
+        <f t="shared" ref="L50" si="75">IF(F50="", "", TEXT(DEC2BIN(F50), "000000"))</f>
         <v>010001</v>
       </c>
-      <c r="M51" s="17" t="str">
-        <f t="shared" ref="M51" si="67">IF(H51="", "", TEXT(DEC2BIN(H51), "000"))</f>
+      <c r="M50" s="17" t="str">
+        <f t="shared" ref="M50" si="76">IF(H50="", "", TEXT(DEC2BIN(H50), "000"))</f>
         <v>000</v>
       </c>
-      <c r="N51" s="17" t="str">
-        <f t="shared" ref="N51" si="68">IF(I51="", "", TEXT(DEC2BIN(I51), "000"))</f>
+      <c r="N50" s="17" t="str">
+        <f t="shared" ref="N50" si="77">IF(I50="", "", TEXT(DEC2BIN(I50), "000"))</f>
         <v>001</v>
       </c>
-      <c r="O51" s="17" t="str">
-        <f t="shared" ref="O51" si="69">IF(J51="", "", TEXT(DEC2BIN(J51), "00000000"))</f>
-        <v/>
-      </c>
-      <c r="P51" s="18" t="str">
-        <f t="shared" ref="P51" si="70">IF(K51="", "", TEXT(DEC2BIN(K51), "00000000"))</f>
-        <v/>
-      </c>
-      <c r="Q51" t="str">
-        <f t="shared" ref="Q51" si="71">BIN2HEX(LEFT(CONCATENATE(L51,IF(M51="", "000", M51)), 8), 2)</f>
+      <c r="O50" s="17" t="str">
+        <f t="shared" ref="O50" si="78">IF(J50="", "", TEXT(DEC2BIN(J50), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="P50" s="18" t="str">
+        <f t="shared" ref="P50" si="79">IF(K50="", "", TEXT(DEC2BIN(K50), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="Q50" t="str">
+        <f t="shared" ref="Q50" si="80">BIN2HEX(LEFT(CONCATENATE(L50,IF(M50="", "000", M50)), 8), 2)</f>
         <v>44</v>
       </c>
-      <c r="R51" t="str">
-        <f t="shared" ref="R51" si="72">BIN2HEX(CONCATENATE(RIGHT(M51, 1), IF(N51 = "", "000", N51), "0000"), 2)</f>
+      <c r="R50" t="str">
+        <f t="shared" ref="R50" si="81">BIN2HEX(CONCATENATE(RIGHT(M50, 1), IF(N50 = "", "000", N50), "0000"), 2)</f>
         <v>10</v>
       </c>
-      <c r="S51" s="13" t="str">
-        <f t="shared" ref="S51" si="73">IF(O51="", BIN2HEX(P51, 2), BIN2HEX(O51,2))</f>
-        <v>00</v>
-      </c>
-    </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S50" s="13" t="str">
+        <f t="shared" ref="S50" si="82">IF(O50="", BIN2HEX(P50, 2), BIN2HEX(O50,2))</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="M51" s="17"/>
+      <c r="N51" s="17"/>
+      <c r="O51" s="17"/>
+    </row>
+    <row r="55" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C55" s="8" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>0</v>
       </c>
       <c r="B56" t="str">
-        <f t="shared" ref="B56:B79" si="74">"0x" &amp; DEC2HEX(A56,3)</f>
+        <f t="shared" ref="B56:B79" si="83">"0x" &amp; DEC2HEX(A56,3)</f>
         <v>0x000</v>
       </c>
       <c r="C56" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+      <c r="F56" s="48" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>3</v>
       </c>
       <c r="B57" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="83"/>
         <v>0x003</v>
       </c>
       <c r="C57" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="E57" s="8"/>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>6</v>
       </c>
       <c r="B58" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="83"/>
         <v>0x006</v>
       </c>
       <c r="C58" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>9</v>
       </c>
       <c r="B59" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="83"/>
         <v>0x009</v>
       </c>
       <c r="C59" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="E59" s="8"/>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>12</v>
       </c>
       <c r="B60" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="83"/>
         <v>0x00C</v>
       </c>
       <c r="C60" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="E60" s="8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>15</v>
       </c>
       <c r="B61" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="83"/>
         <v>0x00F</v>
       </c>
       <c r="C61" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="E61" s="8"/>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>18</v>
       </c>
       <c r="B62" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="83"/>
         <v>0x012</v>
       </c>
       <c r="C62" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="E62" s="8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>21</v>
       </c>
       <c r="B63" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="83"/>
         <v>0x015</v>
       </c>
       <c r="C63" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="E63" s="8"/>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>24</v>
       </c>
       <c r="B64" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="83"/>
         <v>0x018</v>
       </c>
       <c r="C64" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>27</v>
       </c>
       <c r="B65" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="83"/>
         <v>0x01B</v>
       </c>
       <c r="C65" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="E65" s="8"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>30</v>
       </c>
       <c r="B66" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="83"/>
         <v>0x01E</v>
       </c>
       <c r="C66" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="E66" s="8" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>33</v>
       </c>
       <c r="B67" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="83"/>
         <v>0x021</v>
       </c>
       <c r="C67" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="E67" s="8"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>36</v>
       </c>
       <c r="B68" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="83"/>
         <v>0x024</v>
       </c>
       <c r="C68" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="D68" s="7" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="E68" s="8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>39</v>
       </c>
       <c r="B69" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="83"/>
         <v>0x027</v>
       </c>
       <c r="C69" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="E69" s="8"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>42</v>
       </c>
       <c r="B70" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="83"/>
         <v>0x02A</v>
       </c>
       <c r="C70" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="D70" s="7" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>45</v>
       </c>
       <c r="B71" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="83"/>
         <v>0x02D</v>
       </c>
       <c r="C71" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="E71" s="8"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>48</v>
       </c>
       <c r="B72" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="83"/>
         <v>0x030</v>
       </c>
       <c r="C72" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="D72" s="7" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>51</v>
       </c>
       <c r="B73" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="83"/>
         <v>0x033</v>
       </c>
       <c r="C73" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="D73" s="7" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="E73" s="8"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>54</v>
       </c>
       <c r="B74" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="83"/>
         <v>0x036</v>
       </c>
       <c r="C74" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="D74" s="7" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="E74" s="8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>57</v>
       </c>
       <c r="B75" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="83"/>
         <v>0x039</v>
       </c>
       <c r="C75" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="D75" s="7" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="E75" s="8"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>60</v>
       </c>
       <c r="B76" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="83"/>
         <v>0x03C</v>
       </c>
       <c r="C76" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="D76" s="7" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="E76" s="8" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>63</v>
       </c>
       <c r="B77" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="83"/>
         <v>0x03F</v>
       </c>
       <c r="C77" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="D77" s="7" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="E77" s="8"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>66</v>
       </c>
       <c r="B78" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="83"/>
         <v>0x042</v>
       </c>
       <c r="C78" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="D78" s="7" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>69</v>
       </c>
       <c r="B79" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="83"/>
         <v>0x045</v>
       </c>
       <c r="C79" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="D79" s="7" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="E79" s="8"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E80" s="8"/>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="D81"/>
       <c r="E81" s="8"/>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C82" s="8" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="D82"/>
       <c r="E82" s="8"/>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>0</v>
       </c>
       <c r="B83" t="str">
-        <f t="shared" ref="B83:B93" si="75">"0x" &amp; DEC2HEX(A83,3)</f>
+        <f t="shared" ref="B83:B87" si="84">"0x" &amp; DEC2HEX(A83,3)</f>
         <v>0x000</v>
       </c>
       <c r="C83" t="s">
-        <v>177</v>
-      </c>
-      <c r="D83" s="7" t="s">
-        <v>178</v>
-      </c>
+        <v>258</v>
+      </c>
+      <c r="D83"/>
       <c r="E83" s="8" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+        <v>257</v>
+      </c>
+      <c r="F83" s="11">
+        <v>1</v>
+      </c>
+      <c r="G83" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="H83">
+        <f t="shared" ref="H83" si="85">IF(G83="", "", VLOOKUP(G83, $U$3:$V$10, 2))</f>
+        <v>2</v>
+      </c>
+      <c r="K83">
+        <v>0</v>
+      </c>
+      <c r="L83" s="16" t="str">
+        <f t="shared" ref="L83" si="86">IF(F83="", "", TEXT(DEC2BIN(F83), "000000"))</f>
+        <v>000001</v>
+      </c>
+      <c r="M83" s="17" t="str">
+        <f t="shared" ref="M83" si="87">IF(H83="", "", TEXT(DEC2BIN(H83), "000"))</f>
+        <v>010</v>
+      </c>
+      <c r="N83" s="17" t="str">
+        <f t="shared" ref="N83" si="88">IF(I83="", "", TEXT(DEC2BIN(I83), "000"))</f>
+        <v/>
+      </c>
+      <c r="O83" s="17" t="str">
+        <f t="shared" ref="O83" si="89">IF(J83="", "", TEXT(DEC2BIN(J83), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="P83" s="18" t="str">
+        <f t="shared" ref="P83" si="90">IF(K83="", "", TEXT(DEC2BIN(K83), "00000000"))</f>
+        <v>00000000</v>
+      </c>
+      <c r="Q83" t="str">
+        <f t="shared" ref="Q83" si="91">BIN2HEX(LEFT(CONCATENATE(L83,IF(M83="", "000", M83)), 8), 2)</f>
+        <v>05</v>
+      </c>
+      <c r="R83" t="str">
+        <f t="shared" ref="R83" si="92">BIN2HEX(CONCATENATE(RIGHT(M83, 1), IF(N83 = "", "000", N83), "0000"), 2)</f>
+        <v>00</v>
+      </c>
+      <c r="S83" s="13" t="str">
+        <f t="shared" ref="S83" si="93">IF(O83="", BIN2HEX(P83, 2), BIN2HEX(O83,2))</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>3</v>
       </c>
       <c r="B84" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="84"/>
         <v>0x003</v>
       </c>
       <c r="C84" t="s">
-        <v>202</v>
-      </c>
-      <c r="D84" s="7" t="s">
-        <v>201</v>
+        <v>259</v>
       </c>
       <c r="E84" s="8" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+        <v>256</v>
+      </c>
+      <c r="F84" s="11">
+        <v>1</v>
+      </c>
+      <c r="G84" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="H84">
+        <f t="shared" ref="H84:H86" si="94">IF(G84="", "", VLOOKUP(G84, $U$3:$V$10, 2))</f>
+        <v>3</v>
+      </c>
+      <c r="K84">
+        <v>48</v>
+      </c>
+      <c r="L84" s="16" t="str">
+        <f t="shared" ref="L84:L86" si="95">IF(F84="", "", TEXT(DEC2BIN(F84), "000000"))</f>
+        <v>000001</v>
+      </c>
+      <c r="M84" s="17" t="str">
+        <f t="shared" ref="M84:M86" si="96">IF(H84="", "", TEXT(DEC2BIN(H84), "000"))</f>
+        <v>011</v>
+      </c>
+      <c r="N84" s="17" t="str">
+        <f t="shared" ref="N84:N86" si="97">IF(I84="", "", TEXT(DEC2BIN(I84), "000"))</f>
+        <v/>
+      </c>
+      <c r="O84" s="17" t="str">
+        <f t="shared" ref="O84:O86" si="98">IF(J84="", "", TEXT(DEC2BIN(J84), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="P84" s="18" t="str">
+        <f t="shared" ref="P84:P86" si="99">IF(K84="", "", TEXT(DEC2BIN(K84), "00000000"))</f>
+        <v>00110000</v>
+      </c>
+      <c r="Q84" t="str">
+        <f t="shared" ref="Q84:Q86" si="100">BIN2HEX(LEFT(CONCATENATE(L84,IF(M84="", "000", M84)), 8), 2)</f>
+        <v>05</v>
+      </c>
+      <c r="R84" t="str">
+        <f t="shared" ref="R84:R86" si="101">BIN2HEX(CONCATENATE(RIGHT(M84, 1), IF(N84 = "", "000", N84), "0000"), 2)</f>
+        <v>80</v>
+      </c>
+      <c r="S84" s="13" t="str">
+        <f t="shared" ref="S84:S86" si="102">IF(O84="", BIN2HEX(P84, 2), BIN2HEX(O84,2))</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>6</v>
       </c>
       <c r="B85" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="84"/>
         <v>0x006</v>
       </c>
       <c r="C85" t="s">
-        <v>166</v>
-      </c>
-      <c r="D85" s="7" t="s">
-        <v>167</v>
+        <v>182</v>
       </c>
       <c r="E85" s="8" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+      <c r="F85" s="11">
+        <v>1</v>
+      </c>
+      <c r="G85" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="H85">
+        <f t="shared" si="94"/>
+        <v>7</v>
+      </c>
+      <c r="K85">
+        <v>60</v>
+      </c>
+      <c r="L85" s="16" t="str">
+        <f t="shared" si="95"/>
+        <v>000001</v>
+      </c>
+      <c r="M85" s="17" t="str">
+        <f t="shared" si="96"/>
+        <v>111</v>
+      </c>
+      <c r="N85" s="17" t="str">
+        <f t="shared" si="97"/>
+        <v/>
+      </c>
+      <c r="O85" s="17" t="str">
+        <f t="shared" si="98"/>
+        <v/>
+      </c>
+      <c r="P85" s="18" t="str">
+        <f t="shared" si="99"/>
+        <v>00111100</v>
+      </c>
+      <c r="Q85" t="str">
+        <f t="shared" si="100"/>
+        <v>07</v>
+      </c>
+      <c r="R85" t="str">
+        <f t="shared" si="101"/>
+        <v>80</v>
+      </c>
+      <c r="S85" s="13" t="str">
+        <f t="shared" si="102"/>
+        <v>3C</v>
+      </c>
+    </row>
+    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>9</v>
       </c>
       <c r="B86" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="84"/>
         <v>0x009</v>
       </c>
       <c r="C86" t="s">
-        <v>193</v>
-      </c>
-      <c r="D86" s="7" t="s">
-        <v>194</v>
+        <v>255</v>
       </c>
       <c r="E86" s="8" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+      <c r="F86" s="11">
+        <v>4</v>
+      </c>
+      <c r="G86" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="H86">
+        <f t="shared" si="94"/>
+        <v>0</v>
+      </c>
+      <c r="K86">
+        <v>0</v>
+      </c>
+      <c r="L86" s="16" t="str">
+        <f t="shared" si="95"/>
+        <v>000100</v>
+      </c>
+      <c r="M86" s="17" t="str">
+        <f t="shared" si="96"/>
+        <v>000</v>
+      </c>
+      <c r="N86" s="17" t="str">
+        <f t="shared" si="97"/>
+        <v/>
+      </c>
+      <c r="O86" s="17" t="str">
+        <f t="shared" si="98"/>
+        <v/>
+      </c>
+      <c r="P86" s="18" t="str">
+        <f t="shared" si="99"/>
+        <v>00000000</v>
+      </c>
+      <c r="Q86" t="str">
+        <f t="shared" si="100"/>
+        <v>10</v>
+      </c>
+      <c r="R86" t="str">
+        <f t="shared" si="101"/>
+        <v>00</v>
+      </c>
+      <c r="S86" s="13" t="str">
+        <f t="shared" si="102"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>12</v>
       </c>
       <c r="B87" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="84"/>
         <v>0x00C</v>
       </c>
       <c r="C87" t="s">
-        <v>162</v>
-      </c>
-      <c r="D87" t="s">
-        <v>163</v>
-      </c>
+        <v>148</v>
+      </c>
+      <c r="D87"/>
       <c r="E87" s="8" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+      <c r="F87" s="11">
+        <v>17</v>
+      </c>
+      <c r="G87" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="H87">
+        <f t="shared" ref="H87:H89" si="103">IF(G87="", "", VLOOKUP(G87, $U$3:$V$10, 2))</f>
+        <v>0</v>
+      </c>
+      <c r="I87">
+        <v>0</v>
+      </c>
+      <c r="L87" s="16" t="str">
+        <f t="shared" ref="L87" si="104">IF(F87="", "", TEXT(DEC2BIN(F87), "000000"))</f>
+        <v>010001</v>
+      </c>
+      <c r="M87" s="17" t="str">
+        <f t="shared" ref="M87:M89" si="105">IF(H87="", "", TEXT(DEC2BIN(H87), "000"))</f>
+        <v>000</v>
+      </c>
+      <c r="N87" s="17" t="str">
+        <f t="shared" ref="N87:N89" si="106">IF(I87="", "", TEXT(DEC2BIN(I87), "000"))</f>
+        <v>000</v>
+      </c>
+      <c r="O87" s="17" t="str">
+        <f t="shared" ref="O87:O89" si="107">IF(J87="", "", TEXT(DEC2BIN(J87), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="P87" s="18" t="str">
+        <f t="shared" ref="P87:P89" si="108">IF(K87="", "", TEXT(DEC2BIN(K87), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="Q87" t="str">
+        <f t="shared" ref="Q87" si="109">BIN2HEX(LEFT(CONCATENATE(L87,IF(M87="", "000", M87)), 8), 2)</f>
+        <v>44</v>
+      </c>
+      <c r="R87" t="str">
+        <f t="shared" ref="R87" si="110">BIN2HEX(CONCATENATE(RIGHT(M87, 1), IF(N87 = "", "000", N87), "0000"), 2)</f>
+        <v>00</v>
+      </c>
+      <c r="S87" s="13" t="str">
+        <f t="shared" ref="S87" si="111">IF(O87="", BIN2HEX(P87, 2), BIN2HEX(O87,2))</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>15</v>
       </c>
       <c r="B88" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" ref="B88:B93" si="112">"0x" &amp; DEC2HEX(A88,3)</f>
         <v>0x00F</v>
       </c>
       <c r="C88" t="s">
-        <v>59</v>
-      </c>
-      <c r="D88" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="E88" s="42" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+        <v>260</v>
+      </c>
+      <c r="E88" s="49"/>
+      <c r="F88" s="11">
+        <v>40</v>
+      </c>
+      <c r="G88" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="H88">
+        <f t="shared" si="103"/>
+        <v>3</v>
+      </c>
+      <c r="L88" s="16" t="str">
+        <f>IF(F88="", "", TEXT(DEC2BIN(F88), "000000"))</f>
+        <v>101000</v>
+      </c>
+      <c r="M88" s="17" t="str">
+        <f t="shared" si="105"/>
+        <v>011</v>
+      </c>
+      <c r="N88" s="17" t="str">
+        <f t="shared" si="106"/>
+        <v/>
+      </c>
+      <c r="O88" s="17" t="str">
+        <f t="shared" si="107"/>
+        <v/>
+      </c>
+      <c r="P88" s="18" t="str">
+        <f t="shared" si="108"/>
+        <v/>
+      </c>
+      <c r="Q88" t="str">
+        <f>BIN2HEX(LEFT(CONCATENATE(L88,IF(M88="", "000", M88)), 8), 2)</f>
+        <v>A1</v>
+      </c>
+      <c r="R88" t="str">
+        <f>BIN2HEX(CONCATENATE(RIGHT(M88, 1), IF(N88 = "", "000", N88), "0000"), 2)</f>
+        <v>80</v>
+      </c>
+      <c r="S88" s="13" t="str">
+        <f>IF(O88="", BIN2HEX(P88, 2), BIN2HEX(O88,2))</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>18</v>
       </c>
       <c r="B89" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="112"/>
         <v>0x012</v>
       </c>
       <c r="C89" t="s">
-        <v>168</v>
-      </c>
-      <c r="D89" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="E89" s="42"/>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+        <v>264</v>
+      </c>
+      <c r="E89" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="F89" s="11">
+        <v>2</v>
+      </c>
+      <c r="G89" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="H89">
+        <f t="shared" si="103"/>
+        <v>1</v>
+      </c>
+      <c r="I89">
+        <v>3</v>
+      </c>
+      <c r="L89" s="16" t="str">
+        <f t="shared" ref="L89" si="113">IF(F89="", "", TEXT(DEC2BIN(F89), "000000"))</f>
+        <v>000010</v>
+      </c>
+      <c r="M89" s="17" t="str">
+        <f t="shared" si="105"/>
+        <v>001</v>
+      </c>
+      <c r="N89" s="17" t="str">
+        <f t="shared" si="106"/>
+        <v>011</v>
+      </c>
+      <c r="O89" s="17" t="str">
+        <f t="shared" si="107"/>
+        <v/>
+      </c>
+      <c r="P89" s="18" t="str">
+        <f t="shared" si="108"/>
+        <v/>
+      </c>
+      <c r="Q89" t="str">
+        <f t="shared" ref="Q89" si="114">BIN2HEX(LEFT(CONCATENATE(L89,IF(M89="", "000", M89)), 8), 2)</f>
+        <v>08</v>
+      </c>
+      <c r="R89" t="str">
+        <f t="shared" ref="R89" si="115">BIN2HEX(CONCATENATE(RIGHT(M89, 1), IF(N89 = "", "000", N89), "0000"), 2)</f>
+        <v>B0</v>
+      </c>
+      <c r="S89" s="13" t="str">
+        <f t="shared" ref="S89" si="116">IF(O89="", BIN2HEX(P89, 2), BIN2HEX(O89,2))</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>21</v>
       </c>
       <c r="B90" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="112"/>
         <v>0x015</v>
       </c>
       <c r="C90" t="s">
-        <v>62</v>
-      </c>
-      <c r="D90" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="E90" s="42"/>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+        <v>261</v>
+      </c>
+      <c r="E90" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="F90" s="11">
+        <v>33</v>
+      </c>
+      <c r="G90" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="H90">
+        <f t="shared" ref="H90" si="117">IF(G90="", "", VLOOKUP(G90, $U$3:$V$10, 2))</f>
+        <v>3</v>
+      </c>
+      <c r="I90">
+        <v>7</v>
+      </c>
+      <c r="L90" s="16" t="str">
+        <f>IF(F90="", "", TEXT(DEC2BIN(F90), "000000"))</f>
+        <v>100001</v>
+      </c>
+      <c r="M90" s="17" t="str">
+        <f t="shared" ref="M90" si="118">IF(H90="", "", TEXT(DEC2BIN(H90), "000"))</f>
+        <v>011</v>
+      </c>
+      <c r="N90" s="17" t="str">
+        <f t="shared" ref="N90" si="119">IF(I90="", "", TEXT(DEC2BIN(I90), "000"))</f>
+        <v>111</v>
+      </c>
+      <c r="O90" s="17" t="str">
+        <f t="shared" ref="O90" si="120">IF(J90="", "", TEXT(DEC2BIN(J90), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="P90" s="18" t="str">
+        <f t="shared" ref="P90" si="121">IF(K90="", "", TEXT(DEC2BIN(K90), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="Q90" t="str">
+        <f>BIN2HEX(LEFT(CONCATENATE(L90,IF(M90="", "000", M90)), 8), 2)</f>
+        <v>85</v>
+      </c>
+      <c r="R90" t="str">
+        <f>BIN2HEX(CONCATENATE(RIGHT(M90, 1), IF(N90 = "", "000", N90), "0000"), 2)</f>
+        <v>F0</v>
+      </c>
+      <c r="S90" s="13" t="str">
+        <f>IF(O90="", BIN2HEX(P90, 2), BIN2HEX(O90,2))</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>24</v>
       </c>
       <c r="B91" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="112"/>
         <v>0x018</v>
       </c>
       <c r="C91" t="s">
-        <v>176</v>
-      </c>
-      <c r="D91" s="7" t="s">
-        <v>195</v>
+        <v>262</v>
       </c>
       <c r="E91" s="8" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+      <c r="F91" s="11">
+        <v>6</v>
+      </c>
+      <c r="H91" t="str">
+        <f t="shared" ref="H91:H92" si="122">IF(G91="", "", VLOOKUP(G91, $U$3:$V$10, 2))</f>
+        <v/>
+      </c>
+      <c r="J91">
+        <v>24</v>
+      </c>
+      <c r="L91" s="16" t="str">
+        <f>IF(F91="", "", TEXT(DEC2BIN(F91), "000000"))</f>
+        <v>000110</v>
+      </c>
+      <c r="M91" s="17" t="str">
+        <f t="shared" ref="M91:M92" si="123">IF(H91="", "", TEXT(DEC2BIN(H91), "000"))</f>
+        <v/>
+      </c>
+      <c r="N91" s="17" t="str">
+        <f t="shared" ref="N91:N92" si="124">IF(I91="", "", TEXT(DEC2BIN(I91), "000"))</f>
+        <v/>
+      </c>
+      <c r="O91" s="17" t="str">
+        <f t="shared" ref="O91:O92" si="125">IF(J91="", "", TEXT(DEC2BIN(J91), "00000000"))</f>
+        <v>00011000</v>
+      </c>
+      <c r="P91" s="18" t="str">
+        <f t="shared" ref="P91:P92" si="126">IF(K91="", "", TEXT(DEC2BIN(K91), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="Q91" t="str">
+        <f>BIN2HEX(LEFT(CONCATENATE(L91,IF(M91="", "000", M91)), 8), 2)</f>
+        <v>18</v>
+      </c>
+      <c r="R91" t="str">
+        <f>BIN2HEX(CONCATENATE(RIGHT(M91, 1), IF(N91 = "", "000", N91), "0000"), 2)</f>
+        <v>00</v>
+      </c>
+      <c r="S91" s="13" t="str">
+        <f>IF(O91="", BIN2HEX(P91, 2), BIN2HEX(O91,2))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>27</v>
       </c>
       <c r="B92" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="112"/>
         <v>0x01B</v>
       </c>
       <c r="C92" t="s">
-        <v>196</v>
-      </c>
-      <c r="D92" s="7" t="s">
-        <v>197</v>
+        <v>266</v>
       </c>
       <c r="E92" s="8" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+        <v>267</v>
+      </c>
+      <c r="F92" s="11">
+        <v>2</v>
+      </c>
+      <c r="G92" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="H92">
+        <f t="shared" si="122"/>
+        <v>3</v>
+      </c>
+      <c r="I92">
+        <v>1</v>
+      </c>
+      <c r="L92" s="16" t="str">
+        <f t="shared" ref="L92" si="127">IF(F92="", "", TEXT(DEC2BIN(F92), "000000"))</f>
+        <v>000010</v>
+      </c>
+      <c r="M92" s="17" t="str">
+        <f t="shared" si="123"/>
+        <v>011</v>
+      </c>
+      <c r="N92" s="17" t="str">
+        <f t="shared" si="124"/>
+        <v>001</v>
+      </c>
+      <c r="O92" s="17" t="str">
+        <f t="shared" si="125"/>
+        <v/>
+      </c>
+      <c r="P92" s="18" t="str">
+        <f t="shared" si="126"/>
+        <v/>
+      </c>
+      <c r="Q92" t="str">
+        <f t="shared" ref="Q92" si="128">BIN2HEX(LEFT(CONCATENATE(L92,IF(M92="", "000", M92)), 8), 2)</f>
+        <v>09</v>
+      </c>
+      <c r="R92" t="str">
+        <f t="shared" ref="R92" si="129">BIN2HEX(CONCATENATE(RIGHT(M92, 1), IF(N92 = "", "000", N92), "0000"), 2)</f>
+        <v>90</v>
+      </c>
+      <c r="S92" s="13" t="str">
+        <f t="shared" ref="S92" si="130">IF(O92="", BIN2HEX(P92, 2), BIN2HEX(O92,2))</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>30</v>
       </c>
       <c r="B93" t="str">
-        <f t="shared" si="75"/>
+        <f t="shared" si="112"/>
         <v>0x01E</v>
       </c>
       <c r="C93" t="s">
-        <v>92</v>
-      </c>
-      <c r="D93" s="7" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="E93" s="8" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+      <c r="F93" s="11">
+        <v>5</v>
+      </c>
+      <c r="H93" t="str">
+        <f t="shared" ref="H93" si="131">IF(G93="", "", VLOOKUP(G93, $U$3:$V$10, 2))</f>
+        <v/>
+      </c>
+      <c r="J93">
+        <v>9</v>
+      </c>
+      <c r="L93" s="16" t="str">
+        <f>IF(F93="", "", TEXT(DEC2BIN(F93), "000000"))</f>
+        <v>000101</v>
+      </c>
+      <c r="M93" s="17" t="str">
+        <f t="shared" ref="M93" si="132">IF(H93="", "", TEXT(DEC2BIN(H93), "000"))</f>
+        <v/>
+      </c>
+      <c r="N93" s="17" t="str">
+        <f t="shared" ref="N93" si="133">IF(I93="", "", TEXT(DEC2BIN(I93), "000"))</f>
+        <v/>
+      </c>
+      <c r="O93" s="17" t="str">
+        <f t="shared" ref="O93" si="134">IF(J93="", "", TEXT(DEC2BIN(J93), "00000000"))</f>
+        <v>00001001</v>
+      </c>
+      <c r="P93" s="18" t="str">
+        <f t="shared" ref="P93" si="135">IF(K93="", "", TEXT(DEC2BIN(K93), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="Q93" t="str">
+        <f>BIN2HEX(LEFT(CONCATENATE(L93,IF(M93="", "000", M93)), 8), 2)</f>
+        <v>14</v>
+      </c>
+      <c r="R93" t="str">
+        <f>BIN2HEX(CONCATENATE(RIGHT(M93, 1), IF(N93 = "", "000", N93), "0000"), 2)</f>
+        <v>00</v>
+      </c>
+      <c r="S93" s="13" t="str">
+        <f>IF(O93="", BIN2HEX(P93, 2), BIN2HEX(O93,2))</f>
+        <v>09</v>
+      </c>
+    </row>
+    <row r="94" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E94" s="8" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>48</v>
       </c>
       <c r="B95" t="str">
-        <f t="shared" ref="B95:B98" si="76">"0x" &amp; DEC2HEX(A95,3)</f>
+        <f t="shared" ref="B95:B98" si="136">"0x" &amp; DEC2HEX(A95,3)</f>
         <v>0x030</v>
       </c>
       <c r="D95" s="7" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
       <c r="E95" s="8" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>51</v>
       </c>
       <c r="B96" t="str">
-        <f t="shared" si="76"/>
+        <f t="shared" si="136"/>
         <v>0x033</v>
       </c>
       <c r="D96" s="7" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
       <c r="E96" s="9" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>54</v>
       </c>
       <c r="B97" t="str">
-        <f t="shared" si="76"/>
+        <f t="shared" si="136"/>
         <v>0x036</v>
       </c>
       <c r="D97" s="7" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="E97" s="8" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>57</v>
       </c>
       <c r="B98" t="str">
-        <f t="shared" si="76"/>
+        <f t="shared" si="136"/>
         <v>0x039</v>
       </c>
       <c r="D98" s="7" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
       <c r="E98" s="8" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C99" s="5" t="s">
+        <v>268</v>
+      </c>
       <c r="E99" s="8"/>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D100"/>
       <c r="E100" s="8"/>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C101" s="8" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="D101"/>
       <c r="E101" s="8"/>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>0</v>
       </c>
       <c r="B102" t="str">
-        <f t="shared" ref="B102" si="77">"0x" &amp; DEC2HEX(A102,3)</f>
+        <f t="shared" ref="B102" si="137">"0x" &amp; DEC2HEX(A102,3)</f>
         <v>0x000</v>
       </c>
       <c r="C102" t="s">
-        <v>159</v>
-      </c>
-      <c r="D102" s="7" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="E102" s="8" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>3</v>
       </c>
       <c r="B103" t="str">
-        <f t="shared" ref="B103:B113" si="78">"0x" &amp; DEC2HEX(A103,3)</f>
+        <f t="shared" ref="B103:B106" si="138">"0x" &amp; DEC2HEX(A103,3)</f>
         <v>0x003</v>
       </c>
       <c r="C103" t="s">
-        <v>89</v>
-      </c>
-      <c r="D103" s="7" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="E103" s="8" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>6</v>
       </c>
       <c r="B104" t="str">
-        <f t="shared" si="78"/>
+        <f t="shared" si="138"/>
         <v>0x006</v>
       </c>
       <c r="C104" t="s">
-        <v>190</v>
-      </c>
-      <c r="D104" t="s">
-        <v>206</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="D104"/>
       <c r="E104" s="8" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>9</v>
       </c>
       <c r="B105" t="str">
-        <f t="shared" si="78"/>
+        <f t="shared" si="138"/>
         <v>0x009</v>
       </c>
       <c r="C105" t="s">
-        <v>162</v>
-      </c>
-      <c r="D105" s="7" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="E105" s="8"/>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>12</v>
       </c>
       <c r="B106" t="str">
-        <f t="shared" si="78"/>
+        <f t="shared" si="138"/>
         <v>0x00C</v>
       </c>
       <c r="C106" t="s">
-        <v>80</v>
-      </c>
-      <c r="D106" s="7" t="s">
-        <v>86</v>
+        <v>243</v>
       </c>
       <c r="E106" s="8"/>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A107">
-        <v>15</v>
-      </c>
-      <c r="B107" t="str">
-        <f t="shared" si="78"/>
-        <v>0x00F</v>
-      </c>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C107" t="s">
+        <v>85</v>
+      </c>
+      <c r="E107" s="8" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C108" t="s">
+        <v>184</v>
+      </c>
+      <c r="E108" s="8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C109" t="s">
+        <v>81</v>
+      </c>
+      <c r="E109" s="8"/>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C110" t="s">
+        <v>220</v>
+      </c>
+      <c r="E110" s="8" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C111" t="s">
+        <v>84</v>
+      </c>
+      <c r="E111" s="8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C112" t="s">
         <v>82</v>
-      </c>
-      <c r="D107" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="E107" s="8"/>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A108">
-        <v>18</v>
-      </c>
-      <c r="B108" t="str">
-        <f t="shared" si="78"/>
-        <v>0x012</v>
-      </c>
-      <c r="C108" t="s">
-        <v>91</v>
-      </c>
-      <c r="D108" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="E108" s="8" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A109">
-        <v>21</v>
-      </c>
-      <c r="B109" t="str">
-        <f t="shared" si="78"/>
-        <v>0x015</v>
-      </c>
-      <c r="C109" t="s">
-        <v>204</v>
-      </c>
-      <c r="D109" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="E109" s="8" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A110">
-        <v>24</v>
-      </c>
-      <c r="B110" t="str">
-        <f t="shared" si="78"/>
-        <v>0x018</v>
-      </c>
-      <c r="C110" t="s">
-        <v>83</v>
-      </c>
-      <c r="D110" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="E110" s="8"/>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A111">
-        <v>27</v>
-      </c>
-      <c r="B111" t="str">
-        <f t="shared" si="78"/>
-        <v>0x01B</v>
-      </c>
-      <c r="C111" t="s">
-        <v>242</v>
-      </c>
-      <c r="D111" s="7" t="s">
-        <v>243</v>
-      </c>
-      <c r="E111" s="8" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A112">
-        <v>30</v>
-      </c>
-      <c r="B112" t="str">
-        <f t="shared" si="78"/>
-        <v>0x01E</v>
-      </c>
-      <c r="C112" t="s">
-        <v>90</v>
-      </c>
-      <c r="D112" s="7" t="s">
-        <v>95</v>
       </c>
       <c r="E112" s="8" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="113" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A113">
+    <row r="116" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C116" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="117" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>0</v>
+      </c>
+      <c r="B117" t="str">
+        <f t="shared" ref="B117:B121" si="139">"0x" &amp; DEC2HEX(A117,3)</f>
+        <v>0x000</v>
+      </c>
+      <c r="C117" t="s">
+        <v>160</v>
+      </c>
+      <c r="D117" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="E117" s="8" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="118" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>3</v>
+      </c>
+      <c r="B118" t="str">
+        <f t="shared" si="139"/>
+        <v>0x003</v>
+      </c>
+      <c r="C118" t="s">
+        <v>226</v>
+      </c>
+      <c r="D118" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="E118" s="8" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="119" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>6</v>
+      </c>
+      <c r="B119" t="str">
+        <f t="shared" si="139"/>
+        <v>0x006</v>
+      </c>
+      <c r="C119" t="s">
+        <v>188</v>
+      </c>
+      <c r="D119" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="E119" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="F119" s="11">
+        <v>1</v>
+      </c>
+      <c r="G119" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="H119">
+        <f t="shared" ref="H119" si="140">IF(G119="", "", VLOOKUP(G119, $U$3:$V$10, 2))</f>
+        <v>4</v>
+      </c>
+      <c r="K119">
+        <v>96</v>
+      </c>
+      <c r="L119" s="16" t="str">
+        <f>IF(F119="", "", TEXT(DEC2BIN(F119), "000000"))</f>
+        <v>000001</v>
+      </c>
+      <c r="M119" s="17" t="str">
+        <f>IF(H119="", "", TEXT(DEC2BIN(H119), "000"))</f>
+        <v>100</v>
+      </c>
+      <c r="N119" s="17" t="str">
+        <f>IF(I119="", "", TEXT(DEC2BIN(I119), "000"))</f>
+        <v/>
+      </c>
+      <c r="O119" s="17" t="str">
+        <f>IF(J119="", "", TEXT(DEC2BIN(J119), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="P119" s="18" t="str">
+        <f>IF(K119="", "", TEXT(DEC2BIN(K119), "00000000"))</f>
+        <v>01100000</v>
+      </c>
+      <c r="Q119" t="str">
+        <f t="shared" ref="Q119" si="141">BIN2HEX(LEFT(CONCATENATE(L119,IF(M119="", "000", M119)), 8), 2)</f>
+        <v>06</v>
+      </c>
+      <c r="R119" t="str">
+        <f>BIN2HEX(CONCATENATE(RIGHT(M119, 1), IF(N119 = "", "000", N119), "0000"), 2)</f>
+        <v>00</v>
+      </c>
+      <c r="S119" s="13" t="str">
+        <f t="shared" ref="S119" si="142">IF(O119="", BIN2HEX(P119, 2), BIN2HEX(O119,2))</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>9</v>
+      </c>
+      <c r="B120" t="str">
+        <f t="shared" si="139"/>
+        <v>0x009</v>
+      </c>
+      <c r="C120" t="s">
+        <v>150</v>
+      </c>
+      <c r="D120" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="E120" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="121" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>12</v>
+      </c>
+      <c r="B121" t="str">
+        <f t="shared" si="139"/>
+        <v>0x00C</v>
+      </c>
+      <c r="C121" t="s">
+        <v>176</v>
+      </c>
+      <c r="D121" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="E121" s="8" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="122" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>15</v>
+      </c>
+      <c r="B122" t="str">
+        <f t="shared" ref="B122:B135" si="143">"0x" &amp; DEC2HEX(A122,3)</f>
+        <v>0x00F</v>
+      </c>
+      <c r="C122" t="s">
+        <v>189</v>
+      </c>
+      <c r="D122" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="E122" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="F122" s="11">
+        <v>14</v>
+      </c>
+      <c r="G122" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="H122">
+        <f>IF(G122="", "", VLOOKUP(G122, $U$3:$V$10, 2))</f>
+        <v>0</v>
+      </c>
+      <c r="I122">
+        <v>2</v>
+      </c>
+      <c r="L122" s="16" t="str">
+        <f>IF(F122="", "", TEXT(DEC2BIN(F122), "000000"))</f>
+        <v>001110</v>
+      </c>
+      <c r="M122" s="17" t="str">
+        <f>IF(H122="", "", TEXT(DEC2BIN(H122), "000"))</f>
+        <v>000</v>
+      </c>
+      <c r="N122" s="17" t="str">
+        <f>IF(I122="", "", TEXT(DEC2BIN(I122), "000"))</f>
+        <v>010</v>
+      </c>
+      <c r="O122" s="17" t="str">
+        <f>IF(J122="", "", TEXT(DEC2BIN(J122), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="P122" s="18" t="str">
+        <f>IF(K122="", "", TEXT(DEC2BIN(K122), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="Q122" t="str">
+        <f t="shared" ref="Q122" si="144">BIN2HEX(LEFT(CONCATENATE(L122,IF(M122="", "000", M122)), 8), 2)</f>
+        <v>38</v>
+      </c>
+      <c r="R122" t="str">
+        <f>BIN2HEX(CONCATENATE(RIGHT(M122, 1), IF(N122 = "", "000", N122), "0000"), 2)</f>
+        <v>20</v>
+      </c>
+      <c r="S122" s="13" t="str">
+        <f t="shared" ref="S122" si="145">IF(O122="", BIN2HEX(P122, 2), BIN2HEX(O122,2))</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="123" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>18</v>
+      </c>
+      <c r="B123" t="str">
+        <f t="shared" si="143"/>
+        <v>0x012</v>
+      </c>
+      <c r="C123" t="s">
+        <v>59</v>
+      </c>
+      <c r="D123" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="E123" s="44" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="124" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>21</v>
+      </c>
+      <c r="B124" t="str">
+        <f t="shared" si="143"/>
+        <v>0x015</v>
+      </c>
+      <c r="C124" t="s">
+        <v>152</v>
+      </c>
+      <c r="D124" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="E124" s="44"/>
+    </row>
+    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>24</v>
+      </c>
+      <c r="B125" t="str">
+        <f t="shared" si="143"/>
+        <v>0x018</v>
+      </c>
+      <c r="C125" t="s">
+        <v>62</v>
+      </c>
+      <c r="D125" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="E125" s="44"/>
+    </row>
+    <row r="126" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>27</v>
+      </c>
+      <c r="B126" t="str">
+        <f t="shared" si="143"/>
+        <v>0x01B</v>
+      </c>
+      <c r="C126" t="s">
+        <v>159</v>
+      </c>
+      <c r="D126" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="E126" s="8" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="127" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>30</v>
+      </c>
+      <c r="B127" t="str">
+        <f t="shared" si="143"/>
+        <v>0x01E</v>
+      </c>
+      <c r="C127" t="s">
+        <v>198</v>
+      </c>
+      <c r="D127" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="E127" s="8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="128" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A128">
         <v>33</v>
       </c>
-      <c r="B113" t="str">
-        <f t="shared" si="78"/>
+      <c r="B128" t="str">
+        <f t="shared" si="143"/>
         <v>0x021</v>
       </c>
-      <c r="C113" t="s">
-        <v>87</v>
-      </c>
-      <c r="D113" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="E113" s="8" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="117" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="C117" s="8" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="118" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A118">
-        <v>0</v>
-      </c>
-      <c r="B118" t="str">
-        <f t="shared" ref="B118:B122" si="79">"0x" &amp; DEC2HEX(A118,3)</f>
-        <v>0x000</v>
-      </c>
-      <c r="C118" t="s">
-        <v>177</v>
-      </c>
-      <c r="D118" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="E118" s="8" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="119" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A119">
-        <v>3</v>
-      </c>
-      <c r="B119" t="str">
-        <f t="shared" si="79"/>
-        <v>0x003</v>
-      </c>
-      <c r="C119" t="s">
-        <v>249</v>
-      </c>
-      <c r="D119" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="E119" s="8" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="120" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A120">
-        <v>6</v>
-      </c>
-      <c r="B120" t="str">
-        <f t="shared" si="79"/>
-        <v>0x006</v>
-      </c>
-      <c r="C120" t="s">
-        <v>210</v>
-      </c>
-      <c r="D120" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="E120" s="8" t="s">
+      <c r="C128" t="s">
+        <v>196</v>
+      </c>
+      <c r="D128" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="E128" s="44" t="s">
+        <v>195</v>
+      </c>
+      <c r="F128" s="11">
+        <v>2</v>
+      </c>
+      <c r="G128" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="H128">
+        <f t="shared" ref="H128:H130" si="146">IF(G128="", "", VLOOKUP(G128, $U$3:$V$10, 2))</f>
+        <v>0</v>
+      </c>
+      <c r="I128">
+        <v>2</v>
+      </c>
+      <c r="L128" s="16" t="str">
+        <f>IF(F128="", "", TEXT(DEC2BIN(F128), "000000"))</f>
+        <v>000010</v>
+      </c>
+      <c r="M128" s="17" t="str">
+        <f>IF(H128="", "", TEXT(DEC2BIN(H128), "000"))</f>
+        <v>000</v>
+      </c>
+      <c r="N128" s="17" t="str">
+        <f>IF(I128="", "", TEXT(DEC2BIN(I128), "000"))</f>
+        <v>010</v>
+      </c>
+      <c r="O128" s="17" t="str">
+        <f>IF(J128="", "", TEXT(DEC2BIN(J128), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="P128" s="18" t="str">
+        <f>IF(K128="", "", TEXT(DEC2BIN(K128), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="Q128" t="str">
+        <f t="shared" ref="Q128" si="147">BIN2HEX(LEFT(CONCATENATE(L128,IF(M128="", "000", M128)), 8), 2)</f>
+        <v>08</v>
+      </c>
+      <c r="R128" t="str">
+        <f>BIN2HEX(CONCATENATE(RIGHT(M128, 1), IF(N128 = "", "000", N128), "0000"), 2)</f>
+        <v>20</v>
+      </c>
+      <c r="S128" s="13" t="str">
+        <f t="shared" ref="S128" si="148">IF(O128="", BIN2HEX(P128, 2), BIN2HEX(O128,2))</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="129" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>36</v>
+      </c>
+      <c r="B129" t="str">
+        <f t="shared" si="143"/>
+        <v>0x024</v>
+      </c>
+      <c r="C129" t="s">
+        <v>152</v>
+      </c>
+      <c r="D129" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="E129" s="44"/>
+    </row>
+    <row r="130" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>39</v>
+      </c>
+      <c r="B130" t="str">
+        <f t="shared" si="143"/>
+        <v>0x027</v>
+      </c>
+      <c r="C130" t="s">
+        <v>197</v>
+      </c>
+      <c r="D130" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="E130" s="44"/>
+      <c r="F130" s="11">
+        <v>2</v>
+      </c>
+      <c r="G130" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="H130">
+        <f t="shared" si="146"/>
+        <v>4</v>
+      </c>
+      <c r="I130">
+        <v>0</v>
+      </c>
+      <c r="L130" s="16" t="str">
+        <f>IF(F130="", "", TEXT(DEC2BIN(F130), "000000"))</f>
+        <v>000010</v>
+      </c>
+      <c r="M130" s="17" t="str">
+        <f>IF(H130="", "", TEXT(DEC2BIN(H130), "000"))</f>
+        <v>100</v>
+      </c>
+      <c r="N130" s="17" t="str">
+        <f>IF(I130="", "", TEXT(DEC2BIN(I130), "000"))</f>
+        <v>000</v>
+      </c>
+      <c r="O130" s="17" t="str">
+        <f>IF(J130="", "", TEXT(DEC2BIN(J130), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="P130" s="18" t="str">
+        <f>IF(K130="", "", TEXT(DEC2BIN(K130), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="Q130" t="str">
+        <f t="shared" ref="Q130" si="149">BIN2HEX(LEFT(CONCATENATE(L130,IF(M130="", "000", M130)), 8), 2)</f>
+        <v>0A</v>
+      </c>
+      <c r="R130" t="str">
+        <f>BIN2HEX(CONCATENATE(RIGHT(M130, 1), IF(N130 = "", "000", N130), "0000"), 2)</f>
+        <v>00</v>
+      </c>
+      <c r="S130" s="13" t="str">
+        <f t="shared" ref="S130" si="150">IF(O130="", BIN2HEX(P130, 2), BIN2HEX(O130,2))</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="131" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>42</v>
+      </c>
+      <c r="B131" t="str">
+        <f t="shared" si="143"/>
+        <v>0x02A</v>
+      </c>
+      <c r="C131" t="s">
+        <v>193</v>
+      </c>
+      <c r="D131" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="E131" s="8" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="132" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E132" s="8" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="133" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>48</v>
+      </c>
+      <c r="B133" t="str">
+        <f t="shared" si="143"/>
+        <v>0x030</v>
+      </c>
+      <c r="D133" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="F120" s="11">
-        <v>1</v>
-      </c>
-      <c r="G120" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="H120">
-        <f t="shared" ref="H120" si="80">IF(G120="", "", VLOOKUP(G120, $U$3:$V$10, 2))</f>
-        <v>4</v>
-      </c>
-      <c r="K120">
-        <v>96</v>
-      </c>
-      <c r="L120" s="16" t="str">
-        <f>IF(F120="", "", TEXT(DEC2BIN(F120), "000000"))</f>
-        <v>000001</v>
-      </c>
-      <c r="M120" s="17" t="str">
-        <f>IF(H120="", "", TEXT(DEC2BIN(H120), "000"))</f>
-        <v>100</v>
-      </c>
-      <c r="N120" s="17" t="str">
-        <f>IF(I120="", "", TEXT(DEC2BIN(I120), "000"))</f>
-        <v/>
-      </c>
-      <c r="O120" s="17" t="str">
-        <f>IF(J120="", "", TEXT(DEC2BIN(J120), "00000000"))</f>
-        <v/>
-      </c>
-      <c r="P120" s="18" t="str">
-        <f>IF(K120="", "", TEXT(DEC2BIN(K120), "00000000"))</f>
-        <v>01100000</v>
-      </c>
-      <c r="Q120" t="str">
-        <f t="shared" ref="Q120" si="81">BIN2HEX(LEFT(CONCATENATE(L120,IF(M120="", "000", M120)), 8), 2)</f>
-        <v>06</v>
-      </c>
-      <c r="R120" t="str">
-        <f>BIN2HEX(CONCATENATE(RIGHT(M120, 1), IF(N120 = "", "000", N120), "0000"), 2)</f>
-        <v>00</v>
-      </c>
-      <c r="S120" s="13" t="str">
-        <f t="shared" ref="S120" si="82">IF(O120="", BIN2HEX(P120, 2), BIN2HEX(O120,2))</f>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="121" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A121">
-        <v>9</v>
-      </c>
-      <c r="B121" t="str">
-        <f t="shared" si="79"/>
-        <v>0x009</v>
-      </c>
-      <c r="C121" t="s">
-        <v>166</v>
-      </c>
-      <c r="D121" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="E121" s="8" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="122" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A122">
-        <v>12</v>
-      </c>
-      <c r="B122" t="str">
-        <f t="shared" si="79"/>
-        <v>0x00C</v>
-      </c>
-      <c r="C122" t="s">
-        <v>193</v>
-      </c>
-      <c r="D122" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="E122" s="8" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="123" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A123">
-        <v>15</v>
-      </c>
-      <c r="B123" t="str">
-        <f t="shared" ref="B123:B136" si="83">"0x" &amp; DEC2HEX(A123,3)</f>
-        <v>0x00F</v>
-      </c>
-      <c r="C123" t="s">
-        <v>211</v>
-      </c>
-      <c r="D123" s="7" t="s">
-        <v>254</v>
-      </c>
-      <c r="E123" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="F123" s="11">
-        <v>14</v>
-      </c>
-      <c r="G123" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="H123">
-        <f>IF(G123="", "", VLOOKUP(G123, $U$3:$V$10, 2))</f>
-        <v>0</v>
-      </c>
-      <c r="I123">
-        <v>2</v>
-      </c>
-      <c r="L123" s="16" t="str">
-        <f>IF(F123="", "", TEXT(DEC2BIN(F123), "000000"))</f>
-        <v>001110</v>
-      </c>
-      <c r="M123" s="17" t="str">
-        <f>IF(H123="", "", TEXT(DEC2BIN(H123), "000"))</f>
-        <v>000</v>
-      </c>
-      <c r="N123" s="17" t="str">
-        <f>IF(I123="", "", TEXT(DEC2BIN(I123), "000"))</f>
-        <v>010</v>
-      </c>
-      <c r="O123" s="17" t="str">
-        <f>IF(J123="", "", TEXT(DEC2BIN(J123), "00000000"))</f>
-        <v/>
-      </c>
-      <c r="P123" s="18" t="str">
-        <f>IF(K123="", "", TEXT(DEC2BIN(K123), "00000000"))</f>
-        <v/>
-      </c>
-      <c r="Q123" t="str">
-        <f t="shared" ref="Q123" si="84">BIN2HEX(LEFT(CONCATENATE(L123,IF(M123="", "000", M123)), 8), 2)</f>
-        <v>38</v>
-      </c>
-      <c r="R123" t="str">
-        <f>BIN2HEX(CONCATENATE(RIGHT(M123, 1), IF(N123 = "", "000", N123), "0000"), 2)</f>
-        <v>20</v>
-      </c>
-      <c r="S123" s="13" t="str">
-        <f t="shared" ref="S123" si="85">IF(O123="", BIN2HEX(P123, 2), BIN2HEX(O123,2))</f>
-        <v>00</v>
-      </c>
-    </row>
-    <row r="124" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A124">
-        <v>18</v>
-      </c>
-      <c r="B124" t="str">
-        <f t="shared" si="83"/>
-        <v>0x012</v>
-      </c>
-      <c r="C124" t="s">
-        <v>59</v>
-      </c>
-      <c r="D124" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="E124" s="42" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="125" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A125">
-        <v>21</v>
-      </c>
-      <c r="B125" t="str">
-        <f t="shared" si="83"/>
-        <v>0x015</v>
-      </c>
-      <c r="C125" t="s">
-        <v>168</v>
-      </c>
-      <c r="D125" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="E125" s="42"/>
-    </row>
-    <row r="126" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A126">
-        <v>24</v>
-      </c>
-      <c r="B126" t="str">
-        <f t="shared" si="83"/>
-        <v>0x018</v>
-      </c>
-      <c r="C126" t="s">
-        <v>62</v>
-      </c>
-      <c r="D126" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="E126" s="42"/>
-    </row>
-    <row r="127" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A127">
-        <v>27</v>
-      </c>
-      <c r="B127" t="str">
-        <f t="shared" si="83"/>
-        <v>0x01B</v>
-      </c>
-      <c r="C127" t="s">
-        <v>176</v>
-      </c>
-      <c r="D127" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="E127" s="8" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="128" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A128">
-        <v>30</v>
-      </c>
-      <c r="B128" t="str">
-        <f t="shared" si="83"/>
-        <v>0x01E</v>
-      </c>
-      <c r="C128" t="s">
-        <v>220</v>
-      </c>
-      <c r="D128" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="E128" s="8" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="129" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A129">
-        <v>33</v>
-      </c>
-      <c r="B129" t="str">
-        <f t="shared" si="83"/>
-        <v>0x021</v>
-      </c>
-      <c r="C129" t="s">
-        <v>218</v>
-      </c>
-      <c r="D129" s="7" t="s">
-        <v>252</v>
-      </c>
-      <c r="E129" s="42" t="s">
-        <v>217</v>
-      </c>
-      <c r="F129" s="11">
-        <v>2</v>
-      </c>
-      <c r="G129" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="H129">
-        <f t="shared" ref="H129:H131" si="86">IF(G129="", "", VLOOKUP(G129, $U$3:$V$10, 2))</f>
-        <v>0</v>
-      </c>
-      <c r="I129">
-        <v>2</v>
-      </c>
-      <c r="L129" s="16" t="str">
-        <f>IF(F129="", "", TEXT(DEC2BIN(F129), "000000"))</f>
-        <v>000010</v>
-      </c>
-      <c r="M129" s="17" t="str">
-        <f>IF(H129="", "", TEXT(DEC2BIN(H129), "000"))</f>
-        <v>000</v>
-      </c>
-      <c r="N129" s="17" t="str">
-        <f>IF(I129="", "", TEXT(DEC2BIN(I129), "000"))</f>
-        <v>010</v>
-      </c>
-      <c r="O129" s="17" t="str">
-        <f>IF(J129="", "", TEXT(DEC2BIN(J129), "00000000"))</f>
-        <v/>
-      </c>
-      <c r="P129" s="18" t="str">
-        <f>IF(K129="", "", TEXT(DEC2BIN(K129), "00000000"))</f>
-        <v/>
-      </c>
-      <c r="Q129" t="str">
-        <f t="shared" ref="Q129" si="87">BIN2HEX(LEFT(CONCATENATE(L129,IF(M129="", "000", M129)), 8), 2)</f>
-        <v>08</v>
-      </c>
-      <c r="R129" t="str">
-        <f>BIN2HEX(CONCATENATE(RIGHT(M129, 1), IF(N129 = "", "000", N129), "0000"), 2)</f>
-        <v>20</v>
-      </c>
-      <c r="S129" s="13" t="str">
-        <f t="shared" ref="S129" si="88">IF(O129="", BIN2HEX(P129, 2), BIN2HEX(O129,2))</f>
-        <v>00</v>
-      </c>
-    </row>
-    <row r="130" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A130">
-        <v>36</v>
-      </c>
-      <c r="B130" t="str">
-        <f t="shared" si="83"/>
-        <v>0x024</v>
-      </c>
-      <c r="C130" t="s">
-        <v>168</v>
-      </c>
-      <c r="D130" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="E130" s="42"/>
-    </row>
-    <row r="131" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A131">
-        <v>39</v>
-      </c>
-      <c r="B131" t="str">
-        <f t="shared" si="83"/>
-        <v>0x027</v>
-      </c>
-      <c r="C131" t="s">
-        <v>219</v>
-      </c>
-      <c r="D131" s="7" t="s">
-        <v>253</v>
-      </c>
-      <c r="E131" s="42"/>
-      <c r="F131" s="11">
-        <v>2</v>
-      </c>
-      <c r="G131" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="H131">
-        <f t="shared" si="86"/>
-        <v>4</v>
-      </c>
-      <c r="I131">
-        <v>0</v>
-      </c>
-      <c r="L131" s="16" t="str">
-        <f>IF(F131="", "", TEXT(DEC2BIN(F131), "000000"))</f>
-        <v>000010</v>
-      </c>
-      <c r="M131" s="17" t="str">
-        <f>IF(H131="", "", TEXT(DEC2BIN(H131), "000"))</f>
-        <v>100</v>
-      </c>
-      <c r="N131" s="17" t="str">
-        <f>IF(I131="", "", TEXT(DEC2BIN(I131), "000"))</f>
-        <v>000</v>
-      </c>
-      <c r="O131" s="17" t="str">
-        <f>IF(J131="", "", TEXT(DEC2BIN(J131), "00000000"))</f>
-        <v/>
-      </c>
-      <c r="P131" s="18" t="str">
-        <f>IF(K131="", "", TEXT(DEC2BIN(K131), "00000000"))</f>
-        <v/>
-      </c>
-      <c r="Q131" t="str">
-        <f t="shared" ref="Q131" si="89">BIN2HEX(LEFT(CONCATENATE(L131,IF(M131="", "000", M131)), 8), 2)</f>
-        <v>0A</v>
-      </c>
-      <c r="R131" t="str">
-        <f>BIN2HEX(CONCATENATE(RIGHT(M131, 1), IF(N131 = "", "000", N131), "0000"), 2)</f>
-        <v>00</v>
-      </c>
-      <c r="S131" s="13" t="str">
-        <f t="shared" ref="S131" si="90">IF(O131="", BIN2HEX(P131, 2), BIN2HEX(O131,2))</f>
-        <v>00</v>
-      </c>
-    </row>
-    <row r="132" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A132">
-        <v>42</v>
-      </c>
-      <c r="B132" t="str">
-        <f t="shared" si="83"/>
-        <v>0x02A</v>
-      </c>
-      <c r="C132" t="s">
-        <v>215</v>
-      </c>
-      <c r="D132" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="E132" s="8" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="133" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="E133" s="8" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="134" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="134" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A134">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B134" t="str">
-        <f t="shared" si="83"/>
-        <v>0x030</v>
+        <f t="shared" si="143"/>
+        <v>0x033</v>
       </c>
       <c r="D134" s="7" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="135" spans="1:19" x14ac:dyDescent="0.3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="135" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A135">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B135" t="str">
-        <f t="shared" si="83"/>
-        <v>0x033</v>
+        <f t="shared" si="143"/>
+        <v>0x036</v>
       </c>
       <c r="D135" s="7" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="136" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A136">
-        <v>54</v>
-      </c>
-      <c r="B136" t="str">
-        <f t="shared" si="83"/>
-        <v>0x036</v>
-      </c>
-      <c r="D136" s="7" t="s">
-        <v>248</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="U16:V18">
     <sortCondition ref="U13"/>
   </sortState>
-  <mergeCells count="4">
-    <mergeCell ref="E129:E131"/>
+  <mergeCells count="3">
+    <mergeCell ref="E128:E130"/>
     <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="E88:E90"/>
-    <mergeCell ref="E124:E126"/>
+    <mergeCell ref="E123:E125"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W17">
       <formula1>$U$16:$U$18</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G6 G123 G120 G129 G131 G9:G11 G17:G26 G31:G33 G41:G42">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G6 G122 G119 G128 G130 G9:G11 G17:G26 G31:G33 G41:G42 G49 G83:G93">
       <formula1>$U$3:$U$10</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
v.0.14.1 All test programs working fine. Instructions using all addressing modes.
</commit_message>
<xml_diff>
--- a/2nd gen - 8 bit cpu/Instruction control lines.xlsx
+++ b/2nd gen - 8 bit cpu/Instruction control lines.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="7830" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="288" windowWidth="14808" windowHeight="7836" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Control Lines" sheetId="1" r:id="rId1"/>
     <sheet name="Some instructions for test" sheetId="2" r:id="rId2"/>
     <sheet name="Test Programs" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
@@ -22,7 +22,7 @@
     <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="B20" authorId="0">
+    <comment ref="B20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -50,7 +50,7 @@
     <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="H1" authorId="0">
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="250">
   <si>
     <t>LD R1, data</t>
   </si>
@@ -238,9 +238,6 @@
     <t>ST [addr], R1</t>
   </si>
   <si>
-    <t>[RR3]</t>
-  </si>
-  <si>
     <t>[RR3] to MEM_ADDR</t>
   </si>
   <si>
@@ -331,9 +328,6 @@
     <t>LD A, 0x20</t>
   </si>
   <si>
-    <t>SUB A, B</t>
-  </si>
-  <si>
     <t>JP [0x006]</t>
   </si>
   <si>
@@ -376,9 +370,6 @@
     <t>f0</t>
   </si>
   <si>
-    <t>pair of 8-bit registers (as addressing is 12-bit, only lower half of the High register will be used)</t>
-  </si>
-  <si>
     <t>Write byte value of R1 in output selected in R2</t>
   </si>
   <si>
@@ -541,39 +532,21 @@
     <t>LD E, 0x1</t>
   </si>
   <si>
-    <t>06 00 01</t>
-  </si>
-  <si>
     <t>ADD A, E</t>
   </si>
   <si>
-    <t>14 40 00</t>
-  </si>
-  <si>
-    <t>08 80 00</t>
-  </si>
-  <si>
-    <t>// Constant to use in increment</t>
-  </si>
-  <si>
     <t>// Reads char from memory</t>
   </si>
   <si>
     <t>// Print out char to LCD</t>
   </si>
   <si>
-    <t>// Restores value of A register</t>
-  </si>
-  <si>
     <t>SUB A, F</t>
   </si>
   <si>
     <t>LD B, 0x30</t>
   </si>
   <si>
-    <t>04 80 30</t>
-  </si>
-  <si>
     <t>// Data</t>
   </si>
   <si>
@@ -616,24 +589,12 @@
     <t>// next iteration of loop</t>
   </si>
   <si>
-    <t>LD A, [?B]</t>
-  </si>
-  <si>
-    <t>10 10 00</t>
-  </si>
-  <si>
-    <t>18 50 00</t>
-  </si>
-  <si>
     <t>// If true, stops here</t>
   </si>
   <si>
     <t>// If false, next loop iteration</t>
   </si>
   <si>
-    <t>08 10 00</t>
-  </si>
-  <si>
     <t>LD F, 0x3c</t>
   </si>
   <si>
@@ -652,42 +613,15 @@
     <t>// Source addr of last byte + 1</t>
   </si>
   <si>
-    <t>LD C, 0x60</t>
-  </si>
-  <si>
-    <t>ST [?C], A</t>
-  </si>
-  <si>
     <t>// Store byte in destiny addr</t>
   </si>
   <si>
     <t>// Reads byte from memory</t>
   </si>
   <si>
-    <t>// Increments B</t>
-  </si>
-  <si>
     <t>JP [0x00c]</t>
   </si>
   <si>
-    <t>2c 00 0c</t>
-  </si>
-  <si>
-    <t>// Increments C</t>
-  </si>
-  <si>
-    <t>LD A, C</t>
-  </si>
-  <si>
-    <t>LD C, A</t>
-  </si>
-  <si>
-    <t>JP Z, [0x01e]</t>
-  </si>
-  <si>
-    <t>30 00 1e</t>
-  </si>
-  <si>
     <t>Read byte from input selected by R2, and write it to R1</t>
   </si>
   <si>
@@ -769,21 +703,6 @@
     <t>LD F, 0x39</t>
   </si>
   <si>
-    <t>06 80 39</t>
-  </si>
-  <si>
-    <t>05 00 60</t>
-  </si>
-  <si>
-    <t>08 20 00</t>
-  </si>
-  <si>
-    <t>09 00 00</t>
-  </si>
-  <si>
-    <t>38 20 00</t>
-  </si>
-  <si>
     <t>CLOSE_REGS_BRIDGE</t>
   </si>
   <si>
@@ -793,9 +712,6 @@
     <t>All ALU operations take R1 as ALU input A and R2 as ALU input B. Output to R1</t>
   </si>
   <si>
-    <t>In ALU operations R1 are constrained from A to D, and R2 from E to H</t>
-  </si>
-  <si>
     <t>Opcode (Dec)</t>
   </si>
   <si>
@@ -844,15 +760,9 @@
     <t>maybe these two ST instr can use R2 (all 8 registers) instead of R1 (4 regs)</t>
   </si>
   <si>
-    <t>v.0.14.0 Working up to this point</t>
-  </si>
-  <si>
     <t>ST [HL], R1</t>
   </si>
   <si>
-    <t>These machine codes doesn't changed</t>
-  </si>
-  <si>
     <t>LD A, [HL]</t>
   </si>
   <si>
@@ -892,13 +802,46 @@
     <t>// Restores value of L register</t>
   </si>
   <si>
-    <t>Test these 3 programs above in v.0.14.0</t>
+    <t>ST [HL], A</t>
+  </si>
+  <si>
+    <t>INC B</t>
+  </si>
+  <si>
+    <t>// Saves value of B register (current src addr)</t>
+  </si>
+  <si>
+    <t>SUB E, B</t>
+  </si>
+  <si>
+    <t>JP Z, [0x021]</t>
+  </si>
+  <si>
+    <t>// Hi part of both src and dest addresses</t>
+  </si>
+  <si>
+    <t>In ALU operations R1 are constrained to A, B, H and L registers, and R2 from C to F</t>
+  </si>
+  <si>
+    <t>[HL]</t>
+  </si>
+  <si>
+    <t>pair of H and L registers (as addressing is 12-bit, only lower half of the High register will be used)</t>
+  </si>
+  <si>
+    <t>LD E, 0x60</t>
+  </si>
+  <si>
+    <t>LD L, E</t>
+  </si>
+  <si>
+    <t>// Increments E</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1098,7 +1041,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1178,11 +1121,13 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1193,11 +1138,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1218,7 +1164,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1256,9 +1202,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1291,9 +1237,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1326,9 +1289,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1506,23 +1486,23 @@
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P42" sqref="P42"/>
+      <selection pane="bottomLeft" activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16" width="3.28515625" customWidth="1"/>
-    <col min="17" max="18" width="3.28515625" style="4" customWidth="1"/>
-    <col min="19" max="19" width="3.28515625" customWidth="1"/>
-    <col min="20" max="20" width="3.28515625" style="41" customWidth="1"/>
-    <col min="21" max="26" width="3.28515625" customWidth="1"/>
-    <col min="27" max="29" width="5.85546875" customWidth="1"/>
+    <col min="3" max="16" width="3.33203125" customWidth="1"/>
+    <col min="17" max="18" width="3.33203125" style="4" customWidth="1"/>
+    <col min="19" max="19" width="3.33203125" customWidth="1"/>
+    <col min="20" max="20" width="3.33203125" style="41" customWidth="1"/>
+    <col min="21" max="26" width="3.33203125" customWidth="1"/>
+    <col min="27" max="29" width="5.88671875" customWidth="1"/>
     <col min="30" max="30" width="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.3">
       <c r="C1">
         <v>23</v>
       </c>
@@ -1596,12 +1576,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:38" s="1" customFormat="1" ht="130.15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:38" s="1" customFormat="1" ht="129" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
-        <v>236</v>
+        <v>208</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C2" s="29" t="s">
         <v>1</v>
@@ -1625,7 +1605,7 @@
         <v>15</v>
       </c>
       <c r="J2" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K2" s="23" t="s">
         <v>11</v>
@@ -1637,13 +1617,13 @@
         <v>13</v>
       </c>
       <c r="N2" s="24" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="O2" s="23" t="s">
-        <v>233</v>
+        <v>206</v>
       </c>
       <c r="P2" s="23" t="s">
-        <v>232</v>
+        <v>205</v>
       </c>
       <c r="Q2" s="25" t="s">
         <v>20</v>
@@ -1652,10 +1632,10 @@
         <v>21</v>
       </c>
       <c r="S2" s="23" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="T2" s="40" t="s">
-        <v>241</v>
+        <v>213</v>
       </c>
       <c r="U2" s="23" t="s">
         <v>32</v>
@@ -1675,13 +1655,13 @@
       <c r="Z2" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="AA2" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="AB2" s="43"/>
-      <c r="AC2" s="43"/>
-    </row>
-    <row r="3" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="AA2" s="46" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB2" s="46"/>
+      <c r="AC2" s="46"/>
+    </row>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>0</v>
       </c>
@@ -1781,7 +1761,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="4" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -1877,7 +1857,7 @@
         <v>C00000</v>
       </c>
     </row>
-    <row r="5" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -1973,7 +1953,7 @@
         <v>600400</v>
       </c>
     </row>
-    <row r="6" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -2069,12 +2049,12 @@
         <v>5E0000</v>
       </c>
     </row>
-    <row r="7" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>4</v>
       </c>
-      <c r="B7" s="31" t="s">
-        <v>246</v>
+      <c r="B7" s="30" t="s">
+        <v>218</v>
       </c>
       <c r="C7" s="2">
         <v>0</v>
@@ -2165,7 +2145,7 @@
         <v>4F0000</v>
       </c>
     </row>
-    <row r="8" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>5</v>
       </c>
@@ -2261,7 +2241,7 @@
         <v>004000</v>
       </c>
     </row>
-    <row r="9" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>6</v>
       </c>
@@ -2357,7 +2337,7 @@
         <v>006000</v>
       </c>
     </row>
-    <row r="10" spans="1:38" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:38" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="33">
         <v>7</v>
       </c>
@@ -2453,7 +2433,7 @@
         <v>004200</v>
       </c>
     </row>
-    <row r="11" spans="1:38" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:38" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="33">
         <v>8</v>
       </c>
@@ -2549,7 +2529,7 @@
         <v>006200</v>
       </c>
     </row>
-    <row r="12" spans="1:38" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:38" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="33">
         <v>9</v>
       </c>
@@ -2617,7 +2597,7 @@
         <v>000100</v>
       </c>
     </row>
-    <row r="13" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>10</v>
       </c>
@@ -2709,19 +2689,19 @@
         <v>00</v>
       </c>
       <c r="AE13" s="5" t="s">
-        <v>251</v>
+        <v>223</v>
       </c>
       <c r="AL13" s="8" t="str">
         <f t="shared" ref="AL13:AL44" si="4">AA13 &amp; AB13 &amp; AC13</f>
         <v>181800</v>
       </c>
     </row>
-    <row r="14" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>11</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>253</v>
+        <v>224</v>
       </c>
       <c r="C14" s="2">
         <v>0</v>
@@ -2760,7 +2740,7 @@
         <v>1</v>
       </c>
       <c r="O14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P14" s="2">
         <v>0</v>
@@ -2801,7 +2781,7 @@
       </c>
       <c r="AB14" s="12" t="str">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="AC14" s="13" t="str">
         <f t="shared" si="2"/>
@@ -2809,10 +2789,10 @@
       </c>
       <c r="AL14" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>091000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:38" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+        <v>091800</v>
+      </c>
+    </row>
+    <row r="15" spans="1:38" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="33">
         <v>12</v>
       </c>
@@ -2859,7 +2839,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="16" spans="1:38" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:38" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="33">
         <v>13</v>
       </c>
@@ -2906,7 +2886,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="17" spans="1:38" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:38" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="33">
         <v>14</v>
       </c>
@@ -2953,7 +2933,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="18" spans="1:38" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:38" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="33">
         <v>15</v>
       </c>
@@ -3000,12 +2980,12 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="19" spans="1:38" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:38" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="33">
         <v>16</v>
       </c>
       <c r="B19" s="34" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="O19" s="8">
         <v>0</v>
@@ -3032,19 +3012,19 @@
         <v>00</v>
       </c>
       <c r="AE19" s="8" t="s">
-        <v>200</v>
+        <v>178</v>
       </c>
       <c r="AL19" s="8" t="str">
         <f t="shared" si="4"/>
         <v>000000</v>
       </c>
     </row>
-    <row r="20" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>17</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -3131,14 +3111,14 @@
         <v>80</v>
       </c>
       <c r="AE20" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="AL20" s="8" t="str">
         <f t="shared" si="4"/>
         <v>000080</v>
       </c>
     </row>
-    <row r="21" spans="1:38" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:38" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>18</v>
       </c>
@@ -3167,7 +3147,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="22" spans="1:38" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:38" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>19</v>
       </c>
@@ -3196,7 +3176,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="23" spans="1:38" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:38" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>20</v>
       </c>
@@ -3225,7 +3205,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="24" spans="1:38" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:38" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>21</v>
       </c>
@@ -3254,7 +3234,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="25" spans="1:38" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:38" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>22</v>
       </c>
@@ -3283,7 +3263,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="26" spans="1:38" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:38" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>23</v>
       </c>
@@ -3312,7 +3292,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="27" spans="1:38" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:38" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>24</v>
       </c>
@@ -3341,7 +3321,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="28" spans="1:38" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:38" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>25</v>
       </c>
@@ -3370,7 +3350,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="29" spans="1:38" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:38" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>26</v>
       </c>
@@ -3399,7 +3379,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="30" spans="1:38" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:38" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>27</v>
       </c>
@@ -3428,7 +3408,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="31" spans="1:38" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:38" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>28</v>
       </c>
@@ -3457,7 +3437,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="32" spans="1:38" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:38" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>29</v>
       </c>
@@ -3486,7 +3466,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="33" spans="1:38" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:38" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>30</v>
       </c>
@@ -3515,7 +3495,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="34" spans="1:38" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:38" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>31</v>
       </c>
@@ -3544,7 +3524,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="35" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>32</v>
       </c>
@@ -3636,14 +3616,14 @@
         <v>25</v>
       </c>
       <c r="AE35" t="s">
-        <v>234</v>
+        <v>207</v>
       </c>
       <c r="AL35" s="8" t="str">
         <f t="shared" si="4"/>
         <v>408825</v>
       </c>
     </row>
-    <row r="36" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>33</v>
       </c>
@@ -3735,14 +3715,14 @@
         <v>18</v>
       </c>
       <c r="AE36" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
       <c r="AL36" s="8" t="str">
         <f t="shared" si="4"/>
         <v>408818</v>
       </c>
     </row>
-    <row r="37" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>34</v>
       </c>
@@ -3838,7 +3818,7 @@
         <v>408802</v>
       </c>
     </row>
-    <row r="38" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>35</v>
       </c>
@@ -3934,7 +3914,7 @@
         <v>40882E</v>
       </c>
     </row>
-    <row r="39" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>36</v>
       </c>
@@ -4030,7 +4010,7 @@
         <v>40883A</v>
       </c>
     </row>
-    <row r="40" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>37</v>
       </c>
@@ -4126,12 +4106,12 @@
         <v>40881A</v>
       </c>
     </row>
-    <row r="41" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>38</v>
       </c>
       <c r="B41" s="30" t="s">
-        <v>237</v>
+        <v>209</v>
       </c>
       <c r="C41" s="6">
         <v>0</v>
@@ -4222,12 +4202,12 @@
         <v>408806</v>
       </c>
     </row>
-    <row r="42" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>39</v>
       </c>
       <c r="B42" s="30" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="C42" s="6">
         <v>0</v>
@@ -4318,12 +4298,12 @@
         <v>408826</v>
       </c>
     </row>
-    <row r="43" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>40</v>
       </c>
       <c r="B43" s="30" t="s">
-        <v>239</v>
+        <v>211</v>
       </c>
       <c r="C43" s="6">
         <v>0</v>
@@ -4414,12 +4394,12 @@
         <v>408800</v>
       </c>
     </row>
-    <row r="44" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>41</v>
       </c>
       <c r="B44" s="30" t="s">
-        <v>240</v>
+        <v>212</v>
       </c>
       <c r="C44" s="6">
         <v>0</v>
@@ -4510,7 +4490,7 @@
         <v>40883D</v>
       </c>
     </row>
-    <row r="46" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:38" x14ac:dyDescent="0.3">
       <c r="B46" s="3" t="s">
         <v>22</v>
       </c>
@@ -4518,7 +4498,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:38" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:38" x14ac:dyDescent="0.3">
       <c r="B47" s="5" t="s">
         <v>30</v>
       </c>
@@ -4526,23 +4506,23 @@
         <v>31</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B49" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C49" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B50" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C50" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B51" s="1" t="s">
         <v>47</v>
       </c>
@@ -4550,35 +4530,35 @@
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A52"/>
       <c r="B52" s="1" t="s">
-        <v>50</v>
+        <v>245</v>
       </c>
       <c r="C52" t="s">
-        <v>96</v>
+        <v>246</v>
       </c>
       <c r="Q52"/>
       <c r="R52"/>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A53"/>
       <c r="B53" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C53" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q53"/>
       <c r="R53"/>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A54"/>
       <c r="B54" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C54" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="Q54"/>
       <c r="R54"/>
@@ -4601,80 +4581,80 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="9.140625" style="7"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="9.109375" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>54</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>58</v>
-      </c>
       <c r="E4" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>63</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -4682,67 +4662,67 @@
         <v>4</v>
       </c>
       <c r="B6" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>68</v>
-      </c>
       <c r="E6" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" t="s">
         <v>69</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F7" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" t="s">
         <v>74</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F8" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" t="s">
         <v>77</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F9" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -4755,88 +4735,88 @@
   <dimension ref="A1:X135"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J93" sqref="J93"/>
+      <pane ySplit="1" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L131" sqref="L131"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" style="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="3" style="12" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.42578125" style="16" customWidth="1"/>
-    <col min="13" max="14" width="9.140625" style="2"/>
-    <col min="15" max="15" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.85546875" style="18" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="3.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.44140625" style="16" customWidth="1"/>
+    <col min="13" max="14" width="9.109375" style="2"/>
+    <col min="15" max="15" width="10.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.88671875" style="18" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3.44140625" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>212</v>
+        <v>190</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>202</v>
+        <v>180</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>202</v>
+        <v>180</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>203</v>
+        <v>181</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>213</v>
+        <v>191</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>211</v>
+        <v>189</v>
       </c>
       <c r="L1" s="19" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="M1" s="20" t="s">
-        <v>205</v>
+        <v>183</v>
       </c>
       <c r="N1" s="20" t="s">
-        <v>206</v>
+        <v>184</v>
       </c>
       <c r="O1" s="20" t="s">
-        <v>208</v>
+        <v>186</v>
       </c>
       <c r="P1" s="21" t="s">
-        <v>207</v>
-      </c>
-      <c r="Q1" s="45" t="s">
-        <v>210</v>
-      </c>
-      <c r="R1" s="46"/>
-      <c r="S1" s="47"/>
+        <v>185</v>
+      </c>
+      <c r="Q1" s="47" t="s">
+        <v>188</v>
+      </c>
+      <c r="R1" s="48"/>
+      <c r="S1" s="49"/>
       <c r="T1" s="10"/>
     </row>
-    <row r="2" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="8" t="s">
-        <v>242</v>
+        <v>214</v>
       </c>
       <c r="M2" s="17"/>
       <c r="N2" s="17"/>
       <c r="O2" s="17"/>
       <c r="U2" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
@@ -4845,7 +4825,7 @@
         <v>0x000</v>
       </c>
       <c r="C3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="11">
@@ -4900,7 +4880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4909,10 +4889,10 @@
         <v>0x003</v>
       </c>
       <c r="C4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>209</v>
+        <v>187</v>
       </c>
       <c r="F4" s="11">
         <v>1</v>
@@ -4966,7 +4946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>6</v>
       </c>
@@ -4975,7 +4955,7 @@
         <v>0x006</v>
       </c>
       <c r="C5" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="11">
@@ -5030,7 +5010,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>9</v>
       </c>
@@ -5039,7 +5019,7 @@
         <v>0x009</v>
       </c>
       <c r="C6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="11">
@@ -5091,7 +5071,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="E7" s="8"/>
       <c r="M7" s="17"/>
       <c r="N7" s="17"/>
@@ -5103,19 +5083,19 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C8" s="8" t="s">
-        <v>245</v>
+        <v>217</v>
       </c>
       <c r="E8" s="8"/>
       <c r="U8" t="s">
-        <v>218</v>
+        <v>196</v>
       </c>
       <c r="V8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0</v>
       </c>
@@ -5124,7 +5104,7 @@
         <v>0x000</v>
       </c>
       <c r="C9" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="11">
@@ -5173,13 +5153,13 @@
         <v>00</v>
       </c>
       <c r="U9" s="38" t="s">
-        <v>219</v>
+        <v>197</v>
       </c>
       <c r="V9" s="38">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3</v>
       </c>
@@ -5188,7 +5168,7 @@
         <v>0x003</v>
       </c>
       <c r="C10" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
       <c r="F10" s="11">
         <v>40</v>
@@ -5233,13 +5213,13 @@
         <v>00</v>
       </c>
       <c r="U10" s="38" t="s">
-        <v>247</v>
+        <v>219</v>
       </c>
       <c r="V10" s="38">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>6</v>
       </c>
@@ -5248,7 +5228,7 @@
         <v>0x006</v>
       </c>
       <c r="C11" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
       <c r="F11" s="11">
         <v>5</v>
@@ -5293,18 +5273,18 @@
         <v>03</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C16" s="8" t="s">
-        <v>248</v>
+        <v>220</v>
       </c>
       <c r="U16" t="s">
-        <v>216</v>
+        <v>194</v>
       </c>
       <c r="V16">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>0</v>
       </c>
@@ -5313,7 +5293,7 @@
         <v>0x000</v>
       </c>
       <c r="C17" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F17" s="11">
         <v>1</v>
@@ -5361,20 +5341,20 @@
         <v>00</v>
       </c>
       <c r="U17" t="s">
-        <v>214</v>
+        <v>192</v>
       </c>
       <c r="V17">
         <v>1</v>
       </c>
       <c r="W17" t="s">
-        <v>215</v>
+        <v>193</v>
       </c>
       <c r="X17">
         <f>VLOOKUP(W17,U16:V18,2)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>3</v>
       </c>
@@ -5383,7 +5363,7 @@
         <v>0x003</v>
       </c>
       <c r="C18" t="s">
-        <v>249</v>
+        <v>221</v>
       </c>
       <c r="F18" s="11">
         <v>1</v>
@@ -5431,13 +5411,13 @@
         <v>FF</v>
       </c>
       <c r="U18" t="s">
-        <v>215</v>
+        <v>193</v>
       </c>
       <c r="V18">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>6</v>
       </c>
@@ -5446,7 +5426,7 @@
         <v>0x006</v>
       </c>
       <c r="C19" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
       <c r="F19" s="11">
         <v>40</v>
@@ -5491,7 +5471,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="20" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>9</v>
       </c>
@@ -5500,10 +5480,10 @@
         <v>0x009</v>
       </c>
       <c r="C20" t="s">
-        <v>250</v>
+        <v>222</v>
       </c>
       <c r="E20" s="39" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F20" s="11">
         <v>41</v>
@@ -5548,7 +5528,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="21" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>12</v>
       </c>
@@ -5557,7 +5537,7 @@
         <v>0x00C</v>
       </c>
       <c r="C21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E21" s="39"/>
       <c r="F21" s="11">
@@ -5603,43 +5583,43 @@
         <v>06</v>
       </c>
     </row>
-    <row r="22" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="E22" s="39"/>
       <c r="M22" s="17"/>
       <c r="N22" s="17"/>
       <c r="O22" s="17"/>
     </row>
-    <row r="23" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="E23" s="39"/>
       <c r="M23" s="17"/>
       <c r="N23" s="17"/>
       <c r="O23" s="17"/>
     </row>
-    <row r="24" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
       <c r="E24" s="39"/>
       <c r="M24" s="17"/>
       <c r="N24" s="17"/>
       <c r="O24" s="17"/>
     </row>
-    <row r="25" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="E25" s="39"/>
       <c r="M25" s="17"/>
       <c r="N25" s="17"/>
       <c r="O25" s="17"/>
     </row>
-    <row r="26" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
       <c r="M26" s="17"/>
       <c r="N26" s="17"/>
       <c r="O26" s="17"/>
     </row>
-    <row r="30" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="31" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>0</v>
       </c>
@@ -5648,7 +5628,7 @@
         <v>0x000</v>
       </c>
       <c r="C31" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F31" s="11">
         <v>1</v>
@@ -5696,7 +5676,7 @@
         <v>01</v>
       </c>
     </row>
-    <row r="32" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>3</v>
       </c>
@@ -5705,7 +5685,7 @@
         <v>0x003</v>
       </c>
       <c r="C32" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F32" s="11">
         <v>1</v>
@@ -5753,7 +5733,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>6</v>
       </c>
@@ -5762,7 +5742,7 @@
         <v>0x006</v>
       </c>
       <c r="C33" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F33" s="11">
         <v>32</v>
@@ -5810,7 +5790,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>9</v>
       </c>
@@ -5819,7 +5799,7 @@
         <v>0x009</v>
       </c>
       <c r="C34" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F34" s="11">
         <v>6</v>
@@ -5860,7 +5840,7 @@
         <v>0F</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>12</v>
       </c>
@@ -5869,7 +5849,7 @@
         <v>0x00C</v>
       </c>
       <c r="C35" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F35" s="11">
         <v>5</v>
@@ -5910,7 +5890,7 @@
         <v>06</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>15</v>
       </c>
@@ -5919,7 +5899,7 @@
         <v>0x00F</v>
       </c>
       <c r="C36" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F36" s="11">
         <v>5</v>
@@ -5960,12 +5940,12 @@
         <v>0F</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C40" s="8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="41" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>0</v>
       </c>
@@ -5974,7 +5954,7 @@
         <v>0x000</v>
       </c>
       <c r="C41" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F41" s="11">
         <v>3</v>
@@ -6022,7 +6002,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>3</v>
       </c>
@@ -6031,7 +6011,7 @@
         <v>0x003</v>
       </c>
       <c r="C42" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F42" s="11">
         <v>10</v>
@@ -6079,7 +6059,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>6</v>
       </c>
@@ -6088,7 +6068,7 @@
         <v>0x006</v>
       </c>
       <c r="C43" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F43" s="11">
         <v>5</v>
@@ -6129,7 +6109,7 @@
         <v>06</v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>16</v>
       </c>
@@ -6138,23 +6118,21 @@
         <v>0x010</v>
       </c>
       <c r="D44" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="C46" s="38"/>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="C48" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="E44" s="8" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="46" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="C46" s="38" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="48" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="C48" s="8" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="49" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>0</v>
       </c>
@@ -6163,10 +6141,10 @@
         <v>0x000</v>
       </c>
       <c r="C49" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F49" s="11">
         <v>1</v>
@@ -6214,7 +6192,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>3</v>
       </c>
@@ -6223,7 +6201,7 @@
         <v>0x003</v>
       </c>
       <c r="C50" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F50" s="11">
         <v>17</v>
@@ -6267,17 +6245,17 @@
         <v>00</v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
       <c r="M51" s="17"/>
       <c r="N51" s="17"/>
       <c r="O51" s="17"/>
     </row>
-    <row r="55" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C55" s="8" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>0</v>
       </c>
@@ -6286,19 +6264,17 @@
         <v>0x000</v>
       </c>
       <c r="C56" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="F56" s="48" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="57" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+      <c r="F56" s="43"/>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>3</v>
       </c>
@@ -6307,14 +6283,14 @@
         <v>0x003</v>
       </c>
       <c r="C57" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E57" s="8"/>
     </row>
-    <row r="58" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>6</v>
       </c>
@@ -6323,16 +6299,16 @@
         <v>0x006</v>
       </c>
       <c r="C58" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="59" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>9</v>
       </c>
@@ -6341,14 +6317,14 @@
         <v>0x009</v>
       </c>
       <c r="C59" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E59" s="8"/>
     </row>
-    <row r="60" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>12</v>
       </c>
@@ -6357,16 +6333,16 @@
         <v>0x00C</v>
       </c>
       <c r="C60" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E60" s="8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="61" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>15</v>
       </c>
@@ -6375,14 +6351,14 @@
         <v>0x00F</v>
       </c>
       <c r="C61" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E61" s="8"/>
     </row>
-    <row r="62" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>18</v>
       </c>
@@ -6391,16 +6367,16 @@
         <v>0x012</v>
       </c>
       <c r="C62" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E62" s="8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="63" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>21</v>
       </c>
@@ -6409,14 +6385,14 @@
         <v>0x015</v>
       </c>
       <c r="C63" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E63" s="8"/>
     </row>
-    <row r="64" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>24</v>
       </c>
@@ -6425,16 +6401,16 @@
         <v>0x018</v>
       </c>
       <c r="C64" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>27</v>
       </c>
@@ -6443,14 +6419,14 @@
         <v>0x01B</v>
       </c>
       <c r="C65" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E65" s="8"/>
     </row>
-    <row r="66" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>30</v>
       </c>
@@ -6459,16 +6435,16 @@
         <v>0x01E</v>
       </c>
       <c r="C66" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E66" s="8" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>33</v>
       </c>
@@ -6477,14 +6453,14 @@
         <v>0x021</v>
       </c>
       <c r="C67" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E67" s="8"/>
     </row>
-    <row r="68" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>36</v>
       </c>
@@ -6493,16 +6469,16 @@
         <v>0x024</v>
       </c>
       <c r="C68" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D68" s="7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E68" s="8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>39</v>
       </c>
@@ -6511,14 +6487,14 @@
         <v>0x027</v>
       </c>
       <c r="C69" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E69" s="8"/>
     </row>
-    <row r="70" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>42</v>
       </c>
@@ -6527,16 +6503,16 @@
         <v>0x02A</v>
       </c>
       <c r="C70" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D70" s="7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>45</v>
       </c>
@@ -6545,14 +6521,14 @@
         <v>0x02D</v>
       </c>
       <c r="C71" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E71" s="8"/>
     </row>
-    <row r="72" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>48</v>
       </c>
@@ -6561,16 +6537,16 @@
         <v>0x030</v>
       </c>
       <c r="C72" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D72" s="7" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>51</v>
       </c>
@@ -6579,14 +6555,14 @@
         <v>0x033</v>
       </c>
       <c r="C73" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D73" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E73" s="8"/>
     </row>
-    <row r="74" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>54</v>
       </c>
@@ -6595,16 +6571,16 @@
         <v>0x036</v>
       </c>
       <c r="C74" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D74" s="7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E74" s="8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>57</v>
       </c>
@@ -6613,14 +6589,14 @@
         <v>0x039</v>
       </c>
       <c r="C75" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D75" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E75" s="8"/>
     </row>
-    <row r="76" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>60</v>
       </c>
@@ -6629,16 +6605,16 @@
         <v>0x03C</v>
       </c>
       <c r="C76" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D76" s="7" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E76" s="8" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>63</v>
       </c>
@@ -6647,14 +6623,14 @@
         <v>0x03F</v>
       </c>
       <c r="C77" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D77" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E77" s="8"/>
     </row>
-    <row r="78" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>66</v>
       </c>
@@ -6663,16 +6639,16 @@
         <v>0x042</v>
       </c>
       <c r="C78" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D78" s="7" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>69</v>
       </c>
@@ -6681,28 +6657,28 @@
         <v>0x045</v>
       </c>
       <c r="C79" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D79" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E79" s="8"/>
     </row>
-    <row r="80" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E80" s="8"/>
     </row>
-    <row r="81" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D81"/>
       <c r="E81" s="8"/>
     </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C82" s="8" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D82"/>
       <c r="E82" s="8"/>
     </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>0</v>
       </c>
@@ -6711,17 +6687,17 @@
         <v>0x000</v>
       </c>
       <c r="C83" t="s">
-        <v>258</v>
+        <v>228</v>
       </c>
       <c r="D83"/>
       <c r="E83" s="8" t="s">
-        <v>257</v>
+        <v>227</v>
       </c>
       <c r="F83" s="11">
         <v>1</v>
       </c>
       <c r="G83" s="12" t="s">
-        <v>219</v>
+        <v>197</v>
       </c>
       <c r="H83">
         <f t="shared" ref="H83" si="85">IF(G83="", "", VLOOKUP(G83, $U$3:$V$10, 2))</f>
@@ -6763,7 +6739,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>3</v>
       </c>
@@ -6772,16 +6748,16 @@
         <v>0x003</v>
       </c>
       <c r="C84" t="s">
-        <v>259</v>
+        <v>229</v>
       </c>
       <c r="E84" s="8" t="s">
-        <v>256</v>
+        <v>226</v>
       </c>
       <c r="F84" s="11">
         <v>1</v>
       </c>
       <c r="G84" s="12" t="s">
-        <v>247</v>
+        <v>219</v>
       </c>
       <c r="H84">
         <f t="shared" ref="H84:H86" si="94">IF(G84="", "", VLOOKUP(G84, $U$3:$V$10, 2))</f>
@@ -6823,7 +6799,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>6</v>
       </c>
@@ -6832,16 +6808,16 @@
         <v>0x006</v>
       </c>
       <c r="C85" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="E85" s="8" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="F85" s="11">
         <v>1</v>
       </c>
       <c r="G85" s="12" t="s">
-        <v>218</v>
+        <v>196</v>
       </c>
       <c r="H85">
         <f t="shared" si="94"/>
@@ -6883,7 +6859,7 @@
         <v>3C</v>
       </c>
     </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>9</v>
       </c>
@@ -6892,10 +6868,10 @@
         <v>0x009</v>
       </c>
       <c r="C86" t="s">
-        <v>255</v>
+        <v>225</v>
       </c>
       <c r="E86" s="8" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="F86" s="11">
         <v>4</v>
@@ -6905,9 +6881,6 @@
       </c>
       <c r="H86">
         <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="K86">
         <v>0</v>
       </c>
       <c r="L86" s="16" t="str">
@@ -6928,7 +6901,7 @@
       </c>
       <c r="P86" s="18" t="str">
         <f t="shared" si="99"/>
-        <v>00000000</v>
+        <v/>
       </c>
       <c r="Q86" t="str">
         <f t="shared" si="100"/>
@@ -6943,7 +6916,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>12</v>
       </c>
@@ -6952,16 +6925,16 @@
         <v>0x00C</v>
       </c>
       <c r="C87" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D87"/>
       <c r="E87" s="8" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="F87" s="11">
         <v>17</v>
       </c>
-      <c r="G87" s="50" t="s">
+      <c r="G87" s="45" t="s">
         <v>38</v>
       </c>
       <c r="H87">
@@ -7004,7 +6977,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>15</v>
       </c>
@@ -7013,14 +6986,14 @@
         <v>0x00F</v>
       </c>
       <c r="C88" t="s">
-        <v>260</v>
-      </c>
-      <c r="E88" s="49"/>
+        <v>230</v>
+      </c>
+      <c r="E88" s="44"/>
       <c r="F88" s="11">
         <v>40</v>
       </c>
       <c r="G88" s="12" t="s">
-        <v>247</v>
+        <v>219</v>
       </c>
       <c r="H88">
         <f t="shared" si="103"/>
@@ -7059,7 +7032,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>18</v>
       </c>
@@ -7068,10 +7041,10 @@
         <v>0x012</v>
       </c>
       <c r="C89" t="s">
-        <v>264</v>
+        <v>234</v>
       </c>
       <c r="E89" s="8" t="s">
-        <v>265</v>
+        <v>235</v>
       </c>
       <c r="F89" s="11">
         <v>2</v>
@@ -7119,7 +7092,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>21</v>
       </c>
@@ -7128,16 +7101,16 @@
         <v>0x015</v>
       </c>
       <c r="C90" t="s">
-        <v>261</v>
+        <v>231</v>
       </c>
       <c r="E90" s="8" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="F90" s="11">
         <v>33</v>
       </c>
       <c r="G90" s="12" t="s">
-        <v>247</v>
+        <v>219</v>
       </c>
       <c r="H90">
         <f t="shared" ref="H90" si="117">IF(G90="", "", VLOOKUP(G90, $U$3:$V$10, 2))</f>
@@ -7179,7 +7152,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>24</v>
       </c>
@@ -7188,10 +7161,10 @@
         <v>0x018</v>
       </c>
       <c r="C91" t="s">
-        <v>262</v>
+        <v>232</v>
       </c>
       <c r="E91" s="8" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="F91" s="11">
         <v>6</v>
@@ -7236,7 +7209,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>27</v>
       </c>
@@ -7245,16 +7218,16 @@
         <v>0x01B</v>
       </c>
       <c r="C92" t="s">
-        <v>266</v>
+        <v>236</v>
       </c>
       <c r="E92" s="8" t="s">
-        <v>267</v>
+        <v>237</v>
       </c>
       <c r="F92" s="11">
         <v>2</v>
       </c>
       <c r="G92" s="12" t="s">
-        <v>247</v>
+        <v>219</v>
       </c>
       <c r="H92">
         <f t="shared" si="122"/>
@@ -7296,7 +7269,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>30</v>
       </c>
@@ -7305,10 +7278,10 @@
         <v>0x01E</v>
       </c>
       <c r="C93" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E93" s="8" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="F93" s="11">
         <v>5</v>
@@ -7353,12 +7326,12 @@
         <v>09</v>
       </c>
     </row>
-    <row r="94" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E94" s="8" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="95" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>48</v>
       </c>
@@ -7367,13 +7340,13 @@
         <v>0x030</v>
       </c>
       <c r="D95" s="7" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="E95" s="8" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="96" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>51</v>
       </c>
@@ -7382,13 +7355,13 @@
         <v>0x033</v>
       </c>
       <c r="D96" s="7" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="E96" s="9" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>54</v>
       </c>
@@ -7397,13 +7370,13 @@
         <v>0x036</v>
       </c>
       <c r="D97" s="7" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="E97" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>57</v>
       </c>
@@ -7412,30 +7385,28 @@
         <v>0x039</v>
       </c>
       <c r="D98" s="7" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="E98" s="8" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C99" s="5" t="s">
-        <v>268</v>
-      </c>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C99" s="5"/>
       <c r="E99" s="8"/>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D100"/>
       <c r="E100" s="8"/>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C101" s="8" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D101"/>
       <c r="E101" s="8"/>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>0</v>
       </c>
@@ -7444,13 +7415,13 @@
         <v>0x000</v>
       </c>
       <c r="C102" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E102" s="8" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>3</v>
       </c>
@@ -7459,13 +7430,13 @@
         <v>0x003</v>
       </c>
       <c r="C103" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E103" s="8" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>6</v>
       </c>
@@ -7474,14 +7445,14 @@
         <v>0x006</v>
       </c>
       <c r="C104" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="D104"/>
       <c r="E104" s="8" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>9</v>
       </c>
@@ -7490,11 +7461,11 @@
         <v>0x009</v>
       </c>
       <c r="C105" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E105" s="8"/>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>12</v>
       </c>
@@ -7503,126 +7474,259 @@
         <v>0x00C</v>
       </c>
       <c r="C106" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
       <c r="E106" s="8"/>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C107" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E107" s="8" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C108" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="E108" s="8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C109" t="s">
+        <v>241</v>
+      </c>
+      <c r="E109" s="8"/>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C110" t="s">
+        <v>198</v>
+      </c>
+      <c r="E110" s="8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C111" t="s">
+        <v>80</v>
+      </c>
+      <c r="E111" s="8" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="115" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="C115" s="8" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C109" t="s">
-        <v>81</v>
-      </c>
-      <c r="E109" s="8"/>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C110" t="s">
-        <v>220</v>
-      </c>
-      <c r="E110" s="8" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C111" t="s">
-        <v>84</v>
-      </c>
-      <c r="E111" s="8" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C112" t="s">
-        <v>82</v>
-      </c>
-      <c r="E112" s="8" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="116" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C116" s="8" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="117" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A116">
+        <v>0</v>
+      </c>
+      <c r="B116" t="str">
+        <f t="shared" ref="B116:B131" si="139">"0x" &amp; DEC2HEX(A116,3)</f>
+        <v>0x000</v>
+      </c>
+      <c r="C116" t="s">
+        <v>152</v>
+      </c>
+      <c r="E116" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="F116" s="11">
+        <v>1</v>
+      </c>
+      <c r="G116" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="H116">
+        <f t="shared" ref="H116:H117" si="140">IF(G116="", "", VLOOKUP(G116, $U$3:$V$10, 2))</f>
+        <v>1</v>
+      </c>
+      <c r="K116">
+        <v>48</v>
+      </c>
+      <c r="L116" s="16" t="str">
+        <f t="shared" ref="L116:L117" si="141">IF(F116="", "", TEXT(DEC2BIN(F116), "000000"))</f>
+        <v>000001</v>
+      </c>
+      <c r="M116" s="17" t="str">
+        <f t="shared" ref="M116:M117" si="142">IF(H116="", "", TEXT(DEC2BIN(H116), "000"))</f>
+        <v>001</v>
+      </c>
+      <c r="N116" s="17" t="str">
+        <f t="shared" ref="N116:N117" si="143">IF(I116="", "", TEXT(DEC2BIN(I116), "000"))</f>
+        <v/>
+      </c>
+      <c r="O116" s="17" t="str">
+        <f t="shared" ref="O116:O117" si="144">IF(J116="", "", TEXT(DEC2BIN(J116), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="P116" s="18" t="str">
+        <f t="shared" ref="P116:P117" si="145">IF(K116="", "", TEXT(DEC2BIN(K116), "00000000"))</f>
+        <v>00110000</v>
+      </c>
+      <c r="Q116" t="str">
+        <f t="shared" ref="Q116:Q117" si="146">BIN2HEX(LEFT(CONCATENATE(L116,IF(M116="", "000", M116)), 8), 2)</f>
+        <v>04</v>
+      </c>
+      <c r="R116" t="str">
+        <f t="shared" ref="R116:R117" si="147">BIN2HEX(CONCATENATE(RIGHT(M116, 1), IF(N116 = "", "000", N116), "0000"), 2)</f>
+        <v>80</v>
+      </c>
+      <c r="S116" s="13" t="str">
+        <f t="shared" ref="S116:S117" si="148">IF(O116="", BIN2HEX(P116, 2), BIN2HEX(O116,2))</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="117" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A117">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B117" t="str">
-        <f t="shared" ref="B117:B121" si="139">"0x" &amp; DEC2HEX(A117,3)</f>
-        <v>0x000</v>
+        <f t="shared" si="139"/>
+        <v>0x003</v>
       </c>
       <c r="C117" t="s">
-        <v>160</v>
-      </c>
-      <c r="D117" s="7" t="s">
-        <v>161</v>
+        <v>204</v>
       </c>
       <c r="E117" s="8" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="118" spans="1:19" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+      <c r="F117" s="11">
+        <v>1</v>
+      </c>
+      <c r="G117" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="H117">
+        <f t="shared" si="140"/>
+        <v>7</v>
+      </c>
+      <c r="K117">
+        <v>57</v>
+      </c>
+      <c r="L117" s="16" t="str">
+        <f t="shared" si="141"/>
+        <v>000001</v>
+      </c>
+      <c r="M117" s="17" t="str">
+        <f t="shared" si="142"/>
+        <v>111</v>
+      </c>
+      <c r="N117" s="17" t="str">
+        <f t="shared" si="143"/>
+        <v/>
+      </c>
+      <c r="O117" s="17" t="str">
+        <f t="shared" si="144"/>
+        <v/>
+      </c>
+      <c r="P117" s="18" t="str">
+        <f t="shared" si="145"/>
+        <v>00111001</v>
+      </c>
+      <c r="Q117" t="str">
+        <f t="shared" si="146"/>
+        <v>07</v>
+      </c>
+      <c r="R117" t="str">
+        <f t="shared" si="147"/>
+        <v>80</v>
+      </c>
+      <c r="S117" s="13" t="str">
+        <f t="shared" si="148"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="118" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A118">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B118" t="str">
         <f t="shared" si="139"/>
-        <v>0x003</v>
+        <v>0x006</v>
       </c>
       <c r="C118" t="s">
-        <v>226</v>
-      </c>
-      <c r="D118" s="7" t="s">
-        <v>227</v>
+        <v>247</v>
       </c>
       <c r="E118" s="8" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="119" spans="1:19" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+      <c r="F118" s="11">
+        <v>1</v>
+      </c>
+      <c r="G118" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="H118">
+        <f t="shared" ref="H118" si="149">IF(G118="", "", VLOOKUP(G118, $U$3:$V$10, 2))</f>
+        <v>6</v>
+      </c>
+      <c r="K118">
+        <v>96</v>
+      </c>
+      <c r="L118" s="16" t="str">
+        <f>IF(F118="", "", TEXT(DEC2BIN(F118), "000000"))</f>
+        <v>000001</v>
+      </c>
+      <c r="M118" s="17" t="str">
+        <f>IF(H118="", "", TEXT(DEC2BIN(H118), "000"))</f>
+        <v>110</v>
+      </c>
+      <c r="N118" s="17" t="str">
+        <f>IF(I118="", "", TEXT(DEC2BIN(I118), "000"))</f>
+        <v/>
+      </c>
+      <c r="O118" s="17" t="str">
+        <f>IF(J118="", "", TEXT(DEC2BIN(J118), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="P118" s="18" t="str">
+        <f>IF(K118="", "", TEXT(DEC2BIN(K118), "00000000"))</f>
+        <v>01100000</v>
+      </c>
+      <c r="Q118" t="str">
+        <f t="shared" ref="Q118" si="150">BIN2HEX(LEFT(CONCATENATE(L118,IF(M118="", "000", M118)), 8), 2)</f>
+        <v>07</v>
+      </c>
+      <c r="R118" t="str">
+        <f>BIN2HEX(CONCATENATE(RIGHT(M118, 1), IF(N118 = "", "000", N118), "0000"), 2)</f>
+        <v>00</v>
+      </c>
+      <c r="S118" s="13" t="str">
+        <f t="shared" ref="S118" si="151">IF(O118="", BIN2HEX(P118, 2), BIN2HEX(O118,2))</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="119" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A119">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B119" t="str">
         <f t="shared" si="139"/>
-        <v>0x006</v>
+        <v>0x009</v>
       </c>
       <c r="C119" t="s">
-        <v>188</v>
-      </c>
-      <c r="D119" s="7" t="s">
         <v>228</v>
       </c>
       <c r="E119" s="8" t="s">
-        <v>201</v>
+        <v>243</v>
       </c>
       <c r="F119" s="11">
         <v>1</v>
       </c>
       <c r="G119" s="12" t="s">
-        <v>40</v>
+        <v>197</v>
       </c>
       <c r="H119">
-        <f t="shared" ref="H119" si="140">IF(G119="", "", VLOOKUP(G119, $U$3:$V$10, 2))</f>
-        <v>4</v>
+        <f>IF(G119="", "", VLOOKUP(G119, $U$3:$V$10, 2))</f>
+        <v>2</v>
       </c>
       <c r="K119">
-        <v>96</v>
+        <v>0</v>
       </c>
       <c r="L119" s="16" t="str">
         <f>IF(F119="", "", TEXT(DEC2BIN(F119), "000000"))</f>
@@ -7630,7 +7734,7 @@
       </c>
       <c r="M119" s="17" t="str">
         <f>IF(H119="", "", TEXT(DEC2BIN(H119), "000"))</f>
-        <v>100</v>
+        <v>010</v>
       </c>
       <c r="N119" s="17" t="str">
         <f>IF(I119="", "", TEXT(DEC2BIN(I119), "000"))</f>
@@ -7642,222 +7746,496 @@
       </c>
       <c r="P119" s="18" t="str">
         <f>IF(K119="", "", TEXT(DEC2BIN(K119), "00000000"))</f>
-        <v>01100000</v>
+        <v>00000000</v>
       </c>
       <c r="Q119" t="str">
-        <f t="shared" ref="Q119" si="141">BIN2HEX(LEFT(CONCATENATE(L119,IF(M119="", "000", M119)), 8), 2)</f>
-        <v>06</v>
+        <f>BIN2HEX(LEFT(CONCATENATE(L119,IF(M119="", "000", M119)), 8), 2)</f>
+        <v>05</v>
       </c>
       <c r="R119" t="str">
         <f>BIN2HEX(CONCATENATE(RIGHT(M119, 1), IF(N119 = "", "000", N119), "0000"), 2)</f>
         <v>00</v>
       </c>
       <c r="S119" s="13" t="str">
-        <f t="shared" ref="S119" si="142">IF(O119="", BIN2HEX(P119, 2), BIN2HEX(O119,2))</f>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
+        <f>IF(O119="", BIN2HEX(P119, 2), BIN2HEX(O119,2))</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="120" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A120">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B120" t="str">
         <f t="shared" si="139"/>
-        <v>0x009</v>
+        <v>0x00C</v>
       </c>
       <c r="C120" t="s">
-        <v>150</v>
-      </c>
-      <c r="D120" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="E120" s="8" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="121" spans="1:19" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+      <c r="E120" s="8"/>
+      <c r="F120" s="11">
+        <v>2</v>
+      </c>
+      <c r="G120" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="H120">
+        <f t="shared" ref="H120:H121" si="152">IF(G120="", "", VLOOKUP(G120, $U$3:$V$10, 2))</f>
+        <v>3</v>
+      </c>
+      <c r="I120">
+        <v>1</v>
+      </c>
+      <c r="L120" s="16" t="str">
+        <f t="shared" ref="L120:L121" si="153">IF(F120="", "", TEXT(DEC2BIN(F120), "000000"))</f>
+        <v>000010</v>
+      </c>
+      <c r="M120" s="17" t="str">
+        <f t="shared" ref="M120:M121" si="154">IF(H120="", "", TEXT(DEC2BIN(H120), "000"))</f>
+        <v>011</v>
+      </c>
+      <c r="N120" s="17" t="str">
+        <f t="shared" ref="N120:N121" si="155">IF(I120="", "", TEXT(DEC2BIN(I120), "000"))</f>
+        <v>001</v>
+      </c>
+      <c r="O120" s="17" t="str">
+        <f t="shared" ref="O120:O121" si="156">IF(J120="", "", TEXT(DEC2BIN(J120), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="P120" s="18" t="str">
+        <f t="shared" ref="P120:P121" si="157">IF(K120="", "", TEXT(DEC2BIN(K120), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="Q120" t="str">
+        <f t="shared" ref="Q120:Q121" si="158">BIN2HEX(LEFT(CONCATENATE(L120,IF(M120="", "000", M120)), 8), 2)</f>
+        <v>09</v>
+      </c>
+      <c r="R120" t="str">
+        <f t="shared" ref="R120:R121" si="159">BIN2HEX(CONCATENATE(RIGHT(M120, 1), IF(N120 = "", "000", N120), "0000"), 2)</f>
+        <v>90</v>
+      </c>
+      <c r="S120" s="13" t="str">
+        <f t="shared" ref="S120:S121" si="160">IF(O120="", BIN2HEX(P120, 2), BIN2HEX(O120,2))</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="121" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A121">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B121" t="str">
         <f t="shared" si="139"/>
-        <v>0x00C</v>
+        <v>0x00F</v>
       </c>
       <c r="C121" t="s">
+        <v>225</v>
+      </c>
+      <c r="E121" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="D121" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="E121" s="8" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="122" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F121" s="11">
+        <v>4</v>
+      </c>
+      <c r="G121" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="H121">
+        <f t="shared" si="152"/>
+        <v>0</v>
+      </c>
+      <c r="L121" s="16" t="str">
+        <f t="shared" si="153"/>
+        <v>000100</v>
+      </c>
+      <c r="M121" s="17" t="str">
+        <f t="shared" si="154"/>
+        <v>000</v>
+      </c>
+      <c r="N121" s="17" t="str">
+        <f t="shared" si="155"/>
+        <v/>
+      </c>
+      <c r="O121" s="17" t="str">
+        <f t="shared" si="156"/>
+        <v/>
+      </c>
+      <c r="P121" s="18" t="str">
+        <f t="shared" si="157"/>
+        <v/>
+      </c>
+      <c r="Q121" t="str">
+        <f t="shared" si="158"/>
+        <v>10</v>
+      </c>
+      <c r="R121" t="str">
+        <f t="shared" si="159"/>
+        <v>00</v>
+      </c>
+      <c r="S121" s="13" t="str">
+        <f t="shared" si="160"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="122" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A122">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B122" t="str">
-        <f t="shared" ref="B122:B135" si="143">"0x" &amp; DEC2HEX(A122,3)</f>
-        <v>0x00F</v>
+        <f t="shared" si="139"/>
+        <v>0x012</v>
       </c>
       <c r="C122" t="s">
-        <v>189</v>
-      </c>
-      <c r="D122" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="E122" s="8" t="s">
-        <v>190</v>
-      </c>
+        <v>248</v>
+      </c>
+      <c r="E122" s="8"/>
       <c r="F122" s="11">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="G122" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="H122">
+        <f t="shared" ref="H122:H123" si="161">IF(G122="", "", VLOOKUP(G122, $U$3:$V$10, 2))</f>
+        <v>3</v>
+      </c>
+      <c r="I122">
+        <v>6</v>
+      </c>
+      <c r="L122" s="16" t="str">
+        <f t="shared" ref="L122:L123" si="162">IF(F122="", "", TEXT(DEC2BIN(F122), "000000"))</f>
+        <v>000010</v>
+      </c>
+      <c r="M122" s="17" t="str">
+        <f t="shared" ref="M122:M123" si="163">IF(H122="", "", TEXT(DEC2BIN(H122), "000"))</f>
+        <v>011</v>
+      </c>
+      <c r="N122" s="17" t="str">
+        <f t="shared" ref="N122:N123" si="164">IF(I122="", "", TEXT(DEC2BIN(I122), "000"))</f>
+        <v>110</v>
+      </c>
+      <c r="O122" s="17" t="str">
+        <f t="shared" ref="O122:O123" si="165">IF(J122="", "", TEXT(DEC2BIN(J122), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="P122" s="18" t="str">
+        <f t="shared" ref="P122:P123" si="166">IF(K122="", "", TEXT(DEC2BIN(K122), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="Q122" t="str">
+        <f t="shared" ref="Q122:Q123" si="167">BIN2HEX(LEFT(CONCATENATE(L122,IF(M122="", "000", M122)), 8), 2)</f>
+        <v>09</v>
+      </c>
+      <c r="R122" t="str">
+        <f t="shared" ref="R122:R123" si="168">BIN2HEX(CONCATENATE(RIGHT(M122, 1), IF(N122 = "", "000", N122), "0000"), 2)</f>
+        <v>E0</v>
+      </c>
+      <c r="S122" s="13" t="str">
+        <f t="shared" ref="S122:S123" si="169">IF(O122="", BIN2HEX(P122, 2), BIN2HEX(O122,2))</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="123" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A123">
+        <v>21</v>
+      </c>
+      <c r="B123" t="str">
+        <f t="shared" si="139"/>
+        <v>0x015</v>
+      </c>
+      <c r="C123" t="s">
+        <v>238</v>
+      </c>
+      <c r="E123" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="F123" s="11">
+        <v>11</v>
+      </c>
+      <c r="G123" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="H122">
-        <f>IF(G122="", "", VLOOKUP(G122, $U$3:$V$10, 2))</f>
-        <v>0</v>
-      </c>
-      <c r="I122">
+      <c r="H123">
+        <f t="shared" si="161"/>
+        <v>0</v>
+      </c>
+      <c r="L123" s="16" t="str">
+        <f t="shared" si="162"/>
+        <v>001011</v>
+      </c>
+      <c r="M123" s="17" t="str">
+        <f t="shared" si="163"/>
+        <v>000</v>
+      </c>
+      <c r="N123" s="17" t="str">
+        <f t="shared" si="164"/>
+        <v/>
+      </c>
+      <c r="O123" s="17" t="str">
+        <f t="shared" si="165"/>
+        <v/>
+      </c>
+      <c r="P123" s="18" t="str">
+        <f t="shared" si="166"/>
+        <v/>
+      </c>
+      <c r="Q123" t="str">
+        <f t="shared" si="167"/>
+        <v>2C</v>
+      </c>
+      <c r="R123" t="str">
+        <f t="shared" si="168"/>
+        <v>00</v>
+      </c>
+      <c r="S123" s="13" t="str">
+        <f t="shared" si="169"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="124" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A124">
+        <v>24</v>
+      </c>
+      <c r="B124" t="str">
+        <f t="shared" si="139"/>
+        <v>0x018</v>
+      </c>
+      <c r="C124" t="s">
+        <v>239</v>
+      </c>
+      <c r="E124" s="50"/>
+      <c r="F124" s="11">
+        <v>40</v>
+      </c>
+      <c r="G124" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="H124">
+        <f t="shared" ref="H124:H128" si="170">IF(G124="", "", VLOOKUP(G124, $U$3:$V$10, 2))</f>
+        <v>1</v>
+      </c>
+      <c r="L124" s="16" t="str">
+        <f>IF(F124="", "", TEXT(DEC2BIN(F124), "000000"))</f>
+        <v>101000</v>
+      </c>
+      <c r="M124" s="17" t="str">
+        <f>IF(H124="", "", TEXT(DEC2BIN(H124), "000"))</f>
+        <v>001</v>
+      </c>
+      <c r="N124" s="17" t="str">
+        <f>IF(I124="", "", TEXT(DEC2BIN(I124), "000"))</f>
+        <v/>
+      </c>
+      <c r="O124" s="17" t="str">
+        <f>IF(J124="", "", TEXT(DEC2BIN(J124), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="P124" s="18" t="str">
+        <f>IF(K124="", "", TEXT(DEC2BIN(K124), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="Q124" t="str">
+        <f t="shared" ref="Q124:Q125" si="171">BIN2HEX(LEFT(CONCATENATE(L124,IF(M124="", "000", M124)), 8), 2)</f>
+        <v>A0</v>
+      </c>
+      <c r="R124" t="str">
+        <f>BIN2HEX(CONCATENATE(RIGHT(M124, 1), IF(N124 = "", "000", N124), "0000"), 2)</f>
+        <v>80</v>
+      </c>
+      <c r="S124" s="13" t="str">
+        <f t="shared" ref="S124:S125" si="172">IF(O124="", BIN2HEX(P124, 2), BIN2HEX(O124,2))</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="125" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A125">
+        <v>27</v>
+      </c>
+      <c r="B125" t="str">
+        <f t="shared" si="139"/>
+        <v>0x01B</v>
+      </c>
+      <c r="C125" t="s">
+        <v>58</v>
+      </c>
+      <c r="E125" s="50" t="s">
+        <v>240</v>
+      </c>
+      <c r="F125" s="11">
         <v>2</v>
       </c>
-      <c r="L122" s="16" t="str">
-        <f>IF(F122="", "", TEXT(DEC2BIN(F122), "000000"))</f>
-        <v>001110</v>
-      </c>
-      <c r="M122" s="17" t="str">
-        <f>IF(H122="", "", TEXT(DEC2BIN(H122), "000"))</f>
+      <c r="G125" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="H125">
+        <f t="shared" si="170"/>
+        <v>0</v>
+      </c>
+      <c r="I125">
+        <v>1</v>
+      </c>
+      <c r="L125" s="16" t="str">
+        <f t="shared" ref="L125" si="173">IF(F125="", "", TEXT(DEC2BIN(F125), "000000"))</f>
+        <v>000010</v>
+      </c>
+      <c r="M125" s="17" t="str">
+        <f t="shared" ref="M125:M128" si="174">IF(H125="", "", TEXT(DEC2BIN(H125), "000"))</f>
         <v>000</v>
       </c>
-      <c r="N122" s="17" t="str">
-        <f>IF(I122="", "", TEXT(DEC2BIN(I122), "000"))</f>
-        <v>010</v>
-      </c>
-      <c r="O122" s="17" t="str">
-        <f>IF(J122="", "", TEXT(DEC2BIN(J122), "00000000"))</f>
-        <v/>
-      </c>
-      <c r="P122" s="18" t="str">
-        <f>IF(K122="", "", TEXT(DEC2BIN(K122), "00000000"))</f>
-        <v/>
-      </c>
-      <c r="Q122" t="str">
-        <f t="shared" ref="Q122" si="144">BIN2HEX(LEFT(CONCATENATE(L122,IF(M122="", "000", M122)), 8), 2)</f>
+      <c r="N125" s="17" t="str">
+        <f t="shared" ref="N125:N128" si="175">IF(I125="", "", TEXT(DEC2BIN(I125), "000"))</f>
+        <v>001</v>
+      </c>
+      <c r="O125" s="17" t="str">
+        <f t="shared" ref="O125:O128" si="176">IF(J125="", "", TEXT(DEC2BIN(J125), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="P125" s="18" t="str">
+        <f t="shared" ref="P125:P128" si="177">IF(K125="", "", TEXT(DEC2BIN(K125), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="Q125" t="str">
+        <f t="shared" si="171"/>
+        <v>08</v>
+      </c>
+      <c r="R125" t="str">
+        <f t="shared" ref="R125" si="178">BIN2HEX(CONCATENATE(RIGHT(M125, 1), IF(N125 = "", "000", N125), "0000"), 2)</f>
+        <v>10</v>
+      </c>
+      <c r="S125" s="13" t="str">
+        <f t="shared" si="172"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="126" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A126">
+        <v>30</v>
+      </c>
+      <c r="B126" t="str">
+        <f t="shared" si="139"/>
+        <v>0x01E</v>
+      </c>
+      <c r="C126" t="s">
+        <v>151</v>
+      </c>
+      <c r="E126" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="F126" s="11">
+        <v>33</v>
+      </c>
+      <c r="G126" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="R122" t="str">
-        <f>BIN2HEX(CONCATENATE(RIGHT(M122, 1), IF(N122 = "", "000", N122), "0000"), 2)</f>
-        <v>20</v>
-      </c>
-      <c r="S122" s="13" t="str">
-        <f t="shared" ref="S122" si="145">IF(O122="", BIN2HEX(P122, 2), BIN2HEX(O122,2))</f>
-        <v>00</v>
-      </c>
-    </row>
-    <row r="123" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A123">
+      <c r="H126">
+        <f t="shared" si="170"/>
+        <v>0</v>
+      </c>
+      <c r="I126">
+        <v>7</v>
+      </c>
+      <c r="L126" s="16" t="str">
+        <f>IF(F126="", "", TEXT(DEC2BIN(F126), "000000"))</f>
+        <v>100001</v>
+      </c>
+      <c r="M126" s="17" t="str">
+        <f t="shared" si="174"/>
+        <v>000</v>
+      </c>
+      <c r="N126" s="17" t="str">
+        <f t="shared" si="175"/>
+        <v>111</v>
+      </c>
+      <c r="O126" s="17" t="str">
+        <f t="shared" si="176"/>
+        <v/>
+      </c>
+      <c r="P126" s="18" t="str">
+        <f t="shared" si="177"/>
+        <v/>
+      </c>
+      <c r="Q126" t="str">
+        <f>BIN2HEX(LEFT(CONCATENATE(L126,IF(M126="", "000", M126)), 8), 2)</f>
+        <v>84</v>
+      </c>
+      <c r="R126" t="str">
+        <f>BIN2HEX(CONCATENATE(RIGHT(M126, 1), IF(N126 = "", "000", N126), "0000"), 2)</f>
+        <v>70</v>
+      </c>
+      <c r="S126" s="13" t="str">
+        <f>IF(O126="", BIN2HEX(P126, 2), BIN2HEX(O126,2))</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="127" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A127">
+        <v>33</v>
+      </c>
+      <c r="B127" t="str">
+        <f t="shared" si="139"/>
+        <v>0x021</v>
+      </c>
+      <c r="C127" t="s">
+        <v>242</v>
+      </c>
+      <c r="E127" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="F127" s="11">
+        <v>6</v>
+      </c>
+      <c r="H127" t="str">
+        <f t="shared" si="170"/>
+        <v/>
+      </c>
+      <c r="J127">
+        <v>33</v>
+      </c>
+      <c r="L127" s="16" t="str">
+        <f>IF(F127="", "", TEXT(DEC2BIN(F127), "000000"))</f>
+        <v>000110</v>
+      </c>
+      <c r="M127" s="17" t="str">
+        <f t="shared" si="174"/>
+        <v/>
+      </c>
+      <c r="N127" s="17" t="str">
+        <f t="shared" si="175"/>
+        <v/>
+      </c>
+      <c r="O127" s="17" t="str">
+        <f t="shared" si="176"/>
+        <v>00100001</v>
+      </c>
+      <c r="P127" s="18" t="str">
+        <f t="shared" si="177"/>
+        <v/>
+      </c>
+      <c r="Q127" t="str">
+        <f>BIN2HEX(LEFT(CONCATENATE(L127,IF(M127="", "000", M127)), 8), 2)</f>
         <v>18</v>
       </c>
-      <c r="B123" t="str">
-        <f t="shared" si="143"/>
-        <v>0x012</v>
-      </c>
-      <c r="C123" t="s">
-        <v>59</v>
-      </c>
-      <c r="D123" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="E123" s="44" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="124" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A124">
+      <c r="R127" t="str">
+        <f>BIN2HEX(CONCATENATE(RIGHT(M127, 1), IF(N127 = "", "000", N127), "0000"), 2)</f>
+        <v>00</v>
+      </c>
+      <c r="S127" s="13" t="str">
+        <f>IF(O127="", BIN2HEX(P127, 2), BIN2HEX(O127,2))</f>
         <v>21</v>
       </c>
-      <c r="B124" t="str">
-        <f t="shared" si="143"/>
-        <v>0x015</v>
-      </c>
-      <c r="C124" t="s">
-        <v>152</v>
-      </c>
-      <c r="D124" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="E124" s="44"/>
-    </row>
-    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A125">
-        <v>24</v>
-      </c>
-      <c r="B125" t="str">
-        <f t="shared" si="143"/>
-        <v>0x018</v>
-      </c>
-      <c r="C125" t="s">
-        <v>62</v>
-      </c>
-      <c r="D125" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="E125" s="44"/>
-    </row>
-    <row r="126" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A126">
-        <v>27</v>
-      </c>
-      <c r="B126" t="str">
-        <f t="shared" si="143"/>
-        <v>0x01B</v>
-      </c>
-      <c r="C126" t="s">
-        <v>159</v>
-      </c>
-      <c r="D126" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="E126" s="8" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="127" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A127">
-        <v>30</v>
-      </c>
-      <c r="B127" t="str">
-        <f t="shared" si="143"/>
-        <v>0x01E</v>
-      </c>
-      <c r="C127" t="s">
-        <v>198</v>
-      </c>
-      <c r="D127" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="E127" s="8" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="128" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="128" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A128">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B128" t="str">
-        <f t="shared" si="143"/>
-        <v>0x021</v>
+        <f t="shared" si="139"/>
+        <v>0x024</v>
       </c>
       <c r="C128" t="s">
-        <v>196</v>
-      </c>
-      <c r="D128" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="E128" s="44" t="s">
-        <v>195</v>
+        <v>82</v>
+      </c>
+      <c r="E128" s="51" t="s">
+        <v>249</v>
       </c>
       <c r="F128" s="11">
         <v>2</v>
@@ -7866,195 +8244,269 @@
         <v>38</v>
       </c>
       <c r="H128">
-        <f t="shared" ref="H128:H130" si="146">IF(G128="", "", VLOOKUP(G128, $U$3:$V$10, 2))</f>
+        <f t="shared" si="170"/>
         <v>0</v>
       </c>
       <c r="I128">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="L128" s="16" t="str">
-        <f>IF(F128="", "", TEXT(DEC2BIN(F128), "000000"))</f>
+        <f t="shared" ref="L128" si="179">IF(F128="", "", TEXT(DEC2BIN(F128), "000000"))</f>
         <v>000010</v>
       </c>
       <c r="M128" s="17" t="str">
-        <f>IF(H128="", "", TEXT(DEC2BIN(H128), "000"))</f>
+        <f t="shared" si="174"/>
         <v>000</v>
       </c>
       <c r="N128" s="17" t="str">
-        <f>IF(I128="", "", TEXT(DEC2BIN(I128), "000"))</f>
-        <v>010</v>
+        <f t="shared" si="175"/>
+        <v>110</v>
       </c>
       <c r="O128" s="17" t="str">
-        <f>IF(J128="", "", TEXT(DEC2BIN(J128), "00000000"))</f>
+        <f t="shared" si="176"/>
         <v/>
       </c>
       <c r="P128" s="18" t="str">
-        <f>IF(K128="", "", TEXT(DEC2BIN(K128), "00000000"))</f>
+        <f t="shared" si="177"/>
         <v/>
       </c>
       <c r="Q128" t="str">
-        <f t="shared" ref="Q128" si="147">BIN2HEX(LEFT(CONCATENATE(L128,IF(M128="", "000", M128)), 8), 2)</f>
+        <f t="shared" ref="Q128" si="180">BIN2HEX(LEFT(CONCATENATE(L128,IF(M128="", "000", M128)), 8), 2)</f>
         <v>08</v>
       </c>
       <c r="R128" t="str">
-        <f>BIN2HEX(CONCATENATE(RIGHT(M128, 1), IF(N128 = "", "000", N128), "0000"), 2)</f>
-        <v>20</v>
+        <f t="shared" ref="R128" si="181">BIN2HEX(CONCATENATE(RIGHT(M128, 1), IF(N128 = "", "000", N128), "0000"), 2)</f>
+        <v>60</v>
       </c>
       <c r="S128" s="13" t="str">
-        <f t="shared" ref="S128" si="148">IF(O128="", BIN2HEX(P128, 2), BIN2HEX(O128,2))</f>
-        <v>00</v>
-      </c>
-    </row>
-    <row r="129" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" ref="S128" si="182">IF(O128="", BIN2HEX(P128, 2), BIN2HEX(O128,2))</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="129" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A129">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B129" t="str">
-        <f t="shared" si="143"/>
-        <v>0x024</v>
+        <f t="shared" si="139"/>
+        <v>0x027</v>
       </c>
       <c r="C129" t="s">
-        <v>152</v>
-      </c>
-      <c r="D129" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="E129" s="44"/>
-    </row>
-    <row r="130" spans="1:19" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+      <c r="E129" s="51"/>
+      <c r="F129" s="11">
+        <v>40</v>
+      </c>
+      <c r="G129" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="H129">
+        <f t="shared" ref="H129:H131" si="183">IF(G129="", "", VLOOKUP(G129, $U$3:$V$10, 2))</f>
+        <v>0</v>
+      </c>
+      <c r="L129" s="16" t="str">
+        <f>IF(F129="", "", TEXT(DEC2BIN(F129), "000000"))</f>
+        <v>101000</v>
+      </c>
+      <c r="M129" s="17" t="str">
+        <f>IF(H129="", "", TEXT(DEC2BIN(H129), "000"))</f>
+        <v>000</v>
+      </c>
+      <c r="N129" s="17" t="str">
+        <f>IF(I129="", "", TEXT(DEC2BIN(I129), "000"))</f>
+        <v/>
+      </c>
+      <c r="O129" s="17" t="str">
+        <f>IF(J129="", "", TEXT(DEC2BIN(J129), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="P129" s="18" t="str">
+        <f>IF(K129="", "", TEXT(DEC2BIN(K129), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="Q129" t="str">
+        <f t="shared" ref="Q129:Q130" si="184">BIN2HEX(LEFT(CONCATENATE(L129,IF(M129="", "000", M129)), 8), 2)</f>
+        <v>A0</v>
+      </c>
+      <c r="R129" t="str">
+        <f>BIN2HEX(CONCATENATE(RIGHT(M129, 1), IF(N129 = "", "000", N129), "0000"), 2)</f>
+        <v>00</v>
+      </c>
+      <c r="S129" s="13" t="str">
+        <f t="shared" ref="S129:S130" si="185">IF(O129="", BIN2HEX(P129, 2), BIN2HEX(O129,2))</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="130" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A130">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B130" t="str">
-        <f t="shared" si="143"/>
-        <v>0x027</v>
+        <f t="shared" si="139"/>
+        <v>0x02A</v>
       </c>
       <c r="C130" t="s">
-        <v>197</v>
-      </c>
-      <c r="D130" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="E130" s="44"/>
+        <v>83</v>
+      </c>
+      <c r="E130" s="51"/>
       <c r="F130" s="11">
         <v>2</v>
       </c>
       <c r="G130" s="12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H130">
-        <f t="shared" si="146"/>
-        <v>4</v>
+        <f t="shared" si="183"/>
+        <v>6</v>
       </c>
       <c r="I130">
         <v>0</v>
       </c>
       <c r="L130" s="16" t="str">
-        <f>IF(F130="", "", TEXT(DEC2BIN(F130), "000000"))</f>
+        <f t="shared" ref="L130" si="186">IF(F130="", "", TEXT(DEC2BIN(F130), "000000"))</f>
         <v>000010</v>
       </c>
       <c r="M130" s="17" t="str">
-        <f>IF(H130="", "", TEXT(DEC2BIN(H130), "000"))</f>
-        <v>100</v>
+        <f t="shared" ref="M130" si="187">IF(H130="", "", TEXT(DEC2BIN(H130), "000"))</f>
+        <v>110</v>
       </c>
       <c r="N130" s="17" t="str">
-        <f>IF(I130="", "", TEXT(DEC2BIN(I130), "000"))</f>
+        <f t="shared" ref="N130" si="188">IF(I130="", "", TEXT(DEC2BIN(I130), "000"))</f>
         <v>000</v>
       </c>
       <c r="O130" s="17" t="str">
-        <f>IF(J130="", "", TEXT(DEC2BIN(J130), "00000000"))</f>
+        <f t="shared" ref="O130" si="189">IF(J130="", "", TEXT(DEC2BIN(J130), "00000000"))</f>
         <v/>
       </c>
       <c r="P130" s="18" t="str">
-        <f>IF(K130="", "", TEXT(DEC2BIN(K130), "00000000"))</f>
+        <f t="shared" ref="P130" si="190">IF(K130="", "", TEXT(DEC2BIN(K130), "00000000"))</f>
         <v/>
       </c>
       <c r="Q130" t="str">
-        <f t="shared" ref="Q130" si="149">BIN2HEX(LEFT(CONCATENATE(L130,IF(M130="", "000", M130)), 8), 2)</f>
-        <v>0A</v>
+        <f t="shared" si="184"/>
+        <v>0B</v>
       </c>
       <c r="R130" t="str">
-        <f>BIN2HEX(CONCATENATE(RIGHT(M130, 1), IF(N130 = "", "000", N130), "0000"), 2)</f>
+        <f t="shared" ref="R130" si="191">BIN2HEX(CONCATENATE(RIGHT(M130, 1), IF(N130 = "", "000", N130), "0000"), 2)</f>
         <v>00</v>
       </c>
       <c r="S130" s="13" t="str">
-        <f t="shared" ref="S130" si="150">IF(O130="", BIN2HEX(P130, 2), BIN2HEX(O130,2))</f>
-        <v>00</v>
-      </c>
-    </row>
-    <row r="131" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="185"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="131" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A131">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B131" t="str">
-        <f t="shared" si="143"/>
-        <v>0x02A</v>
+        <f t="shared" si="139"/>
+        <v>0x02D</v>
       </c>
       <c r="C131" t="s">
-        <v>193</v>
-      </c>
-      <c r="D131" s="7" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
       <c r="E131" s="8" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="132" spans="1:19" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+      <c r="F131" s="11">
+        <v>5</v>
+      </c>
+      <c r="H131" t="str">
+        <f t="shared" si="183"/>
+        <v/>
+      </c>
+      <c r="J131">
+        <v>12</v>
+      </c>
+      <c r="L131" s="16" t="str">
+        <f>IF(F131="", "", TEXT(DEC2BIN(F131), "000000"))</f>
+        <v>000101</v>
+      </c>
+      <c r="M131" s="17" t="str">
+        <f t="shared" ref="M131" si="192">IF(H131="", "", TEXT(DEC2BIN(H131), "000"))</f>
+        <v/>
+      </c>
+      <c r="N131" s="17" t="str">
+        <f t="shared" ref="N131" si="193">IF(I131="", "", TEXT(DEC2BIN(I131), "000"))</f>
+        <v/>
+      </c>
+      <c r="O131" s="17" t="str">
+        <f t="shared" ref="O131" si="194">IF(J131="", "", TEXT(DEC2BIN(J131), "00000000"))</f>
+        <v>00001100</v>
+      </c>
+      <c r="P131" s="18" t="str">
+        <f t="shared" ref="P131" si="195">IF(K131="", "", TEXT(DEC2BIN(K131), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="Q131" t="str">
+        <f>BIN2HEX(LEFT(CONCATENATE(L131,IF(M131="", "000", M131)), 8), 2)</f>
+        <v>14</v>
+      </c>
+      <c r="R131" t="str">
+        <f>BIN2HEX(CONCATENATE(RIGHT(M131, 1), IF(N131 = "", "000", N131), "0000"), 2)</f>
+        <v>00</v>
+      </c>
+      <c r="S131" s="13" t="str">
+        <f>IF(O131="", BIN2HEX(P131, 2), BIN2HEX(O131,2))</f>
+        <v>0C</v>
+      </c>
+    </row>
+    <row r="132" spans="1:19" x14ac:dyDescent="0.3">
       <c r="E132" s="8" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="133" spans="1:19" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="133" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>48</v>
       </c>
       <c r="B133" t="str">
-        <f t="shared" si="143"/>
+        <f t="shared" ref="B133:B135" si="196">"0x" &amp; DEC2HEX(A133,3)</f>
         <v>0x030</v>
       </c>
       <c r="D133" s="7" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="134" spans="1:19" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="134" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>51</v>
       </c>
       <c r="B134" t="str">
-        <f t="shared" si="143"/>
+        <f t="shared" si="196"/>
         <v>0x033</v>
       </c>
       <c r="D134" s="7" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="135" spans="1:19" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="135" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>54</v>
       </c>
       <c r="B135" t="str">
-        <f t="shared" si="143"/>
+        <f t="shared" si="196"/>
         <v>0x036</v>
       </c>
       <c r="D135" s="7" t="s">
-        <v>225</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="U16:V18">
     <sortCondition ref="U13"/>
   </sortState>
-  <mergeCells count="3">
+  <mergeCells count="2">
+    <mergeCell ref="Q1:S1"/>
     <mergeCell ref="E128:E130"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="E123:E125"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W17">
       <formula1>$U$16:$U$18</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G6 G122 G119 G128 G130 G9:G11 G17:G26 G31:G33 G41:G42 G49 G83:G93">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G6 G9:G11 G17:G26 G31:G33 G41:G42 G49 G83:G93 G116:G131">
       <formula1>$U$3:$U$10</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
v.0.15.1 - Simple animation to LED matrix program
</commit_message>
<xml_diff>
--- a/2nd gen - 8 bit cpu/Instruction control lines.xlsx
+++ b/2nd gen - 8 bit cpu/Instruction control lines.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="288" windowWidth="14808" windowHeight="7836" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="7830" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Control Lines" sheetId="1" r:id="rId1"/>
     <sheet name="Some instructions for test" sheetId="2" r:id="rId2"/>
     <sheet name="Test Programs" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
@@ -22,7 +22,7 @@
     <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="C20" authorId="0" shapeId="0">
+    <comment ref="C20" authorId="0">
       <text>
         <r>
           <rPr>
@@ -51,7 +51,7 @@
     <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="273">
   <si>
     <t>LD R1, data</t>
   </si>
@@ -879,12 +879,39 @@
   </si>
   <si>
     <t>ALL PROGRAMS MUST HAVE THE OUT INSTR REASSEMBLED (NOW USES R1 INSTEAD OF R2)</t>
+  </si>
+  <si>
+    <t>// Addr of first byte (hi)</t>
+  </si>
+  <si>
+    <t>// Addr of first byte (low)</t>
+  </si>
+  <si>
+    <t>// Addr of last byte + 1</t>
+  </si>
+  <si>
+    <t>// Output byte to line indicated by E</t>
+  </si>
+  <si>
+    <t>// If true, start over the animation</t>
+  </si>
+  <si>
+    <t>00 00 00</t>
+  </si>
+  <si>
+    <t>ff 00 00</t>
+  </si>
+  <si>
+    <t>ff</t>
+  </si>
+  <si>
+    <t>LD F, 0x70</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1207,7 +1234,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1245,9 +1272,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1280,26 +1307,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1332,26 +1342,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1532,21 +1525,21 @@
       <selection pane="bottomLeft" activeCell="P35" sqref="P35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.88671875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="17" width="3.33203125" customWidth="1"/>
-    <col min="18" max="19" width="3.33203125" style="4" customWidth="1"/>
-    <col min="20" max="20" width="3.33203125" customWidth="1"/>
-    <col min="21" max="21" width="3.33203125" style="41" customWidth="1"/>
-    <col min="22" max="27" width="3.33203125" customWidth="1"/>
-    <col min="28" max="30" width="5.88671875" customWidth="1"/>
+    <col min="4" max="17" width="3.28515625" customWidth="1"/>
+    <col min="18" max="19" width="3.28515625" style="4" customWidth="1"/>
+    <col min="20" max="20" width="3.28515625" customWidth="1"/>
+    <col min="21" max="21" width="3.28515625" style="41" customWidth="1"/>
+    <col min="22" max="27" width="3.28515625" customWidth="1"/>
+    <col min="28" max="30" width="5.85546875" customWidth="1"/>
     <col min="31" max="31" width="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="D1">
         <v>23</v>
       </c>
@@ -1620,7 +1613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:39" s="1" customFormat="1" ht="130.19999999999999" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:39" s="1" customFormat="1" ht="130.15" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>205</v>
       </c>
@@ -1708,7 +1701,7 @@
       <c r="AC2" s="47"/>
       <c r="AD2" s="47"/>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>0</v>
       </c>
@@ -1812,7 +1805,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -1912,7 +1905,7 @@
         <v>C00000</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -2012,7 +2005,7 @@
         <v>600400</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -2112,7 +2105,7 @@
         <v>5E0000</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -2212,7 +2205,7 @@
         <v>4F0000</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>5</v>
       </c>
@@ -2312,7 +2305,7 @@
         <v>004000</v>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>6</v>
       </c>
@@ -2412,7 +2405,7 @@
         <v>006000</v>
       </c>
     </row>
-    <row r="10" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:39" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="33">
         <v>7</v>
       </c>
@@ -2512,7 +2505,7 @@
         <v>004200</v>
       </c>
     </row>
-    <row r="11" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:39" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="33">
         <v>8</v>
       </c>
@@ -2612,7 +2605,7 @@
         <v>006200</v>
       </c>
     </row>
-    <row r="12" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:39" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="33">
         <v>9</v>
       </c>
@@ -2684,7 +2677,7 @@
         <v>000100</v>
       </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>10</v>
       </c>
@@ -2787,7 +2780,7 @@
         <v>181800</v>
       </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>11</v>
       </c>
@@ -2887,7 +2880,7 @@
         <v>091800</v>
       </c>
     </row>
-    <row r="15" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:39" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="33">
         <v>12</v>
       </c>
@@ -2938,7 +2931,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="16" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:39" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="33">
         <v>13</v>
       </c>
@@ -2989,7 +2982,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="17" spans="1:40" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:40" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="33">
         <v>14</v>
       </c>
@@ -3040,7 +3033,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="18" spans="1:40" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:40" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="33">
         <v>15</v>
       </c>
@@ -3091,7 +3084,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="19" spans="1:40" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:40" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="33">
         <v>16</v>
       </c>
@@ -3134,7 +3127,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>17</v>
       </c>
@@ -3240,7 +3233,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="21" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:40" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>18</v>
       </c>
@@ -3273,7 +3266,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="22" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:40" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>19</v>
       </c>
@@ -3306,7 +3299,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="23" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:40" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>20</v>
       </c>
@@ -3339,7 +3332,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="24" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:40" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>21</v>
       </c>
@@ -3372,7 +3365,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="25" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:40" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>22</v>
       </c>
@@ -3405,7 +3398,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="26" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:40" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>23</v>
       </c>
@@ -3438,7 +3431,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="27" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:40" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>24</v>
       </c>
@@ -3471,7 +3464,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="28" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:40" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>25</v>
       </c>
@@ -3504,7 +3497,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="29" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:40" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>26</v>
       </c>
@@ -3537,7 +3530,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="30" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:40" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>27</v>
       </c>
@@ -3570,7 +3563,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="31" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:40" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>28</v>
       </c>
@@ -3603,7 +3596,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="32" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:40" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>29</v>
       </c>
@@ -3636,7 +3629,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="33" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:40" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>30</v>
       </c>
@@ -3669,7 +3662,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="34" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:40" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>31</v>
       </c>
@@ -3702,7 +3695,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="35" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>32</v>
       </c>
@@ -3805,7 +3798,7 @@
         <v>408825</v>
       </c>
     </row>
-    <row r="36" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>33</v>
       </c>
@@ -3908,7 +3901,7 @@
         <v>408818</v>
       </c>
     </row>
-    <row r="37" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>34</v>
       </c>
@@ -4011,7 +4004,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="38" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>35</v>
       </c>
@@ -4111,7 +4104,7 @@
         <v>40882E</v>
       </c>
     </row>
-    <row r="39" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>36</v>
       </c>
@@ -4211,7 +4204,7 @@
         <v>40883A</v>
       </c>
     </row>
-    <row r="40" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>37</v>
       </c>
@@ -4311,7 +4304,7 @@
         <v>40881A</v>
       </c>
     </row>
-    <row r="41" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>38</v>
       </c>
@@ -4411,7 +4404,7 @@
         <v>408806</v>
       </c>
     </row>
-    <row r="42" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>39</v>
       </c>
@@ -4511,7 +4504,7 @@
         <v>408826</v>
       </c>
     </row>
-    <row r="43" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>40</v>
       </c>
@@ -4611,7 +4604,7 @@
         <v>408800</v>
       </c>
     </row>
-    <row r="44" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>41</v>
       </c>
@@ -4711,7 +4704,7 @@
         <v>40883D</v>
       </c>
     </row>
-    <row r="46" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C46" s="3" t="s">
         <v>22</v>
       </c>
@@ -4719,7 +4712,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C47" s="5" t="s">
         <v>30</v>
       </c>
@@ -4727,7 +4720,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C49" s="1" t="s">
         <v>53</v>
       </c>
@@ -4735,7 +4728,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C50" s="1" t="s">
         <v>62</v>
       </c>
@@ -4743,7 +4736,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C51" s="1" t="s">
         <v>47</v>
       </c>
@@ -4751,7 +4744,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52"/>
       <c r="B52"/>
       <c r="C52" s="1" t="s">
@@ -4763,7 +4756,7 @@
       <c r="R52"/>
       <c r="S52"/>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53"/>
       <c r="B53"/>
       <c r="C53" s="1" t="s">
@@ -4775,7 +4768,7 @@
       <c r="R53"/>
       <c r="S53"/>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54"/>
       <c r="B54"/>
       <c r="C54" s="1" t="s">
@@ -4805,10 +4798,10 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="9.109375" style="7"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="9.140625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -4956,33 +4949,33 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z151"/>
+  <dimension ref="A1:Z191"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C151" sqref="C151"/>
+      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M181" sqref="M181"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" style="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="3" style="12" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.44140625" style="16" customWidth="1"/>
-    <col min="14" max="15" width="9.109375" style="2"/>
-    <col min="16" max="16" width="8.88671875" style="2"/>
-    <col min="17" max="17" width="10.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.88671875" style="18" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="3.44140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.42578125" style="16" customWidth="1"/>
+    <col min="14" max="15" width="9.140625" style="2"/>
+    <col min="16" max="16" width="8.85546875" style="2"/>
+    <col min="17" max="17" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="3.42578125" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>84</v>
       </c>
@@ -5035,7 +5028,7 @@
       <c r="U1" s="50"/>
       <c r="V1" s="10"/>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="8" t="s">
@@ -5049,7 +5042,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
@@ -5114,7 +5107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5181,7 +5174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>6</v>
       </c>
@@ -5246,7 +5239,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>9</v>
       </c>
@@ -5308,7 +5301,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E7" s="8"/>
       <c r="N7" s="17"/>
       <c r="O7" s="17"/>
@@ -5321,7 +5314,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C8" s="8" t="s">
         <v>214</v>
       </c>
@@ -5333,7 +5326,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0</v>
       </c>
@@ -5398,7 +5391,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3</v>
       </c>
@@ -5459,7 +5452,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>6</v>
       </c>
@@ -5514,7 +5507,7 @@
         <v>03</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C16" s="8" t="s">
         <v>217</v>
       </c>
@@ -5525,7 +5518,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>0</v>
       </c>
@@ -5596,7 +5589,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>3</v>
       </c>
@@ -5660,7 +5653,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>6</v>
       </c>
@@ -5715,7 +5708,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>9</v>
       </c>
@@ -5773,7 +5766,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>12</v>
       </c>
@@ -5829,48 +5822,48 @@
         <v>06</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E22" s="39"/>
       <c r="N22" s="17"/>
       <c r="O22" s="17"/>
       <c r="P22" s="17"/>
       <c r="Q22" s="17"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E23" s="39"/>
       <c r="N23" s="17"/>
       <c r="O23" s="17"/>
       <c r="P23" s="17"/>
       <c r="Q23" s="17"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E24" s="39"/>
       <c r="N24" s="17"/>
       <c r="O24" s="17"/>
       <c r="P24" s="17"/>
       <c r="Q24" s="17"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E25" s="39"/>
       <c r="N25" s="17"/>
       <c r="O25" s="17"/>
       <c r="P25" s="17"/>
       <c r="Q25" s="17"/>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="N26" s="17"/>
       <c r="O26" s="17"/>
       <c r="P26" s="17"/>
       <c r="Q26" s="17"/>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="8" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>0</v>
       </c>
@@ -5928,7 +5921,7 @@
         <v>01</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>3</v>
       </c>
@@ -5986,7 +5979,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>6</v>
       </c>
@@ -6044,7 +6037,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>9</v>
       </c>
@@ -6095,7 +6088,7 @@
         <v>0F</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>12</v>
       </c>
@@ -6146,7 +6139,7 @@
         <v>06</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>15</v>
       </c>
@@ -6197,12 +6190,12 @@
         <v>0F</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C40" s="8" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>0</v>
       </c>
@@ -6260,7 +6253,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>3</v>
       </c>
@@ -6318,7 +6311,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>6</v>
       </c>
@@ -6369,7 +6362,7 @@
         <v>06</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>16</v>
       </c>
@@ -6384,15 +6377,15 @@
         <v>151</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C46" s="38"/>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C48" s="8" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>0</v>
       </c>
@@ -6453,7 +6446,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>3</v>
       </c>
@@ -6507,18 +6500,18 @@
         <v>00</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="N51" s="17"/>
       <c r="O51" s="17"/>
       <c r="P51" s="17"/>
       <c r="Q51" s="17"/>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C55" s="8" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>0</v>
       </c>
@@ -6537,7 +6530,7 @@
       </c>
       <c r="F56" s="43"/>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>3</v>
       </c>
@@ -6553,7 +6546,7 @@
       </c>
       <c r="E57" s="8"/>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>6</v>
       </c>
@@ -6571,7 +6564,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>9</v>
       </c>
@@ -6587,7 +6580,7 @@
       </c>
       <c r="E59" s="8"/>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>12</v>
       </c>
@@ -6605,7 +6598,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>15</v>
       </c>
@@ -6621,7 +6614,7 @@
       </c>
       <c r="E61" s="8"/>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>18</v>
       </c>
@@ -6639,7 +6632,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>21</v>
       </c>
@@ -6655,7 +6648,7 @@
       </c>
       <c r="E63" s="8"/>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>24</v>
       </c>
@@ -6673,7 +6666,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>27</v>
       </c>
@@ -6689,7 +6682,7 @@
       </c>
       <c r="E65" s="8"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>30</v>
       </c>
@@ -6707,7 +6700,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>33</v>
       </c>
@@ -6723,7 +6716,7 @@
       </c>
       <c r="E67" s="8"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>36</v>
       </c>
@@ -6741,7 +6734,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>39</v>
       </c>
@@ -6757,7 +6750,7 @@
       </c>
       <c r="E69" s="8"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>42</v>
       </c>
@@ -6775,7 +6768,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>45</v>
       </c>
@@ -6791,7 +6784,7 @@
       </c>
       <c r="E71" s="8"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>48</v>
       </c>
@@ -6809,7 +6802,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>51</v>
       </c>
@@ -6825,7 +6818,7 @@
       </c>
       <c r="E73" s="8"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>54</v>
       </c>
@@ -6843,7 +6836,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>57</v>
       </c>
@@ -6859,7 +6852,7 @@
       </c>
       <c r="E75" s="8"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>60</v>
       </c>
@@ -6877,7 +6870,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>63</v>
       </c>
@@ -6893,7 +6886,7 @@
       </c>
       <c r="E77" s="8"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>66</v>
       </c>
@@ -6911,7 +6904,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>69</v>
       </c>
@@ -6927,21 +6920,21 @@
       </c>
       <c r="E79" s="8"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E80" s="8"/>
     </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="D81"/>
       <c r="E81" s="8"/>
     </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C82" s="8" t="s">
         <v>139</v>
       </c>
       <c r="D82"/>
       <c r="E82" s="8"/>
     </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>0</v>
       </c>
@@ -7003,7 +6996,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>3</v>
       </c>
@@ -7064,7 +7057,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>6</v>
       </c>
@@ -7125,7 +7118,7 @@
         <v>3C</v>
       </c>
     </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>9</v>
       </c>
@@ -7183,7 +7176,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>12</v>
       </c>
@@ -7245,7 +7238,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>15</v>
       </c>
@@ -7301,7 +7294,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>18</v>
       </c>
@@ -7362,7 +7355,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>21</v>
       </c>
@@ -7423,7 +7416,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="91" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>24</v>
       </c>
@@ -7481,7 +7474,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="92" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>27</v>
       </c>
@@ -7542,7 +7535,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="93" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>30</v>
       </c>
@@ -7605,7 +7598,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="95" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>48</v>
       </c>
@@ -7620,7 +7613,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="96" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>51</v>
       </c>
@@ -7635,7 +7628,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="97" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>54</v>
       </c>
@@ -7650,7 +7643,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="98" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>57</v>
       </c>
@@ -7665,25 +7658,25 @@
         <v>159</v>
       </c>
     </row>
-    <row r="99" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C99" s="5"/>
       <c r="E99" s="8"/>
     </row>
-    <row r="100" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C100" s="5" t="s">
         <v>256</v>
       </c>
       <c r="D100"/>
       <c r="E100" s="8"/>
     </row>
-    <row r="101" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C101" s="8" t="s">
         <v>140</v>
       </c>
       <c r="D101"/>
       <c r="E101" s="8"/>
     </row>
-    <row r="102" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>0</v>
       </c>
@@ -7747,7 +7740,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="103" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>3</v>
       </c>
@@ -7811,7 +7804,7 @@
         <v>FF</v>
       </c>
     </row>
-    <row r="104" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>6</v>
       </c>
@@ -7872,7 +7865,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="105" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>9</v>
       </c>
@@ -7930,7 +7923,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="106" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>12</v>
       </c>
@@ -7989,7 +7982,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="107" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>15</v>
       </c>
@@ -8053,7 +8046,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="108" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>18</v>
       </c>
@@ -8117,7 +8110,7 @@
         <v>3A</v>
       </c>
     </row>
-    <row r="109" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>21</v>
       </c>
@@ -8179,7 +8172,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="110" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>24</v>
       </c>
@@ -8240,7 +8233,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="111" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>27</v>
       </c>
@@ -8302,7 +8295,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="112" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>30</v>
       </c>
@@ -8363,12 +8356,12 @@
         <v>06</v>
       </c>
     </row>
-    <row r="116" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C116" s="8" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="117" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>0</v>
       </c>
@@ -8429,7 +8422,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="118" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>3</v>
       </c>
@@ -8490,7 +8483,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="119" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>6</v>
       </c>
@@ -8551,7 +8544,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="120" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>9</v>
       </c>
@@ -8612,7 +8605,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="121" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>12</v>
       </c>
@@ -8671,7 +8664,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="122" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>15</v>
       </c>
@@ -8729,7 +8722,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="123" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>18</v>
       </c>
@@ -8788,7 +8781,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="124" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>21</v>
       </c>
@@ -8846,7 +8839,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="125" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>24</v>
       </c>
@@ -8902,7 +8895,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="126" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>27</v>
       </c>
@@ -8963,7 +8956,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="127" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>30</v>
       </c>
@@ -9024,7 +9017,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="128" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>33</v>
       </c>
@@ -9082,7 +9075,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="129" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>36</v>
       </c>
@@ -9143,7 +9136,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="130" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>39</v>
       </c>
@@ -9199,7 +9192,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="131" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>42</v>
       </c>
@@ -9258,7 +9251,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="132" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>45</v>
       </c>
@@ -9316,12 +9309,12 @@
         <v>0C</v>
       </c>
     </row>
-    <row r="133" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E133" s="8" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="134" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>48</v>
       </c>
@@ -9333,7 +9326,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="135" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>51</v>
       </c>
@@ -9345,7 +9338,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="136" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>54</v>
       </c>
@@ -9357,12 +9350,12 @@
         <v>200</v>
       </c>
     </row>
-    <row r="140" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C140" s="8" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="141" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>0</v>
       </c>
@@ -9392,23 +9385,23 @@
         <v>000001</v>
       </c>
       <c r="N141" s="17" t="str">
-        <f>IF(H141="", "", TEXT(DEC2BIN(H141), "000"))</f>
+        <f t="shared" ref="N141:P144" si="235">IF(H141="", "", TEXT(DEC2BIN(H141), "000"))</f>
         <v>110</v>
       </c>
       <c r="O141" s="17" t="str">
-        <f>IF(I141="", "", TEXT(DEC2BIN(I141), "000"))</f>
+        <f t="shared" si="235"/>
         <v/>
       </c>
       <c r="P141" s="17" t="str">
-        <f>IF(J141="", "", TEXT(DEC2BIN(J141), "000"))</f>
+        <f t="shared" si="235"/>
         <v/>
       </c>
       <c r="Q141" s="17" t="str">
-        <f>IF(K141="", "", TEXT(DEC2BIN(K141), "00000000"))</f>
+        <f t="shared" ref="Q141:R144" si="236">IF(K141="", "", TEXT(DEC2BIN(K141), "00000000"))</f>
         <v/>
       </c>
       <c r="R141" s="18" t="str">
-        <f>IF(L141="", "", TEXT(DEC2BIN(L141), "00000000"))</f>
+        <f t="shared" si="236"/>
         <v>00000000</v>
       </c>
       <c r="S141" t="str">
@@ -9424,7 +9417,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="142" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>3</v>
       </c>
@@ -9443,7 +9436,7 @@
         <v>38</v>
       </c>
       <c r="H142">
-        <f t="shared" ref="H142" si="235">IF(G142="", "", VLOOKUP(G142, $W$3:$X$10, 2))</f>
+        <f t="shared" ref="H142" si="237">IF(G142="", "", VLOOKUP(G142, $W$3:$X$10, 2))</f>
         <v>0</v>
       </c>
       <c r="L142">
@@ -9454,23 +9447,23 @@
         <v>000001</v>
       </c>
       <c r="N142" s="17" t="str">
-        <f>IF(H142="", "", TEXT(DEC2BIN(H142), "000"))</f>
+        <f t="shared" si="235"/>
         <v>000</v>
       </c>
       <c r="O142" s="17" t="str">
-        <f>IF(I142="", "", TEXT(DEC2BIN(I142), "000"))</f>
+        <f t="shared" si="235"/>
         <v/>
       </c>
       <c r="P142" s="17" t="str">
-        <f>IF(J142="", "", TEXT(DEC2BIN(J142), "000"))</f>
+        <f t="shared" si="235"/>
         <v/>
       </c>
       <c r="Q142" s="17" t="str">
-        <f>IF(K142="", "", TEXT(DEC2BIN(K142), "00000000"))</f>
+        <f t="shared" si="236"/>
         <v/>
       </c>
       <c r="R142" s="18" t="str">
-        <f>IF(L142="", "", TEXT(DEC2BIN(L142), "00000000"))</f>
+        <f t="shared" si="236"/>
         <v>11111111</v>
       </c>
       <c r="S142" t="str">
@@ -9486,7 +9479,7 @@
         <v>FF</v>
       </c>
     </row>
-    <row r="143" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>6</v>
       </c>
@@ -9516,23 +9509,23 @@
         <v>000001</v>
       </c>
       <c r="N143" s="17" t="str">
-        <f>IF(H143="", "", TEXT(DEC2BIN(H143), "000"))</f>
+        <f t="shared" si="235"/>
         <v>010</v>
       </c>
       <c r="O143" s="17" t="str">
-        <f>IF(I143="", "", TEXT(DEC2BIN(I143), "000"))</f>
+        <f t="shared" si="235"/>
         <v/>
       </c>
       <c r="P143" s="17" t="str">
-        <f>IF(J143="", "", TEXT(DEC2BIN(J143), "000"))</f>
+        <f t="shared" si="235"/>
         <v/>
       </c>
       <c r="Q143" s="17" t="str">
-        <f>IF(K143="", "", TEXT(DEC2BIN(K143), "00000000"))</f>
+        <f t="shared" si="236"/>
         <v/>
       </c>
       <c r="R143" s="18" t="str">
-        <f>IF(L143="", "", TEXT(DEC2BIN(L143), "00000000"))</f>
+        <f t="shared" si="236"/>
         <v>00000000</v>
       </c>
       <c r="S143" t="str">
@@ -9548,7 +9541,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="144" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C144" t="s">
         <v>261</v>
       </c>
@@ -9574,23 +9567,23 @@
         <v>010001</v>
       </c>
       <c r="N144" s="17" t="str">
-        <f>IF(H144="", "", TEXT(DEC2BIN(H144), "000"))</f>
+        <f t="shared" si="235"/>
         <v>010</v>
       </c>
       <c r="O144" s="17" t="str">
-        <f>IF(I144="", "", TEXT(DEC2BIN(I144), "000"))</f>
+        <f t="shared" si="235"/>
         <v>110</v>
       </c>
       <c r="P144" s="17" t="str">
-        <f>IF(J144="", "", TEXT(DEC2BIN(J144), "000"))</f>
+        <f t="shared" si="235"/>
         <v>001</v>
       </c>
       <c r="Q144" s="17" t="str">
-        <f>IF(K144="", "", TEXT(DEC2BIN(K144), "00000000"))</f>
+        <f t="shared" si="236"/>
         <v/>
       </c>
       <c r="R144" s="18" t="str">
-        <f>IF(L144="", "", TEXT(DEC2BIN(L144), "00000000"))</f>
+        <f t="shared" si="236"/>
         <v/>
       </c>
       <c r="S144" t="str">
@@ -9606,7 +9599,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="145" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C145" t="s">
         <v>258</v>
       </c>
@@ -9618,7 +9611,7 @@
         <v>38</v>
       </c>
       <c r="H145">
-        <f t="shared" ref="H145:H147" si="236">IF(G145="", "", VLOOKUP(G145, $W$3:$X$10, 2))</f>
+        <f t="shared" ref="H145:H147" si="238">IF(G145="", "", VLOOKUP(G145, $W$3:$X$10, 2))</f>
         <v>0</v>
       </c>
       <c r="I145">
@@ -9628,31 +9621,31 @@
         <v>1</v>
       </c>
       <c r="M145" s="16" t="str">
-        <f t="shared" ref="M145:M146" si="237">IF(F145="", "", TEXT(DEC2BIN(F145), "000000"))</f>
+        <f t="shared" ref="M145:M146" si="239">IF(F145="", "", TEXT(DEC2BIN(F145), "000000"))</f>
         <v>010001</v>
       </c>
       <c r="N145" s="17" t="str">
-        <f t="shared" ref="N145:N146" si="238">IF(H145="", "", TEXT(DEC2BIN(H145), "000"))</f>
+        <f t="shared" ref="N145:N146" si="240">IF(H145="", "", TEXT(DEC2BIN(H145), "000"))</f>
         <v>000</v>
       </c>
       <c r="O145" s="17" t="str">
-        <f t="shared" ref="O145:O146" si="239">IF(I145="", "", TEXT(DEC2BIN(I145), "000"))</f>
+        <f t="shared" ref="O145:O146" si="241">IF(I145="", "", TEXT(DEC2BIN(I145), "000"))</f>
         <v>110</v>
       </c>
       <c r="P145" s="17" t="str">
-        <f t="shared" ref="P145" si="240">IF(J145="", "", TEXT(DEC2BIN(J145), "000"))</f>
+        <f t="shared" ref="P145" si="242">IF(J145="", "", TEXT(DEC2BIN(J145), "000"))</f>
         <v>001</v>
       </c>
       <c r="Q145" s="17" t="str">
-        <f t="shared" ref="Q145:Q146" si="241">IF(K145="", "", TEXT(DEC2BIN(K145), "00000000"))</f>
+        <f t="shared" ref="Q145:Q146" si="243">IF(K145="", "", TEXT(DEC2BIN(K145), "00000000"))</f>
         <v/>
       </c>
       <c r="R145" s="18" t="str">
-        <f t="shared" ref="R145:R146" si="242">IF(L145="", "", TEXT(DEC2BIN(L145), "00000000"))</f>
+        <f t="shared" ref="R145:R146" si="244">IF(L145="", "", TEXT(DEC2BIN(L145), "00000000"))</f>
         <v/>
       </c>
       <c r="S145" t="str">
-        <f t="shared" ref="S145:S147" si="243">BIN2HEX(LEFT(CONCATENATE(M145,IF(N145="", "000", N145)), 8), 2)</f>
+        <f t="shared" ref="S145:S147" si="245">BIN2HEX(LEFT(CONCATENATE(M145,IF(N145="", "000", N145)), 8), 2)</f>
         <v>44</v>
       </c>
       <c r="T145" t="str">
@@ -9660,11 +9653,11 @@
         <v>62</v>
       </c>
       <c r="U145" s="13" t="str">
-        <f t="shared" ref="U145:U147" si="244">IF(Q145="", BIN2HEX(R145, 2), BIN2HEX(Q145,2))</f>
-        <v>00</v>
-      </c>
-    </row>
-    <row r="146" spans="3:21" x14ac:dyDescent="0.3">
+        <f t="shared" ref="U145:U147" si="246">IF(Q145="", BIN2HEX(R145, 2), BIN2HEX(Q145,2))</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="146" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C146" t="s">
         <v>259</v>
       </c>
@@ -9676,47 +9669,47 @@
         <v>39</v>
       </c>
       <c r="H146">
-        <f t="shared" si="236"/>
+        <f t="shared" si="238"/>
         <v>1</v>
       </c>
       <c r="I146">
         <v>6</v>
       </c>
       <c r="M146" s="16" t="str">
-        <f t="shared" si="237"/>
+        <f t="shared" si="239"/>
         <v>000010</v>
       </c>
       <c r="N146" s="17" t="str">
-        <f t="shared" si="238"/>
+        <f t="shared" si="240"/>
         <v>001</v>
       </c>
       <c r="O146" s="17" t="str">
-        <f t="shared" si="239"/>
+        <f t="shared" si="241"/>
         <v>110</v>
       </c>
       <c r="P146" s="17"/>
       <c r="Q146" s="17" t="str">
-        <f t="shared" si="241"/>
+        <f t="shared" si="243"/>
         <v/>
       </c>
       <c r="R146" s="18" t="str">
-        <f t="shared" si="242"/>
+        <f t="shared" si="244"/>
         <v/>
       </c>
       <c r="S146" t="str">
-        <f t="shared" si="243"/>
+        <f t="shared" si="245"/>
         <v>08</v>
       </c>
       <c r="T146" t="str">
-        <f t="shared" ref="T146" si="245">BIN2HEX(CONCATENATE(RIGHT(N146, 1), IF(O146 = "", "000", O146), "0000"), 2)</f>
+        <f t="shared" ref="T146" si="247">BIN2HEX(CONCATENATE(RIGHT(N146, 1), IF(O146 = "", "000", O146), "0000"), 2)</f>
         <v>E0</v>
       </c>
       <c r="U146" s="13" t="str">
-        <f t="shared" si="244"/>
-        <v>00</v>
-      </c>
-    </row>
-    <row r="147" spans="3:21" x14ac:dyDescent="0.3">
+        <f t="shared" si="246"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="147" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C147" t="s">
         <v>236</v>
       </c>
@@ -9728,7 +9721,7 @@
         <v>39</v>
       </c>
       <c r="H147">
-        <f t="shared" si="236"/>
+        <f t="shared" si="238"/>
         <v>1</v>
       </c>
       <c r="M147" s="16" t="str">
@@ -9753,7 +9746,7 @@
         <v/>
       </c>
       <c r="S147" t="str">
-        <f t="shared" si="243"/>
+        <f t="shared" si="245"/>
         <v>A0</v>
       </c>
       <c r="T147" t="str">
@@ -9761,11 +9754,11 @@
         <v>80</v>
       </c>
       <c r="U147" s="13" t="str">
-        <f t="shared" si="244"/>
-        <v>00</v>
-      </c>
-    </row>
-    <row r="148" spans="3:21" x14ac:dyDescent="0.3">
+        <f t="shared" si="246"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="148" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C148" t="s">
         <v>260</v>
       </c>
@@ -9777,47 +9770,47 @@
         <v>42</v>
       </c>
       <c r="H148">
-        <f t="shared" ref="H148" si="246">IF(G148="", "", VLOOKUP(G148, $W$3:$X$10, 2))</f>
+        <f t="shared" ref="H148" si="248">IF(G148="", "", VLOOKUP(G148, $W$3:$X$10, 2))</f>
         <v>6</v>
       </c>
       <c r="I148">
         <v>1</v>
       </c>
       <c r="M148" s="16" t="str">
-        <f t="shared" ref="M148" si="247">IF(F148="", "", TEXT(DEC2BIN(F148), "000000"))</f>
+        <f t="shared" ref="M148" si="249">IF(F148="", "", TEXT(DEC2BIN(F148), "000000"))</f>
         <v>000010</v>
       </c>
       <c r="N148" s="17" t="str">
-        <f t="shared" ref="N148" si="248">IF(H148="", "", TEXT(DEC2BIN(H148), "000"))</f>
+        <f t="shared" ref="N148" si="250">IF(H148="", "", TEXT(DEC2BIN(H148), "000"))</f>
         <v>110</v>
       </c>
       <c r="O148" s="17" t="str">
-        <f t="shared" ref="O148" si="249">IF(I148="", "", TEXT(DEC2BIN(I148), "000"))</f>
+        <f t="shared" ref="O148" si="251">IF(I148="", "", TEXT(DEC2BIN(I148), "000"))</f>
         <v>001</v>
       </c>
       <c r="P148" s="17"/>
       <c r="Q148" s="17" t="str">
-        <f t="shared" ref="Q148" si="250">IF(K148="", "", TEXT(DEC2BIN(K148), "00000000"))</f>
+        <f t="shared" ref="Q148" si="252">IF(K148="", "", TEXT(DEC2BIN(K148), "00000000"))</f>
         <v/>
       </c>
       <c r="R148" s="18" t="str">
-        <f t="shared" ref="R148" si="251">IF(L148="", "", TEXT(DEC2BIN(L148), "00000000"))</f>
+        <f t="shared" ref="R148" si="253">IF(L148="", "", TEXT(DEC2BIN(L148), "00000000"))</f>
         <v/>
       </c>
       <c r="S148" t="str">
-        <f t="shared" ref="S148" si="252">BIN2HEX(LEFT(CONCATENATE(M148,IF(N148="", "000", N148)), 8), 2)</f>
+        <f t="shared" ref="S148" si="254">BIN2HEX(LEFT(CONCATENATE(M148,IF(N148="", "000", N148)), 8), 2)</f>
         <v>0B</v>
       </c>
       <c r="T148" t="str">
-        <f t="shared" ref="T148" si="253">BIN2HEX(CONCATENATE(RIGHT(N148, 1), IF(O148 = "", "000", O148), "0000"), 2)</f>
+        <f t="shared" ref="T148" si="255">BIN2HEX(CONCATENATE(RIGHT(N148, 1), IF(O148 = "", "000", O148), "0000"), 2)</f>
         <v>10</v>
       </c>
       <c r="U148" s="13" t="str">
-        <f t="shared" ref="U148" si="254">IF(Q148="", BIN2HEX(R148, 2), BIN2HEX(Q148,2))</f>
-        <v>00</v>
-      </c>
-    </row>
-    <row r="149" spans="3:21" x14ac:dyDescent="0.3">
+        <f t="shared" ref="U148" si="256">IF(Q148="", BIN2HEX(R148, 2), BIN2HEX(Q148,2))</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="149" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C149" t="s">
         <v>82</v>
       </c>
@@ -9825,38 +9818,38 @@
         <v>5</v>
       </c>
       <c r="H149" t="str">
-        <f t="shared" ref="H143:H149" si="255">IF(G149="", "", VLOOKUP(G149, $W$3:$X$10, 2))</f>
+        <f t="shared" ref="H149" si="257">IF(G149="", "", VLOOKUP(G149, $W$3:$X$10, 2))</f>
         <v/>
       </c>
       <c r="K149">
         <v>9</v>
       </c>
       <c r="M149" s="16" t="str">
-        <f t="shared" ref="M149" si="256">IF(F149="", "", TEXT(DEC2BIN(F149), "000000"))</f>
+        <f t="shared" ref="M149" si="258">IF(F149="", "", TEXT(DEC2BIN(F149), "000000"))</f>
         <v>000101</v>
       </c>
       <c r="N149" s="17" t="str">
-        <f t="shared" ref="N149" si="257">IF(H149="", "", TEXT(DEC2BIN(H149), "000"))</f>
+        <f t="shared" ref="N149" si="259">IF(H149="", "", TEXT(DEC2BIN(H149), "000"))</f>
         <v/>
       </c>
       <c r="O149" s="17" t="str">
-        <f t="shared" ref="O149" si="258">IF(I149="", "", TEXT(DEC2BIN(I149), "000"))</f>
+        <f t="shared" ref="O149" si="260">IF(I149="", "", TEXT(DEC2BIN(I149), "000"))</f>
         <v/>
       </c>
       <c r="P149" s="17" t="str">
-        <f t="shared" ref="P149" si="259">IF(J149="", "", TEXT(DEC2BIN(J149), "000"))</f>
+        <f t="shared" ref="P149" si="261">IF(J149="", "", TEXT(DEC2BIN(J149), "000"))</f>
         <v/>
       </c>
       <c r="Q149" s="17" t="str">
-        <f t="shared" ref="Q149" si="260">IF(K149="", "", TEXT(DEC2BIN(K149), "00000000"))</f>
+        <f t="shared" ref="Q149" si="262">IF(K149="", "", TEXT(DEC2BIN(K149), "00000000"))</f>
         <v>00001001</v>
       </c>
       <c r="R149" s="18" t="str">
-        <f t="shared" ref="R149" si="261">IF(L149="", "", TEXT(DEC2BIN(L149), "00000000"))</f>
+        <f t="shared" ref="R149" si="263">IF(L149="", "", TEXT(DEC2BIN(L149), "00000000"))</f>
         <v/>
       </c>
       <c r="S149" t="str">
-        <f t="shared" ref="S149" si="262">BIN2HEX(LEFT(CONCATENATE(M149,IF(N149="", "000", N149)), 8), 2)</f>
+        <f t="shared" ref="S149" si="264">BIN2HEX(LEFT(CONCATENATE(M149,IF(N149="", "000", N149)), 8), 2)</f>
         <v>14</v>
       </c>
       <c r="T149" t="str">
@@ -9864,28 +9857,1205 @@
         <v>00</v>
       </c>
       <c r="U149" s="13" t="str">
-        <f t="shared" ref="U149" si="263">IF(Q149="", BIN2HEX(R149, 2), BIN2HEX(Q149,2))</f>
+        <f t="shared" ref="U149" si="265">IF(Q149="", BIN2HEX(R149, 2), BIN2HEX(Q149,2))</f>
         <v>09</v>
       </c>
     </row>
-    <row r="151" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C151" s="5" t="s">
         <v>263</v>
+      </c>
+    </row>
+    <row r="153" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C153" s="8" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="154" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A154">
+        <v>0</v>
+      </c>
+      <c r="B154" t="str">
+        <f t="shared" ref="B154:B168" si="266">"0x" &amp; DEC2HEX(A154,3)</f>
+        <v>0x000</v>
+      </c>
+      <c r="C154" t="s">
+        <v>254</v>
+      </c>
+      <c r="E154" s="8"/>
+      <c r="F154" s="11">
+        <v>1</v>
+      </c>
+      <c r="G154" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="H154">
+        <f t="shared" ref="H154" si="267">IF(G154="", "", VLOOKUP(G154, $W$3:$X$10, 2))</f>
+        <v>6</v>
+      </c>
+      <c r="L154">
+        <v>0</v>
+      </c>
+      <c r="M154" s="16" t="str">
+        <f>IF(F154="", "", TEXT(DEC2BIN(F154), "000000"))</f>
+        <v>000001</v>
+      </c>
+      <c r="N154" s="17" t="str">
+        <f t="shared" ref="N154" si="268">IF(H154="", "", TEXT(DEC2BIN(H154), "000"))</f>
+        <v>110</v>
+      </c>
+      <c r="O154" s="17" t="str">
+        <f t="shared" ref="O154" si="269">IF(I154="", "", TEXT(DEC2BIN(I154), "000"))</f>
+        <v/>
+      </c>
+      <c r="P154" s="17" t="str">
+        <f t="shared" ref="P154" si="270">IF(J154="", "", TEXT(DEC2BIN(J154), "000"))</f>
+        <v/>
+      </c>
+      <c r="Q154" s="17" t="str">
+        <f t="shared" ref="Q154" si="271">IF(K154="", "", TEXT(DEC2BIN(K154), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="R154" s="18" t="str">
+        <f t="shared" ref="R154" si="272">IF(L154="", "", TEXT(DEC2BIN(L154), "00000000"))</f>
+        <v>00000000</v>
+      </c>
+      <c r="S154" t="str">
+        <f>BIN2HEX(LEFT(CONCATENATE(M154,IF(N154="", "000", N154)), 8), 2)</f>
+        <v>07</v>
+      </c>
+      <c r="T154" t="str">
+        <f>BIN2HEX(CONCATENATE(RIGHT(N154, 1), IF(O154 = "", "000", O154), IF(P154 = "", "000", P154), "0"), 2)</f>
+        <v>00</v>
+      </c>
+      <c r="U154" s="13" t="str">
+        <f>IF(Q154="", BIN2HEX(R154, 2), BIN2HEX(Q154,2))</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="155" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>3</v>
+      </c>
+      <c r="B155" t="str">
+        <f t="shared" si="266"/>
+        <v>0x003</v>
+      </c>
+      <c r="C155" t="s">
+        <v>225</v>
+      </c>
+      <c r="D155"/>
+      <c r="E155" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="F155" s="11">
+        <v>1</v>
+      </c>
+      <c r="G155" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="H155">
+        <f t="shared" ref="H155:H168" si="273">IF(G155="", "", VLOOKUP(G155, $W$3:$X$10, 2))</f>
+        <v>2</v>
+      </c>
+      <c r="L155">
+        <v>0</v>
+      </c>
+      <c r="M155" s="16" t="str">
+        <f t="shared" ref="M155:M159" si="274">IF(F155="", "", TEXT(DEC2BIN(F155), "000000"))</f>
+        <v>000001</v>
+      </c>
+      <c r="N155" s="17" t="str">
+        <f t="shared" ref="N155:N168" si="275">IF(H155="", "", TEXT(DEC2BIN(H155), "000"))</f>
+        <v>010</v>
+      </c>
+      <c r="O155" s="17" t="str">
+        <f t="shared" ref="O155:O168" si="276">IF(I155="", "", TEXT(DEC2BIN(I155), "000"))</f>
+        <v/>
+      </c>
+      <c r="P155" s="17"/>
+      <c r="Q155" s="17" t="str">
+        <f t="shared" ref="Q155:Q168" si="277">IF(K155="", "", TEXT(DEC2BIN(K155), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="R155" s="18" t="str">
+        <f t="shared" ref="R155:R168" si="278">IF(L155="", "", TEXT(DEC2BIN(L155), "00000000"))</f>
+        <v>00000000</v>
+      </c>
+      <c r="S155" t="str">
+        <f t="shared" ref="S155:S159" si="279">BIN2HEX(LEFT(CONCATENATE(M155,IF(N155="", "000", N155)), 8), 2)</f>
+        <v>05</v>
+      </c>
+      <c r="T155" t="str">
+        <f t="shared" ref="T155:T158" si="280">BIN2HEX(CONCATENATE(RIGHT(N155, 1), IF(O155 = "", "000", O155), "0000"), 2)</f>
+        <v>00</v>
+      </c>
+      <c r="U155" s="13" t="str">
+        <f t="shared" ref="U155:U159" si="281">IF(Q155="", BIN2HEX(R155, 2), BIN2HEX(Q155,2))</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="156" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>6</v>
+      </c>
+      <c r="B156" t="str">
+        <f t="shared" si="266"/>
+        <v>0x006</v>
+      </c>
+      <c r="C156" t="s">
+        <v>226</v>
+      </c>
+      <c r="E156" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="F156" s="11">
+        <v>1</v>
+      </c>
+      <c r="G156" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="H156">
+        <f t="shared" si="273"/>
+        <v>3</v>
+      </c>
+      <c r="L156">
+        <v>48</v>
+      </c>
+      <c r="M156" s="16" t="str">
+        <f t="shared" si="274"/>
+        <v>000001</v>
+      </c>
+      <c r="N156" s="17" t="str">
+        <f t="shared" si="275"/>
+        <v>011</v>
+      </c>
+      <c r="O156" s="17" t="str">
+        <f t="shared" si="276"/>
+        <v/>
+      </c>
+      <c r="P156" s="17"/>
+      <c r="Q156" s="17" t="str">
+        <f t="shared" si="277"/>
+        <v/>
+      </c>
+      <c r="R156" s="18" t="str">
+        <f t="shared" si="278"/>
+        <v>00110000</v>
+      </c>
+      <c r="S156" t="str">
+        <f t="shared" si="279"/>
+        <v>05</v>
+      </c>
+      <c r="T156" t="str">
+        <f t="shared" si="280"/>
+        <v>80</v>
+      </c>
+      <c r="U156" s="13" t="str">
+        <f t="shared" si="281"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="157" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>9</v>
+      </c>
+      <c r="B157" t="str">
+        <f t="shared" si="266"/>
+        <v>0x009</v>
+      </c>
+      <c r="C157" t="s">
+        <v>272</v>
+      </c>
+      <c r="E157" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="F157" s="11">
+        <v>1</v>
+      </c>
+      <c r="G157" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="H157">
+        <f t="shared" si="273"/>
+        <v>7</v>
+      </c>
+      <c r="L157">
+        <v>112</v>
+      </c>
+      <c r="M157" s="16" t="str">
+        <f t="shared" si="274"/>
+        <v>000001</v>
+      </c>
+      <c r="N157" s="17" t="str">
+        <f t="shared" si="275"/>
+        <v>111</v>
+      </c>
+      <c r="O157" s="17" t="str">
+        <f t="shared" si="276"/>
+        <v/>
+      </c>
+      <c r="P157" s="17"/>
+      <c r="Q157" s="17" t="str">
+        <f t="shared" si="277"/>
+        <v/>
+      </c>
+      <c r="R157" s="18" t="str">
+        <f t="shared" si="278"/>
+        <v>01110000</v>
+      </c>
+      <c r="S157" t="str">
+        <f t="shared" si="279"/>
+        <v>07</v>
+      </c>
+      <c r="T157" t="str">
+        <f t="shared" si="280"/>
+        <v>80</v>
+      </c>
+      <c r="U157" s="13" t="str">
+        <f t="shared" si="281"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="158" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>12</v>
+      </c>
+      <c r="B158" t="str">
+        <f t="shared" si="266"/>
+        <v>0x00C</v>
+      </c>
+      <c r="C158" t="s">
+        <v>222</v>
+      </c>
+      <c r="E158" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="F158" s="11">
+        <v>4</v>
+      </c>
+      <c r="G158" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="H158">
+        <f t="shared" si="273"/>
+        <v>0</v>
+      </c>
+      <c r="M158" s="16" t="str">
+        <f t="shared" si="274"/>
+        <v>000100</v>
+      </c>
+      <c r="N158" s="17" t="str">
+        <f t="shared" si="275"/>
+        <v>000</v>
+      </c>
+      <c r="O158" s="17" t="str">
+        <f t="shared" si="276"/>
+        <v/>
+      </c>
+      <c r="P158" s="17"/>
+      <c r="Q158" s="17" t="str">
+        <f t="shared" si="277"/>
+        <v/>
+      </c>
+      <c r="R158" s="18" t="str">
+        <f t="shared" si="278"/>
+        <v/>
+      </c>
+      <c r="S158" t="str">
+        <f t="shared" si="279"/>
+        <v>10</v>
+      </c>
+      <c r="T158" t="str">
+        <f t="shared" si="280"/>
+        <v>00</v>
+      </c>
+      <c r="U158" s="13" t="str">
+        <f t="shared" si="281"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="159" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>15</v>
+      </c>
+      <c r="B159" t="str">
+        <f t="shared" si="266"/>
+        <v>0x00F</v>
+      </c>
+      <c r="C159" t="s">
+        <v>258</v>
+      </c>
+      <c r="E159" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="F159" s="11">
+        <v>17</v>
+      </c>
+      <c r="G159" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="H159">
+        <f t="shared" si="273"/>
+        <v>0</v>
+      </c>
+      <c r="I159">
+        <v>6</v>
+      </c>
+      <c r="J159">
+        <v>1</v>
+      </c>
+      <c r="M159" s="16" t="str">
+        <f t="shared" si="274"/>
+        <v>010001</v>
+      </c>
+      <c r="N159" s="17" t="str">
+        <f t="shared" si="275"/>
+        <v>000</v>
+      </c>
+      <c r="O159" s="17" t="str">
+        <f t="shared" si="276"/>
+        <v>110</v>
+      </c>
+      <c r="P159" s="17" t="str">
+        <f t="shared" ref="P159" si="282">IF(J159="", "", TEXT(DEC2BIN(J159), "000"))</f>
+        <v>001</v>
+      </c>
+      <c r="Q159" s="17" t="str">
+        <f t="shared" si="277"/>
+        <v/>
+      </c>
+      <c r="R159" s="18" t="str">
+        <f t="shared" si="278"/>
+        <v/>
+      </c>
+      <c r="S159" t="str">
+        <f t="shared" si="279"/>
+        <v>44</v>
+      </c>
+      <c r="T159" t="str">
+        <f>BIN2HEX(CONCATENATE(RIGHT(N159, 1), IF(O159 = "", "000", O159), IF(P159 = "", "000", P159), "0"), 2)</f>
+        <v>62</v>
+      </c>
+      <c r="U159" s="13" t="str">
+        <f t="shared" si="281"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="160" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>18</v>
+      </c>
+      <c r="B160" t="str">
+        <f t="shared" si="266"/>
+        <v>0x012</v>
+      </c>
+      <c r="C160" t="s">
+        <v>227</v>
+      </c>
+      <c r="E160" s="44"/>
+      <c r="F160" s="11">
+        <v>40</v>
+      </c>
+      <c r="G160" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="H160">
+        <f t="shared" si="273"/>
+        <v>3</v>
+      </c>
+      <c r="M160" s="16" t="str">
+        <f>IF(F160="", "", TEXT(DEC2BIN(F160), "000000"))</f>
+        <v>101000</v>
+      </c>
+      <c r="N160" s="17" t="str">
+        <f t="shared" si="275"/>
+        <v>011</v>
+      </c>
+      <c r="O160" s="17" t="str">
+        <f t="shared" si="276"/>
+        <v/>
+      </c>
+      <c r="P160" s="17"/>
+      <c r="Q160" s="17" t="str">
+        <f t="shared" si="277"/>
+        <v/>
+      </c>
+      <c r="R160" s="18" t="str">
+        <f t="shared" si="278"/>
+        <v/>
+      </c>
+      <c r="S160" t="str">
+        <f>BIN2HEX(LEFT(CONCATENATE(M160,IF(N160="", "000", N160)), 8), 2)</f>
+        <v>A1</v>
+      </c>
+      <c r="T160" t="str">
+        <f>BIN2HEX(CONCATENATE(RIGHT(N160, 1), IF(O160 = "", "000", O160), "0000"), 2)</f>
+        <v>80</v>
+      </c>
+      <c r="U160" s="13" t="str">
+        <f>IF(Q160="", BIN2HEX(R160, 2), BIN2HEX(Q160,2))</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="161" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>21</v>
+      </c>
+      <c r="B161" t="str">
+        <f t="shared" si="266"/>
+        <v>0x015</v>
+      </c>
+      <c r="C161" t="s">
+        <v>231</v>
+      </c>
+      <c r="E161" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="F161" s="11">
+        <v>2</v>
+      </c>
+      <c r="G161" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="H161">
+        <f t="shared" si="273"/>
+        <v>1</v>
+      </c>
+      <c r="I161">
+        <v>3</v>
+      </c>
+      <c r="M161" s="16" t="str">
+        <f t="shared" ref="M161" si="283">IF(F161="", "", TEXT(DEC2BIN(F161), "000000"))</f>
+        <v>000010</v>
+      </c>
+      <c r="N161" s="17" t="str">
+        <f t="shared" si="275"/>
+        <v>001</v>
+      </c>
+      <c r="O161" s="17" t="str">
+        <f t="shared" si="276"/>
+        <v>011</v>
+      </c>
+      <c r="P161" s="17"/>
+      <c r="Q161" s="17" t="str">
+        <f t="shared" si="277"/>
+        <v/>
+      </c>
+      <c r="R161" s="18" t="str">
+        <f t="shared" si="278"/>
+        <v/>
+      </c>
+      <c r="S161" t="str">
+        <f t="shared" ref="S161" si="284">BIN2HEX(LEFT(CONCATENATE(M161,IF(N161="", "000", N161)), 8), 2)</f>
+        <v>08</v>
+      </c>
+      <c r="T161" t="str">
+        <f t="shared" ref="T161" si="285">BIN2HEX(CONCATENATE(RIGHT(N161, 1), IF(O161 = "", "000", O161), "0000"), 2)</f>
+        <v>B0</v>
+      </c>
+      <c r="U161" s="13" t="str">
+        <f t="shared" ref="U161" si="286">IF(Q161="", BIN2HEX(R161, 2), BIN2HEX(Q161,2))</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="162" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>24</v>
+      </c>
+      <c r="B162" t="str">
+        <f t="shared" si="266"/>
+        <v>0x018</v>
+      </c>
+      <c r="C162" t="s">
+        <v>228</v>
+      </c>
+      <c r="E162" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="F162" s="11">
+        <v>33</v>
+      </c>
+      <c r="G162" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="H162">
+        <f t="shared" si="273"/>
+        <v>3</v>
+      </c>
+      <c r="I162">
+        <v>7</v>
+      </c>
+      <c r="M162" s="16" t="str">
+        <f>IF(F162="", "", TEXT(DEC2BIN(F162), "000000"))</f>
+        <v>100001</v>
+      </c>
+      <c r="N162" s="17" t="str">
+        <f t="shared" si="275"/>
+        <v>011</v>
+      </c>
+      <c r="O162" s="17" t="str">
+        <f t="shared" si="276"/>
+        <v>111</v>
+      </c>
+      <c r="P162" s="17"/>
+      <c r="Q162" s="17" t="str">
+        <f t="shared" si="277"/>
+        <v/>
+      </c>
+      <c r="R162" s="18" t="str">
+        <f t="shared" si="278"/>
+        <v/>
+      </c>
+      <c r="S162" t="str">
+        <f>BIN2HEX(LEFT(CONCATENATE(M162,IF(N162="", "000", N162)), 8), 2)</f>
+        <v>85</v>
+      </c>
+      <c r="T162" t="str">
+        <f>BIN2HEX(CONCATENATE(RIGHT(N162, 1), IF(O162 = "", "000", O162), "0000"), 2)</f>
+        <v>F0</v>
+      </c>
+      <c r="U162" s="13" t="str">
+        <f>IF(Q162="", BIN2HEX(R162, 2), BIN2HEX(Q162,2))</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="163" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>27</v>
+      </c>
+      <c r="B163" t="str">
+        <f t="shared" si="266"/>
+        <v>0x01B</v>
+      </c>
+      <c r="C163" t="s">
+        <v>195</v>
+      </c>
+      <c r="E163" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="F163" s="11">
+        <v>6</v>
+      </c>
+      <c r="H163" t="str">
+        <f t="shared" si="273"/>
+        <v/>
+      </c>
+      <c r="K163">
+        <v>24</v>
+      </c>
+      <c r="M163" s="16" t="str">
+        <f>IF(F163="", "", TEXT(DEC2BIN(F163), "000000"))</f>
+        <v>000110</v>
+      </c>
+      <c r="N163" s="17" t="str">
+        <f t="shared" si="275"/>
+        <v/>
+      </c>
+      <c r="O163" s="17" t="str">
+        <f t="shared" si="276"/>
+        <v/>
+      </c>
+      <c r="P163" s="17"/>
+      <c r="Q163" s="17" t="str">
+        <f t="shared" si="277"/>
+        <v>00011000</v>
+      </c>
+      <c r="R163" s="18" t="str">
+        <f t="shared" si="278"/>
+        <v/>
+      </c>
+      <c r="S163" t="str">
+        <f>BIN2HEX(LEFT(CONCATENATE(M163,IF(N163="", "000", N163)), 8), 2)</f>
+        <v>18</v>
+      </c>
+      <c r="T163" t="str">
+        <f>BIN2HEX(CONCATENATE(RIGHT(N163, 1), IF(O163 = "", "000", O163), "0000"), 2)</f>
+        <v>00</v>
+      </c>
+      <c r="U163" s="13" t="str">
+        <f>IF(Q163="", BIN2HEX(R163, 2), BIN2HEX(Q163,2))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="164" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>30</v>
+      </c>
+      <c r="B164" t="str">
+        <f t="shared" si="266"/>
+        <v>0x01E</v>
+      </c>
+      <c r="C164" t="s">
+        <v>233</v>
+      </c>
+      <c r="E164" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="F164" s="11">
+        <v>2</v>
+      </c>
+      <c r="G164" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="H164">
+        <f t="shared" si="273"/>
+        <v>3</v>
+      </c>
+      <c r="I164">
+        <v>1</v>
+      </c>
+      <c r="M164" s="16" t="str">
+        <f t="shared" ref="M164:M165" si="287">IF(F164="", "", TEXT(DEC2BIN(F164), "000000"))</f>
+        <v>000010</v>
+      </c>
+      <c r="N164" s="17" t="str">
+        <f t="shared" si="275"/>
+        <v>011</v>
+      </c>
+      <c r="O164" s="17" t="str">
+        <f t="shared" si="276"/>
+        <v>001</v>
+      </c>
+      <c r="P164" s="17"/>
+      <c r="Q164" s="17" t="str">
+        <f t="shared" si="277"/>
+        <v/>
+      </c>
+      <c r="R164" s="18" t="str">
+        <f t="shared" si="278"/>
+        <v/>
+      </c>
+      <c r="S164" t="str">
+        <f t="shared" ref="S164:S167" si="288">BIN2HEX(LEFT(CONCATENATE(M164,IF(N164="", "000", N164)), 8), 2)</f>
+        <v>09</v>
+      </c>
+      <c r="T164" t="str">
+        <f t="shared" ref="T164:T165" si="289">BIN2HEX(CONCATENATE(RIGHT(N164, 1), IF(O164 = "", "000", O164), "0000"), 2)</f>
+        <v>90</v>
+      </c>
+      <c r="U164" s="13" t="str">
+        <f t="shared" ref="U164:U167" si="290">IF(Q164="", BIN2HEX(R164, 2), BIN2HEX(Q164,2))</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="165" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>33</v>
+      </c>
+      <c r="B165" t="str">
+        <f t="shared" si="266"/>
+        <v>0x021</v>
+      </c>
+      <c r="C165" t="s">
+        <v>259</v>
+      </c>
+      <c r="E165" s="51" t="s">
+        <v>245</v>
+      </c>
+      <c r="F165" s="11">
+        <v>2</v>
+      </c>
+      <c r="G165" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="H165">
+        <f t="shared" si="273"/>
+        <v>1</v>
+      </c>
+      <c r="I165">
+        <v>6</v>
+      </c>
+      <c r="M165" s="16" t="str">
+        <f t="shared" si="287"/>
+        <v>000010</v>
+      </c>
+      <c r="N165" s="17" t="str">
+        <f t="shared" si="275"/>
+        <v>001</v>
+      </c>
+      <c r="O165" s="17" t="str">
+        <f t="shared" si="276"/>
+        <v>110</v>
+      </c>
+      <c r="P165" s="17"/>
+      <c r="Q165" s="17" t="str">
+        <f t="shared" si="277"/>
+        <v/>
+      </c>
+      <c r="R165" s="18" t="str">
+        <f t="shared" si="278"/>
+        <v/>
+      </c>
+      <c r="S165" t="str">
+        <f t="shared" si="288"/>
+        <v>08</v>
+      </c>
+      <c r="T165" t="str">
+        <f t="shared" si="289"/>
+        <v>E0</v>
+      </c>
+      <c r="U165" s="13" t="str">
+        <f t="shared" si="290"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="166" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>36</v>
+      </c>
+      <c r="B166" t="str">
+        <f t="shared" si="266"/>
+        <v>0x024</v>
+      </c>
+      <c r="C166" t="s">
+        <v>236</v>
+      </c>
+      <c r="E166" s="51"/>
+      <c r="F166" s="11">
+        <v>40</v>
+      </c>
+      <c r="G166" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="H166">
+        <f t="shared" si="273"/>
+        <v>1</v>
+      </c>
+      <c r="M166" s="16" t="str">
+        <f>IF(F166="", "", TEXT(DEC2BIN(F166), "000000"))</f>
+        <v>101000</v>
+      </c>
+      <c r="N166" s="17" t="str">
+        <f>IF(H166="", "", TEXT(DEC2BIN(H166), "000"))</f>
+        <v>001</v>
+      </c>
+      <c r="O166" s="17" t="str">
+        <f>IF(I166="", "", TEXT(DEC2BIN(I166), "000"))</f>
+        <v/>
+      </c>
+      <c r="P166" s="17"/>
+      <c r="Q166" s="17" t="str">
+        <f>IF(K166="", "", TEXT(DEC2BIN(K166), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="R166" s="18" t="str">
+        <f>IF(L166="", "", TEXT(DEC2BIN(L166), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="S166" t="str">
+        <f t="shared" si="288"/>
+        <v>A0</v>
+      </c>
+      <c r="T166" t="str">
+        <f>BIN2HEX(CONCATENATE(RIGHT(N166, 1), IF(O166 = "", "000", O166), "0000"), 2)</f>
+        <v>80</v>
+      </c>
+      <c r="U166" s="13" t="str">
+        <f t="shared" si="290"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="167" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>39</v>
+      </c>
+      <c r="B167" t="str">
+        <f t="shared" si="266"/>
+        <v>0x027</v>
+      </c>
+      <c r="C167" t="s">
+        <v>260</v>
+      </c>
+      <c r="E167" s="51"/>
+      <c r="F167" s="11">
+        <v>2</v>
+      </c>
+      <c r="G167" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="H167">
+        <f t="shared" si="273"/>
+        <v>6</v>
+      </c>
+      <c r="I167">
+        <v>1</v>
+      </c>
+      <c r="M167" s="16" t="str">
+        <f t="shared" ref="M167" si="291">IF(F167="", "", TEXT(DEC2BIN(F167), "000000"))</f>
+        <v>000010</v>
+      </c>
+      <c r="N167" s="17" t="str">
+        <f t="shared" ref="N167" si="292">IF(H167="", "", TEXT(DEC2BIN(H167), "000"))</f>
+        <v>110</v>
+      </c>
+      <c r="O167" s="17" t="str">
+        <f t="shared" ref="O167" si="293">IF(I167="", "", TEXT(DEC2BIN(I167), "000"))</f>
+        <v>001</v>
+      </c>
+      <c r="P167" s="17"/>
+      <c r="Q167" s="17" t="str">
+        <f t="shared" ref="Q167" si="294">IF(K167="", "", TEXT(DEC2BIN(K167), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="R167" s="18" t="str">
+        <f t="shared" ref="R167" si="295">IF(L167="", "", TEXT(DEC2BIN(L167), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="S167" t="str">
+        <f t="shared" si="288"/>
+        <v>0B</v>
+      </c>
+      <c r="T167" t="str">
+        <f t="shared" ref="T167" si="296">BIN2HEX(CONCATENATE(RIGHT(N167, 1), IF(O167 = "", "000", O167), "0000"), 2)</f>
+        <v>10</v>
+      </c>
+      <c r="U167" s="13" t="str">
+        <f t="shared" si="290"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="168" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>42</v>
+      </c>
+      <c r="B168" t="str">
+        <f t="shared" si="266"/>
+        <v>0x02A</v>
+      </c>
+      <c r="C168" t="s">
+        <v>82</v>
+      </c>
+      <c r="E168" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="F168" s="11">
+        <v>5</v>
+      </c>
+      <c r="H168" t="str">
+        <f t="shared" si="273"/>
+        <v/>
+      </c>
+      <c r="K168">
+        <v>9</v>
+      </c>
+      <c r="M168" s="16" t="str">
+        <f>IF(F168="", "", TEXT(DEC2BIN(F168), "000000"))</f>
+        <v>000101</v>
+      </c>
+      <c r="N168" s="17" t="str">
+        <f t="shared" si="275"/>
+        <v/>
+      </c>
+      <c r="O168" s="17" t="str">
+        <f t="shared" si="276"/>
+        <v/>
+      </c>
+      <c r="P168" s="17"/>
+      <c r="Q168" s="17" t="str">
+        <f t="shared" si="277"/>
+        <v>00001001</v>
+      </c>
+      <c r="R168" s="18" t="str">
+        <f t="shared" si="278"/>
+        <v/>
+      </c>
+      <c r="S168" t="str">
+        <f>BIN2HEX(LEFT(CONCATENATE(M168,IF(N168="", "000", N168)), 8), 2)</f>
+        <v>14</v>
+      </c>
+      <c r="T168" t="str">
+        <f>BIN2HEX(CONCATENATE(RIGHT(N168, 1), IF(O168 = "", "000", O168), "0000"), 2)</f>
+        <v>00</v>
+      </c>
+      <c r="U168" s="13" t="str">
+        <f>IF(Q168="", BIN2HEX(R168, 2), BIN2HEX(Q168,2))</f>
+        <v>09</v>
+      </c>
+    </row>
+    <row r="169" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E169" s="8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="170" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>48</v>
+      </c>
+      <c r="B170" t="str">
+        <f t="shared" ref="B170:B173" si="297">"0x" &amp; DEC2HEX(A170,3)</f>
+        <v>0x030</v>
+      </c>
+      <c r="D170" s="7" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="171" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>51</v>
+      </c>
+      <c r="B171" t="str">
+        <f t="shared" si="297"/>
+        <v>0x033</v>
+      </c>
+      <c r="D171" s="7" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="172" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>54</v>
+      </c>
+      <c r="B172" t="str">
+        <f t="shared" si="297"/>
+        <v>0x036</v>
+      </c>
+      <c r="D172" s="7" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="173" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>57</v>
+      </c>
+      <c r="B173" t="str">
+        <f t="shared" si="297"/>
+        <v>0x039</v>
+      </c>
+      <c r="D173" s="7" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="174" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>60</v>
+      </c>
+      <c r="B174" t="str">
+        <f t="shared" ref="B174:B181" si="298">"0x" &amp; DEC2HEX(A174,3)</f>
+        <v>0x03C</v>
+      </c>
+      <c r="D174" s="7" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="175" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>63</v>
+      </c>
+      <c r="B175" t="str">
+        <f t="shared" si="298"/>
+        <v>0x03F</v>
+      </c>
+      <c r="D175" s="7" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="176" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>66</v>
+      </c>
+      <c r="B176" t="str">
+        <f t="shared" si="298"/>
+        <v>0x042</v>
+      </c>
+      <c r="D176" s="7" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>69</v>
+      </c>
+      <c r="B177" t="str">
+        <f t="shared" si="298"/>
+        <v>0x045</v>
+      </c>
+      <c r="D177" s="7" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>72</v>
+      </c>
+      <c r="B178" t="str">
+        <f t="shared" si="298"/>
+        <v>0x048</v>
+      </c>
+      <c r="D178" s="7" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>75</v>
+      </c>
+      <c r="B179" t="str">
+        <f t="shared" si="298"/>
+        <v>0x04B</v>
+      </c>
+      <c r="D179" s="7" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>78</v>
+      </c>
+      <c r="B180" t="str">
+        <f t="shared" si="298"/>
+        <v>0x04E</v>
+      </c>
+      <c r="D180" s="7" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>81</v>
+      </c>
+      <c r="B181" t="str">
+        <f t="shared" si="298"/>
+        <v>0x051</v>
+      </c>
+      <c r="D181" s="7" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>84</v>
+      </c>
+      <c r="B182" t="str">
+        <f t="shared" ref="B182:B191" si="299">"0x" &amp; DEC2HEX(A182,3)</f>
+        <v>0x054</v>
+      </c>
+      <c r="D182" s="7" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>87</v>
+      </c>
+      <c r="B183" t="str">
+        <f t="shared" si="299"/>
+        <v>0x057</v>
+      </c>
+      <c r="D183" s="7" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>90</v>
+      </c>
+      <c r="B184" t="str">
+        <f t="shared" si="299"/>
+        <v>0x05A</v>
+      </c>
+      <c r="D184" s="7" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>93</v>
+      </c>
+      <c r="B185" t="str">
+        <f t="shared" si="299"/>
+        <v>0x05D</v>
+      </c>
+      <c r="D185" s="7" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>96</v>
+      </c>
+      <c r="B186" t="str">
+        <f t="shared" si="299"/>
+        <v>0x060</v>
+      </c>
+      <c r="D186" s="7" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>99</v>
+      </c>
+      <c r="B187" t="str">
+        <f t="shared" si="299"/>
+        <v>0x063</v>
+      </c>
+      <c r="D187" s="7" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>102</v>
+      </c>
+      <c r="B188" t="str">
+        <f t="shared" si="299"/>
+        <v>0x066</v>
+      </c>
+      <c r="D188" s="7" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>105</v>
+      </c>
+      <c r="B189" t="str">
+        <f t="shared" si="299"/>
+        <v>0x069</v>
+      </c>
+      <c r="D189" s="7" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>108</v>
+      </c>
+      <c r="B190" t="str">
+        <f t="shared" si="299"/>
+        <v>0x06C</v>
+      </c>
+      <c r="D190" s="7" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>111</v>
+      </c>
+      <c r="B191" t="str">
+        <f t="shared" si="299"/>
+        <v>0x06F</v>
+      </c>
+      <c r="D191" s="7" t="s">
+        <v>271</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="W16:X18">
     <sortCondition ref="W13"/>
   </sortState>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="S1:U1"/>
     <mergeCell ref="E129:E131"/>
+    <mergeCell ref="E165:E167"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y17">
       <formula1>$W$16:$W$18</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G6 G9:G11 G17:G26 G31:G33 G41:G42 G49 G83:G93 G117:G132 G102:G112 G144 G141:G143 G145:G149">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G6 G9:G11 G17:G26 G31:G33 G41:G42 G49 G83:G93 G117:G132 G102:G112 G141:G149 G154:G168">
       <formula1>$W$3:$W$10</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
v.0.15.2 - Output to led matrix improved by adding an extra layer of flip flops to make animations smoothier.
</commit_message>
<xml_diff>
--- a/2nd gen - 8 bit cpu/Instruction control lines.xlsx
+++ b/2nd gen - 8 bit cpu/Instruction control lines.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="7830" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="288" windowWidth="14808" windowHeight="7836" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Control Lines" sheetId="1" r:id="rId1"/>
     <sheet name="Some instructions for test" sheetId="2" r:id="rId2"/>
     <sheet name="Test Programs" sheetId="3" r:id="rId3"/>
+    <sheet name="Animations" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
@@ -22,7 +23,7 @@
     <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="C20" authorId="0">
+    <comment ref="C20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -51,7 +52,7 @@
     <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="H1" authorId="0">
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -87,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="275">
   <si>
     <t>LD R1, data</t>
   </si>
@@ -906,12 +907,18 @@
   </si>
   <si>
     <t>LD F, 0x70</t>
+  </si>
+  <si>
+    <t>SUB B, F</t>
+  </si>
+  <si>
+    <t>Frame #</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1022,7 +1029,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1107,11 +1114,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1214,6 +1230,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1234,7 +1254,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1272,9 +1292,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1307,9 +1327,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1342,9 +1379,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1525,21 +1579,21 @@
       <selection pane="bottomLeft" activeCell="P35" sqref="P35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="7.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.88671875" style="2" customWidth="1"/>
     <col min="3" max="3" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="17" width="3.28515625" customWidth="1"/>
-    <col min="18" max="19" width="3.28515625" style="4" customWidth="1"/>
-    <col min="20" max="20" width="3.28515625" customWidth="1"/>
-    <col min="21" max="21" width="3.28515625" style="41" customWidth="1"/>
-    <col min="22" max="27" width="3.28515625" customWidth="1"/>
-    <col min="28" max="30" width="5.85546875" customWidth="1"/>
+    <col min="4" max="17" width="3.33203125" customWidth="1"/>
+    <col min="18" max="19" width="3.33203125" style="4" customWidth="1"/>
+    <col min="20" max="20" width="3.33203125" customWidth="1"/>
+    <col min="21" max="21" width="3.33203125" style="41" customWidth="1"/>
+    <col min="22" max="27" width="3.33203125" customWidth="1"/>
+    <col min="28" max="30" width="5.88671875" customWidth="1"/>
     <col min="31" max="31" width="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.3">
       <c r="D1">
         <v>23</v>
       </c>
@@ -1613,7 +1667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:39" s="1" customFormat="1" ht="130.15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:39" s="1" customFormat="1" ht="129" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>205</v>
       </c>
@@ -1701,7 +1755,7 @@
       <c r="AC2" s="47"/>
       <c r="AD2" s="47"/>
     </row>
-    <row r="3" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>0</v>
       </c>
@@ -1805,7 +1859,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="4" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -1905,7 +1959,7 @@
         <v>C00000</v>
       </c>
     </row>
-    <row r="5" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -2005,7 +2059,7 @@
         <v>600400</v>
       </c>
     </row>
-    <row r="6" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -2105,7 +2159,7 @@
         <v>5E0000</v>
       </c>
     </row>
-    <row r="7" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -2205,7 +2259,7 @@
         <v>4F0000</v>
       </c>
     </row>
-    <row r="8" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>5</v>
       </c>
@@ -2305,7 +2359,7 @@
         <v>004000</v>
       </c>
     </row>
-    <row r="9" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>6</v>
       </c>
@@ -2405,7 +2459,7 @@
         <v>006000</v>
       </c>
     </row>
-    <row r="10" spans="1:39" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="33">
         <v>7</v>
       </c>
@@ -2505,7 +2559,7 @@
         <v>004200</v>
       </c>
     </row>
-    <row r="11" spans="1:39" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="33">
         <v>8</v>
       </c>
@@ -2605,7 +2659,7 @@
         <v>006200</v>
       </c>
     </row>
-    <row r="12" spans="1:39" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="33">
         <v>9</v>
       </c>
@@ -2677,7 +2731,7 @@
         <v>000100</v>
       </c>
     </row>
-    <row r="13" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>10</v>
       </c>
@@ -2780,7 +2834,7 @@
         <v>181800</v>
       </c>
     </row>
-    <row r="14" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>11</v>
       </c>
@@ -2880,7 +2934,7 @@
         <v>091800</v>
       </c>
     </row>
-    <row r="15" spans="1:39" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="33">
         <v>12</v>
       </c>
@@ -2931,7 +2985,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="16" spans="1:39" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="33">
         <v>13</v>
       </c>
@@ -2982,7 +3036,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="17" spans="1:40" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:40" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="33">
         <v>14</v>
       </c>
@@ -3033,7 +3087,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="18" spans="1:40" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:40" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="33">
         <v>15</v>
       </c>
@@ -3084,7 +3138,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="19" spans="1:40" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:40" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="33">
         <v>16</v>
       </c>
@@ -3127,7 +3181,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="20" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>17</v>
       </c>
@@ -3233,7 +3287,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="21" spans="1:40" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>18</v>
       </c>
@@ -3266,7 +3320,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="22" spans="1:40" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>19</v>
       </c>
@@ -3299,7 +3353,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="23" spans="1:40" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>20</v>
       </c>
@@ -3332,7 +3386,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="24" spans="1:40" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>21</v>
       </c>
@@ -3365,7 +3419,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="25" spans="1:40" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>22</v>
       </c>
@@ -3398,7 +3452,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="26" spans="1:40" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>23</v>
       </c>
@@ -3431,7 +3485,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="27" spans="1:40" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>24</v>
       </c>
@@ -3464,7 +3518,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="28" spans="1:40" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>25</v>
       </c>
@@ -3497,7 +3551,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="29" spans="1:40" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>26</v>
       </c>
@@ -3530,7 +3584,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="30" spans="1:40" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>27</v>
       </c>
@@ -3563,7 +3617,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="31" spans="1:40" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>28</v>
       </c>
@@ -3596,7 +3650,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="32" spans="1:40" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>29</v>
       </c>
@@ -3629,7 +3683,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="33" spans="1:40" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>30</v>
       </c>
@@ -3662,7 +3716,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="34" spans="1:40" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>31</v>
       </c>
@@ -3695,7 +3749,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="35" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>32</v>
       </c>
@@ -3798,7 +3852,7 @@
         <v>408825</v>
       </c>
     </row>
-    <row r="36" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>33</v>
       </c>
@@ -3901,7 +3955,7 @@
         <v>408818</v>
       </c>
     </row>
-    <row r="37" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>34</v>
       </c>
@@ -4004,7 +4058,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="38" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>35</v>
       </c>
@@ -4104,7 +4158,7 @@
         <v>40882E</v>
       </c>
     </row>
-    <row r="39" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>36</v>
       </c>
@@ -4204,7 +4258,7 @@
         <v>40883A</v>
       </c>
     </row>
-    <row r="40" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>37</v>
       </c>
@@ -4304,7 +4358,7 @@
         <v>40881A</v>
       </c>
     </row>
-    <row r="41" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>38</v>
       </c>
@@ -4404,7 +4458,7 @@
         <v>408806</v>
       </c>
     </row>
-    <row r="42" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>39</v>
       </c>
@@ -4504,7 +4558,7 @@
         <v>408826</v>
       </c>
     </row>
-    <row r="43" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>40</v>
       </c>
@@ -4604,7 +4658,7 @@
         <v>408800</v>
       </c>
     </row>
-    <row r="44" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>41</v>
       </c>
@@ -4704,7 +4758,7 @@
         <v>40883D</v>
       </c>
     </row>
-    <row r="46" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:40" x14ac:dyDescent="0.3">
       <c r="C46" s="3" t="s">
         <v>22</v>
       </c>
@@ -4712,7 +4766,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:40" x14ac:dyDescent="0.3">
       <c r="C47" s="5" t="s">
         <v>30</v>
       </c>
@@ -4720,7 +4774,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C49" s="1" t="s">
         <v>53</v>
       </c>
@@ -4728,7 +4782,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C50" s="1" t="s">
         <v>62</v>
       </c>
@@ -4736,7 +4790,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C51" s="1" t="s">
         <v>47</v>
       </c>
@@ -4744,7 +4798,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A52"/>
       <c r="B52"/>
       <c r="C52" s="1" t="s">
@@ -4756,7 +4810,7 @@
       <c r="R52"/>
       <c r="S52"/>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A53"/>
       <c r="B53"/>
       <c r="C53" s="1" t="s">
@@ -4768,7 +4822,7 @@
       <c r="R53"/>
       <c r="S53"/>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A54"/>
       <c r="B54"/>
       <c r="C54" s="1" t="s">
@@ -4798,10 +4852,10 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="9.140625" style="7"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="9.109375" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -4949,33 +5003,33 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z191"/>
+  <dimension ref="A1:Z190"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M181" sqref="M181"/>
+      <pane ySplit="1" topLeftCell="A151" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L174" sqref="L174"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" style="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="3" style="12" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.42578125" style="16" customWidth="1"/>
-    <col min="14" max="15" width="9.140625" style="2"/>
-    <col min="16" max="16" width="8.85546875" style="2"/>
-    <col min="17" max="17" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.85546875" style="18" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="3.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.44140625" style="16" customWidth="1"/>
+    <col min="14" max="15" width="9.109375" style="2"/>
+    <col min="16" max="16" width="8.88671875" style="2"/>
+    <col min="17" max="17" width="10.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.88671875" style="18" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="3.44140625" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>84</v>
       </c>
@@ -5028,7 +5082,7 @@
       <c r="U1" s="50"/>
       <c r="V1" s="10"/>
     </row>
-    <row r="2" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="8" t="s">
@@ -5042,7 +5096,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
@@ -5107,7 +5161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5174,7 +5228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>6</v>
       </c>
@@ -5239,7 +5293,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>9</v>
       </c>
@@ -5301,7 +5355,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="E7" s="8"/>
       <c r="N7" s="17"/>
       <c r="O7" s="17"/>
@@ -5314,7 +5368,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C8" s="8" t="s">
         <v>214</v>
       </c>
@@ -5326,7 +5380,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0</v>
       </c>
@@ -5391,7 +5445,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3</v>
       </c>
@@ -5452,7 +5506,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>6</v>
       </c>
@@ -5507,7 +5561,7 @@
         <v>03</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C16" s="8" t="s">
         <v>217</v>
       </c>
@@ -5518,7 +5572,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>0</v>
       </c>
@@ -5589,7 +5643,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>3</v>
       </c>
@@ -5653,7 +5707,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>6</v>
       </c>
@@ -5708,7 +5762,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="20" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>9</v>
       </c>
@@ -5766,7 +5820,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="21" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>12</v>
       </c>
@@ -5822,48 +5876,48 @@
         <v>06</v>
       </c>
     </row>
-    <row r="22" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
       <c r="E22" s="39"/>
       <c r="N22" s="17"/>
       <c r="O22" s="17"/>
       <c r="P22" s="17"/>
       <c r="Q22" s="17"/>
     </row>
-    <row r="23" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
       <c r="E23" s="39"/>
       <c r="N23" s="17"/>
       <c r="O23" s="17"/>
       <c r="P23" s="17"/>
       <c r="Q23" s="17"/>
     </row>
-    <row r="24" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
       <c r="E24" s="39"/>
       <c r="N24" s="17"/>
       <c r="O24" s="17"/>
       <c r="P24" s="17"/>
       <c r="Q24" s="17"/>
     </row>
-    <row r="25" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
       <c r="E25" s="39"/>
       <c r="N25" s="17"/>
       <c r="O25" s="17"/>
       <c r="P25" s="17"/>
       <c r="Q25" s="17"/>
     </row>
-    <row r="26" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
       <c r="N26" s="17"/>
       <c r="O26" s="17"/>
       <c r="P26" s="17"/>
       <c r="Q26" s="17"/>
     </row>
-    <row r="30" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="8" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>0</v>
       </c>
@@ -5921,7 +5975,7 @@
         <v>01</v>
       </c>
     </row>
-    <row r="32" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>3</v>
       </c>
@@ -5979,7 +6033,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>6</v>
       </c>
@@ -6037,7 +6091,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="34" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>9</v>
       </c>
@@ -6088,7 +6142,7 @@
         <v>0F</v>
       </c>
     </row>
-    <row r="35" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>12</v>
       </c>
@@ -6139,7 +6193,7 @@
         <v>06</v>
       </c>
     </row>
-    <row r="36" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>15</v>
       </c>
@@ -6190,12 +6244,12 @@
         <v>0F</v>
       </c>
     </row>
-    <row r="40" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C40" s="8" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="41" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>0</v>
       </c>
@@ -6253,7 +6307,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>3</v>
       </c>
@@ -6311,7 +6365,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>6</v>
       </c>
@@ -6362,7 +6416,7 @@
         <v>06</v>
       </c>
     </row>
-    <row r="44" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>16</v>
       </c>
@@ -6377,15 +6431,15 @@
         <v>151</v>
       </c>
     </row>
-    <row r="46" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C46" s="38"/>
     </row>
-    <row r="48" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C48" s="8" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>0</v>
       </c>
@@ -6446,7 +6500,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="50" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>3</v>
       </c>
@@ -6500,18 +6554,18 @@
         <v>00</v>
       </c>
     </row>
-    <row r="51" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
       <c r="N51" s="17"/>
       <c r="O51" s="17"/>
       <c r="P51" s="17"/>
       <c r="Q51" s="17"/>
     </row>
-    <row r="55" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C55" s="8" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="56" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>0</v>
       </c>
@@ -6530,7 +6584,7 @@
       </c>
       <c r="F56" s="43"/>
     </row>
-    <row r="57" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>3</v>
       </c>
@@ -6546,7 +6600,7 @@
       </c>
       <c r="E57" s="8"/>
     </row>
-    <row r="58" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>6</v>
       </c>
@@ -6564,7 +6618,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="59" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>9</v>
       </c>
@@ -6580,7 +6634,7 @@
       </c>
       <c r="E59" s="8"/>
     </row>
-    <row r="60" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>12</v>
       </c>
@@ -6598,7 +6652,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="61" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>15</v>
       </c>
@@ -6614,7 +6668,7 @@
       </c>
       <c r="E61" s="8"/>
     </row>
-    <row r="62" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>18</v>
       </c>
@@ -6632,7 +6686,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="63" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>21</v>
       </c>
@@ -6648,7 +6702,7 @@
       </c>
       <c r="E63" s="8"/>
     </row>
-    <row r="64" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>24</v>
       </c>
@@ -6666,7 +6720,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>27</v>
       </c>
@@ -6682,7 +6736,7 @@
       </c>
       <c r="E65" s="8"/>
     </row>
-    <row r="66" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>30</v>
       </c>
@@ -6700,7 +6754,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>33</v>
       </c>
@@ -6716,7 +6770,7 @@
       </c>
       <c r="E67" s="8"/>
     </row>
-    <row r="68" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>36</v>
       </c>
@@ -6734,7 +6788,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>39</v>
       </c>
@@ -6750,7 +6804,7 @@
       </c>
       <c r="E69" s="8"/>
     </row>
-    <row r="70" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>42</v>
       </c>
@@ -6768,7 +6822,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>45</v>
       </c>
@@ -6784,7 +6838,7 @@
       </c>
       <c r="E71" s="8"/>
     </row>
-    <row r="72" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>48</v>
       </c>
@@ -6802,7 +6856,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>51</v>
       </c>
@@ -6818,7 +6872,7 @@
       </c>
       <c r="E73" s="8"/>
     </row>
-    <row r="74" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>54</v>
       </c>
@@ -6836,7 +6890,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>57</v>
       </c>
@@ -6852,7 +6906,7 @@
       </c>
       <c r="E75" s="8"/>
     </row>
-    <row r="76" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>60</v>
       </c>
@@ -6870,7 +6924,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>63</v>
       </c>
@@ -6886,7 +6940,7 @@
       </c>
       <c r="E77" s="8"/>
     </row>
-    <row r="78" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>66</v>
       </c>
@@ -6904,7 +6958,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>69</v>
       </c>
@@ -6920,21 +6974,21 @@
       </c>
       <c r="E79" s="8"/>
     </row>
-    <row r="80" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E80" s="8"/>
     </row>
-    <row r="81" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:21" x14ac:dyDescent="0.3">
       <c r="D81"/>
       <c r="E81" s="8"/>
     </row>
-    <row r="82" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C82" s="8" t="s">
         <v>139</v>
       </c>
       <c r="D82"/>
       <c r="E82" s="8"/>
     </row>
-    <row r="83" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>0</v>
       </c>
@@ -6996,7 +7050,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="84" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>3</v>
       </c>
@@ -7057,7 +7111,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="85" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>6</v>
       </c>
@@ -7118,7 +7172,7 @@
         <v>3C</v>
       </c>
     </row>
-    <row r="86" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>9</v>
       </c>
@@ -7176,7 +7230,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="87" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>12</v>
       </c>
@@ -7238,7 +7292,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="88" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>15</v>
       </c>
@@ -7294,7 +7348,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="89" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>18</v>
       </c>
@@ -7355,7 +7409,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="90" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>21</v>
       </c>
@@ -7416,7 +7470,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="91" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>24</v>
       </c>
@@ -7474,7 +7528,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="92" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>27</v>
       </c>
@@ -7535,7 +7589,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="93" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>30</v>
       </c>
@@ -7598,7 +7652,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="95" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>48</v>
       </c>
@@ -7613,7 +7667,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="96" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>51</v>
       </c>
@@ -7628,7 +7682,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="97" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>54</v>
       </c>
@@ -7643,7 +7697,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="98" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>57</v>
       </c>
@@ -7658,25 +7712,25 @@
         <v>159</v>
       </c>
     </row>
-    <row r="99" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C99" s="5"/>
       <c r="E99" s="8"/>
     </row>
-    <row r="100" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C100" s="5" t="s">
         <v>256</v>
       </c>
       <c r="D100"/>
       <c r="E100" s="8"/>
     </row>
-    <row r="101" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C101" s="8" t="s">
         <v>140</v>
       </c>
       <c r="D101"/>
       <c r="E101" s="8"/>
     </row>
-    <row r="102" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>0</v>
       </c>
@@ -7740,7 +7794,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="103" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>3</v>
       </c>
@@ -7804,7 +7858,7 @@
         <v>FF</v>
       </c>
     </row>
-    <row r="104" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>6</v>
       </c>
@@ -7865,7 +7919,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="105" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>9</v>
       </c>
@@ -7923,7 +7977,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="106" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>12</v>
       </c>
@@ -7982,7 +8036,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="107" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>15</v>
       </c>
@@ -8046,7 +8100,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="108" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>18</v>
       </c>
@@ -8110,7 +8164,7 @@
         <v>3A</v>
       </c>
     </row>
-    <row r="109" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>21</v>
       </c>
@@ -8172,7 +8226,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="110" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>24</v>
       </c>
@@ -8233,7 +8287,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="111" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>27</v>
       </c>
@@ -8295,7 +8349,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="112" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>30</v>
       </c>
@@ -8356,12 +8410,12 @@
         <v>06</v>
       </c>
     </row>
-    <row r="116" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C116" s="8" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="117" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>0</v>
       </c>
@@ -8422,7 +8476,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="118" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>3</v>
       </c>
@@ -8483,7 +8537,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="119" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>6</v>
       </c>
@@ -8544,7 +8598,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="120" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>9</v>
       </c>
@@ -8605,7 +8659,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="121" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>12</v>
       </c>
@@ -8664,7 +8718,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="122" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>15</v>
       </c>
@@ -8722,7 +8776,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="123" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>18</v>
       </c>
@@ -8781,7 +8835,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="124" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>21</v>
       </c>
@@ -8839,7 +8893,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="125" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>24</v>
       </c>
@@ -8895,7 +8949,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="126" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>27</v>
       </c>
@@ -8956,7 +9010,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="127" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>30</v>
       </c>
@@ -9017,7 +9071,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="128" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>33</v>
       </c>
@@ -9075,7 +9129,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="129" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>36</v>
       </c>
@@ -9136,7 +9190,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="130" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>39</v>
       </c>
@@ -9192,7 +9246,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="131" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>42</v>
       </c>
@@ -9251,7 +9305,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="132" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>45</v>
       </c>
@@ -9309,12 +9363,12 @@
         <v>0C</v>
       </c>
     </row>
-    <row r="133" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:21" x14ac:dyDescent="0.3">
       <c r="E133" s="8" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="134" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>48</v>
       </c>
@@ -9326,7 +9380,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="135" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>51</v>
       </c>
@@ -9338,7 +9392,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="136" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>54</v>
       </c>
@@ -9350,12 +9404,12 @@
         <v>200</v>
       </c>
     </row>
-    <row r="140" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C140" s="8" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="141" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>0</v>
       </c>
@@ -9417,7 +9471,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="142" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>3</v>
       </c>
@@ -9479,7 +9533,7 @@
         <v>FF</v>
       </c>
     </row>
-    <row r="143" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>6</v>
       </c>
@@ -9541,7 +9595,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="144" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C144" t="s">
         <v>261</v>
       </c>
@@ -9599,7 +9653,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="145" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C145" t="s">
         <v>258</v>
       </c>
@@ -9657,7 +9711,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="146" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C146" t="s">
         <v>259</v>
       </c>
@@ -9709,7 +9763,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="147" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C147" t="s">
         <v>236</v>
       </c>
@@ -9758,7 +9812,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="148" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C148" t="s">
         <v>260</v>
       </c>
@@ -9810,7 +9864,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="149" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C149" t="s">
         <v>82</v>
       </c>
@@ -9861,22 +9915,22 @@
         <v>09</v>
       </c>
     </row>
-    <row r="151" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C151" s="5" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="153" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C153" s="8" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="154" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>0</v>
       </c>
       <c r="B154" t="str">
-        <f t="shared" ref="B154:B168" si="266">"0x" &amp; DEC2HEX(A154,3)</f>
+        <f t="shared" ref="B154:B167" si="266">"0x" &amp; DEC2HEX(A154,3)</f>
         <v>0x000</v>
       </c>
       <c r="C154" t="s">
@@ -9933,7 +9987,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="155" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>3</v>
       </c>
@@ -9955,7 +10009,7 @@
         <v>194</v>
       </c>
       <c r="H155">
-        <f t="shared" ref="H155:H168" si="273">IF(G155="", "", VLOOKUP(G155, $W$3:$X$10, 2))</f>
+        <f t="shared" ref="H155:H167" si="273">IF(G155="", "", VLOOKUP(G155, $W$3:$X$10, 2))</f>
         <v>2</v>
       </c>
       <c r="L155">
@@ -9966,20 +10020,20 @@
         <v>000001</v>
       </c>
       <c r="N155" s="17" t="str">
-        <f t="shared" ref="N155:N168" si="275">IF(H155="", "", TEXT(DEC2BIN(H155), "000"))</f>
+        <f t="shared" ref="N155:N167" si="275">IF(H155="", "", TEXT(DEC2BIN(H155), "000"))</f>
         <v>010</v>
       </c>
       <c r="O155" s="17" t="str">
-        <f t="shared" ref="O155:O168" si="276">IF(I155="", "", TEXT(DEC2BIN(I155), "000"))</f>
+        <f t="shared" ref="O155:O167" si="276">IF(I155="", "", TEXT(DEC2BIN(I155), "000"))</f>
         <v/>
       </c>
       <c r="P155" s="17"/>
       <c r="Q155" s="17" t="str">
-        <f t="shared" ref="Q155:Q168" si="277">IF(K155="", "", TEXT(DEC2BIN(K155), "00000000"))</f>
+        <f t="shared" ref="Q155:Q167" si="277">IF(K155="", "", TEXT(DEC2BIN(K155), "00000000"))</f>
         <v/>
       </c>
       <c r="R155" s="18" t="str">
-        <f t="shared" ref="R155:R168" si="278">IF(L155="", "", TEXT(DEC2BIN(L155), "00000000"))</f>
+        <f t="shared" ref="R155:R167" si="278">IF(L155="", "", TEXT(DEC2BIN(L155), "00000000"))</f>
         <v>00000000</v>
       </c>
       <c r="S155" t="str">
@@ -9995,7 +10049,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="156" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>6</v>
       </c>
@@ -10056,7 +10110,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="157" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>9</v>
       </c>
@@ -10117,7 +10171,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="158" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>12</v>
       </c>
@@ -10175,7 +10229,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="159" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>15</v>
       </c>
@@ -10242,7 +10296,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="160" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>18</v>
       </c>
@@ -10298,7 +10352,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="161" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>21</v>
       </c>
@@ -10309,9 +10363,7 @@
       <c r="C161" t="s">
         <v>231</v>
       </c>
-      <c r="E161" s="8" t="s">
-        <v>232</v>
-      </c>
+      <c r="E161" s="8"/>
       <c r="F161" s="11">
         <v>2</v>
       </c>
@@ -10359,7 +10411,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="162" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>24</v>
       </c>
@@ -10368,7 +10420,7 @@
         <v>0x018</v>
       </c>
       <c r="C162" t="s">
-        <v>228</v>
+        <v>273</v>
       </c>
       <c r="E162" s="8" t="s">
         <v>160</v>
@@ -10377,11 +10429,11 @@
         <v>33</v>
       </c>
       <c r="G162" s="12" t="s">
-        <v>216</v>
+        <v>39</v>
       </c>
       <c r="H162">
         <f t="shared" si="273"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I162">
         <v>7</v>
@@ -10392,7 +10444,7 @@
       </c>
       <c r="N162" s="17" t="str">
         <f t="shared" si="275"/>
-        <v>011</v>
+        <v>001</v>
       </c>
       <c r="O162" s="17" t="str">
         <f t="shared" si="276"/>
@@ -10409,7 +10461,7 @@
       </c>
       <c r="S162" t="str">
         <f>BIN2HEX(LEFT(CONCATENATE(M162,IF(N162="", "000", N162)), 8), 2)</f>
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="T162" t="str">
         <f>BIN2HEX(CONCATENATE(RIGHT(N162, 1), IF(O162 = "", "000", O162), "0000"), 2)</f>
@@ -10420,7 +10472,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="163" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>27</v>
       </c>
@@ -10442,7 +10494,7 @@
         <v/>
       </c>
       <c r="K163">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="M163" s="16" t="str">
         <f>IF(F163="", "", TEXT(DEC2BIN(F163), "000000"))</f>
@@ -10459,7 +10511,7 @@
       <c r="P163" s="17"/>
       <c r="Q163" s="17" t="str">
         <f t="shared" si="277"/>
-        <v>00011000</v>
+        <v>00000000</v>
       </c>
       <c r="R163" s="18" t="str">
         <f t="shared" si="278"/>
@@ -10475,10 +10527,10 @@
       </c>
       <c r="U163" s="13" t="str">
         <f>IF(Q163="", BIN2HEX(R163, 2), BIN2HEX(Q163,2))</f>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="164" spans="1:21" x14ac:dyDescent="0.25">
+        <v>00</v>
+      </c>
+    </row>
+    <row r="164" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>30</v>
       </c>
@@ -10487,35 +10539,35 @@
         <v>0x01E</v>
       </c>
       <c r="C164" t="s">
-        <v>233</v>
-      </c>
-      <c r="E164" s="8" t="s">
-        <v>234</v>
+        <v>259</v>
+      </c>
+      <c r="E164" s="51" t="s">
+        <v>245</v>
       </c>
       <c r="F164" s="11">
         <v>2</v>
       </c>
       <c r="G164" s="12" t="s">
-        <v>216</v>
+        <v>39</v>
       </c>
       <c r="H164">
         <f t="shared" si="273"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I164">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="M164" s="16" t="str">
-        <f t="shared" ref="M164:M165" si="287">IF(F164="", "", TEXT(DEC2BIN(F164), "000000"))</f>
+        <f t="shared" ref="M164" si="287">IF(F164="", "", TEXT(DEC2BIN(F164), "000000"))</f>
         <v>000010</v>
       </c>
       <c r="N164" s="17" t="str">
         <f t="shared" si="275"/>
-        <v>011</v>
+        <v>001</v>
       </c>
       <c r="O164" s="17" t="str">
         <f t="shared" si="276"/>
-        <v>001</v>
+        <v>110</v>
       </c>
       <c r="P164" s="17"/>
       <c r="Q164" s="17" t="str">
@@ -10527,19 +10579,19 @@
         <v/>
       </c>
       <c r="S164" t="str">
-        <f t="shared" ref="S164:S167" si="288">BIN2HEX(LEFT(CONCATENATE(M164,IF(N164="", "000", N164)), 8), 2)</f>
-        <v>09</v>
+        <f t="shared" ref="S164:S166" si="288">BIN2HEX(LEFT(CONCATENATE(M164,IF(N164="", "000", N164)), 8), 2)</f>
+        <v>08</v>
       </c>
       <c r="T164" t="str">
-        <f t="shared" ref="T164:T165" si="289">BIN2HEX(CONCATENATE(RIGHT(N164, 1), IF(O164 = "", "000", O164), "0000"), 2)</f>
-        <v>90</v>
+        <f t="shared" ref="T164" si="289">BIN2HEX(CONCATENATE(RIGHT(N164, 1), IF(O164 = "", "000", O164), "0000"), 2)</f>
+        <v>E0</v>
       </c>
       <c r="U164" s="13" t="str">
-        <f t="shared" ref="U164:U167" si="290">IF(Q164="", BIN2HEX(R164, 2), BIN2HEX(Q164,2))</f>
-        <v>00</v>
-      </c>
-    </row>
-    <row r="165" spans="1:21" x14ac:dyDescent="0.25">
+        <f t="shared" ref="U164:U166" si="290">IF(Q164="", BIN2HEX(R164, 2), BIN2HEX(Q164,2))</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="165" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>33</v>
       </c>
@@ -10548,13 +10600,11 @@
         <v>0x021</v>
       </c>
       <c r="C165" t="s">
-        <v>259</v>
-      </c>
-      <c r="E165" s="51" t="s">
-        <v>245</v>
-      </c>
+        <v>236</v>
+      </c>
+      <c r="E165" s="51"/>
       <c r="F165" s="11">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="G165" s="12" t="s">
         <v>39</v>
@@ -10563,44 +10613,41 @@
         <f t="shared" si="273"/>
         <v>1</v>
       </c>
-      <c r="I165">
-        <v>6</v>
-      </c>
       <c r="M165" s="16" t="str">
-        <f t="shared" si="287"/>
-        <v>000010</v>
+        <f>IF(F165="", "", TEXT(DEC2BIN(F165), "000000"))</f>
+        <v>101000</v>
       </c>
       <c r="N165" s="17" t="str">
-        <f t="shared" si="275"/>
+        <f>IF(H165="", "", TEXT(DEC2BIN(H165), "000"))</f>
         <v>001</v>
       </c>
       <c r="O165" s="17" t="str">
-        <f t="shared" si="276"/>
-        <v>110</v>
+        <f>IF(I165="", "", TEXT(DEC2BIN(I165), "000"))</f>
+        <v/>
       </c>
       <c r="P165" s="17"/>
       <c r="Q165" s="17" t="str">
-        <f t="shared" si="277"/>
+        <f>IF(K165="", "", TEXT(DEC2BIN(K165), "00000000"))</f>
         <v/>
       </c>
       <c r="R165" s="18" t="str">
-        <f t="shared" si="278"/>
+        <f>IF(L165="", "", TEXT(DEC2BIN(L165), "00000000"))</f>
         <v/>
       </c>
       <c r="S165" t="str">
         <f t="shared" si="288"/>
-        <v>08</v>
+        <v>A0</v>
       </c>
       <c r="T165" t="str">
-        <f t="shared" si="289"/>
-        <v>E0</v>
+        <f>BIN2HEX(CONCATENATE(RIGHT(N165, 1), IF(O165 = "", "000", O165), "0000"), 2)</f>
+        <v>80</v>
       </c>
       <c r="U165" s="13" t="str">
         <f t="shared" si="290"/>
         <v>00</v>
       </c>
     </row>
-    <row r="166" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>36</v>
       </c>
@@ -10609,54 +10656,57 @@
         <v>0x024</v>
       </c>
       <c r="C166" t="s">
-        <v>236</v>
+        <v>260</v>
       </c>
       <c r="E166" s="51"/>
       <c r="F166" s="11">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="G166" s="12" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H166">
         <f t="shared" si="273"/>
+        <v>6</v>
+      </c>
+      <c r="I166">
         <v>1</v>
       </c>
       <c r="M166" s="16" t="str">
-        <f>IF(F166="", "", TEXT(DEC2BIN(F166), "000000"))</f>
-        <v>101000</v>
+        <f t="shared" ref="M166" si="291">IF(F166="", "", TEXT(DEC2BIN(F166), "000000"))</f>
+        <v>000010</v>
       </c>
       <c r="N166" s="17" t="str">
-        <f>IF(H166="", "", TEXT(DEC2BIN(H166), "000"))</f>
+        <f t="shared" ref="N166" si="292">IF(H166="", "", TEXT(DEC2BIN(H166), "000"))</f>
+        <v>110</v>
+      </c>
+      <c r="O166" s="17" t="str">
+        <f t="shared" ref="O166" si="293">IF(I166="", "", TEXT(DEC2BIN(I166), "000"))</f>
         <v>001</v>
-      </c>
-      <c r="O166" s="17" t="str">
-        <f>IF(I166="", "", TEXT(DEC2BIN(I166), "000"))</f>
-        <v/>
       </c>
       <c r="P166" s="17"/>
       <c r="Q166" s="17" t="str">
-        <f>IF(K166="", "", TEXT(DEC2BIN(K166), "00000000"))</f>
+        <f t="shared" ref="Q166" si="294">IF(K166="", "", TEXT(DEC2BIN(K166), "00000000"))</f>
         <v/>
       </c>
       <c r="R166" s="18" t="str">
-        <f>IF(L166="", "", TEXT(DEC2BIN(L166), "00000000"))</f>
+        <f t="shared" ref="R166" si="295">IF(L166="", "", TEXT(DEC2BIN(L166), "00000000"))</f>
         <v/>
       </c>
       <c r="S166" t="str">
         <f t="shared" si="288"/>
-        <v>A0</v>
+        <v>0B</v>
       </c>
       <c r="T166" t="str">
-        <f>BIN2HEX(CONCATENATE(RIGHT(N166, 1), IF(O166 = "", "000", O166), "0000"), 2)</f>
-        <v>80</v>
+        <f t="shared" ref="T166" si="296">BIN2HEX(CONCATENATE(RIGHT(N166, 1), IF(O166 = "", "000", O166), "0000"), 2)</f>
+        <v>10</v>
       </c>
       <c r="U166" s="13" t="str">
         <f t="shared" si="290"/>
         <v>00</v>
       </c>
     </row>
-    <row r="167" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>39</v>
       </c>
@@ -10665,380 +10715,321 @@
         <v>0x027</v>
       </c>
       <c r="C167" t="s">
-        <v>260</v>
-      </c>
-      <c r="E167" s="51"/>
+        <v>174</v>
+      </c>
+      <c r="E167" s="8" t="s">
+        <v>165</v>
+      </c>
       <c r="F167" s="11">
-        <v>2</v>
-      </c>
-      <c r="G167" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="H167">
+        <v>5</v>
+      </c>
+      <c r="H167" t="str">
         <f t="shared" si="273"/>
-        <v>6</v>
-      </c>
-      <c r="I167">
-        <v>1</v>
+        <v/>
+      </c>
+      <c r="K167">
+        <v>12</v>
       </c>
       <c r="M167" s="16" t="str">
-        <f t="shared" ref="M167" si="291">IF(F167="", "", TEXT(DEC2BIN(F167), "000000"))</f>
-        <v>000010</v>
+        <f>IF(F167="", "", TEXT(DEC2BIN(F167), "000000"))</f>
+        <v>000101</v>
       </c>
       <c r="N167" s="17" t="str">
-        <f t="shared" ref="N167" si="292">IF(H167="", "", TEXT(DEC2BIN(H167), "000"))</f>
-        <v>110</v>
+        <f t="shared" si="275"/>
+        <v/>
       </c>
       <c r="O167" s="17" t="str">
-        <f t="shared" ref="O167" si="293">IF(I167="", "", TEXT(DEC2BIN(I167), "000"))</f>
-        <v>001</v>
+        <f t="shared" si="276"/>
+        <v/>
       </c>
       <c r="P167" s="17"/>
       <c r="Q167" s="17" t="str">
-        <f t="shared" ref="Q167" si="294">IF(K167="", "", TEXT(DEC2BIN(K167), "00000000"))</f>
-        <v/>
+        <f t="shared" si="277"/>
+        <v>00001100</v>
       </c>
       <c r="R167" s="18" t="str">
-        <f t="shared" ref="R167" si="295">IF(L167="", "", TEXT(DEC2BIN(L167), "00000000"))</f>
+        <f t="shared" si="278"/>
         <v/>
       </c>
       <c r="S167" t="str">
-        <f t="shared" si="288"/>
-        <v>0B</v>
+        <f>BIN2HEX(LEFT(CONCATENATE(M167,IF(N167="", "000", N167)), 8), 2)</f>
+        <v>14</v>
       </c>
       <c r="T167" t="str">
-        <f t="shared" ref="T167" si="296">BIN2HEX(CONCATENATE(RIGHT(N167, 1), IF(O167 = "", "000", O167), "0000"), 2)</f>
-        <v>10</v>
+        <f>BIN2HEX(CONCATENATE(RIGHT(N167, 1), IF(O167 = "", "000", O167), "0000"), 2)</f>
+        <v>00</v>
       </c>
       <c r="U167" s="13" t="str">
-        <f t="shared" si="290"/>
-        <v>00</v>
-      </c>
-    </row>
-    <row r="168" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A168">
-        <v>42</v>
-      </c>
-      <c r="B168" t="str">
-        <f t="shared" si="266"/>
-        <v>0x02A</v>
-      </c>
-      <c r="C168" t="s">
-        <v>82</v>
-      </c>
+        <f>IF(Q167="", BIN2HEX(R167, 2), BIN2HEX(Q167,2))</f>
+        <v>0C</v>
+      </c>
+    </row>
+    <row r="168" spans="1:21" x14ac:dyDescent="0.3">
       <c r="E168" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="F168" s="11">
-        <v>5</v>
-      </c>
-      <c r="H168" t="str">
-        <f t="shared" si="273"/>
-        <v/>
-      </c>
-      <c r="K168">
-        <v>9</v>
-      </c>
-      <c r="M168" s="16" t="str">
-        <f>IF(F168="", "", TEXT(DEC2BIN(F168), "000000"))</f>
-        <v>000101</v>
-      </c>
-      <c r="N168" s="17" t="str">
-        <f t="shared" si="275"/>
-        <v/>
-      </c>
-      <c r="O168" s="17" t="str">
-        <f t="shared" si="276"/>
-        <v/>
-      </c>
-      <c r="P168" s="17"/>
-      <c r="Q168" s="17" t="str">
-        <f t="shared" si="277"/>
-        <v>00001001</v>
-      </c>
-      <c r="R168" s="18" t="str">
-        <f t="shared" si="278"/>
-        <v/>
-      </c>
-      <c r="S168" t="str">
-        <f>BIN2HEX(LEFT(CONCATENATE(M168,IF(N168="", "000", N168)), 8), 2)</f>
-        <v>14</v>
-      </c>
-      <c r="T168" t="str">
-        <f>BIN2HEX(CONCATENATE(RIGHT(N168, 1), IF(O168 = "", "000", O168), "0000"), 2)</f>
-        <v>00</v>
-      </c>
-      <c r="U168" s="13" t="str">
-        <f>IF(Q168="", BIN2HEX(R168, 2), BIN2HEX(Q168,2))</f>
-        <v>09</v>
-      </c>
-    </row>
-    <row r="169" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="E169" s="8" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="170" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A169">
+        <v>48</v>
+      </c>
+      <c r="B169" t="str">
+        <f t="shared" ref="B169:B172" si="297">"0x" &amp; DEC2HEX(A169,3)</f>
+        <v>0x030</v>
+      </c>
+      <c r="D169" s="7" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="170" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A170">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B170" t="str">
-        <f t="shared" ref="B170:B173" si="297">"0x" &amp; DEC2HEX(A170,3)</f>
-        <v>0x030</v>
+        <f t="shared" si="297"/>
+        <v>0x033</v>
       </c>
       <c r="D170" s="7" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="171" spans="1:21" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="171" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A171">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B171" t="str">
         <f t="shared" si="297"/>
-        <v>0x033</v>
+        <v>0x036</v>
       </c>
       <c r="D171" s="7" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="172" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A172">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B172" t="str">
         <f t="shared" si="297"/>
-        <v>0x036</v>
+        <v>0x039</v>
       </c>
       <c r="D172" s="7" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="173" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A173">
+        <v>60</v>
+      </c>
+      <c r="B173" t="str">
+        <f t="shared" ref="B173:B180" si="298">"0x" &amp; DEC2HEX(A173,3)</f>
+        <v>0x03C</v>
+      </c>
+      <c r="D173" s="7" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="173" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A173">
-        <v>57</v>
-      </c>
-      <c r="B173" t="str">
-        <f t="shared" si="297"/>
-        <v>0x039</v>
-      </c>
-      <c r="D173" s="7" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="174" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A174">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B174" t="str">
-        <f t="shared" ref="B174:B181" si="298">"0x" &amp; DEC2HEX(A174,3)</f>
-        <v>0x03C</v>
+        <f t="shared" si="298"/>
+        <v>0x03F</v>
       </c>
       <c r="D174" s="7" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="175" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A175">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B175" t="str">
         <f t="shared" si="298"/>
-        <v>0x03F</v>
+        <v>0x042</v>
       </c>
       <c r="D175" s="7" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="176" spans="1:21" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="176" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A176">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B176" t="str">
         <f t="shared" si="298"/>
-        <v>0x042</v>
+        <v>0x045</v>
       </c>
       <c r="D176" s="7" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B177" t="str">
         <f t="shared" si="298"/>
-        <v>0x045</v>
+        <v>0x048</v>
       </c>
       <c r="D177" s="7" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B178" t="str">
         <f t="shared" si="298"/>
-        <v>0x048</v>
+        <v>0x04B</v>
       </c>
       <c r="D178" s="7" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B179" t="str">
         <f t="shared" si="298"/>
-        <v>0x04B</v>
+        <v>0x04E</v>
       </c>
       <c r="D179" s="7" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B180" t="str">
         <f t="shared" si="298"/>
-        <v>0x04E</v>
+        <v>0x051</v>
       </c>
       <c r="D180" s="7" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B181" t="str">
-        <f t="shared" si="298"/>
-        <v>0x051</v>
+        <f t="shared" ref="B181:B190" si="299">"0x" &amp; DEC2HEX(A181,3)</f>
+        <v>0x054</v>
       </c>
       <c r="D181" s="7" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A182">
+        <v>87</v>
+      </c>
+      <c r="B182" t="str">
+        <f t="shared" si="299"/>
+        <v>0x057</v>
+      </c>
+      <c r="D182" s="7" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182">
-        <v>84</v>
-      </c>
-      <c r="B182" t="str">
-        <f t="shared" ref="B182:B191" si="299">"0x" &amp; DEC2HEX(A182,3)</f>
-        <v>0x054</v>
-      </c>
-      <c r="D182" s="7" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B183" t="str">
         <f t="shared" si="299"/>
-        <v>0x057</v>
+        <v>0x05A</v>
       </c>
       <c r="D183" s="7" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B184" t="str">
         <f t="shared" si="299"/>
-        <v>0x05A</v>
+        <v>0x05D</v>
       </c>
       <c r="D184" s="7" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B185" t="str">
         <f t="shared" si="299"/>
-        <v>0x05D</v>
+        <v>0x060</v>
       </c>
       <c r="D185" s="7" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B186" t="str">
         <f t="shared" si="299"/>
-        <v>0x060</v>
+        <v>0x063</v>
       </c>
       <c r="D186" s="7" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B187" t="str">
         <f t="shared" si="299"/>
-        <v>0x063</v>
+        <v>0x066</v>
       </c>
       <c r="D187" s="7" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B188" t="str">
         <f t="shared" si="299"/>
-        <v>0x066</v>
+        <v>0x069</v>
       </c>
       <c r="D188" s="7" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B189" t="str">
         <f t="shared" si="299"/>
-        <v>0x069</v>
+        <v>0x06C</v>
       </c>
       <c r="D189" s="7" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B190" t="str">
         <f t="shared" si="299"/>
-        <v>0x06C</v>
+        <v>0x06F</v>
       </c>
       <c r="D190" s="7" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A191">
-        <v>111</v>
-      </c>
-      <c r="B191" t="str">
-        <f t="shared" si="299"/>
-        <v>0x06F</v>
-      </c>
-      <c r="D191" s="7" t="s">
         <v>271</v>
       </c>
     </row>
@@ -11049,13 +11040,13 @@
   <mergeCells count="3">
     <mergeCell ref="S1:U1"/>
     <mergeCell ref="E129:E131"/>
-    <mergeCell ref="E165:E167"/>
+    <mergeCell ref="E164:E166"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y17">
       <formula1>$W$16:$W$18</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G6 G9:G11 G17:G26 G31:G33 G41:G42 G49 G83:G93 G117:G132 G102:G112 G141:G149 G154:G168">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G6 G9:G11 G17:G26 G31:G33 G41:G42 G49 G83:G93 G117:G132 G102:G112 G141:G149 G154:G167">
       <formula1>$W$3:$W$10</formula1>
     </dataValidation>
   </dataValidations>
@@ -11063,4 +11054,697 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D65"/>
+  <sheetViews>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C65"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="22.5546875" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>11111111</v>
+      </c>
+      <c r="C2" t="str">
+        <f>BIN2HEX(B2, 2)</f>
+        <v>FF</v>
+      </c>
+      <c r="D2" t="str">
+        <f>BIN2HEX(B2, 2) &amp; " " &amp; BIN2HEX(B3,2) &amp; " " &amp; BIN2HEX(B4,2)</f>
+        <v>FF 81 81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="2">
+        <v>10000001</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C65" si="0">BIN2HEX(B3, 2)</f>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="2">
+        <v>10000001</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B5" s="2">
+        <v>10000001</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>81</v>
+      </c>
+      <c r="D5" t="str">
+        <f>BIN2HEX(B5, 2) &amp; " " &amp; BIN2HEX(B6,2) &amp; " " &amp; BIN2HEX(B7,2)</f>
+        <v>81 81 81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="2">
+        <v>10000001</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B7" s="2">
+        <v>10000001</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="2">
+        <v>10000001</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>81</v>
+      </c>
+      <c r="D8" t="str">
+        <f>BIN2HEX(B8, 2) &amp; " " &amp; BIN2HEX(B9,2) &amp; " " &amp; BIN2HEX(B10,2)</f>
+        <v>81 FF 00</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="53">
+        <v>11111111</v>
+      </c>
+      <c r="C9" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>FF</v>
+      </c>
+      <c r="D9" s="52"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2" t="str">
+        <f>"00000000"</f>
+        <v>00000000</v>
+      </c>
+      <c r="C10" t="str">
+        <f>BIN2HEX(B10, 2)</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="str">
+        <f>"01111110"</f>
+        <v>01111110</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>7E</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B12" s="2" t="str">
+        <f>"01000010"</f>
+        <v>01000010</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B13" s="2" t="str">
+        <f t="shared" ref="B13:B15" si="1">"01000010"</f>
+        <v>01000010</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B14" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>01000010</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B15" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>01000010</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B16" s="2" t="str">
+        <f>"01111110"</f>
+        <v>01111110</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>7E</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B17" s="53" t="str">
+        <f>"00000000"</f>
+        <v>00000000</v>
+      </c>
+      <c r="C17" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" s="2" t="str">
+        <f>"00000000"</f>
+        <v>00000000</v>
+      </c>
+      <c r="C18" t="str">
+        <f>BIN2HEX(B18, 2)</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B19" s="2" t="str">
+        <f>"00000000"</f>
+        <v>00000000</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B20" s="2" t="str">
+        <f>"00111100"</f>
+        <v>00111100</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>3C</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B21" s="2" t="str">
+        <f>"00100100"</f>
+        <v>00100100</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B22" s="2" t="str">
+        <f>"00100100"</f>
+        <v>00100100</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B23" s="2" t="str">
+        <f>"00111100"</f>
+        <v>00111100</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>3C</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B24" s="2" t="str">
+        <f>"00000000"</f>
+        <v>00000000</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B25" s="53" t="str">
+        <f>"00000000"</f>
+        <v>00000000</v>
+      </c>
+      <c r="C25" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>3</v>
+      </c>
+      <c r="B26" s="2" t="str">
+        <f>"00000000"</f>
+        <v>00000000</v>
+      </c>
+      <c r="C26" t="str">
+        <f>BIN2HEX(B26, 2)</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B27" s="2" t="str">
+        <f>"00000000"</f>
+        <v>00000000</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B28" s="2" t="str">
+        <f>"00000000"</f>
+        <v>00000000</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B29" s="2" t="str">
+        <f>"00011000"</f>
+        <v>00011000</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B30" s="2" t="str">
+        <f>"00011000"</f>
+        <v>00011000</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B31" s="2" t="str">
+        <f>"00000000"</f>
+        <v>00000000</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B32" s="2" t="str">
+        <f>"00000000"</f>
+        <v>00000000</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B33" s="53" t="str">
+        <f>"00000000"</f>
+        <v>00000000</v>
+      </c>
+      <c r="C33" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>4</v>
+      </c>
+      <c r="B34" s="2" t="str">
+        <f>"00000000"</f>
+        <v>00000000</v>
+      </c>
+      <c r="C34" t="str">
+        <f>BIN2HEX(B34, 2)</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B35" s="2" t="str">
+        <f>"00000000"</f>
+        <v>00000000</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="0"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B36" s="2" t="str">
+        <f>"00000000"</f>
+        <v>00000000</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="0"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B37" s="2" t="str">
+        <f t="shared" ref="B37:B38" si="2">"00000000"</f>
+        <v>00000000</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="0"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B38" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="0"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B39" s="2" t="str">
+        <f>"00000000"</f>
+        <v>00000000</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="0"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B40" s="2" t="str">
+        <f>"00000000"</f>
+        <v>00000000</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="0"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B41" s="53" t="str">
+        <f>"00000000"</f>
+        <v>00000000</v>
+      </c>
+      <c r="C41" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>5</v>
+      </c>
+      <c r="B42" s="2" t="str">
+        <f>"00000000"</f>
+        <v>00000000</v>
+      </c>
+      <c r="C42" t="str">
+        <f>BIN2HEX(B42, 2)</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B43" s="2" t="str">
+        <f>"00000000"</f>
+        <v>00000000</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" si="0"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B44" s="2" t="str">
+        <f>"00000000"</f>
+        <v>00000000</v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" si="0"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B45" s="2" t="str">
+        <f>"00011000"</f>
+        <v>00011000</v>
+      </c>
+      <c r="C45" t="str">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B46" s="2" t="str">
+        <f>"00011000"</f>
+        <v>00011000</v>
+      </c>
+      <c r="C46" t="str">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B47" s="2" t="str">
+        <f>"00000000"</f>
+        <v>00000000</v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" si="0"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B48" s="2" t="str">
+        <f>"00000000"</f>
+        <v>00000000</v>
+      </c>
+      <c r="C48" t="str">
+        <f t="shared" si="0"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B49" s="53" t="str">
+        <f>"00000000"</f>
+        <v>00000000</v>
+      </c>
+      <c r="C49" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>6</v>
+      </c>
+      <c r="B50" s="2" t="str">
+        <f>"00000000"</f>
+        <v>00000000</v>
+      </c>
+      <c r="C50" t="str">
+        <f>BIN2HEX(B50, 2)</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B51" s="2" t="str">
+        <f>"00000000"</f>
+        <v>00000000</v>
+      </c>
+      <c r="C51" t="str">
+        <f t="shared" si="0"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B52" s="2" t="str">
+        <f>"00111100"</f>
+        <v>00111100</v>
+      </c>
+      <c r="C52" t="str">
+        <f t="shared" si="0"/>
+        <v>3C</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B53" s="2" t="str">
+        <f>"00100100"</f>
+        <v>00100100</v>
+      </c>
+      <c r="C53" t="str">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B54" s="2" t="str">
+        <f>"00100100"</f>
+        <v>00100100</v>
+      </c>
+      <c r="C54" t="str">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B55" s="2" t="str">
+        <f>"00111100"</f>
+        <v>00111100</v>
+      </c>
+      <c r="C55" t="str">
+        <f t="shared" si="0"/>
+        <v>3C</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B56" s="2" t="str">
+        <f>"00000000"</f>
+        <v>00000000</v>
+      </c>
+      <c r="C56" t="str">
+        <f t="shared" si="0"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B57" s="53" t="str">
+        <f>"00000000"</f>
+        <v>00000000</v>
+      </c>
+      <c r="C57" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>7</v>
+      </c>
+      <c r="B58" s="2" t="str">
+        <f>"00000000"</f>
+        <v>00000000</v>
+      </c>
+      <c r="C58" t="str">
+        <f>BIN2HEX(B58, 2)</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B59" s="2" t="str">
+        <f>"01111110"</f>
+        <v>01111110</v>
+      </c>
+      <c r="C59" t="str">
+        <f t="shared" si="0"/>
+        <v>7E</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B60" s="2" t="str">
+        <f>"01000010"</f>
+        <v>01000010</v>
+      </c>
+      <c r="C60" t="str">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B61" s="2" t="str">
+        <f t="shared" ref="B61:B63" si="3">"01000010"</f>
+        <v>01000010</v>
+      </c>
+      <c r="C61" t="str">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B62" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>01000010</v>
+      </c>
+      <c r="C62" t="str">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B63" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>01000010</v>
+      </c>
+      <c r="C63" t="str">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B64" s="2" t="str">
+        <f>"01111110"</f>
+        <v>01111110</v>
+      </c>
+      <c r="C64" t="str">
+        <f t="shared" si="0"/>
+        <v>7E</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B65" s="53" t="str">
+        <f>"00000000"</f>
+        <v>00000000</v>
+      </c>
+      <c r="C65" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>00</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
New logisim circuit image / small changes
</commit_message>
<xml_diff>
--- a/2nd gen - 8 bit cpu/Instruction control lines.xlsx
+++ b/2nd gen - 8 bit cpu/Instruction control lines.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="345" windowWidth="14805" windowHeight="7770" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="345" windowWidth="14805" windowHeight="7770"/>
   </bookViews>
   <sheets>
     <sheet name="Control Lines" sheetId="1" r:id="rId1"/>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="316">
   <si>
     <t>LD R1, data</t>
   </si>
@@ -790,12 +790,6 @@
     <t>44 80 00</t>
   </si>
   <si>
-    <t>CLOSE_REGS_BRIDGE = 1 would allow to output all registers, instead of only the first four</t>
-  </si>
-  <si>
-    <t>One register ALU instructions can be modified to use all registers, as the above OUT instruction</t>
-  </si>
-  <si>
     <t>// 1 - Increments A, starting in 32</t>
   </si>
   <si>
@@ -1037,13 +1031,16 @@
   </si>
   <si>
     <t>JP [0x021]</t>
+  </si>
+  <si>
+    <t>One register ALU instructions can be modified to use all registers, by using CLOSE_REGS_BRIDGE=1 and EN_R1_OUT=0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1135,6 +1132,14 @@
     <font>
       <sz val="11"/>
       <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1258,7 +1263,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1350,6 +1355,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1368,10 +1377,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1678,16 +1684,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN54"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
+      <selection pane="bottomLeft" activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="17" width="3.28515625" customWidth="1"/>
     <col min="18" max="19" width="3.28515625" style="4" customWidth="1"/>
     <col min="20" max="20" width="3.28515625" customWidth="1"/>
@@ -1771,7 +1777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:39" s="1" customFormat="1" ht="129" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:39" s="1" customFormat="1" ht="131.25" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>173</v>
       </c>
@@ -1853,11 +1859,11 @@
       <c r="AA2" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="AB2" s="49" t="s">
+      <c r="AB2" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="AC2" s="49"/>
-      <c r="AD2" s="49"/>
+      <c r="AC2" s="51"/>
+      <c r="AD2" s="51"/>
     </row>
     <row r="3" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -2835,7 +2841,7 @@
         <v>000100</v>
       </c>
     </row>
-    <row r="13" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>10</v>
       </c>
@@ -2930,7 +2936,7 @@
         <f t="shared" si="2"/>
         <v>00</v>
       </c>
-      <c r="AF13" s="5" t="s">
+      <c r="AF13" s="57" t="s">
         <v>185</v>
       </c>
       <c r="AM13" s="8" t="str">
@@ -3285,7 +3291,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="20" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>17</v>
       </c>
@@ -3293,7 +3299,7 @@
         <f t="shared" si="4"/>
         <v>0x11</v>
       </c>
-      <c r="C20" s="31" t="s">
+      <c r="C20" s="30" t="s">
         <v>113</v>
       </c>
       <c r="D20">
@@ -3387,9 +3393,7 @@
         <f t="shared" si="5"/>
         <v>000880</v>
       </c>
-      <c r="AN20" s="5" t="s">
-        <v>234</v>
-      </c>
+      <c r="AN20" s="5"/>
     </row>
     <row r="21" spans="1:40" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
@@ -4059,7 +4063,7 @@
         <v>408818</v>
       </c>
     </row>
-    <row r="37" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>34</v>
       </c>
@@ -4158,8 +4162,8 @@
         <f t="shared" si="5"/>
         <v>408802</v>
       </c>
-      <c r="AN37" s="5" t="s">
-        <v>235</v>
+      <c r="AN37" s="57" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="38" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
@@ -4952,14 +4956,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA249"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A171" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E176" sqref="E176:E197"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A216" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G234" sqref="G234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="55" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="49" customWidth="1"/>
     <col min="2" max="2" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" style="7" bestFit="1" customWidth="1"/>
@@ -4979,13 +4983,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
-        <v>301</v>
-      </c>
-      <c r="B1" s="56" t="s">
+      <c r="A1" s="50" t="s">
+        <v>299</v>
+      </c>
+      <c r="B1" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="56" t="s">
+      <c r="C1" s="50" t="s">
         <v>70</v>
       </c>
       <c r="G1" s="14" t="s">
@@ -5027,18 +5031,18 @@
       <c r="S1" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="T1" s="50" t="s">
+      <c r="T1" s="52" t="s">
         <v>153</v>
       </c>
-      <c r="U1" s="51"/>
-      <c r="V1" s="52"/>
+      <c r="U1" s="53"/>
+      <c r="V1" s="54"/>
       <c r="W1" s="10"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="8" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="O2" s="17"/>
       <c r="P2" s="17"/>
@@ -5334,7 +5338,7 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="D8" s="8" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F8" s="8"/>
       <c r="X8" t="s">
@@ -5536,7 +5540,7 @@
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="D16" s="8" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="X16" t="s">
         <v>159</v>
@@ -5902,7 +5906,7 @@
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="31" spans="2:27" x14ac:dyDescent="0.25">
@@ -6252,7 +6256,7 @@
     </row>
     <row r="40" spans="2:22" x14ac:dyDescent="0.25">
       <c r="D40" s="8" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="41" spans="2:22" x14ac:dyDescent="0.25">
@@ -6451,7 +6455,7 @@
     </row>
     <row r="48" spans="2:22" x14ac:dyDescent="0.25">
       <c r="D48" s="8" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="49" spans="2:22" x14ac:dyDescent="0.25">
@@ -6587,7 +6591,7 @@
     </row>
     <row r="55" spans="2:22" x14ac:dyDescent="0.25">
       <c r="D55" s="8" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="56" spans="2:22" x14ac:dyDescent="0.25">
@@ -7008,7 +7012,7 @@
     </row>
     <row r="82" spans="2:22" x14ac:dyDescent="0.25">
       <c r="D82" s="8" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E82"/>
       <c r="F82" s="8"/>
@@ -7781,7 +7785,7 @@
     </row>
     <row r="101" spans="2:22" x14ac:dyDescent="0.25">
       <c r="D101" s="8" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E101"/>
       <c r="F101" s="8"/>
@@ -8476,7 +8480,7 @@
     </row>
     <row r="116" spans="2:22" x14ac:dyDescent="0.25">
       <c r="D116" s="8" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="117" spans="2:22" x14ac:dyDescent="0.25">
@@ -9240,7 +9244,7 @@
       <c r="D129" t="s">
         <v>56</v>
       </c>
-      <c r="F129" s="53" t="s">
+      <c r="F129" s="55" t="s">
         <v>210</v>
       </c>
       <c r="G129" s="11">
@@ -9304,7 +9308,7 @@
       <c r="D130" t="s">
         <v>179</v>
       </c>
-      <c r="F130" s="53"/>
+      <c r="F130" s="55"/>
       <c r="G130" s="11">
         <v>40</v>
       </c>
@@ -9363,7 +9367,7 @@
       <c r="D131" t="s">
         <v>57</v>
       </c>
-      <c r="F131" s="53"/>
+      <c r="F131" s="55"/>
       <c r="G131" s="11">
         <v>2</v>
       </c>
@@ -9518,7 +9522,7 @@
     </row>
     <row r="140" spans="2:22" x14ac:dyDescent="0.25">
       <c r="D140" s="8" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="141" spans="2:22" x14ac:dyDescent="0.25">
@@ -10041,7 +10045,7 @@
     </row>
     <row r="153" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D153" s="8" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="154" spans="1:22" x14ac:dyDescent="0.25">
@@ -10119,7 +10123,7 @@
       </c>
       <c r="E155"/>
       <c r="F155" s="8" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G155" s="11">
         <v>1</v>
@@ -10180,7 +10184,7 @@
         <v>0x006</v>
       </c>
       <c r="D156" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F156" s="8" t="s">
         <v>224</v>
@@ -10244,7 +10248,7 @@
         <v>0x009</v>
       </c>
       <c r="D157" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="F157" s="8" t="s">
         <v>225</v>
@@ -10300,21 +10304,21 @@
       </c>
     </row>
     <row r="158" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A158" s="55" t="s">
-        <v>291</v>
+      <c r="A158" s="49" t="s">
+        <v>289</v>
       </c>
       <c r="B158">
         <v>12</v>
       </c>
       <c r="C158" t="str">
-        <f t="shared" ref="C158:C174" si="172">"0x" &amp; DEC2HEX(B158,3)</f>
+        <f t="shared" ref="C158:C167" si="172">"0x" &amp; DEC2HEX(B158,3)</f>
         <v>0x00C</v>
       </c>
       <c r="D158" s="10" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F158" s="8" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="G158" s="11">
         <v>1</v>
@@ -10375,10 +10379,10 @@
         <v>0x00F</v>
       </c>
       <c r="D159" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="F159" s="8" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G159" s="11">
         <v>35</v>
@@ -10498,7 +10502,7 @@
         <v>0x015</v>
       </c>
       <c r="D161" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F161" s="8"/>
       <c r="G161" s="11">
@@ -10549,8 +10553,8 @@
       </c>
     </row>
     <row r="162" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A162" s="55" t="s">
-        <v>308</v>
+      <c r="A162" s="49" t="s">
+        <v>306</v>
       </c>
       <c r="B162">
         <v>24</v>
@@ -10560,10 +10564,10 @@
         <v>0x018</v>
       </c>
       <c r="D162" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F162" s="8" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="G162" s="11">
         <v>1</v>
@@ -10624,10 +10628,10 @@
         <v>0x01B</v>
       </c>
       <c r="D163" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="F163" s="8" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="G163" s="11">
         <v>17</v>
@@ -10694,7 +10698,7 @@
         <v>217</v>
       </c>
       <c r="F164" s="8" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G164" s="11">
         <v>1</v>
@@ -10747,8 +10751,8 @@
       </c>
     </row>
     <row r="165" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A165" s="55" t="s">
-        <v>312</v>
+      <c r="A165" s="49" t="s">
+        <v>310</v>
       </c>
       <c r="B165">
         <v>33</v>
@@ -11134,7 +11138,7 @@
       <c r="D171" t="s">
         <v>221</v>
       </c>
-      <c r="F171" s="53" t="s">
+      <c r="F171" s="55" t="s">
         <v>210</v>
       </c>
       <c r="G171" s="11">
@@ -11198,7 +11202,7 @@
       <c r="D172" t="s">
         <v>201</v>
       </c>
-      <c r="F172" s="53"/>
+      <c r="F172" s="55"/>
       <c r="G172" s="11">
         <v>40</v>
       </c>
@@ -11257,7 +11261,7 @@
       <c r="D173" t="s">
         <v>222</v>
       </c>
-      <c r="F173" s="53"/>
+      <c r="F173" s="55"/>
       <c r="G173" s="11">
         <v>2</v>
       </c>
@@ -11640,7 +11644,7 @@
     </row>
     <row r="200" spans="2:22" x14ac:dyDescent="0.25">
       <c r="D200" s="8" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="201" spans="2:22" x14ac:dyDescent="0.25">
@@ -11652,10 +11656,10 @@
         <v>0x000</v>
       </c>
       <c r="D201" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F201" s="8" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="G201" s="11">
         <v>1</v>
@@ -11716,10 +11720,10 @@
         <v>0x003</v>
       </c>
       <c r="D202" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F202" s="8" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G202" s="11">
         <v>1</v>
@@ -11839,7 +11843,7 @@
         <v>0x009</v>
       </c>
       <c r="D204" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F204" s="8"/>
       <c r="G204" s="11">
@@ -11901,7 +11905,7 @@
         <v>115</v>
       </c>
       <c r="F205" s="8" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G205" s="11">
         <v>32</v>
@@ -11964,8 +11968,8 @@
       <c r="D206" t="s">
         <v>221</v>
       </c>
-      <c r="F206" s="54" t="s">
-        <v>255</v>
+      <c r="F206" s="56" t="s">
+        <v>253</v>
       </c>
       <c r="G206" s="11">
         <v>2</v>
@@ -12028,7 +12032,7 @@
       <c r="D207" t="s">
         <v>57</v>
       </c>
-      <c r="F207" s="54"/>
+      <c r="F207" s="56"/>
       <c r="G207" s="11">
         <v>2</v>
       </c>
@@ -12090,7 +12094,7 @@
       <c r="D208" t="s">
         <v>51</v>
       </c>
-      <c r="F208" s="54"/>
+      <c r="F208" s="56"/>
       <c r="G208" s="11">
         <v>2</v>
       </c>
@@ -12150,10 +12154,10 @@
         <v>0x018</v>
       </c>
       <c r="D209" t="s">
+        <v>252</v>
+      </c>
+      <c r="F209" s="8" t="s">
         <v>254</v>
-      </c>
-      <c r="F209" s="8" t="s">
-        <v>256</v>
       </c>
       <c r="G209" s="11">
         <v>33</v>
@@ -12217,7 +12221,7 @@
         <v>53</v>
       </c>
       <c r="F210" s="8" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G210" s="11">
         <v>34</v>
@@ -12275,10 +12279,10 @@
         <v>0x01E</v>
       </c>
       <c r="D211" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F211" s="8" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="G211" s="11">
         <v>35</v>
@@ -12339,10 +12343,10 @@
         <v>0x021</v>
       </c>
       <c r="D212" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F212" s="8" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="G212" s="11">
         <v>36</v>
@@ -12403,10 +12407,10 @@
         <v>0x024</v>
       </c>
       <c r="D213" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="F213" s="8" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G213" s="11">
         <v>37</v>
@@ -12467,10 +12471,10 @@
         <v>0x027</v>
       </c>
       <c r="D214" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F214" s="8" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="G214" s="11">
         <v>38</v>
@@ -12531,10 +12535,10 @@
         <v>0x02A</v>
       </c>
       <c r="D215" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F215" s="8" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G215" s="11">
         <v>39</v>
@@ -12595,10 +12599,10 @@
         <v>0x02D</v>
       </c>
       <c r="D216" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F216" s="8" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G216" s="11">
         <v>41</v>
@@ -12656,7 +12660,7 @@
         <v>0x030</v>
       </c>
       <c r="D217" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F217" s="8"/>
       <c r="G217" s="11">
@@ -12718,10 +12722,10 @@
         <v>0x033</v>
       </c>
       <c r="D218" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F218" s="8" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G218" s="11">
         <v>3</v>
@@ -12785,7 +12789,7 @@
         <v>190</v>
       </c>
       <c r="F219" s="8" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="G219" s="11">
         <v>1</v>
@@ -12846,10 +12850,10 @@
         <v>0x039</v>
       </c>
       <c r="D220" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F220" s="8" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="G220" s="11">
         <v>1</v>
@@ -12910,10 +12914,10 @@
         <v>0x03C</v>
       </c>
       <c r="D221" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F221" s="8" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G221" s="11">
         <v>4</v>
@@ -12971,7 +12975,7 @@
         <v>0x03F</v>
       </c>
       <c r="D222" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F222" s="8"/>
       <c r="G222" s="11">
@@ -13030,10 +13034,10 @@
         <v>0x042</v>
       </c>
       <c r="D223" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="F223" s="8" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="G223" s="11">
         <v>4</v>
@@ -13091,10 +13095,10 @@
         <v>0x045</v>
       </c>
       <c r="D224" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F224" s="8" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G224" s="11">
         <v>4</v>
@@ -13145,7 +13149,7 @@
     </row>
     <row r="225" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F225" s="8" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="226" spans="1:22" x14ac:dyDescent="0.25">
@@ -13156,7 +13160,7 @@
     </row>
     <row r="228" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D228" s="8" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F228" s="8"/>
     </row>
@@ -13169,10 +13173,10 @@
         <v>0x000</v>
       </c>
       <c r="D229" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F229" s="8" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="G229" s="11">
         <v>1</v>
@@ -13287,8 +13291,8 @@
       </c>
     </row>
     <row r="231" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A231" s="55" t="s">
-        <v>286</v>
+      <c r="A231" s="49" t="s">
+        <v>284</v>
       </c>
       <c r="B231">
         <v>6</v>
@@ -13298,10 +13302,10 @@
         <v>0x006</v>
       </c>
       <c r="D231" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F231" s="8" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="G231" s="11">
         <v>1</v>
@@ -13362,7 +13366,7 @@
         <v>0x009</v>
       </c>
       <c r="D232" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F232" s="8"/>
       <c r="G232" s="11">
@@ -13416,8 +13420,8 @@
       </c>
     </row>
     <row r="233" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A233" s="55" t="s">
-        <v>291</v>
+      <c r="A233" s="49" t="s">
+        <v>289</v>
       </c>
       <c r="B233">
         <v>12</v>
@@ -13427,10 +13431,10 @@
         <v>0x00C</v>
       </c>
       <c r="D233" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F233" s="8" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G233" s="11">
         <v>2</v>
@@ -13491,7 +13495,7 @@
         <v>0x00F</v>
       </c>
       <c r="D234" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F234" s="8"/>
       <c r="G234" s="11">
@@ -13553,7 +13557,7 @@
         <v>0x012</v>
       </c>
       <c r="D235" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F235" s="8"/>
       <c r="G235" s="11">
@@ -13612,7 +13616,7 @@
         <v>0x015</v>
       </c>
       <c r="D236" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F236" s="8"/>
       <c r="G236" s="11">
@@ -13674,10 +13678,10 @@
         <v>0x018</v>
       </c>
       <c r="D237" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="F237" s="8" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G237" s="11">
         <v>32</v>
@@ -13797,7 +13801,7 @@
         <v>0x01E</v>
       </c>
       <c r="D239" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="F239" s="8"/>
       <c r="G239" s="11">
@@ -13848,8 +13852,8 @@
       </c>
     </row>
     <row r="240" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A240" s="55" t="s">
-        <v>292</v>
+      <c r="A240" s="49" t="s">
+        <v>290</v>
       </c>
       <c r="B240">
         <v>33</v>
@@ -13862,7 +13866,7 @@
         <v>223</v>
       </c>
       <c r="F240" s="8" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="G240" s="11">
         <v>17</v>
@@ -13926,10 +13930,10 @@
         <v>0x024</v>
       </c>
       <c r="D241" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F241" s="8" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="G241" s="11">
         <v>1</v>

</xml_diff>

<commit_message>
Pixel animation using Draw pixel subroutine test program (not working yet)
</commit_message>
<xml_diff>
--- a/2nd gen - 8 bit cpu/Instruction control lines.xlsx
+++ b/2nd gen - 8 bit cpu/Instruction control lines.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="345" windowWidth="14805" windowHeight="7770"/>
+    <workbookView xWindow="240" yWindow="345" windowWidth="14805" windowHeight="7770" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Control Lines" sheetId="1" r:id="rId1"/>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="329">
   <si>
     <t>LD R1, data</t>
   </si>
@@ -1034,6 +1034,45 @@
   </si>
   <si>
     <t>One register ALU instructions can be modified to use all registers, by using CLOSE_REGS_BRIDGE=1 and EN_R1_OUT=0</t>
+  </si>
+  <si>
+    <t>// 14 - Pixel animation using Draw pixel subroutine</t>
+  </si>
+  <si>
+    <t>JP 0x0</t>
+  </si>
+  <si>
+    <t>// Else reset E register (y value)</t>
+  </si>
+  <si>
+    <t>// Decrements A (x value)</t>
+  </si>
+  <si>
+    <t>// go to next loop iteration</t>
+  </si>
+  <si>
+    <t>// Alu op just to set Z flag and make conditional jump possible</t>
+  </si>
+  <si>
+    <t>reset_a:</t>
+  </si>
+  <si>
+    <t>// If A = 0 then to reset_a</t>
+  </si>
+  <si>
+    <t>JP Z, 0x3c</t>
+  </si>
+  <si>
+    <t>LD F, 0</t>
+  </si>
+  <si>
+    <t>// Start of loop testing</t>
+  </si>
+  <si>
+    <t>// restart from the very beginning</t>
+  </si>
+  <si>
+    <t>JP 0x6</t>
   </si>
 </sst>
 </file>
@@ -1359,6 +1398,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1377,7 +1417,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1684,8 +1723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
@@ -1859,11 +1898,11 @@
       <c r="AA2" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="AB2" s="51" t="s">
+      <c r="AB2" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="AC2" s="51"/>
-      <c r="AD2" s="51"/>
+      <c r="AC2" s="52"/>
+      <c r="AD2" s="52"/>
     </row>
     <row r="3" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -2936,7 +2975,7 @@
         <f t="shared" si="2"/>
         <v>00</v>
       </c>
-      <c r="AF13" s="57" t="s">
+      <c r="AF13" s="51" t="s">
         <v>185</v>
       </c>
       <c r="AM13" s="8" t="str">
@@ -4162,7 +4201,7 @@
         <f t="shared" si="5"/>
         <v>408802</v>
       </c>
-      <c r="AN37" s="57" t="s">
+      <c r="AN37" s="51" t="s">
         <v>315</v>
       </c>
     </row>
@@ -4954,11 +4993,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA249"/>
+  <dimension ref="A1:AA270"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A216" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G234" sqref="G234"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A234" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F257" sqref="F257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5031,11 +5070,11 @@
       <c r="S1" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="T1" s="52" t="s">
+      <c r="T1" s="53" t="s">
         <v>153</v>
       </c>
-      <c r="U1" s="53"/>
-      <c r="V1" s="54"/>
+      <c r="U1" s="54"/>
+      <c r="V1" s="55"/>
       <c r="W1" s="10"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
@@ -9244,7 +9283,7 @@
       <c r="D129" t="s">
         <v>56</v>
       </c>
-      <c r="F129" s="55" t="s">
+      <c r="F129" s="56" t="s">
         <v>210</v>
       </c>
       <c r="G129" s="11">
@@ -9308,7 +9347,7 @@
       <c r="D130" t="s">
         <v>179</v>
       </c>
-      <c r="F130" s="55"/>
+      <c r="F130" s="56"/>
       <c r="G130" s="11">
         <v>40</v>
       </c>
@@ -9367,7 +9406,7 @@
       <c r="D131" t="s">
         <v>57</v>
       </c>
-      <c r="F131" s="55"/>
+      <c r="F131" s="56"/>
       <c r="G131" s="11">
         <v>2</v>
       </c>
@@ -11138,7 +11177,7 @@
       <c r="D171" t="s">
         <v>221</v>
       </c>
-      <c r="F171" s="55" t="s">
+      <c r="F171" s="56" t="s">
         <v>210</v>
       </c>
       <c r="G171" s="11">
@@ -11202,7 +11241,7 @@
       <c r="D172" t="s">
         <v>201</v>
       </c>
-      <c r="F172" s="55"/>
+      <c r="F172" s="56"/>
       <c r="G172" s="11">
         <v>40</v>
       </c>
@@ -11261,7 +11300,7 @@
       <c r="D173" t="s">
         <v>222</v>
       </c>
-      <c r="F173" s="55"/>
+      <c r="F173" s="56"/>
       <c r="G173" s="11">
         <v>2</v>
       </c>
@@ -11968,7 +12007,7 @@
       <c r="D206" t="s">
         <v>221</v>
       </c>
-      <c r="F206" s="56" t="s">
+      <c r="F206" s="57" t="s">
         <v>253</v>
       </c>
       <c r="G206" s="11">
@@ -12032,7 +12071,7 @@
       <c r="D207" t="s">
         <v>57</v>
       </c>
-      <c r="F207" s="56"/>
+      <c r="F207" s="57"/>
       <c r="G207" s="11">
         <v>2</v>
       </c>
@@ -12094,7 +12133,7 @@
       <c r="D208" t="s">
         <v>51</v>
       </c>
-      <c r="F208" s="56"/>
+      <c r="F208" s="57"/>
       <c r="G208" s="11">
         <v>2</v>
       </c>
@@ -13921,7 +13960,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="241" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B241">
         <v>36</v>
       </c>
@@ -13985,7 +14024,7 @@
         <v>08</v>
       </c>
     </row>
-    <row r="242" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B242">
         <v>39</v>
       </c>
@@ -14050,26 +14089,1410 @@
         <v>00</v>
       </c>
     </row>
-    <row r="243" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F243" s="8"/>
     </row>
-    <row r="244" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F244" s="8"/>
     </row>
-    <row r="245" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F245" s="8"/>
     </row>
-    <row r="246" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D246" s="8" t="s">
+        <v>316</v>
+      </c>
       <c r="F246" s="8"/>
     </row>
-    <row r="247" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="F247" s="8"/>
-    </row>
-    <row r="248" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B247">
+        <v>0</v>
+      </c>
+      <c r="C247" t="str">
+        <f t="shared" ref="C247:C260" si="353">"0x" &amp; DEC2HEX(B247,3)</f>
+        <v>0x000</v>
+      </c>
+      <c r="D247" t="s">
+        <v>296</v>
+      </c>
+      <c r="F247" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="G247" s="11">
+        <v>1</v>
+      </c>
+      <c r="H247" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="I247">
+        <f t="shared" ref="I247:I257" si="354">IF(H247="", "", VLOOKUP(H247, $X$3:$Y$10, 2))</f>
+        <v>0</v>
+      </c>
+      <c r="M247">
+        <v>7</v>
+      </c>
+      <c r="N247" s="16" t="str">
+        <f t="shared" ref="N247:N261" si="355">IF(G247="", "", TEXT(DEC2BIN(G247), "000000"))</f>
+        <v>000001</v>
+      </c>
+      <c r="O247" s="17" t="str">
+        <f t="shared" ref="O247:O261" si="356">IF(I247="", "", TEXT(DEC2BIN(I247), "000"))</f>
+        <v>000</v>
+      </c>
+      <c r="P247" s="17" t="str">
+        <f t="shared" ref="P247:P261" si="357">IF(J247="", "", TEXT(DEC2BIN(J247), "000"))</f>
+        <v/>
+      </c>
+      <c r="Q247" s="17" t="str">
+        <f t="shared" ref="Q247:Q261" si="358">IF(K247="", "", TEXT(DEC2BIN(K247), "000"))</f>
+        <v/>
+      </c>
+      <c r="R247" s="17" t="str">
+        <f t="shared" ref="R247:R261" si="359">IF(L247="", "", TEXT(DEC2BIN(L247), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="S247" s="18" t="str">
+        <f t="shared" ref="S247:S261" si="360">IF(M247="", "", TEXT(DEC2BIN(M247), "00000000"))</f>
+        <v>00000111</v>
+      </c>
+      <c r="T247" t="str">
+        <f t="shared" ref="T247:T261" si="361">BIN2HEX(LEFT(CONCATENATE(N247,IF(O247="", "000", O247)), 8), 2)</f>
+        <v>04</v>
+      </c>
+      <c r="U247" t="str">
+        <f t="shared" ref="U247:U261" si="362">BIN2HEX(CONCATENATE(RIGHT(O247, 1), IF(P247 = "", "000", P247), IF(Q247 = "", "000", Q247), "0"), 2)</f>
+        <v>00</v>
+      </c>
+      <c r="V247" s="13" t="str">
+        <f t="shared" ref="V247:V261" si="363">IF(R247="", BIN2HEX(S247, 2), BIN2HEX(R247,2))</f>
+        <v>07</v>
+      </c>
+    </row>
+    <row r="248" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B248">
+        <v>3</v>
+      </c>
+      <c r="C248" t="str">
+        <f t="shared" si="353"/>
+        <v>0x003</v>
+      </c>
+      <c r="D248" t="s">
+        <v>217</v>
+      </c>
       <c r="F248" s="8"/>
-    </row>
-    <row r="249" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="F249" s="8"/>
+      <c r="G248" s="11">
+        <v>1</v>
+      </c>
+      <c r="H248" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I248">
+        <f t="shared" si="354"/>
+        <v>6</v>
+      </c>
+      <c r="M248">
+        <v>0</v>
+      </c>
+      <c r="N248" s="16" t="str">
+        <f t="shared" si="355"/>
+        <v>000001</v>
+      </c>
+      <c r="O248" s="17" t="str">
+        <f t="shared" si="356"/>
+        <v>110</v>
+      </c>
+      <c r="P248" s="17" t="str">
+        <f t="shared" si="357"/>
+        <v/>
+      </c>
+      <c r="Q248" s="17" t="str">
+        <f t="shared" si="358"/>
+        <v/>
+      </c>
+      <c r="R248" s="17" t="str">
+        <f t="shared" si="359"/>
+        <v/>
+      </c>
+      <c r="S248" s="18" t="str">
+        <f t="shared" si="360"/>
+        <v>00000000</v>
+      </c>
+      <c r="T248" t="str">
+        <f t="shared" si="361"/>
+        <v>07</v>
+      </c>
+      <c r="U248" t="str">
+        <f t="shared" si="362"/>
+        <v>00</v>
+      </c>
+      <c r="V248" s="13" t="str">
+        <f t="shared" si="363"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="249" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A249" s="49" t="s">
+        <v>284</v>
+      </c>
+      <c r="B249">
+        <v>6</v>
+      </c>
+      <c r="C249" t="str">
+        <f t="shared" si="353"/>
+        <v>0x006</v>
+      </c>
+      <c r="D249" t="s">
+        <v>281</v>
+      </c>
+      <c r="F249" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="G249" s="11">
+        <v>1</v>
+      </c>
+      <c r="H249" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="I249">
+        <f t="shared" si="354"/>
+        <v>2</v>
+      </c>
+      <c r="M249">
+        <v>1</v>
+      </c>
+      <c r="N249" s="16" t="str">
+        <f t="shared" si="355"/>
+        <v>000001</v>
+      </c>
+      <c r="O249" s="17" t="str">
+        <f t="shared" si="356"/>
+        <v>010</v>
+      </c>
+      <c r="P249" s="17" t="str">
+        <f t="shared" si="357"/>
+        <v/>
+      </c>
+      <c r="Q249" s="17" t="str">
+        <f t="shared" si="358"/>
+        <v/>
+      </c>
+      <c r="R249" s="17" t="str">
+        <f t="shared" si="359"/>
+        <v/>
+      </c>
+      <c r="S249" s="18" t="str">
+        <f t="shared" si="360"/>
+        <v>00000001</v>
+      </c>
+      <c r="T249" t="str">
+        <f t="shared" si="361"/>
+        <v>05</v>
+      </c>
+      <c r="U249" t="str">
+        <f t="shared" si="362"/>
+        <v>00</v>
+      </c>
+      <c r="V249" s="13" t="str">
+        <f t="shared" si="363"/>
+        <v>01</v>
+      </c>
+    </row>
+    <row r="250" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B250">
+        <v>9</v>
+      </c>
+      <c r="C250" t="str">
+        <f t="shared" si="353"/>
+        <v>0x009</v>
+      </c>
+      <c r="D250" t="s">
+        <v>283</v>
+      </c>
+      <c r="F250" s="8"/>
+      <c r="G250" s="11">
+        <v>1</v>
+      </c>
+      <c r="H250" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="I250">
+        <f t="shared" si="354"/>
+        <v>4</v>
+      </c>
+      <c r="M250">
+        <v>7</v>
+      </c>
+      <c r="N250" s="16" t="str">
+        <f t="shared" si="355"/>
+        <v>000001</v>
+      </c>
+      <c r="O250" s="17" t="str">
+        <f t="shared" si="356"/>
+        <v>100</v>
+      </c>
+      <c r="P250" s="17" t="str">
+        <f t="shared" si="357"/>
+        <v/>
+      </c>
+      <c r="Q250" s="17" t="str">
+        <f t="shared" si="358"/>
+        <v/>
+      </c>
+      <c r="R250" s="17" t="str">
+        <f t="shared" si="359"/>
+        <v/>
+      </c>
+      <c r="S250" s="18" t="str">
+        <f t="shared" si="360"/>
+        <v>00000111</v>
+      </c>
+      <c r="T250" t="str">
+        <f t="shared" si="361"/>
+        <v>06</v>
+      </c>
+      <c r="U250" t="str">
+        <f t="shared" si="362"/>
+        <v>00</v>
+      </c>
+      <c r="V250" s="13" t="str">
+        <f t="shared" si="363"/>
+        <v>07</v>
+      </c>
+    </row>
+    <row r="251" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A251" s="49" t="s">
+        <v>289</v>
+      </c>
+      <c r="B251">
+        <v>12</v>
+      </c>
+      <c r="C251" t="str">
+        <f t="shared" si="353"/>
+        <v>0x00C</v>
+      </c>
+      <c r="D251" t="s">
+        <v>285</v>
+      </c>
+      <c r="F251" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="G251" s="11">
+        <v>2</v>
+      </c>
+      <c r="H251" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="I251">
+        <f t="shared" si="354"/>
+        <v>3</v>
+      </c>
+      <c r="J251">
+        <v>0</v>
+      </c>
+      <c r="N251" s="16" t="str">
+        <f t="shared" si="355"/>
+        <v>000010</v>
+      </c>
+      <c r="O251" s="17" t="str">
+        <f t="shared" si="356"/>
+        <v>011</v>
+      </c>
+      <c r="P251" s="17" t="str">
+        <f t="shared" si="357"/>
+        <v>000</v>
+      </c>
+      <c r="Q251" s="17" t="str">
+        <f t="shared" si="358"/>
+        <v/>
+      </c>
+      <c r="R251" s="17" t="str">
+        <f t="shared" si="359"/>
+        <v/>
+      </c>
+      <c r="S251" s="18" t="str">
+        <f t="shared" si="360"/>
+        <v/>
+      </c>
+      <c r="T251" t="str">
+        <f t="shared" si="361"/>
+        <v>09</v>
+      </c>
+      <c r="U251" t="str">
+        <f t="shared" si="362"/>
+        <v>80</v>
+      </c>
+      <c r="V251" s="13" t="str">
+        <f t="shared" si="363"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="252" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B252">
+        <v>15</v>
+      </c>
+      <c r="C252" t="str">
+        <f t="shared" si="353"/>
+        <v>0x00F</v>
+      </c>
+      <c r="D252" t="s">
+        <v>287</v>
+      </c>
+      <c r="F252" s="8"/>
+      <c r="G252" s="11">
+        <v>33</v>
+      </c>
+      <c r="H252" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="I252">
+        <f t="shared" si="354"/>
+        <v>3</v>
+      </c>
+      <c r="J252">
+        <v>4</v>
+      </c>
+      <c r="N252" s="16" t="str">
+        <f t="shared" si="355"/>
+        <v>100001</v>
+      </c>
+      <c r="O252" s="17" t="str">
+        <f t="shared" si="356"/>
+        <v>011</v>
+      </c>
+      <c r="P252" s="17" t="str">
+        <f t="shared" si="357"/>
+        <v>100</v>
+      </c>
+      <c r="Q252" s="17" t="str">
+        <f t="shared" si="358"/>
+        <v/>
+      </c>
+      <c r="R252" s="17" t="str">
+        <f t="shared" si="359"/>
+        <v/>
+      </c>
+      <c r="S252" s="18" t="str">
+        <f t="shared" si="360"/>
+        <v/>
+      </c>
+      <c r="T252" t="str">
+        <f t="shared" si="361"/>
+        <v>85</v>
+      </c>
+      <c r="U252" t="str">
+        <f t="shared" si="362"/>
+        <v>C0</v>
+      </c>
+      <c r="V252" s="13" t="str">
+        <f t="shared" si="363"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="253" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B253">
+        <v>18</v>
+      </c>
+      <c r="C253" t="str">
+        <f t="shared" si="353"/>
+        <v>0x012</v>
+      </c>
+      <c r="D253" t="s">
+        <v>295</v>
+      </c>
+      <c r="F253" s="8"/>
+      <c r="G253" s="11">
+        <v>6</v>
+      </c>
+      <c r="I253" t="str">
+        <f t="shared" si="354"/>
+        <v/>
+      </c>
+      <c r="L253">
+        <v>33</v>
+      </c>
+      <c r="N253" s="16" t="str">
+        <f t="shared" si="355"/>
+        <v>000110</v>
+      </c>
+      <c r="O253" s="17" t="str">
+        <f t="shared" si="356"/>
+        <v/>
+      </c>
+      <c r="P253" s="17" t="str">
+        <f t="shared" si="357"/>
+        <v/>
+      </c>
+      <c r="Q253" s="17" t="str">
+        <f t="shared" si="358"/>
+        <v/>
+      </c>
+      <c r="R253" s="17" t="str">
+        <f t="shared" si="359"/>
+        <v>00100001</v>
+      </c>
+      <c r="S253" s="18" t="str">
+        <f t="shared" si="360"/>
+        <v/>
+      </c>
+      <c r="T253" t="str">
+        <f t="shared" si="361"/>
+        <v>18</v>
+      </c>
+      <c r="U253" t="str">
+        <f t="shared" si="362"/>
+        <v>00</v>
+      </c>
+      <c r="V253" s="13" t="str">
+        <f t="shared" si="363"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="254" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B254">
+        <v>21</v>
+      </c>
+      <c r="C254" t="str">
+        <f t="shared" si="353"/>
+        <v>0x015</v>
+      </c>
+      <c r="D254" t="s">
+        <v>293</v>
+      </c>
+      <c r="F254" s="8"/>
+      <c r="G254" s="11">
+        <v>2</v>
+      </c>
+      <c r="H254" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="I254">
+        <f t="shared" si="354"/>
+        <v>5</v>
+      </c>
+      <c r="J254">
+        <v>2</v>
+      </c>
+      <c r="N254" s="16" t="str">
+        <f t="shared" si="355"/>
+        <v>000010</v>
+      </c>
+      <c r="O254" s="17" t="str">
+        <f t="shared" si="356"/>
+        <v>101</v>
+      </c>
+      <c r="P254" s="17" t="str">
+        <f t="shared" si="357"/>
+        <v>010</v>
+      </c>
+      <c r="Q254" s="17" t="str">
+        <f t="shared" si="358"/>
+        <v/>
+      </c>
+      <c r="R254" s="17" t="str">
+        <f t="shared" si="359"/>
+        <v/>
+      </c>
+      <c r="S254" s="18" t="str">
+        <f t="shared" si="360"/>
+        <v/>
+      </c>
+      <c r="T254" t="str">
+        <f t="shared" si="361"/>
+        <v>0A</v>
+      </c>
+      <c r="U254" t="str">
+        <f t="shared" si="362"/>
+        <v>A0</v>
+      </c>
+      <c r="V254" s="13" t="str">
+        <f t="shared" si="363"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="255" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B255">
+        <v>24</v>
+      </c>
+      <c r="C255" t="str">
+        <f t="shared" si="353"/>
+        <v>0x018</v>
+      </c>
+      <c r="D255" t="s">
+        <v>294</v>
+      </c>
+      <c r="F255" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="G255" s="11">
+        <v>32</v>
+      </c>
+      <c r="H255" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="I255">
+        <f t="shared" si="354"/>
+        <v>2</v>
+      </c>
+      <c r="J255">
+        <v>5</v>
+      </c>
+      <c r="N255" s="16" t="str">
+        <f t="shared" si="355"/>
+        <v>100000</v>
+      </c>
+      <c r="O255" s="17" t="str">
+        <f t="shared" si="356"/>
+        <v>010</v>
+      </c>
+      <c r="P255" s="17" t="str">
+        <f t="shared" si="357"/>
+        <v>101</v>
+      </c>
+      <c r="Q255" s="17" t="str">
+        <f t="shared" si="358"/>
+        <v/>
+      </c>
+      <c r="R255" s="17" t="str">
+        <f t="shared" si="359"/>
+        <v/>
+      </c>
+      <c r="S255" s="18" t="str">
+        <f t="shared" si="360"/>
+        <v/>
+      </c>
+      <c r="T255" t="str">
+        <f t="shared" si="361"/>
+        <v>81</v>
+      </c>
+      <c r="U255" t="str">
+        <f t="shared" si="362"/>
+        <v>50</v>
+      </c>
+      <c r="V255" s="13" t="str">
+        <f t="shared" si="363"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="256" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B256">
+        <v>27</v>
+      </c>
+      <c r="C256" t="str">
+        <f t="shared" si="353"/>
+        <v>0x01B</v>
+      </c>
+      <c r="D256" t="s">
+        <v>179</v>
+      </c>
+      <c r="F256" s="8"/>
+      <c r="G256" s="11">
+        <v>40</v>
+      </c>
+      <c r="H256" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="I256">
+        <f t="shared" si="354"/>
+        <v>0</v>
+      </c>
+      <c r="N256" s="16" t="str">
+        <f t="shared" si="355"/>
+        <v>101000</v>
+      </c>
+      <c r="O256" s="17" t="str">
+        <f t="shared" si="356"/>
+        <v>000</v>
+      </c>
+      <c r="P256" s="17" t="str">
+        <f t="shared" si="357"/>
+        <v/>
+      </c>
+      <c r="Q256" s="17" t="str">
+        <f t="shared" si="358"/>
+        <v/>
+      </c>
+      <c r="R256" s="17" t="str">
+        <f t="shared" si="359"/>
+        <v/>
+      </c>
+      <c r="S256" s="18" t="str">
+        <f t="shared" si="360"/>
+        <v/>
+      </c>
+      <c r="T256" t="str">
+        <f t="shared" si="361"/>
+        <v>A0</v>
+      </c>
+      <c r="U256" t="str">
+        <f t="shared" si="362"/>
+        <v>00</v>
+      </c>
+      <c r="V256" s="13" t="str">
+        <f t="shared" si="363"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="257" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B257">
+        <v>30</v>
+      </c>
+      <c r="C257" t="str">
+        <f t="shared" si="353"/>
+        <v>0x01E</v>
+      </c>
+      <c r="D257" t="s">
+        <v>291</v>
+      </c>
+      <c r="F257" s="8"/>
+      <c r="G257" s="11">
+        <v>5</v>
+      </c>
+      <c r="I257" t="str">
+        <f t="shared" si="354"/>
+        <v/>
+      </c>
+      <c r="L257">
+        <v>12</v>
+      </c>
+      <c r="N257" s="16" t="str">
+        <f t="shared" si="355"/>
+        <v>000101</v>
+      </c>
+      <c r="O257" s="17" t="str">
+        <f t="shared" si="356"/>
+        <v/>
+      </c>
+      <c r="P257" s="17" t="str">
+        <f t="shared" si="357"/>
+        <v/>
+      </c>
+      <c r="Q257" s="17" t="str">
+        <f t="shared" si="358"/>
+        <v/>
+      </c>
+      <c r="R257" s="17" t="str">
+        <f t="shared" si="359"/>
+        <v>00001100</v>
+      </c>
+      <c r="S257" s="18" t="str">
+        <f t="shared" si="360"/>
+        <v/>
+      </c>
+      <c r="T257" t="str">
+        <f t="shared" si="361"/>
+        <v>14</v>
+      </c>
+      <c r="U257" t="str">
+        <f t="shared" si="362"/>
+        <v>00</v>
+      </c>
+      <c r="V257" s="13" t="str">
+        <f t="shared" si="363"/>
+        <v>0C</v>
+      </c>
+    </row>
+    <row r="258" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A258" s="49" t="s">
+        <v>290</v>
+      </c>
+      <c r="B258">
+        <v>33</v>
+      </c>
+      <c r="C258" t="str">
+        <f t="shared" si="353"/>
+        <v>0x021</v>
+      </c>
+      <c r="D258" t="s">
+        <v>223</v>
+      </c>
+      <c r="F258" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="G258" s="11">
+        <v>17</v>
+      </c>
+      <c r="H258" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="I258">
+        <f>IF(H258="", "", VLOOKUP(H258, $X$3:$Y$10, 2))</f>
+        <v>2</v>
+      </c>
+      <c r="J258">
+        <v>6</v>
+      </c>
+      <c r="K258">
+        <v>1</v>
+      </c>
+      <c r="N258" s="16" t="str">
+        <f t="shared" si="355"/>
+        <v>010001</v>
+      </c>
+      <c r="O258" s="17" t="str">
+        <f t="shared" si="356"/>
+        <v>010</v>
+      </c>
+      <c r="P258" s="17" t="str">
+        <f t="shared" si="357"/>
+        <v>110</v>
+      </c>
+      <c r="Q258" s="17" t="str">
+        <f t="shared" si="358"/>
+        <v>001</v>
+      </c>
+      <c r="R258" s="17" t="str">
+        <f t="shared" si="359"/>
+        <v/>
+      </c>
+      <c r="S258" s="18" t="str">
+        <f t="shared" si="360"/>
+        <v/>
+      </c>
+      <c r="T258" t="str">
+        <f t="shared" si="361"/>
+        <v>45</v>
+      </c>
+      <c r="U258" t="str">
+        <f t="shared" si="362"/>
+        <v>62</v>
+      </c>
+      <c r="V258" s="13" t="str">
+        <f t="shared" si="363"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="259" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B259">
+        <v>36</v>
+      </c>
+      <c r="C259" t="str">
+        <f t="shared" si="353"/>
+        <v>0x024</v>
+      </c>
+      <c r="D259" t="s">
+        <v>301</v>
+      </c>
+      <c r="F259" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="G259" s="11">
+        <v>1</v>
+      </c>
+      <c r="H259" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I259">
+        <f t="shared" ref="I259" si="364">IF(H259="", "", VLOOKUP(H259, $X$3:$Y$10, 2))</f>
+        <v>6</v>
+      </c>
+      <c r="M259">
+        <v>8</v>
+      </c>
+      <c r="N259" s="16" t="str">
+        <f t="shared" si="355"/>
+        <v>000001</v>
+      </c>
+      <c r="O259" s="17" t="str">
+        <f t="shared" si="356"/>
+        <v>110</v>
+      </c>
+      <c r="P259" s="17" t="str">
+        <f t="shared" si="357"/>
+        <v/>
+      </c>
+      <c r="Q259" s="17" t="str">
+        <f t="shared" si="358"/>
+        <v/>
+      </c>
+      <c r="R259" s="17" t="str">
+        <f t="shared" si="359"/>
+        <v/>
+      </c>
+      <c r="S259" s="18" t="str">
+        <f t="shared" si="360"/>
+        <v>00001000</v>
+      </c>
+      <c r="T259" t="str">
+        <f t="shared" si="361"/>
+        <v>07</v>
+      </c>
+      <c r="U259" t="str">
+        <f t="shared" si="362"/>
+        <v>00</v>
+      </c>
+      <c r="V259" s="13" t="str">
+        <f t="shared" si="363"/>
+        <v>08</v>
+      </c>
+    </row>
+    <row r="260" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B260">
+        <v>39</v>
+      </c>
+      <c r="C260" t="str">
+        <f t="shared" si="353"/>
+        <v>0x027</v>
+      </c>
+      <c r="D260" t="s">
+        <v>223</v>
+      </c>
+      <c r="F260" s="8"/>
+      <c r="G260" s="11">
+        <v>17</v>
+      </c>
+      <c r="H260" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="I260">
+        <f>IF(H260="", "", VLOOKUP(H260, $X$3:$Y$10, 2))</f>
+        <v>2</v>
+      </c>
+      <c r="J260">
+        <v>6</v>
+      </c>
+      <c r="K260">
+        <v>1</v>
+      </c>
+      <c r="N260" s="16" t="str">
+        <f t="shared" si="355"/>
+        <v>010001</v>
+      </c>
+      <c r="O260" s="17" t="str">
+        <f t="shared" si="356"/>
+        <v>010</v>
+      </c>
+      <c r="P260" s="17" t="str">
+        <f t="shared" si="357"/>
+        <v>110</v>
+      </c>
+      <c r="Q260" s="17" t="str">
+        <f t="shared" si="358"/>
+        <v>001</v>
+      </c>
+      <c r="R260" s="17" t="str">
+        <f t="shared" si="359"/>
+        <v/>
+      </c>
+      <c r="S260" s="18" t="str">
+        <f t="shared" si="360"/>
+        <v/>
+      </c>
+      <c r="T260" t="str">
+        <f t="shared" si="361"/>
+        <v>45</v>
+      </c>
+      <c r="U260" t="str">
+        <f t="shared" si="362"/>
+        <v>62</v>
+      </c>
+      <c r="V260" s="13" t="str">
+        <f t="shared" si="363"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="261" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B261">
+        <v>42</v>
+      </c>
+      <c r="C261" t="str">
+        <f t="shared" ref="C261:C265" si="365">"0x" &amp; DEC2HEX(B261,3)</f>
+        <v>0x02A</v>
+      </c>
+      <c r="D261" t="s">
+        <v>325</v>
+      </c>
+      <c r="F261" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="G261" s="11">
+        <v>1</v>
+      </c>
+      <c r="H261" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="I261">
+        <f t="shared" ref="I261:I263" si="366">IF(H261="", "", VLOOKUP(H261, $X$3:$Y$10, 2))</f>
+        <v>7</v>
+      </c>
+      <c r="M261">
+        <v>0</v>
+      </c>
+      <c r="N261" s="16" t="str">
+        <f t="shared" si="355"/>
+        <v>000001</v>
+      </c>
+      <c r="O261" s="17" t="str">
+        <f t="shared" si="356"/>
+        <v>111</v>
+      </c>
+      <c r="P261" s="17" t="str">
+        <f t="shared" si="357"/>
+        <v/>
+      </c>
+      <c r="Q261" s="17" t="str">
+        <f t="shared" si="358"/>
+        <v/>
+      </c>
+      <c r="R261" s="17" t="str">
+        <f t="shared" si="359"/>
+        <v/>
+      </c>
+      <c r="S261" s="18" t="str">
+        <f t="shared" si="360"/>
+        <v>00000000</v>
+      </c>
+      <c r="T261" t="str">
+        <f t="shared" si="361"/>
+        <v>07</v>
+      </c>
+      <c r="U261" t="str">
+        <f t="shared" si="362"/>
+        <v>80</v>
+      </c>
+      <c r="V261" s="13" t="str">
+        <f t="shared" si="363"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="262" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B262">
+        <v>45</v>
+      </c>
+      <c r="C262" t="str">
+        <f t="shared" si="365"/>
+        <v>0x02D</v>
+      </c>
+      <c r="D262" t="s">
+        <v>118</v>
+      </c>
+      <c r="F262" s="8" t="s">
+        <v>321</v>
+      </c>
+      <c r="G262" s="11">
+        <v>33</v>
+      </c>
+      <c r="H262" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="I262">
+        <f t="shared" si="366"/>
+        <v>0</v>
+      </c>
+      <c r="J262">
+        <v>7</v>
+      </c>
+      <c r="N262" s="16" t="str">
+        <f t="shared" ref="N262:N263" si="367">IF(G262="", "", TEXT(DEC2BIN(G262), "000000"))</f>
+        <v>100001</v>
+      </c>
+      <c r="O262" s="17" t="str">
+        <f t="shared" ref="O262:O263" si="368">IF(I262="", "", TEXT(DEC2BIN(I262), "000"))</f>
+        <v>000</v>
+      </c>
+      <c r="P262" s="17" t="str">
+        <f t="shared" ref="P262:P263" si="369">IF(J262="", "", TEXT(DEC2BIN(J262), "000"))</f>
+        <v>111</v>
+      </c>
+      <c r="Q262" s="17" t="str">
+        <f t="shared" ref="Q262:Q263" si="370">IF(K262="", "", TEXT(DEC2BIN(K262), "000"))</f>
+        <v/>
+      </c>
+      <c r="R262" s="17" t="str">
+        <f t="shared" ref="R262:R263" si="371">IF(L262="", "", TEXT(DEC2BIN(L262), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="S262" s="18" t="str">
+        <f t="shared" ref="S262:S263" si="372">IF(M262="", "", TEXT(DEC2BIN(M262), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="T262" t="str">
+        <f t="shared" ref="T262:T263" si="373">BIN2HEX(LEFT(CONCATENATE(N262,IF(O262="", "000", O262)), 8), 2)</f>
+        <v>84</v>
+      </c>
+      <c r="U262" t="str">
+        <f t="shared" ref="U262:U263" si="374">BIN2HEX(CONCATENATE(RIGHT(O262, 1), IF(P262 = "", "000", P262), IF(Q262 = "", "000", Q262), "0"), 2)</f>
+        <v>70</v>
+      </c>
+      <c r="V262" s="13" t="str">
+        <f t="shared" ref="V262:V263" si="375">IF(R262="", BIN2HEX(S262, 2), BIN2HEX(R262,2))</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="263" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B263">
+        <v>48</v>
+      </c>
+      <c r="C263" t="str">
+        <f t="shared" si="365"/>
+        <v>0x030</v>
+      </c>
+      <c r="D263" t="s">
+        <v>324</v>
+      </c>
+      <c r="F263" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="G263" s="11">
+        <v>6</v>
+      </c>
+      <c r="I263" t="str">
+        <f t="shared" si="366"/>
+        <v/>
+      </c>
+      <c r="L263">
+        <v>60</v>
+      </c>
+      <c r="N263" s="16" t="str">
+        <f t="shared" si="367"/>
+        <v>000110</v>
+      </c>
+      <c r="O263" s="17" t="str">
+        <f t="shared" si="368"/>
+        <v/>
+      </c>
+      <c r="P263" s="17" t="str">
+        <f t="shared" si="369"/>
+        <v/>
+      </c>
+      <c r="Q263" s="17" t="str">
+        <f t="shared" si="370"/>
+        <v/>
+      </c>
+      <c r="R263" s="17" t="str">
+        <f t="shared" si="371"/>
+        <v>00111100</v>
+      </c>
+      <c r="S263" s="18" t="str">
+        <f t="shared" si="372"/>
+        <v/>
+      </c>
+      <c r="T263" t="str">
+        <f t="shared" si="373"/>
+        <v>18</v>
+      </c>
+      <c r="U263" t="str">
+        <f t="shared" si="374"/>
+        <v>00</v>
+      </c>
+      <c r="V263" s="13" t="str">
+        <f t="shared" si="375"/>
+        <v>3C</v>
+      </c>
+    </row>
+    <row r="264" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B264">
+        <v>51</v>
+      </c>
+      <c r="C264" t="str">
+        <f t="shared" si="365"/>
+        <v>0x033</v>
+      </c>
+      <c r="D264" t="s">
+        <v>217</v>
+      </c>
+      <c r="F264" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="G264" s="11">
+        <v>1</v>
+      </c>
+      <c r="H264" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I264">
+        <f t="shared" ref="I264:I266" si="376">IF(H264="", "", VLOOKUP(H264, $X$3:$Y$10, 2))</f>
+        <v>6</v>
+      </c>
+      <c r="M264">
+        <v>0</v>
+      </c>
+      <c r="N264" s="16" t="str">
+        <f t="shared" ref="N264:N266" si="377">IF(G264="", "", TEXT(DEC2BIN(G264), "000000"))</f>
+        <v>000001</v>
+      </c>
+      <c r="O264" s="17" t="str">
+        <f t="shared" ref="O264:O266" si="378">IF(I264="", "", TEXT(DEC2BIN(I264), "000"))</f>
+        <v>110</v>
+      </c>
+      <c r="P264" s="17" t="str">
+        <f t="shared" ref="P264:P266" si="379">IF(J264="", "", TEXT(DEC2BIN(J264), "000"))</f>
+        <v/>
+      </c>
+      <c r="Q264" s="17" t="str">
+        <f t="shared" ref="Q264:Q266" si="380">IF(K264="", "", TEXT(DEC2BIN(K264), "000"))</f>
+        <v/>
+      </c>
+      <c r="R264" s="17" t="str">
+        <f t="shared" ref="R264:R266" si="381">IF(L264="", "", TEXT(DEC2BIN(L264), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="S264" s="18" t="str">
+        <f t="shared" ref="S264:S266" si="382">IF(M264="", "", TEXT(DEC2BIN(M264), "00000000"))</f>
+        <v>00000000</v>
+      </c>
+      <c r="T264" t="str">
+        <f t="shared" ref="T264:T266" si="383">BIN2HEX(LEFT(CONCATENATE(N264,IF(O264="", "000", O264)), 8), 2)</f>
+        <v>07</v>
+      </c>
+      <c r="U264" t="str">
+        <f t="shared" ref="U264:U266" si="384">BIN2HEX(CONCATENATE(RIGHT(O264, 1), IF(P264 = "", "000", P264), IF(Q264 = "", "000", Q264), "0"), 2)</f>
+        <v>00</v>
+      </c>
+      <c r="V264" s="13" t="str">
+        <f t="shared" ref="V264:V266" si="385">IF(R264="", BIN2HEX(S264, 2), BIN2HEX(R264,2))</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="265" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B265">
+        <v>54</v>
+      </c>
+      <c r="C265" t="str">
+        <f t="shared" si="365"/>
+        <v>0x036</v>
+      </c>
+      <c r="D265" t="s">
+        <v>248</v>
+      </c>
+      <c r="F265" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="G265" s="11">
+        <v>41</v>
+      </c>
+      <c r="H265" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="I265">
+        <f t="shared" si="376"/>
+        <v>0</v>
+      </c>
+      <c r="N265" s="16" t="str">
+        <f t="shared" si="377"/>
+        <v>101001</v>
+      </c>
+      <c r="O265" s="17" t="str">
+        <f t="shared" si="378"/>
+        <v>000</v>
+      </c>
+      <c r="P265" s="17" t="str">
+        <f t="shared" si="379"/>
+        <v/>
+      </c>
+      <c r="Q265" s="17" t="str">
+        <f t="shared" si="380"/>
+        <v/>
+      </c>
+      <c r="R265" s="17" t="str">
+        <f t="shared" si="381"/>
+        <v/>
+      </c>
+      <c r="S265" s="18" t="str">
+        <f t="shared" si="382"/>
+        <v/>
+      </c>
+      <c r="T265" t="str">
+        <f t="shared" si="383"/>
+        <v>A4</v>
+      </c>
+      <c r="U265" t="str">
+        <f t="shared" si="384"/>
+        <v>00</v>
+      </c>
+      <c r="V265" s="13" t="str">
+        <f t="shared" si="385"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="266" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B266">
+        <v>57</v>
+      </c>
+      <c r="C266" t="str">
+        <f t="shared" ref="C266:C268" si="386">"0x" &amp; DEC2HEX(B266,3)</f>
+        <v>0x039</v>
+      </c>
+      <c r="D266" t="s">
+        <v>328</v>
+      </c>
+      <c r="F266" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="G266" s="11">
+        <v>5</v>
+      </c>
+      <c r="I266" t="str">
+        <f t="shared" si="376"/>
+        <v/>
+      </c>
+      <c r="L266">
+        <v>6</v>
+      </c>
+      <c r="N266" s="16" t="str">
+        <f t="shared" si="377"/>
+        <v>000101</v>
+      </c>
+      <c r="O266" s="17" t="str">
+        <f t="shared" si="378"/>
+        <v/>
+      </c>
+      <c r="P266" s="17" t="str">
+        <f t="shared" si="379"/>
+        <v/>
+      </c>
+      <c r="Q266" s="17" t="str">
+        <f t="shared" si="380"/>
+        <v/>
+      </c>
+      <c r="R266" s="17" t="str">
+        <f t="shared" si="381"/>
+        <v>00000110</v>
+      </c>
+      <c r="S266" s="18" t="str">
+        <f t="shared" si="382"/>
+        <v/>
+      </c>
+      <c r="T266" t="str">
+        <f t="shared" si="383"/>
+        <v>14</v>
+      </c>
+      <c r="U266" t="str">
+        <f t="shared" si="384"/>
+        <v>00</v>
+      </c>
+      <c r="V266" s="13" t="str">
+        <f t="shared" si="385"/>
+        <v>06</v>
+      </c>
+    </row>
+    <row r="267" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A267" s="49" t="s">
+        <v>322</v>
+      </c>
+      <c r="B267">
+        <v>60</v>
+      </c>
+      <c r="C267" t="str">
+        <f t="shared" si="386"/>
+        <v>0x03C</v>
+      </c>
+      <c r="D267" t="s">
+        <v>296</v>
+      </c>
+      <c r="F267" s="8"/>
+      <c r="G267" s="11">
+        <v>1</v>
+      </c>
+      <c r="H267" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="I267">
+        <f t="shared" ref="I267:I268" si="387">IF(H267="", "", VLOOKUP(H267, $X$3:$Y$10, 2))</f>
+        <v>0</v>
+      </c>
+      <c r="M267">
+        <v>7</v>
+      </c>
+      <c r="N267" s="16" t="str">
+        <f t="shared" ref="N267:N268" si="388">IF(G267="", "", TEXT(DEC2BIN(G267), "000000"))</f>
+        <v>000001</v>
+      </c>
+      <c r="O267" s="17" t="str">
+        <f t="shared" ref="O267:O268" si="389">IF(I267="", "", TEXT(DEC2BIN(I267), "000"))</f>
+        <v>000</v>
+      </c>
+      <c r="P267" s="17" t="str">
+        <f t="shared" ref="P267:P268" si="390">IF(J267="", "", TEXT(DEC2BIN(J267), "000"))</f>
+        <v/>
+      </c>
+      <c r="Q267" s="17" t="str">
+        <f t="shared" ref="Q267:Q268" si="391">IF(K267="", "", TEXT(DEC2BIN(K267), "000"))</f>
+        <v/>
+      </c>
+      <c r="R267" s="17" t="str">
+        <f t="shared" ref="R267:R268" si="392">IF(L267="", "", TEXT(DEC2BIN(L267), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="S267" s="18" t="str">
+        <f t="shared" ref="S267:S268" si="393">IF(M267="", "", TEXT(DEC2BIN(M267), "00000000"))</f>
+        <v>00000111</v>
+      </c>
+      <c r="T267" t="str">
+        <f t="shared" ref="T267:T268" si="394">BIN2HEX(LEFT(CONCATENATE(N267,IF(O267="", "000", O267)), 8), 2)</f>
+        <v>04</v>
+      </c>
+      <c r="U267" t="str">
+        <f t="shared" ref="U267:U268" si="395">BIN2HEX(CONCATENATE(RIGHT(O267, 1), IF(P267 = "", "000", P267), IF(Q267 = "", "000", Q267), "0"), 2)</f>
+        <v>00</v>
+      </c>
+      <c r="V267" s="13" t="str">
+        <f t="shared" ref="V267:V268" si="396">IF(R267="", BIN2HEX(S267, 2), BIN2HEX(R267,2))</f>
+        <v>07</v>
+      </c>
+    </row>
+    <row r="268" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B268">
+        <v>63</v>
+      </c>
+      <c r="C268" t="str">
+        <f t="shared" si="386"/>
+        <v>0x03F</v>
+      </c>
+      <c r="D268" t="s">
+        <v>317</v>
+      </c>
+      <c r="F268" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="G268" s="11">
+        <v>5</v>
+      </c>
+      <c r="I268" t="str">
+        <f t="shared" si="387"/>
+        <v/>
+      </c>
+      <c r="L268">
+        <v>0</v>
+      </c>
+      <c r="N268" s="16" t="str">
+        <f t="shared" si="388"/>
+        <v>000101</v>
+      </c>
+      <c r="O268" s="17" t="str">
+        <f t="shared" si="389"/>
+        <v/>
+      </c>
+      <c r="P268" s="17" t="str">
+        <f t="shared" si="390"/>
+        <v/>
+      </c>
+      <c r="Q268" s="17" t="str">
+        <f t="shared" si="391"/>
+        <v/>
+      </c>
+      <c r="R268" s="17" t="str">
+        <f t="shared" si="392"/>
+        <v>00000000</v>
+      </c>
+      <c r="S268" s="18" t="str">
+        <f t="shared" si="393"/>
+        <v/>
+      </c>
+      <c r="T268" t="str">
+        <f t="shared" si="394"/>
+        <v>14</v>
+      </c>
+      <c r="U268" t="str">
+        <f t="shared" si="395"/>
+        <v>00</v>
+      </c>
+      <c r="V268" s="13" t="str">
+        <f t="shared" si="396"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="270" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F270" s="8"/>
     </row>
   </sheetData>
   <sortState ref="X16:Y18">
@@ -14085,7 +15508,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z17">
       <formula1>$X$16:$X$18</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H6 H9:H11 H201:H224 H141:H149 H102:H112 H117:H132 H83:H93 H49 H41:H42 H31:H33 H17:H26 H229:H242 H154:H174">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H6 H9:H11 H201:H224 H141:H149 H102:H112 H117:H132 H83:H93 H49 H41:H42 H31:H33 H17:H26 H229:H242 H154:H174 H247:H268">
       <formula1>$X$3:$X$10</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
v.0.17.3 Mag comp instr test programs working OK.
</commit_message>
<xml_diff>
--- a/2nd gen - 8 bit cpu/Instruction control lines.xlsx
+++ b/2nd gen - 8 bit cpu/Instruction control lines.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="345" windowWidth="14805" windowHeight="7770" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="345" windowWidth="14805" windowHeight="7770" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Control Lines" sheetId="1" r:id="rId1"/>
@@ -90,6 +90,19 @@
         </r>
       </text>
     </comment>
+    <comment ref="C48" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shift Left (multiply by 2)</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -136,7 +149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="388">
   <si>
     <t>LD R1, data</t>
   </si>
@@ -1185,9 +1198,6 @@
     <t>SUBM R1, R2</t>
   </si>
   <si>
-    <t xml:space="preserve">JP C, </t>
-  </si>
-  <si>
     <t>SUB</t>
   </si>
   <si>
@@ -1236,28 +1246,73 @@
     <t>// R1 &gt; R2</t>
   </si>
   <si>
-    <t>// 18 - Test mag comp instr</t>
-  </si>
-  <si>
-    <t>LD A, 0</t>
-  </si>
-  <si>
-    <t>LD C, 5</t>
-  </si>
-  <si>
     <t>SUB A, C</t>
   </si>
   <si>
-    <t>// ASCII char '&lt;'</t>
-  </si>
-  <si>
-    <t>LD B, 0x3c</t>
-  </si>
-  <si>
-    <t>LD H, 0x3e</t>
-  </si>
-  <si>
-    <t>// ASCII char '&gt;'</t>
+    <t>// ASCII char 'A'</t>
+  </si>
+  <si>
+    <t>// ASCII char 'C'</t>
+  </si>
+  <si>
+    <t>r2_higher:</t>
+  </si>
+  <si>
+    <t>inc:</t>
+  </si>
+  <si>
+    <t>LD F, A</t>
+  </si>
+  <si>
+    <t>LD A, F</t>
+  </si>
+  <si>
+    <t>// Expected output:</t>
+  </si>
+  <si>
+    <t>LD H, 0x43</t>
+  </si>
+  <si>
+    <t>// R1 &gt;= R2; Print out 'A'</t>
+  </si>
+  <si>
+    <t>// Print out 'C'</t>
+  </si>
+  <si>
+    <t>// CCCCCAAAAAAA (...)</t>
+  </si>
+  <si>
+    <t>JP 0x00c</t>
+  </si>
+  <si>
+    <t>JP C, 0x01e</t>
+  </si>
+  <si>
+    <t>JP 0x021</t>
+  </si>
+  <si>
+    <t>LD C, 0x5</t>
+  </si>
+  <si>
+    <t>SHL R1</t>
+  </si>
+  <si>
+    <t>// 18 - Test magnitude comparison instruction</t>
+  </si>
+  <si>
+    <t>// 19 - Test magnitude comparison instruction (2)</t>
+  </si>
+  <si>
+    <t>SUBM A, C</t>
+  </si>
+  <si>
+    <t>// R1 &gt; R2; Print out 'A'</t>
+  </si>
+  <si>
+    <t>// CCCCCCAAAAAAA (...)</t>
+  </si>
+  <si>
+    <t>// ALU op to set C flag used in comparison instruction</t>
   </si>
 </sst>
 </file>
@@ -1515,7 +1570,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1616,6 +1671,17 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1628,16 +1694,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1984,11 +2043,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN57"/>
+  <dimension ref="A1:AN58"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K52" sqref="K52"/>
+      <selection pane="bottomLeft" activeCell="AN53" sqref="AN53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2137,7 +2196,7 @@
       <c r="T2" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="U2" s="66" t="s">
+      <c r="U2" s="62" t="s">
         <v>345</v>
       </c>
       <c r="V2" s="35" t="s">
@@ -2158,11 +2217,11 @@
       <c r="AA2" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="AB2" s="58" t="s">
+      <c r="AB2" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="AC2" s="58"/>
-      <c r="AD2" s="58"/>
+      <c r="AC2" s="63"/>
+      <c r="AD2" s="63"/>
     </row>
     <row r="3" spans="1:39" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="29">
@@ -5477,81 +5536,111 @@
         <f t="shared" si="26"/>
         <v>19</v>
       </c>
-      <c r="AF47" s="31" t="s">
-        <v>199</v>
-      </c>
       <c r="AM47" s="42" t="str">
         <f t="shared" si="27"/>
         <v>408819</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="C49" s="57" t="s">
+    <row r="48" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="C48" s="9" t="s">
+        <v>381</v>
+      </c>
+      <c r="D48" s="56"/>
+      <c r="E48" s="56"/>
+      <c r="F48" s="56"/>
+      <c r="G48" s="56"/>
+      <c r="H48" s="56"/>
+      <c r="I48" s="56"/>
+      <c r="J48" s="56"/>
+      <c r="K48" s="56"/>
+      <c r="L48" s="56"/>
+      <c r="M48" s="56"/>
+      <c r="N48" s="56"/>
+      <c r="O48" s="56"/>
+      <c r="P48" s="56"/>
+      <c r="Q48" s="56"/>
+      <c r="R48" s="56"/>
+      <c r="S48" s="56"/>
+      <c r="T48" s="56"/>
+      <c r="U48" s="56"/>
+      <c r="V48" s="68"/>
+      <c r="W48" s="29"/>
+      <c r="X48" s="29"/>
+      <c r="Y48" s="29"/>
+      <c r="Z48" s="29"/>
+      <c r="AA48" s="29"/>
+      <c r="AB48" s="45"/>
+      <c r="AC48" s="45"/>
+      <c r="AD48" s="45"/>
+      <c r="AM48" s="42"/>
+    </row>
+    <row r="50" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C50" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="D49" s="31" t="s">
+      <c r="D50" s="31" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="C50" s="54" t="s">
+    <row r="51" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C51" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="D50" s="31" t="s">
+      <c r="D51" s="31" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="C52" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="D52" s="31" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C53" s="30" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D53" s="31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C54" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D54" s="31" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C55" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="D54" s="31" t="s">
+      <c r="D55" s="31" t="s">
         <v>208</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A55" s="31"/>
-      <c r="B55" s="31"/>
-      <c r="C55" s="30" t="s">
-        <v>200</v>
-      </c>
-      <c r="D55" s="31" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A56" s="31"/>
       <c r="B56" s="31"/>
       <c r="C56" s="30" t="s">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="D56" s="31" t="s">
-        <v>96</v>
+        <v>201</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A57" s="31"/>
       <c r="B57" s="31"/>
       <c r="C57" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="D57" s="31" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A58" s="31"/>
+      <c r="B58" s="31"/>
+      <c r="C58" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="D57" s="31" t="s">
+      <c r="D58" s="31" t="s">
         <v>95</v>
       </c>
     </row>
@@ -5567,11 +5656,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA313"/>
+  <dimension ref="A1:AA339"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A280" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F309" sqref="F309"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A299" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F312" sqref="F312"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5649,11 +5738,11 @@
       <c r="S1" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="T1" s="59" t="s">
+      <c r="T1" s="64" t="s">
         <v>148</v>
       </c>
-      <c r="U1" s="60"/>
-      <c r="V1" s="61"/>
+      <c r="U1" s="65"/>
+      <c r="V1" s="66"/>
     </row>
     <row r="2" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="10"/>
@@ -17242,56 +17331,1650 @@
         <v>00</v>
       </c>
     </row>
-    <row r="306" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D306" s="2" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="307" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B307" s="6">
+        <v>0</v>
+      </c>
+      <c r="C307" s="6" t="str">
+        <f t="shared" ref="C307:C308" si="438">"0x" &amp; DEC2HEX(B307,3)</f>
+        <v>0x000</v>
+      </c>
+      <c r="D307" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="F307" s="2" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="307" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D307" s="27" t="s">
+      <c r="G307" s="16">
+        <v>1</v>
+      </c>
+      <c r="H307" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="I307" s="6">
+        <f t="shared" ref="I307:I308" si="439">IF(H307="", "", VLOOKUP(H307, $X$3:$Y$10, 2))</f>
+        <v>1</v>
+      </c>
+      <c r="M307" s="6">
+        <v>65</v>
+      </c>
+      <c r="N307" s="18" t="str">
+        <f t="shared" ref="N307:N308" si="440">IF(G307="", "", TEXT(DEC2BIN(G307), "000000"))</f>
+        <v>000001</v>
+      </c>
+      <c r="O307" s="19" t="str">
+        <f t="shared" ref="O307:O308" si="441">IF(I307="", "", TEXT(DEC2BIN(I307), "000"))</f>
+        <v>001</v>
+      </c>
+      <c r="P307" s="19" t="str">
+        <f t="shared" ref="P307:P308" si="442">IF(J307="", "", TEXT(DEC2BIN(J307), "000"))</f>
+        <v/>
+      </c>
+      <c r="Q307" s="19" t="str">
+        <f t="shared" ref="Q307:Q308" si="443">IF(K307="", "", TEXT(DEC2BIN(K307), "000"))</f>
+        <v/>
+      </c>
+      <c r="R307" s="19" t="str">
+        <f t="shared" ref="R307:R308" si="444">IF(L307="", "", TEXT(DEC2BIN(L307), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="S307" s="20" t="str">
+        <f t="shared" ref="S307:S308" si="445">IF(M307="", "", TEXT(DEC2BIN(M307), "00000000"))</f>
+        <v>01000001</v>
+      </c>
+      <c r="T307" s="6" t="str">
+        <f t="shared" ref="T307:T308" si="446">BIN2HEX(LEFT(CONCATENATE(N307,IF(O307="", "000", O307)), 8), 2)</f>
+        <v>04</v>
+      </c>
+      <c r="U307" s="6" t="str">
+        <f t="shared" ref="U307:U308" si="447">BIN2HEX(CONCATENATE(RIGHT(O307, 1), IF(P307 = "", "000", P307), IF(Q307 = "", "000", Q307), "0"), 2)</f>
+        <v>80</v>
+      </c>
+      <c r="V307" s="21" t="str">
+        <f t="shared" ref="V307:V308" si="448">IF(R307="", BIN2HEX(S307, 2), BIN2HEX(R307,2))</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="308" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B308" s="6">
+        <v>3</v>
+      </c>
+      <c r="C308" s="6" t="str">
+        <f t="shared" si="438"/>
+        <v>0x003</v>
+      </c>
+      <c r="D308" s="27" t="s">
+        <v>373</v>
+      </c>
+      <c r="F308" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="G308" s="16">
+        <v>1</v>
+      </c>
+      <c r="H308" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="I308" s="6">
+        <f t="shared" si="439"/>
+        <v>2</v>
+      </c>
+      <c r="M308" s="6">
+        <v>67</v>
+      </c>
+      <c r="N308" s="18" t="str">
+        <f t="shared" si="440"/>
+        <v>000001</v>
+      </c>
+      <c r="O308" s="19" t="str">
+        <f t="shared" si="441"/>
+        <v>010</v>
+      </c>
+      <c r="P308" s="19" t="str">
+        <f t="shared" si="442"/>
+        <v/>
+      </c>
+      <c r="Q308" s="19" t="str">
+        <f t="shared" si="443"/>
+        <v/>
+      </c>
+      <c r="R308" s="19" t="str">
+        <f t="shared" si="444"/>
+        <v/>
+      </c>
+      <c r="S308" s="20" t="str">
+        <f t="shared" si="445"/>
+        <v>01000011</v>
+      </c>
+      <c r="T308" s="6" t="str">
+        <f t="shared" si="446"/>
+        <v>05</v>
+      </c>
+      <c r="U308" s="6" t="str">
+        <f t="shared" si="447"/>
+        <v>00</v>
+      </c>
+      <c r="V308" s="21" t="str">
+        <f t="shared" si="448"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="309" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B309" s="6">
+        <v>6</v>
+      </c>
+      <c r="C309" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(B309,3)</f>
+        <v>0x006</v>
+      </c>
+      <c r="D309" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="G309" s="16">
+        <v>1</v>
+      </c>
+      <c r="H309" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="I309" s="6">
+        <f t="shared" ref="I309:I312" si="449">IF(H309="", "", VLOOKUP(H309, $X$3:$Y$10, 2))</f>
+        <v>0</v>
+      </c>
+      <c r="M309" s="6">
+        <v>0</v>
+      </c>
+      <c r="N309" s="18" t="str">
+        <f t="shared" ref="N309:N312" si="450">IF(G309="", "", TEXT(DEC2BIN(G309), "000000"))</f>
+        <v>000001</v>
+      </c>
+      <c r="O309" s="19" t="str">
+        <f t="shared" ref="O309:O312" si="451">IF(I309="", "", TEXT(DEC2BIN(I309), "000"))</f>
+        <v>000</v>
+      </c>
+      <c r="P309" s="19" t="str">
+        <f t="shared" ref="P309:P312" si="452">IF(J309="", "", TEXT(DEC2BIN(J309), "000"))</f>
+        <v/>
+      </c>
+      <c r="Q309" s="19" t="str">
+        <f t="shared" ref="Q309:Q312" si="453">IF(K309="", "", TEXT(DEC2BIN(K309), "000"))</f>
+        <v/>
+      </c>
+      <c r="R309" s="19" t="str">
+        <f t="shared" ref="R309:R312" si="454">IF(L309="", "", TEXT(DEC2BIN(L309), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="S309" s="20" t="str">
+        <f t="shared" ref="S309:S312" si="455">IF(M309="", "", TEXT(DEC2BIN(M309), "00000000"))</f>
+        <v>00000000</v>
+      </c>
+      <c r="T309" s="6" t="str">
+        <f t="shared" ref="T309:T312" si="456">BIN2HEX(LEFT(CONCATENATE(N309,IF(O309="", "000", O309)), 8), 2)</f>
+        <v>04</v>
+      </c>
+      <c r="U309" s="6" t="str">
+        <f t="shared" ref="U309:U312" si="457">BIN2HEX(CONCATENATE(RIGHT(O309, 1), IF(P309 = "", "000", P309), IF(Q309 = "", "000", Q309), "0"), 2)</f>
+        <v>00</v>
+      </c>
+      <c r="V309" s="21" t="str">
+        <f t="shared" ref="V309:V312" si="458">IF(R309="", BIN2HEX(S309, 2), BIN2HEX(R309,2))</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="310" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B310" s="6">
+        <v>9</v>
+      </c>
+      <c r="C310" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(B310,3)</f>
+        <v>0x009</v>
+      </c>
+      <c r="D310" s="27" t="s">
+        <v>380</v>
+      </c>
+      <c r="G310" s="16">
+        <v>1</v>
+      </c>
+      <c r="H310" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="I310" s="6">
+        <f t="shared" si="449"/>
+        <v>4</v>
+      </c>
+      <c r="M310" s="6">
+        <v>5</v>
+      </c>
+      <c r="N310" s="18" t="str">
+        <f t="shared" si="450"/>
+        <v>000001</v>
+      </c>
+      <c r="O310" s="19" t="str">
+        <f t="shared" si="451"/>
+        <v>100</v>
+      </c>
+      <c r="P310" s="19" t="str">
+        <f t="shared" si="452"/>
+        <v/>
+      </c>
+      <c r="Q310" s="19" t="str">
+        <f t="shared" si="453"/>
+        <v/>
+      </c>
+      <c r="R310" s="19" t="str">
+        <f t="shared" si="454"/>
+        <v/>
+      </c>
+      <c r="S310" s="20" t="str">
+        <f t="shared" si="455"/>
+        <v>00000101</v>
+      </c>
+      <c r="T310" s="6" t="str">
+        <f t="shared" si="456"/>
+        <v>06</v>
+      </c>
+      <c r="U310" s="6" t="str">
+        <f t="shared" si="457"/>
+        <v>00</v>
+      </c>
+      <c r="V310" s="21" t="str">
+        <f t="shared" si="458"/>
+        <v>05</v>
+      </c>
+    </row>
+    <row r="311" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A311" s="14" t="s">
+        <v>283</v>
+      </c>
+      <c r="B311" s="6">
+        <v>12</v>
+      </c>
+      <c r="C311" s="6" t="str">
+        <f t="shared" ref="C311:C319" si="459">"0x" &amp; DEC2HEX(B311,3)</f>
+        <v>0x00C</v>
+      </c>
+      <c r="D311" s="27" t="s">
+        <v>370</v>
+      </c>
+      <c r="G311" s="16">
+        <v>2</v>
+      </c>
+      <c r="H311" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="I311" s="6">
+        <f t="shared" si="449"/>
+        <v>7</v>
+      </c>
+      <c r="J311" s="6">
+        <v>0</v>
+      </c>
+      <c r="N311" s="18" t="str">
+        <f t="shared" si="450"/>
+        <v>000010</v>
+      </c>
+      <c r="O311" s="19" t="str">
+        <f t="shared" si="451"/>
+        <v>111</v>
+      </c>
+      <c r="P311" s="19" t="str">
+        <f t="shared" si="452"/>
+        <v>000</v>
+      </c>
+      <c r="Q311" s="19" t="str">
+        <f t="shared" si="453"/>
+        <v/>
+      </c>
+      <c r="R311" s="19" t="str">
+        <f t="shared" si="454"/>
+        <v/>
+      </c>
+      <c r="S311" s="20" t="str">
+        <f t="shared" si="455"/>
+        <v/>
+      </c>
+      <c r="T311" s="6" t="str">
+        <f t="shared" si="456"/>
+        <v>0B</v>
+      </c>
+      <c r="U311" s="6" t="str">
+        <f t="shared" si="457"/>
+        <v>80</v>
+      </c>
+      <c r="V311" s="21" t="str">
+        <f t="shared" si="458"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="312" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B312" s="6">
+        <v>15</v>
+      </c>
+      <c r="C312" s="6" t="str">
+        <f t="shared" si="459"/>
+        <v>0x00F</v>
+      </c>
+      <c r="D312" s="27" t="s">
+        <v>365</v>
+      </c>
+      <c r="F312" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="G312" s="16">
+        <v>33</v>
+      </c>
+      <c r="H312" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="I312" s="6">
+        <f t="shared" si="449"/>
+        <v>0</v>
+      </c>
+      <c r="J312" s="6">
+        <v>4</v>
+      </c>
+      <c r="N312" s="18" t="str">
+        <f t="shared" si="450"/>
+        <v>100001</v>
+      </c>
+      <c r="O312" s="19" t="str">
+        <f t="shared" si="451"/>
+        <v>000</v>
+      </c>
+      <c r="P312" s="19" t="str">
+        <f t="shared" si="452"/>
+        <v>100</v>
+      </c>
+      <c r="Q312" s="19" t="str">
+        <f t="shared" si="453"/>
+        <v/>
+      </c>
+      <c r="R312" s="19" t="str">
+        <f t="shared" si="454"/>
+        <v/>
+      </c>
+      <c r="S312" s="20" t="str">
+        <f t="shared" si="455"/>
+        <v/>
+      </c>
+      <c r="T312" s="6" t="str">
+        <f t="shared" si="456"/>
+        <v>84</v>
+      </c>
+      <c r="U312" s="6" t="str">
+        <f t="shared" si="457"/>
+        <v>40</v>
+      </c>
+      <c r="V312" s="21" t="str">
+        <f t="shared" si="458"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="313" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B313" s="6">
+        <v>18</v>
+      </c>
+      <c r="C313" s="6" t="str">
+        <f t="shared" si="459"/>
+        <v>0x012</v>
+      </c>
+      <c r="D313" s="27" t="s">
         <v>371</v>
       </c>
-      <c r="F307" s="2" t="s">
+      <c r="G313" s="16">
+        <v>2</v>
+      </c>
+      <c r="H313" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="I313" s="6">
+        <f t="shared" ref="I313:I315" si="460">IF(H313="", "", VLOOKUP(H313, $X$3:$Y$10, 2))</f>
+        <v>0</v>
+      </c>
+      <c r="J313" s="6">
+        <v>7</v>
+      </c>
+      <c r="N313" s="18" t="str">
+        <f t="shared" ref="N313:N315" si="461">IF(G313="", "", TEXT(DEC2BIN(G313), "000000"))</f>
+        <v>000010</v>
+      </c>
+      <c r="O313" s="19" t="str">
+        <f t="shared" ref="O313" si="462">IF(I313="", "", TEXT(DEC2BIN(I313), "000"))</f>
+        <v>000</v>
+      </c>
+      <c r="P313" s="19" t="str">
+        <f t="shared" ref="P313:P315" si="463">IF(J313="", "", TEXT(DEC2BIN(J313), "000"))</f>
+        <v>111</v>
+      </c>
+      <c r="Q313" s="19" t="str">
+        <f t="shared" ref="Q313:Q315" si="464">IF(K313="", "", TEXT(DEC2BIN(K313), "000"))</f>
+        <v/>
+      </c>
+      <c r="R313" s="19" t="str">
+        <f t="shared" ref="R313:R315" si="465">IF(L313="", "", TEXT(DEC2BIN(L313), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="S313" s="20" t="str">
+        <f t="shared" ref="S313:S315" si="466">IF(M313="", "", TEXT(DEC2BIN(M313), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="T313" s="6" t="str">
+        <f t="shared" ref="T313:T315" si="467">BIN2HEX(LEFT(CONCATENATE(N313,IF(O313="", "000", O313)), 8), 2)</f>
+        <v>08</v>
+      </c>
+      <c r="U313" s="6" t="str">
+        <f t="shared" ref="U313:U315" si="468">BIN2HEX(CONCATENATE(RIGHT(O313, 1), IF(P313 = "", "000", P313), IF(Q313 = "", "000", Q313), "0"), 2)</f>
+        <v>70</v>
+      </c>
+      <c r="V313" s="21" t="str">
+        <f t="shared" ref="V313:V315" si="469">IF(R313="", BIN2HEX(S313, 2), BIN2HEX(R313,2))</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="314" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B314" s="6">
+        <v>21</v>
+      </c>
+      <c r="C314" s="6" t="str">
+        <f t="shared" si="459"/>
+        <v>0x015</v>
+      </c>
+      <c r="D314" s="27" t="s">
+        <v>378</v>
+      </c>
+      <c r="F314" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="G314" s="16">
+        <v>12</v>
+      </c>
+      <c r="I314" s="6" t="str">
+        <f t="shared" si="460"/>
+        <v/>
+      </c>
+      <c r="L314" s="6">
+        <v>30</v>
+      </c>
+      <c r="N314" s="18" t="str">
+        <f t="shared" si="461"/>
+        <v>001100</v>
+      </c>
+      <c r="O314" s="19" t="str">
+        <f>IF(I314="", "", TEXT(DEC2BIN(I314), "000"))</f>
+        <v/>
+      </c>
+      <c r="P314" s="19" t="str">
+        <f t="shared" si="463"/>
+        <v/>
+      </c>
+      <c r="Q314" s="19" t="str">
+        <f t="shared" si="464"/>
+        <v/>
+      </c>
+      <c r="R314" s="19" t="str">
+        <f t="shared" si="465"/>
+        <v>00011110</v>
+      </c>
+      <c r="S314" s="20" t="str">
+        <f t="shared" si="466"/>
+        <v/>
+      </c>
+      <c r="T314" s="6" t="str">
+        <f t="shared" si="467"/>
+        <v>30</v>
+      </c>
+      <c r="U314" s="6" t="str">
+        <f t="shared" si="468"/>
+        <v>00</v>
+      </c>
+      <c r="V314" s="21" t="str">
+        <f t="shared" si="469"/>
+        <v>1E</v>
+      </c>
+    </row>
+    <row r="315" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B315" s="6">
+        <v>24</v>
+      </c>
+      <c r="C315" s="6" t="str">
+        <f t="shared" si="459"/>
+        <v>0x018</v>
+      </c>
+      <c r="D315" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="F315" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="G315" s="16">
+        <v>17</v>
+      </c>
+      <c r="H315" s="67" t="s">
+        <v>39</v>
+      </c>
+      <c r="I315" s="6">
+        <f t="shared" si="460"/>
+        <v>1</v>
+      </c>
+      <c r="K315" s="6">
+        <v>0</v>
+      </c>
+      <c r="N315" s="18" t="str">
+        <f t="shared" si="461"/>
+        <v>010001</v>
+      </c>
+      <c r="O315" s="19" t="str">
+        <f t="shared" ref="O315" si="470">IF(I315="", "", TEXT(DEC2BIN(I315), "000"))</f>
+        <v>001</v>
+      </c>
+      <c r="P315" s="19" t="str">
+        <f t="shared" si="463"/>
+        <v/>
+      </c>
+      <c r="Q315" s="19" t="str">
+        <f t="shared" si="464"/>
+        <v>000</v>
+      </c>
+      <c r="R315" s="19" t="str">
+        <f t="shared" si="465"/>
+        <v/>
+      </c>
+      <c r="S315" s="20" t="str">
+        <f t="shared" si="466"/>
+        <v/>
+      </c>
+      <c r="T315" s="6" t="str">
+        <f t="shared" si="467"/>
+        <v>44</v>
+      </c>
+      <c r="U315" s="6" t="str">
+        <f t="shared" si="468"/>
+        <v>80</v>
+      </c>
+      <c r="V315" s="21" t="str">
+        <f t="shared" si="469"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="316" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B316" s="6">
+        <v>27</v>
+      </c>
+      <c r="C316" s="6" t="str">
+        <f t="shared" si="459"/>
+        <v>0x01B</v>
+      </c>
+      <c r="D316" s="27" t="s">
+        <v>379</v>
+      </c>
+      <c r="G316" s="16">
+        <v>5</v>
+      </c>
+      <c r="I316" s="6" t="str">
+        <f t="shared" ref="I316" si="471">IF(H316="", "", VLOOKUP(H316, $X$3:$Y$10, 2))</f>
+        <v/>
+      </c>
+      <c r="L316" s="6">
+        <v>33</v>
+      </c>
+      <c r="N316" s="18" t="str">
+        <f t="shared" ref="N316" si="472">IF(G316="", "", TEXT(DEC2BIN(G316), "000000"))</f>
+        <v>000101</v>
+      </c>
+      <c r="O316" s="19" t="str">
+        <f>IF(I316="", "", TEXT(DEC2BIN(I316), "000"))</f>
+        <v/>
+      </c>
+      <c r="P316" s="19" t="str">
+        <f t="shared" ref="P316" si="473">IF(J316="", "", TEXT(DEC2BIN(J316), "000"))</f>
+        <v/>
+      </c>
+      <c r="Q316" s="19" t="str">
+        <f t="shared" ref="Q316" si="474">IF(K316="", "", TEXT(DEC2BIN(K316), "000"))</f>
+        <v/>
+      </c>
+      <c r="R316" s="19" t="str">
+        <f t="shared" ref="R316" si="475">IF(L316="", "", TEXT(DEC2BIN(L316), "00000000"))</f>
+        <v>00100001</v>
+      </c>
+      <c r="S316" s="20" t="str">
+        <f t="shared" ref="S316" si="476">IF(M316="", "", TEXT(DEC2BIN(M316), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="T316" s="6" t="str">
+        <f t="shared" ref="T316" si="477">BIN2HEX(LEFT(CONCATENATE(N316,IF(O316="", "000", O316)), 8), 2)</f>
+        <v>14</v>
+      </c>
+      <c r="U316" s="6" t="str">
+        <f t="shared" ref="U316" si="478">BIN2HEX(CONCATENATE(RIGHT(O316, 1), IF(P316 = "", "000", P316), IF(Q316 = "", "000", Q316), "0"), 2)</f>
+        <v>00</v>
+      </c>
+      <c r="V316" s="21" t="str">
+        <f t="shared" ref="V316" si="479">IF(R316="", BIN2HEX(S316, 2), BIN2HEX(R316,2))</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="317" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A317" s="14" t="s">
+        <v>368</v>
+      </c>
+      <c r="B317" s="6">
+        <v>30</v>
+      </c>
+      <c r="C317" s="6" t="str">
+        <f t="shared" si="459"/>
+        <v>0x01E</v>
+      </c>
+      <c r="D317" s="27" t="s">
+        <v>207</v>
+      </c>
+      <c r="F317" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="G317" s="16">
+        <v>17</v>
+      </c>
+      <c r="H317" s="67" t="s">
+        <v>157</v>
+      </c>
+      <c r="I317" s="6">
+        <f t="shared" ref="I317:I318" si="480">IF(H317="", "", VLOOKUP(H317, $X$3:$Y$10, 2))</f>
+        <v>2</v>
+      </c>
+      <c r="K317" s="6">
+        <v>0</v>
+      </c>
+      <c r="N317" s="18" t="str">
+        <f t="shared" ref="N317:N318" si="481">IF(G317="", "", TEXT(DEC2BIN(G317), "000000"))</f>
+        <v>010001</v>
+      </c>
+      <c r="O317" s="19" t="str">
+        <f t="shared" ref="O317:O318" si="482">IF(I317="", "", TEXT(DEC2BIN(I317), "000"))</f>
+        <v>010</v>
+      </c>
+      <c r="P317" s="19" t="str">
+        <f t="shared" ref="P317:P318" si="483">IF(J317="", "", TEXT(DEC2BIN(J317), "000"))</f>
+        <v/>
+      </c>
+      <c r="Q317" s="19" t="str">
+        <f t="shared" ref="Q317:Q318" si="484">IF(K317="", "", TEXT(DEC2BIN(K317), "000"))</f>
+        <v>000</v>
+      </c>
+      <c r="R317" s="19" t="str">
+        <f t="shared" ref="R317:R318" si="485">IF(L317="", "", TEXT(DEC2BIN(L317), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="S317" s="20" t="str">
+        <f t="shared" ref="S317:S318" si="486">IF(M317="", "", TEXT(DEC2BIN(M317), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="T317" s="6" t="str">
+        <f t="shared" ref="T317:T318" si="487">BIN2HEX(LEFT(CONCATENATE(N317,IF(O317="", "000", O317)), 8), 2)</f>
+        <v>45</v>
+      </c>
+      <c r="U317" s="6" t="str">
+        <f t="shared" ref="U317:U318" si="488">BIN2HEX(CONCATENATE(RIGHT(O317, 1), IF(P317 = "", "000", P317), IF(Q317 = "", "000", Q317), "0"), 2)</f>
+        <v>00</v>
+      </c>
+      <c r="V317" s="21" t="str">
+        <f t="shared" ref="V317:V318" si="489">IF(R317="", BIN2HEX(S317, 2), BIN2HEX(R317,2))</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="318" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A318" s="14" t="s">
+        <v>369</v>
+      </c>
+      <c r="B318" s="6">
+        <v>33</v>
+      </c>
+      <c r="C318" s="6" t="str">
+        <f t="shared" si="459"/>
+        <v>0x021</v>
+      </c>
+      <c r="D318" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="G318" s="16">
+        <v>40</v>
+      </c>
+      <c r="H318" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="I318" s="6">
+        <f t="shared" si="480"/>
+        <v>0</v>
+      </c>
+      <c r="N318" s="18" t="str">
+        <f t="shared" si="481"/>
+        <v>101000</v>
+      </c>
+      <c r="O318" s="19" t="str">
+        <f t="shared" si="482"/>
+        <v>000</v>
+      </c>
+      <c r="P318" s="19" t="str">
+        <f t="shared" si="483"/>
+        <v/>
+      </c>
+      <c r="Q318" s="19" t="str">
+        <f t="shared" si="484"/>
+        <v/>
+      </c>
+      <c r="R318" s="19" t="str">
+        <f t="shared" si="485"/>
+        <v/>
+      </c>
+      <c r="S318" s="20" t="str">
+        <f t="shared" si="486"/>
+        <v/>
+      </c>
+      <c r="T318" s="6" t="str">
+        <f t="shared" si="487"/>
+        <v>A0</v>
+      </c>
+      <c r="U318" s="6" t="str">
+        <f t="shared" si="488"/>
+        <v>00</v>
+      </c>
+      <c r="V318" s="21" t="str">
+        <f t="shared" si="489"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="319" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B319" s="6">
+        <v>36</v>
+      </c>
+      <c r="C319" s="6" t="str">
+        <f t="shared" si="459"/>
+        <v>0x024</v>
+      </c>
+      <c r="D319" s="27" t="s">
+        <v>377</v>
+      </c>
+      <c r="G319" s="16">
+        <v>5</v>
+      </c>
+      <c r="I319" s="6" t="str">
+        <f t="shared" ref="I319" si="490">IF(H319="", "", VLOOKUP(H319, $X$3:$Y$10, 2))</f>
+        <v/>
+      </c>
+      <c r="L319" s="6">
+        <v>12</v>
+      </c>
+      <c r="N319" s="18" t="str">
+        <f t="shared" ref="N319" si="491">IF(G319="", "", TEXT(DEC2BIN(G319), "000000"))</f>
+        <v>000101</v>
+      </c>
+      <c r="O319" s="19" t="str">
+        <f>IF(I319="", "", TEXT(DEC2BIN(I319), "000"))</f>
+        <v/>
+      </c>
+      <c r="P319" s="19" t="str">
+        <f t="shared" ref="P319" si="492">IF(J319="", "", TEXT(DEC2BIN(J319), "000"))</f>
+        <v/>
+      </c>
+      <c r="Q319" s="19" t="str">
+        <f t="shared" ref="Q319" si="493">IF(K319="", "", TEXT(DEC2BIN(K319), "000"))</f>
+        <v/>
+      </c>
+      <c r="R319" s="19" t="str">
+        <f t="shared" ref="R319" si="494">IF(L319="", "", TEXT(DEC2BIN(L319), "00000000"))</f>
+        <v>00001100</v>
+      </c>
+      <c r="S319" s="20" t="str">
+        <f t="shared" ref="S319" si="495">IF(M319="", "", TEXT(DEC2BIN(M319), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="T319" s="6" t="str">
+        <f t="shared" ref="T319" si="496">BIN2HEX(LEFT(CONCATENATE(N319,IF(O319="", "000", O319)), 8), 2)</f>
+        <v>14</v>
+      </c>
+      <c r="U319" s="6" t="str">
+        <f t="shared" ref="U319" si="497">BIN2HEX(CONCATENATE(RIGHT(O319, 1), IF(P319 = "", "000", P319), IF(Q319 = "", "000", Q319), "0"), 2)</f>
+        <v>00</v>
+      </c>
+      <c r="V319" s="21" t="str">
+        <f t="shared" ref="V319" si="498">IF(R319="", BIN2HEX(S319, 2), BIN2HEX(R319,2))</f>
+        <v>0C</v>
+      </c>
+    </row>
+    <row r="320" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F320" s="2" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="321" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F321" s="2" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="324" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D324" s="2" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="325" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B325" s="6">
+        <v>0</v>
+      </c>
+      <c r="C325" s="6" t="str">
+        <f t="shared" ref="C325:C326" si="499">"0x" &amp; DEC2HEX(B325,3)</f>
+        <v>0x000</v>
+      </c>
+      <c r="D325" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="F325" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="G325" s="16">
+        <v>1</v>
+      </c>
+      <c r="H325" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="I325" s="6">
+        <f t="shared" ref="I325:I337" si="500">IF(H325="", "", VLOOKUP(H325, $X$3:$Y$10, 2))</f>
+        <v>1</v>
+      </c>
+      <c r="M325" s="6">
+        <v>65</v>
+      </c>
+      <c r="N325" s="18" t="str">
+        <f t="shared" ref="N325:N337" si="501">IF(G325="", "", TEXT(DEC2BIN(G325), "000000"))</f>
+        <v>000001</v>
+      </c>
+      <c r="O325" s="19" t="str">
+        <f t="shared" ref="O325:O331" si="502">IF(I325="", "", TEXT(DEC2BIN(I325), "000"))</f>
+        <v>001</v>
+      </c>
+      <c r="P325" s="19" t="str">
+        <f t="shared" ref="P325:P337" si="503">IF(J325="", "", TEXT(DEC2BIN(J325), "000"))</f>
+        <v/>
+      </c>
+      <c r="Q325" s="19" t="str">
+        <f t="shared" ref="Q325:Q337" si="504">IF(K325="", "", TEXT(DEC2BIN(K325), "000"))</f>
+        <v/>
+      </c>
+      <c r="R325" s="19" t="str">
+        <f t="shared" ref="R325:R337" si="505">IF(L325="", "", TEXT(DEC2BIN(L325), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="S325" s="20" t="str">
+        <f t="shared" ref="S325:S337" si="506">IF(M325="", "", TEXT(DEC2BIN(M325), "00000000"))</f>
+        <v>01000001</v>
+      </c>
+      <c r="T325" s="6" t="str">
+        <f t="shared" ref="T325:T337" si="507">BIN2HEX(LEFT(CONCATENATE(N325,IF(O325="", "000", O325)), 8), 2)</f>
+        <v>04</v>
+      </c>
+      <c r="U325" s="6" t="str">
+        <f t="shared" ref="U325:U337" si="508">BIN2HEX(CONCATENATE(RIGHT(O325, 1), IF(P325 = "", "000", P325), IF(Q325 = "", "000", Q325), "0"), 2)</f>
+        <v>80</v>
+      </c>
+      <c r="V325" s="21" t="str">
+        <f t="shared" ref="V325:V337" si="509">IF(R325="", BIN2HEX(S325, 2), BIN2HEX(R325,2))</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="326" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B326" s="6">
+        <v>3</v>
+      </c>
+      <c r="C326" s="6" t="str">
+        <f t="shared" si="499"/>
+        <v>0x003</v>
+      </c>
+      <c r="D326" s="27" t="s">
+        <v>373</v>
+      </c>
+      <c r="F326" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="G326" s="16">
+        <v>1</v>
+      </c>
+      <c r="H326" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="I326" s="6">
+        <f t="shared" si="500"/>
+        <v>2</v>
+      </c>
+      <c r="M326" s="6">
+        <v>67</v>
+      </c>
+      <c r="N326" s="18" t="str">
+        <f t="shared" si="501"/>
+        <v>000001</v>
+      </c>
+      <c r="O326" s="19" t="str">
+        <f t="shared" si="502"/>
+        <v>010</v>
+      </c>
+      <c r="P326" s="19" t="str">
+        <f t="shared" si="503"/>
+        <v/>
+      </c>
+      <c r="Q326" s="19" t="str">
+        <f t="shared" si="504"/>
+        <v/>
+      </c>
+      <c r="R326" s="19" t="str">
+        <f t="shared" si="505"/>
+        <v/>
+      </c>
+      <c r="S326" s="20" t="str">
+        <f t="shared" si="506"/>
+        <v>01000011</v>
+      </c>
+      <c r="T326" s="6" t="str">
+        <f t="shared" si="507"/>
+        <v>05</v>
+      </c>
+      <c r="U326" s="6" t="str">
+        <f t="shared" si="508"/>
+        <v>00</v>
+      </c>
+      <c r="V326" s="21" t="str">
+        <f t="shared" si="509"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="327" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B327" s="6">
+        <v>6</v>
+      </c>
+      <c r="C327" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(B327,3)</f>
+        <v>0x006</v>
+      </c>
+      <c r="D327" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="G327" s="16">
+        <v>1</v>
+      </c>
+      <c r="H327" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="I327" s="6">
+        <f t="shared" si="500"/>
+        <v>0</v>
+      </c>
+      <c r="M327" s="6">
+        <v>0</v>
+      </c>
+      <c r="N327" s="18" t="str">
+        <f t="shared" si="501"/>
+        <v>000001</v>
+      </c>
+      <c r="O327" s="19" t="str">
+        <f t="shared" si="502"/>
+        <v>000</v>
+      </c>
+      <c r="P327" s="19" t="str">
+        <f t="shared" si="503"/>
+        <v/>
+      </c>
+      <c r="Q327" s="19" t="str">
+        <f t="shared" si="504"/>
+        <v/>
+      </c>
+      <c r="R327" s="19" t="str">
+        <f t="shared" si="505"/>
+        <v/>
+      </c>
+      <c r="S327" s="20" t="str">
+        <f t="shared" si="506"/>
+        <v>00000000</v>
+      </c>
+      <c r="T327" s="6" t="str">
+        <f t="shared" si="507"/>
+        <v>04</v>
+      </c>
+      <c r="U327" s="6" t="str">
+        <f t="shared" si="508"/>
+        <v>00</v>
+      </c>
+      <c r="V327" s="21" t="str">
+        <f t="shared" si="509"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="328" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B328" s="6">
+        <v>9</v>
+      </c>
+      <c r="C328" s="6" t="str">
+        <f>"0x" &amp; DEC2HEX(B328,3)</f>
+        <v>0x009</v>
+      </c>
+      <c r="D328" s="27" t="s">
+        <v>380</v>
+      </c>
+      <c r="G328" s="16">
+        <v>1</v>
+      </c>
+      <c r="H328" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="I328" s="6">
+        <f t="shared" si="500"/>
+        <v>4</v>
+      </c>
+      <c r="M328" s="6">
+        <v>5</v>
+      </c>
+      <c r="N328" s="18" t="str">
+        <f t="shared" si="501"/>
+        <v>000001</v>
+      </c>
+      <c r="O328" s="19" t="str">
+        <f t="shared" si="502"/>
+        <v>100</v>
+      </c>
+      <c r="P328" s="19" t="str">
+        <f t="shared" si="503"/>
+        <v/>
+      </c>
+      <c r="Q328" s="19" t="str">
+        <f t="shared" si="504"/>
+        <v/>
+      </c>
+      <c r="R328" s="19" t="str">
+        <f t="shared" si="505"/>
+        <v/>
+      </c>
+      <c r="S328" s="20" t="str">
+        <f t="shared" si="506"/>
+        <v>00000101</v>
+      </c>
+      <c r="T328" s="6" t="str">
+        <f t="shared" si="507"/>
+        <v>06</v>
+      </c>
+      <c r="U328" s="6" t="str">
+        <f t="shared" si="508"/>
+        <v>00</v>
+      </c>
+      <c r="V328" s="21" t="str">
+        <f t="shared" si="509"/>
+        <v>05</v>
+      </c>
+    </row>
+    <row r="329" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A329" s="14" t="s">
+        <v>283</v>
+      </c>
+      <c r="B329" s="6">
+        <v>12</v>
+      </c>
+      <c r="C329" s="6" t="str">
+        <f t="shared" ref="C329:C337" si="510">"0x" &amp; DEC2HEX(B329,3)</f>
+        <v>0x00C</v>
+      </c>
+      <c r="D329" s="27" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="308" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D308" s="27" t="s">
+      <c r="G329" s="16">
+        <v>2</v>
+      </c>
+      <c r="H329" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="I329" s="6">
+        <f t="shared" si="500"/>
+        <v>7</v>
+      </c>
+      <c r="J329" s="6">
+        <v>0</v>
+      </c>
+      <c r="N329" s="18" t="str">
+        <f t="shared" si="501"/>
+        <v>000010</v>
+      </c>
+      <c r="O329" s="19" t="str">
+        <f t="shared" si="502"/>
+        <v>111</v>
+      </c>
+      <c r="P329" s="19" t="str">
+        <f t="shared" si="503"/>
+        <v>000</v>
+      </c>
+      <c r="Q329" s="19" t="str">
+        <f t="shared" si="504"/>
+        <v/>
+      </c>
+      <c r="R329" s="19" t="str">
+        <f t="shared" si="505"/>
+        <v/>
+      </c>
+      <c r="S329" s="20" t="str">
+        <f t="shared" si="506"/>
+        <v/>
+      </c>
+      <c r="T329" s="6" t="str">
+        <f t="shared" si="507"/>
+        <v>0B</v>
+      </c>
+      <c r="U329" s="6" t="str">
+        <f t="shared" si="508"/>
+        <v>80</v>
+      </c>
+      <c r="V329" s="21" t="str">
+        <f t="shared" si="509"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="330" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B330" s="6">
+        <v>15</v>
+      </c>
+      <c r="C330" s="6" t="str">
+        <f t="shared" si="510"/>
+        <v>0x00F</v>
+      </c>
+      <c r="D330" s="27" t="s">
+        <v>384</v>
+      </c>
+      <c r="F330" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="G330" s="16">
+        <v>43</v>
+      </c>
+      <c r="H330" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="I330" s="6">
+        <f t="shared" si="500"/>
+        <v>0</v>
+      </c>
+      <c r="J330" s="6">
+        <v>4</v>
+      </c>
+      <c r="N330" s="18" t="str">
+        <f t="shared" si="501"/>
+        <v>101011</v>
+      </c>
+      <c r="O330" s="19" t="str">
+        <f t="shared" si="502"/>
+        <v>000</v>
+      </c>
+      <c r="P330" s="19" t="str">
+        <f t="shared" si="503"/>
+        <v>100</v>
+      </c>
+      <c r="Q330" s="19" t="str">
+        <f t="shared" si="504"/>
+        <v/>
+      </c>
+      <c r="R330" s="19" t="str">
+        <f t="shared" si="505"/>
+        <v/>
+      </c>
+      <c r="S330" s="20" t="str">
+        <f t="shared" si="506"/>
+        <v/>
+      </c>
+      <c r="T330" s="6" t="str">
+        <f t="shared" si="507"/>
+        <v>AC</v>
+      </c>
+      <c r="U330" s="6" t="str">
+        <f t="shared" si="508"/>
+        <v>40</v>
+      </c>
+      <c r="V330" s="21" t="str">
+        <f t="shared" si="509"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="331" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B331" s="6">
+        <v>18</v>
+      </c>
+      <c r="C331" s="6" t="str">
+        <f t="shared" si="510"/>
+        <v>0x012</v>
+      </c>
+      <c r="D331" s="27" t="s">
+        <v>371</v>
+      </c>
+      <c r="G331" s="16">
+        <v>2</v>
+      </c>
+      <c r="H331" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="I331" s="6">
+        <f t="shared" si="500"/>
+        <v>0</v>
+      </c>
+      <c r="J331" s="6">
+        <v>7</v>
+      </c>
+      <c r="N331" s="18" t="str">
+        <f t="shared" si="501"/>
+        <v>000010</v>
+      </c>
+      <c r="O331" s="19" t="str">
+        <f t="shared" si="502"/>
+        <v>000</v>
+      </c>
+      <c r="P331" s="19" t="str">
+        <f t="shared" si="503"/>
+        <v>111</v>
+      </c>
+      <c r="Q331" s="19" t="str">
+        <f t="shared" si="504"/>
+        <v/>
+      </c>
+      <c r="R331" s="19" t="str">
+        <f t="shared" si="505"/>
+        <v/>
+      </c>
+      <c r="S331" s="20" t="str">
+        <f t="shared" si="506"/>
+        <v/>
+      </c>
+      <c r="T331" s="6" t="str">
+        <f t="shared" si="507"/>
+        <v>08</v>
+      </c>
+      <c r="U331" s="6" t="str">
+        <f t="shared" si="508"/>
+        <v>70</v>
+      </c>
+      <c r="V331" s="21" t="str">
+        <f t="shared" si="509"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="332" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B332" s="6">
+        <v>21</v>
+      </c>
+      <c r="C332" s="6" t="str">
+        <f t="shared" si="510"/>
+        <v>0x015</v>
+      </c>
+      <c r="D332" s="27" t="s">
+        <v>378</v>
+      </c>
+      <c r="F332" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="G332" s="16">
+        <v>12</v>
+      </c>
+      <c r="I332" s="6" t="str">
+        <f t="shared" si="500"/>
+        <v/>
+      </c>
+      <c r="L332" s="6">
+        <v>30</v>
+      </c>
+      <c r="N332" s="18" t="str">
+        <f t="shared" si="501"/>
+        <v>001100</v>
+      </c>
+      <c r="O332" s="19" t="str">
+        <f>IF(I332="", "", TEXT(DEC2BIN(I332), "000"))</f>
+        <v/>
+      </c>
+      <c r="P332" s="19" t="str">
+        <f t="shared" si="503"/>
+        <v/>
+      </c>
+      <c r="Q332" s="19" t="str">
+        <f t="shared" si="504"/>
+        <v/>
+      </c>
+      <c r="R332" s="19" t="str">
+        <f t="shared" si="505"/>
+        <v>00011110</v>
+      </c>
+      <c r="S332" s="20" t="str">
+        <f t="shared" si="506"/>
+        <v/>
+      </c>
+      <c r="T332" s="6" t="str">
+        <f t="shared" si="507"/>
+        <v>30</v>
+      </c>
+      <c r="U332" s="6" t="str">
+        <f t="shared" si="508"/>
+        <v>00</v>
+      </c>
+      <c r="V332" s="21" t="str">
+        <f t="shared" si="509"/>
+        <v>1E</v>
+      </c>
+    </row>
+    <row r="333" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B333" s="6">
+        <v>24</v>
+      </c>
+      <c r="C333" s="6" t="str">
+        <f t="shared" si="510"/>
+        <v>0x018</v>
+      </c>
+      <c r="D333" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="F333" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="G333" s="16">
+        <v>17</v>
+      </c>
+      <c r="H333" s="67" t="s">
+        <v>39</v>
+      </c>
+      <c r="I333" s="6">
+        <f t="shared" si="500"/>
+        <v>1</v>
+      </c>
+      <c r="K333" s="6">
+        <v>0</v>
+      </c>
+      <c r="N333" s="18" t="str">
+        <f t="shared" si="501"/>
+        <v>010001</v>
+      </c>
+      <c r="O333" s="19" t="str">
+        <f t="shared" ref="O333" si="511">IF(I333="", "", TEXT(DEC2BIN(I333), "000"))</f>
+        <v>001</v>
+      </c>
+      <c r="P333" s="19" t="str">
+        <f t="shared" si="503"/>
+        <v/>
+      </c>
+      <c r="Q333" s="19" t="str">
+        <f t="shared" si="504"/>
+        <v>000</v>
+      </c>
+      <c r="R333" s="19" t="str">
+        <f t="shared" si="505"/>
+        <v/>
+      </c>
+      <c r="S333" s="20" t="str">
+        <f t="shared" si="506"/>
+        <v/>
+      </c>
+      <c r="T333" s="6" t="str">
+        <f t="shared" si="507"/>
+        <v>44</v>
+      </c>
+      <c r="U333" s="6" t="str">
+        <f t="shared" si="508"/>
+        <v>80</v>
+      </c>
+      <c r="V333" s="21" t="str">
+        <f t="shared" si="509"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="334" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B334" s="6">
+        <v>27</v>
+      </c>
+      <c r="C334" s="6" t="str">
+        <f t="shared" si="510"/>
+        <v>0x01B</v>
+      </c>
+      <c r="D334" s="27" t="s">
+        <v>379</v>
+      </c>
+      <c r="G334" s="16">
+        <v>5</v>
+      </c>
+      <c r="I334" s="6" t="str">
+        <f t="shared" si="500"/>
+        <v/>
+      </c>
+      <c r="L334" s="6">
+        <v>33</v>
+      </c>
+      <c r="N334" s="18" t="str">
+        <f t="shared" si="501"/>
+        <v>000101</v>
+      </c>
+      <c r="O334" s="19" t="str">
+        <f>IF(I334="", "", TEXT(DEC2BIN(I334), "000"))</f>
+        <v/>
+      </c>
+      <c r="P334" s="19" t="str">
+        <f t="shared" si="503"/>
+        <v/>
+      </c>
+      <c r="Q334" s="19" t="str">
+        <f t="shared" si="504"/>
+        <v/>
+      </c>
+      <c r="R334" s="19" t="str">
+        <f t="shared" si="505"/>
+        <v>00100001</v>
+      </c>
+      <c r="S334" s="20" t="str">
+        <f t="shared" si="506"/>
+        <v/>
+      </c>
+      <c r="T334" s="6" t="str">
+        <f t="shared" si="507"/>
+        <v>14</v>
+      </c>
+      <c r="U334" s="6" t="str">
+        <f t="shared" si="508"/>
+        <v>00</v>
+      </c>
+      <c r="V334" s="21" t="str">
+        <f t="shared" si="509"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="335" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A335" s="14" t="s">
+        <v>368</v>
+      </c>
+      <c r="B335" s="6">
+        <v>30</v>
+      </c>
+      <c r="C335" s="6" t="str">
+        <f t="shared" si="510"/>
+        <v>0x01E</v>
+      </c>
+      <c r="D335" s="27" t="s">
+        <v>207</v>
+      </c>
+      <c r="F335" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="G335" s="16">
+        <v>17</v>
+      </c>
+      <c r="H335" s="67" t="s">
+        <v>157</v>
+      </c>
+      <c r="I335" s="6">
+        <f t="shared" si="500"/>
+        <v>2</v>
+      </c>
+      <c r="K335" s="6">
+        <v>0</v>
+      </c>
+      <c r="N335" s="18" t="str">
+        <f t="shared" si="501"/>
+        <v>010001</v>
+      </c>
+      <c r="O335" s="19" t="str">
+        <f t="shared" ref="O335:O336" si="512">IF(I335="", "", TEXT(DEC2BIN(I335), "000"))</f>
+        <v>010</v>
+      </c>
+      <c r="P335" s="19" t="str">
+        <f t="shared" si="503"/>
+        <v/>
+      </c>
+      <c r="Q335" s="19" t="str">
+        <f t="shared" si="504"/>
+        <v>000</v>
+      </c>
+      <c r="R335" s="19" t="str">
+        <f t="shared" si="505"/>
+        <v/>
+      </c>
+      <c r="S335" s="20" t="str">
+        <f t="shared" si="506"/>
+        <v/>
+      </c>
+      <c r="T335" s="6" t="str">
+        <f t="shared" si="507"/>
+        <v>45</v>
+      </c>
+      <c r="U335" s="6" t="str">
+        <f t="shared" si="508"/>
+        <v>00</v>
+      </c>
+      <c r="V335" s="21" t="str">
+        <f t="shared" si="509"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="336" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A336" s="14" t="s">
+        <v>369</v>
+      </c>
+      <c r="B336" s="6">
+        <v>33</v>
+      </c>
+      <c r="C336" s="6" t="str">
+        <f t="shared" si="510"/>
+        <v>0x021</v>
+      </c>
+      <c r="D336" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="G336" s="16">
+        <v>40</v>
+      </c>
+      <c r="H336" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="I336" s="6">
+        <f t="shared" si="500"/>
+        <v>0</v>
+      </c>
+      <c r="N336" s="18" t="str">
+        <f t="shared" si="501"/>
+        <v>101000</v>
+      </c>
+      <c r="O336" s="19" t="str">
+        <f t="shared" si="512"/>
+        <v>000</v>
+      </c>
+      <c r="P336" s="19" t="str">
+        <f t="shared" si="503"/>
+        <v/>
+      </c>
+      <c r="Q336" s="19" t="str">
+        <f t="shared" si="504"/>
+        <v/>
+      </c>
+      <c r="R336" s="19" t="str">
+        <f t="shared" si="505"/>
+        <v/>
+      </c>
+      <c r="S336" s="20" t="str">
+        <f t="shared" si="506"/>
+        <v/>
+      </c>
+      <c r="T336" s="6" t="str">
+        <f t="shared" si="507"/>
+        <v>A0</v>
+      </c>
+      <c r="U336" s="6" t="str">
+        <f t="shared" si="508"/>
+        <v>00</v>
+      </c>
+      <c r="V336" s="21" t="str">
+        <f t="shared" si="509"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="337" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B337" s="6">
+        <v>36</v>
+      </c>
+      <c r="C337" s="6" t="str">
+        <f t="shared" si="510"/>
+        <v>0x024</v>
+      </c>
+      <c r="D337" s="27" t="s">
+        <v>377</v>
+      </c>
+      <c r="G337" s="16">
+        <v>5</v>
+      </c>
+      <c r="I337" s="6" t="str">
+        <f t="shared" si="500"/>
+        <v/>
+      </c>
+      <c r="L337" s="6">
+        <v>12</v>
+      </c>
+      <c r="N337" s="18" t="str">
+        <f t="shared" si="501"/>
+        <v>000101</v>
+      </c>
+      <c r="O337" s="19" t="str">
+        <f>IF(I337="", "", TEXT(DEC2BIN(I337), "000"))</f>
+        <v/>
+      </c>
+      <c r="P337" s="19" t="str">
+        <f t="shared" si="503"/>
+        <v/>
+      </c>
+      <c r="Q337" s="19" t="str">
+        <f t="shared" si="504"/>
+        <v/>
+      </c>
+      <c r="R337" s="19" t="str">
+        <f t="shared" si="505"/>
+        <v>00001100</v>
+      </c>
+      <c r="S337" s="20" t="str">
+        <f t="shared" si="506"/>
+        <v/>
+      </c>
+      <c r="T337" s="6" t="str">
+        <f t="shared" si="507"/>
+        <v>14</v>
+      </c>
+      <c r="U337" s="6" t="str">
+        <f t="shared" si="508"/>
+        <v>00</v>
+      </c>
+      <c r="V337" s="21" t="str">
+        <f t="shared" si="509"/>
+        <v>0C</v>
+      </c>
+    </row>
+    <row r="338" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="F338" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="F308" s="2" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="309" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D309" s="27" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="310" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D310" s="27" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="311" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D311" s="27" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="312" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D312" s="27" t="s">
-        <v>349</v>
-      </c>
-      <c r="F312" s="2" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="313" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D313" s="27" t="s">
-        <v>107</v>
-      </c>
-      <c r="F313" s="2" t="s">
-        <v>362</v>
+    </row>
+    <row r="339" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="F339" s="2" t="s">
+        <v>386</v>
       </c>
     </row>
   </sheetData>
@@ -17305,7 +18988,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z17">
       <formula1>$X$16:$X$18</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H6 H9:H11 H201:H224 H141:H149 H102:H112 H117:H132 H83:H93 H49 H41:H42 H31:H33 H17:H26 H229:H242 H154:H174 H276 H247:H273 H282:H283 H278:H280 H293:H294 H288:H291 H299:H302">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H6 H9:H11 H201:H224 H141:H149 H102:H112 H117:H132 H83:H93 H49 H41:H42 H31:H33 H17:H26 H229:H242 H154:H174 H276 H247:H273 H282:H283 H278:H280 H293:H294 H288:H291 H299:H302 H307:H319 H325:H337">
       <formula1>$X$3:$X$10</formula1>
     </dataValidation>
   </dataValidations>
@@ -18012,8 +19695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:L29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18024,58 +19707,58 @@
   </cols>
   <sheetData>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="J6" s="62" t="s">
+      <c r="J6" s="58" t="s">
+        <v>356</v>
+      </c>
+      <c r="K6" s="59" t="s">
+        <v>355</v>
+      </c>
+      <c r="L6" s="59" t="s">
         <v>357</v>
       </c>
-      <c r="K6" s="63" t="s">
-        <v>356</v>
-      </c>
-      <c r="L6" s="63" t="s">
-        <v>358</v>
-      </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="J7" s="64" t="s">
+      <c r="J7" s="60" t="s">
+        <v>352</v>
+      </c>
+      <c r="K7" s="61" t="s">
+        <v>157</v>
+      </c>
+      <c r="L7" s="61" t="s">
         <v>353</v>
       </c>
-      <c r="K7" s="65" t="s">
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J8" s="60" t="s">
+        <v>349</v>
+      </c>
+      <c r="K8" s="61" t="s">
         <v>157</v>
       </c>
-      <c r="L7" s="65" t="s">
+      <c r="L8" s="61" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="J8" s="64" t="s">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J9" s="60" t="s">
+        <v>352</v>
+      </c>
+      <c r="K9" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="L9" s="61" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J10" s="60" t="s">
+        <v>349</v>
+      </c>
+      <c r="K10" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="L10" s="61" t="s">
         <v>350</v>
-      </c>
-      <c r="K8" s="65" t="s">
-        <v>157</v>
-      </c>
-      <c r="L8" s="65" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="J9" s="64" t="s">
-        <v>353</v>
-      </c>
-      <c r="K9" s="65" t="s">
-        <v>176</v>
-      </c>
-      <c r="L9" s="65" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="J10" s="64" t="s">
-        <v>350</v>
-      </c>
-      <c r="K10" s="65" t="s">
-        <v>176</v>
-      </c>
-      <c r="L10" s="65" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
@@ -18085,23 +19768,23 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C18" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C20" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -18111,23 +19794,23 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C27" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C29" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v.0.18.2 SHL instr (finally) implemented
</commit_message>
<xml_diff>
--- a/2nd gen - 8 bit cpu/Instruction control lines.xlsx
+++ b/2nd gen - 8 bit cpu/Instruction control lines.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="345" windowWidth="14805" windowHeight="7770" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="348" windowWidth="14808" windowHeight="7776" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Control Lines" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Animations" sheetId="4" r:id="rId3"/>
     <sheet name="Magnitude comparison instr" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
@@ -20,10 +20,10 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="C20" authorId="0">
+    <comment ref="C20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -41,7 +41,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C46" authorId="0">
+    <comment ref="C46" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -65,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C47" authorId="0">
+    <comment ref="C47" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -90,7 +90,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C48" authorId="0">
+    <comment ref="C48" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -99,7 +99,9 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Shift Left (multiply by 2)</t>
+          <t xml:space="preserve">Shift Left (multiply by 2)
+74181 operation: A PLUS A
+</t>
         </r>
       </text>
     </comment>
@@ -110,10 +112,10 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="I1" authorId="0">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -149,7 +151,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="398">
   <si>
     <t>LD R1, data</t>
   </si>
@@ -1319,12 +1321,36 @@
   </si>
   <si>
     <t>Read byte from input selected by ID_addr, and write it to R1</t>
+  </si>
+  <si>
+    <t>SHR R1</t>
+  </si>
+  <si>
+    <t>// 21 - Shift Left test</t>
+  </si>
+  <si>
+    <t>LD A, 0x1</t>
+  </si>
+  <si>
+    <t>LD C, 0x0</t>
+  </si>
+  <si>
+    <t>LD D, 0x8</t>
+  </si>
+  <si>
+    <t>OUT 1, A, D</t>
+  </si>
+  <si>
+    <t>SHL A</t>
+  </si>
+  <si>
+    <t>JP Z, 0x0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1595,7 +1621,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1735,6 +1761,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1772,7 +1804,7 @@
         <xdr:cNvPr id="2" name="Imagem 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1800,9 +1832,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1840,9 +1872,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1875,9 +1907,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1910,9 +1959,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2086,25 +2152,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO58"/>
+  <dimension ref="A1:AO59"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AG20" sqref="AG20"/>
+      <pane ySplit="2" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" style="29" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" style="29" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" style="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="28" width="3.28515625" style="31" customWidth="1"/>
-    <col min="29" max="29" width="5.85546875" style="61" customWidth="1"/>
-    <col min="30" max="32" width="5.85546875" style="31" customWidth="1"/>
-    <col min="33" max="16384" width="8.85546875" style="31"/>
+    <col min="1" max="1" width="7.88671875" style="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.88671875" style="29" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" style="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="28" width="3.33203125" style="31" customWidth="1"/>
+    <col min="29" max="29" width="5.88671875" style="61" customWidth="1"/>
+    <col min="30" max="32" width="5.88671875" style="31" customWidth="1"/>
+    <col min="33" max="16384" width="8.88671875" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.3">
       <c r="D1" s="31">
         <v>24</v>
       </c>
@@ -2181,7 +2247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:40" s="30" customFormat="1" ht="130.9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:40" s="30" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
         <v>160</v>
       </c>
@@ -2273,7 +2339,7 @@
       <c r="AE2" s="66"/>
       <c r="AF2" s="67"/>
     </row>
-    <row r="3" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A3" s="29">
         <v>0</v>
       </c>
@@ -2380,7 +2446,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="4" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A4" s="29">
         <v>1</v>
       </c>
@@ -2487,7 +2553,7 @@
         <v>C00000</v>
       </c>
     </row>
-    <row r="5" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A5" s="29">
         <v>2</v>
       </c>
@@ -2594,7 +2660,7 @@
         <v>600400</v>
       </c>
     </row>
-    <row r="6" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A6" s="29">
         <v>3</v>
       </c>
@@ -2701,7 +2767,7 @@
         <v>5E0000</v>
       </c>
     </row>
-    <row r="7" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A7" s="29">
         <v>4</v>
       </c>
@@ -2808,7 +2874,7 @@
         <v>4F0000</v>
       </c>
     </row>
-    <row r="8" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A8" s="29">
         <v>5</v>
       </c>
@@ -2915,7 +2981,7 @@
         <v>004000</v>
       </c>
     </row>
-    <row r="9" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A9" s="29">
         <v>6</v>
       </c>
@@ -3022,7 +3088,7 @@
         <v>006000</v>
       </c>
     </row>
-    <row r="10" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A10" s="29">
         <v>7</v>
       </c>
@@ -3129,7 +3195,7 @@
         <v>004200</v>
       </c>
     </row>
-    <row r="11" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A11" s="29">
         <v>8</v>
       </c>
@@ -3236,7 +3302,7 @@
         <v>006200</v>
       </c>
     </row>
-    <row r="12" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A12" s="29">
         <v>9</v>
       </c>
@@ -3343,7 +3409,7 @@
         <v>000100</v>
       </c>
     </row>
-    <row r="13" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A13" s="29">
         <v>10</v>
       </c>
@@ -3453,7 +3519,7 @@
         <v>181800</v>
       </c>
     </row>
-    <row r="14" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A14" s="29">
         <v>11</v>
       </c>
@@ -3560,7 +3626,7 @@
         <v>091800</v>
       </c>
     </row>
-    <row r="15" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A15" s="29">
         <v>12</v>
       </c>
@@ -3668,7 +3734,7 @@
         <v>004040</v>
       </c>
     </row>
-    <row r="16" spans="1:40" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A16" s="29">
         <v>13</v>
       </c>
@@ -3776,7 +3842,7 @@
         <v>004240</v>
       </c>
     </row>
-    <row r="17" spans="1:41" s="40" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:41" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="45">
         <v>14</v>
       </c>
@@ -3827,7 +3893,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="18" spans="1:41" s="40" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:41" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="45">
         <v>15</v>
       </c>
@@ -3878,7 +3944,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A19" s="29">
         <v>16</v>
       </c>
@@ -3977,7 +4043,7 @@
       </c>
       <c r="AO19" s="50"/>
     </row>
-    <row r="20" spans="1:41" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A20" s="29">
         <v>17</v>
       </c>
@@ -4085,7 +4151,7 @@
       </c>
       <c r="AO20" s="50"/>
     </row>
-    <row r="21" spans="1:41" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="29">
         <v>18</v>
       </c>
@@ -4118,7 +4184,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="22" spans="1:41" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="29">
         <v>19</v>
       </c>
@@ -4151,7 +4217,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="23" spans="1:41" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="29">
         <v>20</v>
       </c>
@@ -4184,7 +4250,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="24" spans="1:41" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="29">
         <v>21</v>
       </c>
@@ -4217,7 +4283,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="25" spans="1:41" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="29">
         <v>22</v>
       </c>
@@ -4250,7 +4316,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="26" spans="1:41" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="29">
         <v>23</v>
       </c>
@@ -4283,7 +4349,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="27" spans="1:41" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="29">
         <v>24</v>
       </c>
@@ -4316,7 +4382,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="28" spans="1:41" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="29">
         <v>25</v>
       </c>
@@ -4349,7 +4415,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="29" spans="1:41" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="29">
         <v>26</v>
       </c>
@@ -4382,7 +4448,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="30" spans="1:41" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="29">
         <v>27</v>
       </c>
@@ -4415,7 +4481,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="31" spans="1:41" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="29">
         <v>28</v>
       </c>
@@ -4448,7 +4514,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="32" spans="1:41" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="29">
         <v>29</v>
       </c>
@@ -4481,7 +4547,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="33" spans="1:41" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="29">
         <v>30</v>
       </c>
@@ -4514,7 +4580,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="34" spans="1:41" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="29">
         <v>31</v>
       </c>
@@ -4547,7 +4613,7 @@
         <v>000000</v>
       </c>
     </row>
-    <row r="35" spans="1:41" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:41" x14ac:dyDescent="0.3">
       <c r="C35" s="51"/>
       <c r="W35" s="41"/>
       <c r="X35" s="29"/>
@@ -4561,7 +4627,7 @@
       <c r="AF35" s="43"/>
       <c r="AN35" s="40"/>
     </row>
-    <row r="36" spans="1:41" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A36" s="29">
         <v>32</v>
       </c>
@@ -4671,7 +4737,7 @@
         <v>408825</v>
       </c>
     </row>
-    <row r="37" spans="1:41" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A37" s="29">
         <v>33</v>
       </c>
@@ -4781,7 +4847,7 @@
         <v>408818</v>
       </c>
     </row>
-    <row r="38" spans="1:41" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A38" s="29">
         <v>34</v>
       </c>
@@ -4891,7 +4957,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="39" spans="1:41" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A39" s="29">
         <v>35</v>
       </c>
@@ -4998,7 +5064,7 @@
         <v>40882E</v>
       </c>
     </row>
-    <row r="40" spans="1:41" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A40" s="29">
         <v>36</v>
       </c>
@@ -5105,7 +5171,7 @@
         <v>40883A</v>
       </c>
     </row>
-    <row r="41" spans="1:41" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A41" s="29">
         <v>37</v>
       </c>
@@ -5212,7 +5278,7 @@
         <v>40881A</v>
       </c>
     </row>
-    <row r="42" spans="1:41" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A42" s="29">
         <v>38</v>
       </c>
@@ -5319,7 +5385,7 @@
         <v>408806</v>
       </c>
     </row>
-    <row r="43" spans="1:41" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A43" s="29">
         <v>39</v>
       </c>
@@ -5426,7 +5492,7 @@
         <v>408826</v>
       </c>
     </row>
-    <row r="44" spans="1:41" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A44" s="29">
         <v>40</v>
       </c>
@@ -5533,7 +5599,7 @@
         <v>408800</v>
       </c>
     </row>
-    <row r="45" spans="1:41" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A45" s="29">
         <v>41</v>
       </c>
@@ -5640,7 +5706,7 @@
         <v>40883D</v>
       </c>
     </row>
-    <row r="46" spans="1:41" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A46" s="29">
         <v>42</v>
       </c>
@@ -5747,12 +5813,12 @@
         <v>408801</v>
       </c>
     </row>
-    <row r="47" spans="1:41" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A47" s="29">
         <v>43</v>
       </c>
       <c r="B47" s="29" t="str">
-        <f t="shared" ref="B47" si="30">"0x" &amp; DEC2HEX(A47)</f>
+        <f t="shared" ref="B47:B48" si="30">"0x" &amp; DEC2HEX(A47)</f>
         <v>0x2B</v>
       </c>
       <c r="C47" s="37" t="s">
@@ -5854,107 +5920,215 @@
         <v>408819</v>
       </c>
     </row>
-    <row r="48" spans="1:41" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A48" s="29">
+        <v>44</v>
+      </c>
+      <c r="B48" s="29" t="str">
+        <f t="shared" si="30"/>
+        <v>0x2C</v>
+      </c>
       <c r="C48" s="9" t="s">
         <v>369</v>
       </c>
-      <c r="D48" s="52"/>
-      <c r="E48" s="52"/>
-      <c r="F48" s="52"/>
-      <c r="G48" s="52"/>
-      <c r="H48" s="52"/>
-      <c r="I48" s="52"/>
-      <c r="J48" s="52"/>
-      <c r="K48" s="52"/>
-      <c r="L48" s="52"/>
-      <c r="M48" s="52"/>
-      <c r="N48" s="52"/>
-      <c r="O48" s="52"/>
-      <c r="P48" s="52"/>
-      <c r="Q48" s="52"/>
-      <c r="R48" s="52"/>
-      <c r="S48" s="52"/>
-      <c r="T48" s="52"/>
-      <c r="U48" s="52"/>
-      <c r="V48" s="52"/>
-      <c r="W48" s="60"/>
-      <c r="X48" s="29"/>
-      <c r="Y48" s="29"/>
-      <c r="Z48" s="29"/>
-      <c r="AA48" s="29"/>
-      <c r="AB48" s="29"/>
-      <c r="AD48" s="42"/>
-      <c r="AE48" s="42"/>
-      <c r="AF48" s="42"/>
+      <c r="D48" s="52">
+        <v>0</v>
+      </c>
+      <c r="E48" s="52">
+        <v>0</v>
+      </c>
+      <c r="F48" s="52">
+        <v>1</v>
+      </c>
+      <c r="G48" s="52">
+        <v>0</v>
+      </c>
+      <c r="H48" s="52">
+        <v>0</v>
+      </c>
+      <c r="I48" s="52">
+        <v>0</v>
+      </c>
+      <c r="J48" s="52" t="s">
+        <v>14</v>
+      </c>
+      <c r="K48" s="52">
+        <v>0</v>
+      </c>
+      <c r="L48" s="52">
+        <v>0</v>
+      </c>
+      <c r="M48" s="52">
+        <v>1</v>
+      </c>
+      <c r="N48" s="52">
+        <v>0</v>
+      </c>
+      <c r="O48" s="52">
+        <v>0</v>
+      </c>
+      <c r="P48" s="52">
+        <v>0</v>
+      </c>
+      <c r="Q48" s="52">
+        <v>1</v>
+      </c>
+      <c r="R48" s="52">
+        <v>0</v>
+      </c>
+      <c r="S48" s="52">
+        <v>0</v>
+      </c>
+      <c r="T48" s="52">
+        <v>0</v>
+      </c>
+      <c r="U48" s="52">
+        <v>0</v>
+      </c>
+      <c r="V48" s="52">
+        <v>0</v>
+      </c>
+      <c r="W48" s="60">
+        <v>1</v>
+      </c>
+      <c r="X48" s="29">
+        <v>1</v>
+      </c>
+      <c r="Y48" s="29">
+        <v>0</v>
+      </c>
+      <c r="Z48" s="29">
+        <v>0</v>
+      </c>
+      <c r="AA48" s="29">
+        <v>0</v>
+      </c>
+      <c r="AB48" s="29">
+        <v>1</v>
+      </c>
+      <c r="AC48" s="62" t="str">
+        <f t="shared" ref="AC48" si="31">BIN2HEX("0000000"+D48, 2)</f>
+        <v>00</v>
+      </c>
+      <c r="AD48" s="42" t="str">
+        <f t="shared" ref="AD48" si="32">BIN2HEX(IF(E48="x", 0, E48) &amp; IF(F48="x", 0, F48) &amp; IF(G48="x", 0, G48) &amp; IF(H48="x", 0, H48) &amp; IF(I48="x", 0, I48) &amp; IF(J48="x", 0, J48) &amp; IF(K48="x", 0, K48) &amp; IF(L48="x", 0, L48), 2)</f>
+        <v>40</v>
+      </c>
+      <c r="AE48" s="42" t="str">
+        <f t="shared" ref="AE48" si="33">BIN2HEX(IF(M48="x", 0, M48) &amp; IF(N48="x", 0, N48) &amp; IF(O48="x", 0, O48) &amp; IF(P48="x", 0, P48) &amp;  IF(Q48="x", 0, Q48) &amp; IF(R48="x", 0, R48) &amp; IF(S48="x", 0, S48) &amp; IF(T48="x", 0, T48), 2)</f>
+        <v>88</v>
+      </c>
+      <c r="AF48" s="43" t="str">
+        <f t="shared" ref="AF48" si="34">BIN2HEX(IF(U48="x", 0, U48) &amp; IF(V48="x", 0, V48) &amp; IF(W48="x", 0, W48) &amp; IF(X48="x", 0, X48) &amp; IF(Y48="x", 0, Y48) &amp; IF(Z48="x", 0, Z48) &amp; IF(AA48="x", 0, AA48) &amp; IF(AB48="x", 0, AB48), 2)</f>
+        <v>31</v>
+      </c>
       <c r="AN48" s="40"/>
     </row>
-    <row r="50" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="C50" s="53" t="s">
+    <row r="49" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="C49" s="9" t="s">
+        <v>390</v>
+      </c>
+      <c r="D49" s="52"/>
+      <c r="E49" s="52"/>
+      <c r="F49" s="52"/>
+      <c r="G49" s="52"/>
+      <c r="H49" s="52"/>
+      <c r="I49" s="52"/>
+      <c r="J49" s="52"/>
+      <c r="K49" s="52"/>
+      <c r="L49" s="52"/>
+      <c r="M49" s="52"/>
+      <c r="N49" s="52"/>
+      <c r="O49" s="52"/>
+      <c r="P49" s="52"/>
+      <c r="Q49" s="52"/>
+      <c r="R49" s="52"/>
+      <c r="S49" s="52"/>
+      <c r="T49" s="52"/>
+      <c r="U49" s="52"/>
+      <c r="V49" s="52"/>
+      <c r="W49" s="60"/>
+      <c r="X49" s="29"/>
+      <c r="Y49" s="29"/>
+      <c r="Z49" s="29"/>
+      <c r="AA49" s="29"/>
+      <c r="AB49" s="29"/>
+      <c r="AC49" s="72"/>
+      <c r="AD49" s="42"/>
+      <c r="AE49" s="42"/>
+      <c r="AF49" s="42"/>
+      <c r="AN49" s="40"/>
+    </row>
+    <row r="50" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AC50" s="71"/>
+    </row>
+    <row r="51" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="C51" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="E50" s="31" t="s">
+      <c r="E51" s="31" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="C51" s="50" t="s">
+    <row r="52" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="C52" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="E51" s="31" t="s">
+      <c r="E52" s="31" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="C53" s="30" t="s">
+    <row r="54" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="C54" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="E53" s="31" t="s">
+      <c r="E54" s="31" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="C54" s="30" t="s">
+    <row r="55" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="C55" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="E54" s="31" t="s">
+      <c r="E55" s="31" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="C55" s="30" t="s">
+    <row r="56" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="C56" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="E55" s="31" t="s">
+      <c r="E56" s="31" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A56" s="31"/>
-      <c r="B56" s="31"/>
-      <c r="C56" s="30" t="s">
-        <v>189</v>
-      </c>
-      <c r="E56" s="31" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A57" s="31"/>
       <c r="B57" s="31"/>
       <c r="C57" s="30" t="s">
-        <v>96</v>
+        <v>189</v>
       </c>
       <c r="E57" s="31" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="58" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A58" s="31"/>
       <c r="B58" s="31"/>
       <c r="C58" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="E58" s="31" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="59" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="A59" s="31"/>
+      <c r="B59" s="31"/>
+      <c r="C59" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="E58" s="31" t="s">
+      <c r="E59" s="31" t="s">
         <v>91</v>
       </c>
     </row>
@@ -5970,40 +6144,40 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA357"/>
+  <dimension ref="A1:AA362"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A325" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G352" sqref="G352"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A342" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L357" sqref="L357"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="14" customWidth="1"/>
-    <col min="2" max="2" width="4.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" style="6"/>
+    <col min="1" max="1" width="12.44140625" style="14" customWidth="1"/>
+    <col min="2" max="2" width="4.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="6"/>
     <col min="4" max="4" width="19" style="6" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="78.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="78.5546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" style="16" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="3" style="17" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="3" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="3.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" style="6"/>
-    <col min="14" max="14" width="15.42578125" style="18" customWidth="1"/>
-    <col min="15" max="16" width="9.140625" style="22"/>
-    <col min="17" max="17" width="8.85546875" style="22"/>
-    <col min="18" max="18" width="10.85546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="3.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="3.42578125" style="21" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.85546875" style="6"/>
-    <col min="24" max="24" width="9.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="8.85546875" style="6"/>
+    <col min="11" max="11" width="3.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.88671875" style="6"/>
+    <col min="14" max="14" width="15.44140625" style="18" customWidth="1"/>
+    <col min="15" max="16" width="9.109375" style="22"/>
+    <col min="17" max="17" width="8.88671875" style="22"/>
+    <col min="18" max="18" width="10.88671875" style="22" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="3.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="3.44140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.88671875" style="6"/>
+    <col min="24" max="24" width="9.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>282</v>
       </c>
@@ -6058,7 +6232,7 @@
       <c r="U1" s="69"/>
       <c r="V1" s="70"/>
     </row>
-    <row r="2" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
       <c r="D2" s="15" t="s">
@@ -6072,7 +6246,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="6">
         <v>0</v>
       </c>
@@ -6139,7 +6313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="6">
         <v>3</v>
       </c>
@@ -6209,7 +6383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="6">
         <v>6</v>
       </c>
@@ -6276,7 +6450,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="6">
         <v>9</v>
       </c>
@@ -6340,7 +6514,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O7" s="19"/>
       <c r="P7" s="19"/>
       <c r="Q7" s="19"/>
@@ -6352,7 +6526,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D8" s="15" t="s">
         <v>218</v>
       </c>
@@ -6363,7 +6537,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="6">
         <v>0</v>
       </c>
@@ -6430,7 +6604,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="6">
         <v>3</v>
       </c>
@@ -6494,7 +6668,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="6">
         <v>6</v>
       </c>
@@ -6552,7 +6726,7 @@
         <v>03</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D16" s="15" t="s">
         <v>219</v>
       </c>
@@ -6563,7 +6737,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="2:27" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="6">
         <v>0</v>
       </c>
@@ -6637,7 +6811,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:27" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="6">
         <v>3</v>
       </c>
@@ -6704,7 +6878,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="2:27" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="6">
         <v>6</v>
       </c>
@@ -6762,7 +6936,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="20" spans="2:27" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="6">
         <v>9</v>
       </c>
@@ -6823,7 +6997,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="21" spans="2:27" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="6">
         <v>12</v>
       </c>
@@ -6881,44 +7055,44 @@
         <v>06</v>
       </c>
     </row>
-    <row r="22" spans="2:27" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O22" s="19"/>
       <c r="P22" s="19"/>
       <c r="Q22" s="19"/>
       <c r="R22" s="19"/>
     </row>
-    <row r="23" spans="2:27" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O23" s="19"/>
       <c r="P23" s="19"/>
       <c r="Q23" s="19"/>
       <c r="R23" s="19"/>
     </row>
-    <row r="24" spans="2:27" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O24" s="19"/>
       <c r="P24" s="19"/>
       <c r="Q24" s="19"/>
       <c r="R24" s="19"/>
     </row>
-    <row r="25" spans="2:27" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O25" s="19"/>
       <c r="P25" s="19"/>
       <c r="Q25" s="19"/>
       <c r="R25" s="19"/>
     </row>
-    <row r="26" spans="2:27" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O26" s="19"/>
       <c r="P26" s="19"/>
       <c r="Q26" s="19"/>
       <c r="R26" s="19"/>
     </row>
-    <row r="30" spans="2:27" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
       <c r="D30" s="15" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="31" spans="2:27" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="6">
         <v>0</v>
       </c>
@@ -6979,7 +7153,7 @@
         <v>01</v>
       </c>
     </row>
-    <row r="32" spans="2:27" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="6">
         <v>3</v>
       </c>
@@ -7040,7 +7214,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="6">
         <v>6</v>
       </c>
@@ -7101,7 +7275,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="34" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="6">
         <v>9</v>
       </c>
@@ -7155,7 +7329,7 @@
         <v>0F</v>
       </c>
     </row>
-    <row r="35" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="6">
         <v>12</v>
       </c>
@@ -7209,7 +7383,7 @@
         <v>06</v>
       </c>
     </row>
-    <row r="36" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="6">
         <v>15</v>
       </c>
@@ -7263,12 +7437,12 @@
         <v>0F</v>
       </c>
     </row>
-    <row r="40" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D40" s="15" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="41" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="6">
         <v>0</v>
       </c>
@@ -7329,7 +7503,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="6">
         <v>3</v>
       </c>
@@ -7390,7 +7564,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="6">
         <v>6</v>
       </c>
@@ -7444,7 +7618,7 @@
         <v>06</v>
       </c>
     </row>
-    <row r="44" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="6">
         <v>16</v>
       </c>
@@ -7459,15 +7633,15 @@
         <v>110</v>
       </c>
     </row>
-    <row r="46" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D46" s="23"/>
     </row>
-    <row r="48" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D48" s="15" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="49" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B49" s="6">
         <v>0</v>
       </c>
@@ -7531,7 +7705,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="50" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="6">
         <v>3</v>
       </c>
@@ -7592,18 +7766,18 @@
         <v>00</v>
       </c>
     </row>
-    <row r="51" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O51" s="19"/>
       <c r="P51" s="19"/>
       <c r="Q51" s="19"/>
       <c r="R51" s="19"/>
     </row>
-    <row r="55" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D55" s="15" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="56" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B56" s="6">
         <v>0</v>
       </c>
@@ -7622,7 +7796,7 @@
       </c>
       <c r="G56" s="24"/>
     </row>
-    <row r="57" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B57" s="6">
         <v>3</v>
       </c>
@@ -7637,7 +7811,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="58" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B58" s="6">
         <v>6</v>
       </c>
@@ -7655,7 +7829,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="59" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B59" s="6">
         <v>9</v>
       </c>
@@ -7670,7 +7844,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="60" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B60" s="6">
         <v>12</v>
       </c>
@@ -7688,7 +7862,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="61" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B61" s="6">
         <v>15</v>
       </c>
@@ -7703,7 +7877,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="62" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B62" s="6">
         <v>18</v>
       </c>
@@ -7721,7 +7895,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B63" s="6">
         <v>21</v>
       </c>
@@ -7736,7 +7910,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="64" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B64" s="6">
         <v>24</v>
       </c>
@@ -7754,7 +7928,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="65" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B65" s="6">
         <v>27</v>
       </c>
@@ -7769,7 +7943,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="66" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B66" s="6">
         <v>30</v>
       </c>
@@ -7787,7 +7961,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="67" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B67" s="6">
         <v>33</v>
       </c>
@@ -7802,7 +7976,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="68" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B68" s="6">
         <v>36</v>
       </c>
@@ -7820,7 +7994,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="69" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B69" s="6">
         <v>39</v>
       </c>
@@ -7835,7 +8009,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="70" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B70" s="6">
         <v>42</v>
       </c>
@@ -7853,7 +8027,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="71" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B71" s="6">
         <v>45</v>
       </c>
@@ -7868,7 +8042,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="72" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B72" s="6">
         <v>48</v>
       </c>
@@ -7886,7 +8060,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="73" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B73" s="6">
         <v>51</v>
       </c>
@@ -7901,7 +8075,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="74" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B74" s="6">
         <v>54</v>
       </c>
@@ -7919,7 +8093,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="75" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B75" s="6">
         <v>57</v>
       </c>
@@ -7934,7 +8108,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="76" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B76" s="6">
         <v>60</v>
       </c>
@@ -7952,7 +8126,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="77" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B77" s="6">
         <v>63</v>
       </c>
@@ -7967,7 +8141,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="78" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B78" s="6">
         <v>66</v>
       </c>
@@ -7985,7 +8159,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="79" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B79" s="6">
         <v>69</v>
       </c>
@@ -8000,17 +8174,17 @@
         <v>216</v>
       </c>
     </row>
-    <row r="80" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="81" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="81" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E81" s="6"/>
     </row>
-    <row r="82" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D82" s="15" t="s">
         <v>224</v>
       </c>
       <c r="E82" s="6"/>
     </row>
-    <row r="83" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B83" s="6">
         <v>0</v>
       </c>
@@ -8075,7 +8249,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="84" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B84" s="6">
         <v>3</v>
       </c>
@@ -8139,7 +8313,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="85" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B85" s="6">
         <v>6</v>
       </c>
@@ -8203,7 +8377,7 @@
         <v>3C</v>
       </c>
     </row>
-    <row r="86" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B86" s="6">
         <v>9</v>
       </c>
@@ -8264,7 +8438,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="87" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B87" s="6">
         <v>12</v>
       </c>
@@ -8329,7 +8503,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="88" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B88" s="6">
         <v>15</v>
       </c>
@@ -8387,7 +8561,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="89" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B89" s="6">
         <v>18</v>
       </c>
@@ -8451,7 +8625,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="90" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B90" s="6">
         <v>21</v>
       </c>
@@ -8515,7 +8689,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="91" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B91" s="6">
         <v>24</v>
       </c>
@@ -8576,7 +8750,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="92" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B92" s="6">
         <v>27</v>
       </c>
@@ -8640,7 +8814,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="93" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B93" s="6">
         <v>30</v>
       </c>
@@ -8706,7 +8880,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="95" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B95" s="6">
         <v>48</v>
       </c>
@@ -8721,7 +8895,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="96" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B96" s="6">
         <v>51</v>
       </c>
@@ -8736,7 +8910,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="97" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B97" s="6">
         <v>54</v>
       </c>
@@ -8751,7 +8925,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="98" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B98" s="6">
         <v>57</v>
       </c>
@@ -8766,20 +8940,20 @@
         <v>118</v>
       </c>
     </row>
-    <row r="99" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D99" s="26"/>
     </row>
-    <row r="100" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D100" s="26"/>
       <c r="E100" s="6"/>
     </row>
-    <row r="101" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D101" s="15" t="s">
         <v>225</v>
       </c>
       <c r="E101" s="6"/>
     </row>
-    <row r="102" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B102" s="6">
         <v>0</v>
       </c>
@@ -8843,7 +9017,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="103" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B103" s="6">
         <v>3</v>
       </c>
@@ -8907,7 +9081,7 @@
         <v>FF</v>
       </c>
     </row>
-    <row r="104" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B104" s="6">
         <v>6</v>
       </c>
@@ -8972,7 +9146,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="105" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B105" s="6">
         <v>9</v>
       </c>
@@ -9033,7 +9207,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="106" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B106" s="6">
         <v>12</v>
       </c>
@@ -9091,7 +9265,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="107" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B107" s="6">
         <v>15</v>
       </c>
@@ -9155,7 +9329,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="108" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B108" s="6">
         <v>18</v>
       </c>
@@ -9219,7 +9393,7 @@
         <v>3A</v>
       </c>
     </row>
-    <row r="109" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B109" s="6">
         <v>21</v>
       </c>
@@ -9280,7 +9454,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="110" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B110" s="6">
         <v>24</v>
       </c>
@@ -9341,7 +9515,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="111" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B111" s="6">
         <v>27</v>
       </c>
@@ -9402,7 +9576,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="112" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B112" s="6">
         <v>30</v>
       </c>
@@ -9463,12 +9637,12 @@
         <v>06</v>
       </c>
     </row>
-    <row r="116" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D116" s="15" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="117" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B117" s="6">
         <v>0</v>
       </c>
@@ -9532,7 +9706,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="118" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B118" s="6">
         <v>3</v>
       </c>
@@ -9596,7 +9770,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="119" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B119" s="6">
         <v>6</v>
       </c>
@@ -9660,7 +9834,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="120" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B120" s="6">
         <v>9</v>
       </c>
@@ -9724,7 +9898,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="121" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B121" s="6">
         <v>12</v>
       </c>
@@ -9785,7 +9959,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="122" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B122" s="6">
         <v>15</v>
       </c>
@@ -9846,7 +10020,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="123" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B123" s="6">
         <v>18</v>
       </c>
@@ -9907,7 +10081,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="124" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B124" s="6">
         <v>21</v>
       </c>
@@ -9968,7 +10142,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="125" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B125" s="6">
         <v>24</v>
       </c>
@@ -10026,7 +10200,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="126" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B126" s="6">
         <v>27</v>
       </c>
@@ -10090,7 +10264,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="127" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B127" s="6">
         <v>30</v>
       </c>
@@ -10154,7 +10328,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="128" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B128" s="6">
         <v>33</v>
       </c>
@@ -10215,7 +10389,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="129" spans="2:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B129" s="6">
         <v>36</v>
       </c>
@@ -10279,7 +10453,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="130" spans="2:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B130" s="6">
         <v>39</v>
       </c>
@@ -10337,7 +10511,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="131" spans="2:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B131" s="6">
         <v>42</v>
       </c>
@@ -10398,7 +10572,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="132" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B132" s="6">
         <v>45</v>
       </c>
@@ -10459,12 +10633,12 @@
         <v>0C</v>
       </c>
     </row>
-    <row r="133" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F133" s="15" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="134" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B134" s="6">
         <v>48</v>
       </c>
@@ -10476,7 +10650,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="135" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B135" s="6">
         <v>51</v>
       </c>
@@ -10488,7 +10662,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="136" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B136" s="6">
         <v>54</v>
       </c>
@@ -10500,12 +10674,12 @@
         <v>155</v>
       </c>
     </row>
-    <row r="140" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D140" s="15" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="141" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B141" s="6">
         <v>0</v>
       </c>
@@ -10566,7 +10740,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="142" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B142" s="6">
         <v>3</v>
       </c>
@@ -10627,7 +10801,7 @@
         <v>FF</v>
       </c>
     </row>
-    <row r="143" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B143" s="6">
         <v>6</v>
       </c>
@@ -10688,7 +10862,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="144" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D144" s="6" t="s">
         <v>206</v>
       </c>
@@ -10745,7 +10919,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="145" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D145" s="6" t="s">
         <v>203</v>
       </c>
@@ -10802,7 +10976,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="146" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D146" s="6" t="s">
         <v>204</v>
       </c>
@@ -10856,7 +11030,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="147" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D147" s="6" t="s">
         <v>185</v>
       </c>
@@ -10907,7 +11081,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="148" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D148" s="6" t="s">
         <v>205</v>
       </c>
@@ -10961,7 +11135,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="149" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D149" s="27" t="s">
         <v>381</v>
       </c>
@@ -11012,15 +11186,15 @@
         <v>09</v>
       </c>
     </row>
-    <row r="151" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D151" s="26"/>
     </row>
-    <row r="153" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D153" s="15" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="154" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B154" s="6">
         <v>0</v>
       </c>
@@ -11081,7 +11255,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="155" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B155" s="6">
         <v>3</v>
       </c>
@@ -11146,7 +11320,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="156" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B156" s="6">
         <v>6</v>
       </c>
@@ -11210,7 +11384,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="157" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B157" s="6">
         <v>9</v>
       </c>
@@ -11274,7 +11448,7 @@
         <v>A0</v>
       </c>
     </row>
-    <row r="158" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="14" t="s">
         <v>272</v>
       </c>
@@ -11341,7 +11515,7 @@
         <v>07</v>
       </c>
     </row>
-    <row r="159" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B159" s="6">
         <v>15</v>
       </c>
@@ -11405,7 +11579,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="160" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B160" s="6">
         <v>18</v>
       </c>
@@ -11463,7 +11637,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="161" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B161" s="6">
         <v>21</v>
       </c>
@@ -11521,7 +11695,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="162" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="14" t="s">
         <v>289</v>
       </c>
@@ -11588,7 +11762,7 @@
         <v>08</v>
       </c>
     </row>
-    <row r="163" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B163" s="6">
         <v>27</v>
       </c>
@@ -11655,7 +11829,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="164" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B164" s="6">
         <v>30</v>
       </c>
@@ -11719,7 +11893,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="165" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" s="14" t="s">
         <v>293</v>
       </c>
@@ -11783,7 +11957,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="166" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B166" s="6">
         <v>36</v>
       </c>
@@ -11850,7 +12024,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="167" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B167" s="6">
         <v>39</v>
       </c>
@@ -11908,7 +12082,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="168" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B168" s="6">
         <v>42</v>
       </c>
@@ -11969,7 +12143,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="169" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B169" s="6">
         <v>45</v>
       </c>
@@ -12033,7 +12207,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="170" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B170" s="6">
         <v>48</v>
       </c>
@@ -12094,7 +12268,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="171" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B171" s="6">
         <v>51</v>
       </c>
@@ -12158,7 +12332,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="172" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B172" s="6">
         <v>54</v>
       </c>
@@ -12216,7 +12390,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="173" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B173" s="6">
         <v>57</v>
       </c>
@@ -12277,7 +12451,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="174" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B174" s="6">
         <v>60</v>
       </c>
@@ -12338,12 +12512,12 @@
         <v>0C</v>
       </c>
     </row>
-    <row r="175" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F175" s="15" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="176" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B176" s="6">
         <v>96</v>
       </c>
@@ -12355,7 +12529,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="177" spans="2:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B177" s="6">
         <v>99</v>
       </c>
@@ -12367,7 +12541,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="178" spans="2:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B178" s="6">
         <v>102</v>
       </c>
@@ -12379,7 +12553,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="179" spans="2:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B179" s="6">
         <v>105</v>
       </c>
@@ -12391,7 +12565,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="180" spans="2:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B180" s="6">
         <v>108</v>
       </c>
@@ -12403,7 +12577,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="181" spans="2:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B181" s="6">
         <v>111</v>
       </c>
@@ -12415,7 +12589,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="182" spans="2:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B182" s="6">
         <v>114</v>
       </c>
@@ -12427,7 +12601,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="183" spans="2:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B183" s="6">
         <v>117</v>
       </c>
@@ -12439,7 +12613,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="184" spans="2:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B184" s="6">
         <v>120</v>
       </c>
@@ -12451,7 +12625,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="185" spans="2:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B185" s="6">
         <v>123</v>
       </c>
@@ -12463,7 +12637,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="186" spans="2:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B186" s="6">
         <v>126</v>
       </c>
@@ -12475,7 +12649,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="187" spans="2:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B187" s="6">
         <v>129</v>
       </c>
@@ -12487,7 +12661,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="188" spans="2:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B188" s="6">
         <v>132</v>
       </c>
@@ -12499,7 +12673,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="189" spans="2:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B189" s="6">
         <v>135</v>
       </c>
@@ -12511,7 +12685,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="190" spans="2:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B190" s="6">
         <v>138</v>
       </c>
@@ -12523,7 +12697,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="191" spans="2:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B191" s="6">
         <v>141</v>
       </c>
@@ -12535,7 +12709,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="192" spans="2:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B192" s="6">
         <v>144</v>
       </c>
@@ -12547,7 +12721,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="193" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B193" s="6">
         <v>147</v>
       </c>
@@ -12559,7 +12733,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="194" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B194" s="6">
         <v>150</v>
       </c>
@@ -12571,7 +12745,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="195" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B195" s="6">
         <v>153</v>
       </c>
@@ -12583,7 +12757,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="196" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B196" s="6">
         <v>156</v>
       </c>
@@ -12595,7 +12769,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="197" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B197" s="6">
         <v>159</v>
       </c>
@@ -12607,12 +12781,12 @@
         <v>213</v>
       </c>
     </row>
-    <row r="200" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D200" s="15" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="201" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B201" s="6">
         <v>0</v>
       </c>
@@ -12676,7 +12850,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="202" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B202" s="6">
         <v>3</v>
       </c>
@@ -12740,7 +12914,7 @@
         <v>C7</v>
       </c>
     </row>
-    <row r="203" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B203" s="6">
         <v>6</v>
       </c>
@@ -12798,7 +12972,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="204" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B204" s="6">
         <v>9</v>
       </c>
@@ -12856,7 +13030,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="205" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B205" s="6">
         <v>12</v>
       </c>
@@ -12920,7 +13094,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="206" spans="2:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="206" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B206" s="6">
         <v>15</v>
       </c>
@@ -12984,7 +13158,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="207" spans="2:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="207" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B207" s="6">
         <v>18</v>
       </c>
@@ -13045,7 +13219,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="208" spans="2:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="208" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B208" s="6">
         <v>21</v>
       </c>
@@ -13106,7 +13280,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="209" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B209" s="6">
         <v>24</v>
       </c>
@@ -13170,7 +13344,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="210" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B210" s="6">
         <v>27</v>
       </c>
@@ -13231,7 +13405,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="211" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B211" s="6">
         <v>30</v>
       </c>
@@ -13295,7 +13469,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="212" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B212" s="6">
         <v>33</v>
       </c>
@@ -13359,7 +13533,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="213" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B213" s="6">
         <v>36</v>
       </c>
@@ -13423,7 +13597,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="214" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B214" s="6">
         <v>39</v>
       </c>
@@ -13487,7 +13661,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="215" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B215" s="6">
         <v>42</v>
       </c>
@@ -13551,7 +13725,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="216" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B216" s="6">
         <v>45</v>
       </c>
@@ -13612,7 +13786,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="217" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B217" s="6">
         <v>48</v>
       </c>
@@ -13673,7 +13847,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="218" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B218" s="6">
         <v>51</v>
       </c>
@@ -13737,7 +13911,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="219" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B219" s="6">
         <v>54</v>
       </c>
@@ -13801,7 +13975,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="220" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B220" s="6">
         <v>57</v>
       </c>
@@ -13865,7 +14039,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="221" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B221" s="6">
         <v>60</v>
       </c>
@@ -13926,7 +14100,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="222" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B222" s="6">
         <v>63</v>
       </c>
@@ -13984,7 +14158,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="223" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B223" s="6">
         <v>66</v>
       </c>
@@ -14045,7 +14219,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="224" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B224" s="6">
         <v>69</v>
       </c>
@@ -14106,19 +14280,19 @@
         <v>00</v>
       </c>
     </row>
-    <row r="225" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F225" s="15" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="226" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="227" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="228" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="227" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="228" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D228" s="15" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="229" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B229" s="6">
         <v>0</v>
       </c>
@@ -14182,7 +14356,7 @@
         <v>07</v>
       </c>
     </row>
-    <row r="230" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B230" s="6">
         <v>3</v>
       </c>
@@ -14243,7 +14417,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="231" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A231" s="14" t="s">
         <v>267</v>
       </c>
@@ -14310,7 +14484,7 @@
         <v>01</v>
       </c>
     </row>
-    <row r="232" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B232" s="6">
         <v>9</v>
       </c>
@@ -14371,7 +14545,7 @@
         <v>07</v>
       </c>
     </row>
-    <row r="233" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A233" s="14" t="s">
         <v>272</v>
       </c>
@@ -14438,7 +14612,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="234" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B234" s="6">
         <v>15</v>
       </c>
@@ -14499,7 +14673,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="235" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B235" s="6">
         <v>18</v>
       </c>
@@ -14557,7 +14731,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="236" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B236" s="6">
         <v>21</v>
       </c>
@@ -14618,7 +14792,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="237" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B237" s="6">
         <v>24</v>
       </c>
@@ -14682,7 +14856,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="238" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B238" s="6">
         <v>27</v>
       </c>
@@ -14740,7 +14914,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="239" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B239" s="6">
         <v>30</v>
       </c>
@@ -14798,7 +14972,7 @@
         <v>0C</v>
       </c>
     </row>
-    <row r="240" spans="1:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A240" s="14" t="s">
         <v>273</v>
       </c>
@@ -14868,7 +15042,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="241" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B241" s="6">
         <v>36</v>
       </c>
@@ -14932,7 +15106,7 @@
         <v>08</v>
       </c>
     </row>
-    <row r="242" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B242" s="6">
         <v>39</v>
       </c>
@@ -14996,14 +15170,14 @@
         <v>00</v>
       </c>
     </row>
-    <row r="243" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="245" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="246" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="245" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="246" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D246" s="15" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="247" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B247" s="6">
         <v>0</v>
       </c>
@@ -15068,7 +15242,7 @@
       </c>
       <c r="Y247" s="21"/>
     </row>
-    <row r="248" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A248" s="14" t="s">
         <v>316</v>
       </c>
@@ -15136,7 +15310,7 @@
       </c>
       <c r="Y248" s="21"/>
     </row>
-    <row r="249" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B249" s="6">
         <v>6</v>
       </c>
@@ -15201,7 +15375,7 @@
       </c>
       <c r="Y249" s="21"/>
     </row>
-    <row r="250" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B250" s="6">
         <v>9</v>
       </c>
@@ -15266,7 +15440,7 @@
       </c>
       <c r="Y250" s="21"/>
     </row>
-    <row r="251" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B251" s="6">
         <v>12</v>
       </c>
@@ -15331,7 +15505,7 @@
       </c>
       <c r="Y251" s="21"/>
     </row>
-    <row r="252" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A252" s="14" t="s">
         <v>267</v>
       </c>
@@ -15399,7 +15573,7 @@
       </c>
       <c r="Y252" s="21"/>
     </row>
-    <row r="253" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A253" s="14" t="s">
         <v>272</v>
       </c>
@@ -15467,7 +15641,7 @@
       </c>
       <c r="Y253" s="21"/>
     </row>
-    <row r="254" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B254" s="6">
         <v>21</v>
       </c>
@@ -15529,7 +15703,7 @@
       </c>
       <c r="Y254" s="21"/>
     </row>
-    <row r="255" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A255" s="6"/>
       <c r="B255" s="6">
         <v>24</v>
@@ -15589,7 +15763,7 @@
       </c>
       <c r="Y255" s="21"/>
     </row>
-    <row r="256" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B256" s="6">
         <v>27</v>
       </c>
@@ -15651,7 +15825,7 @@
       </c>
       <c r="Y256" s="21"/>
     </row>
-    <row r="257" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B257" s="6">
         <v>30</v>
       </c>
@@ -15716,7 +15890,7 @@
       </c>
       <c r="Y257" s="21"/>
     </row>
-    <row r="258" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B258" s="6">
         <v>33</v>
       </c>
@@ -15775,7 +15949,7 @@
       </c>
       <c r="Y258" s="21"/>
     </row>
-    <row r="259" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B259" s="6">
         <v>36</v>
       </c>
@@ -15834,7 +16008,7 @@
       </c>
       <c r="Y259" s="21"/>
     </row>
-    <row r="260" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A260" s="14" t="s">
         <v>273</v>
       </c>
@@ -15905,7 +16079,7 @@
       </c>
       <c r="Y260" s="21"/>
     </row>
-    <row r="261" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B261" s="6">
         <v>42</v>
       </c>
@@ -15967,7 +16141,7 @@
       </c>
       <c r="Y261" s="21"/>
     </row>
-    <row r="262" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B262" s="6">
         <v>45</v>
       </c>
@@ -16035,7 +16209,7 @@
       </c>
       <c r="Y262" s="21"/>
     </row>
-    <row r="263" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B263" s="6">
         <v>48</v>
       </c>
@@ -16097,7 +16271,7 @@
       </c>
       <c r="Y263" s="21"/>
     </row>
-    <row r="264" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A264" s="6"/>
       <c r="B264" s="6">
         <v>51</v>
@@ -16163,7 +16337,7 @@
       </c>
       <c r="Y264" s="21"/>
     </row>
-    <row r="265" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B265" s="6">
         <v>54</v>
       </c>
@@ -16225,7 +16399,7 @@
       </c>
       <c r="Y265" s="21"/>
     </row>
-    <row r="266" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B266" s="6">
         <v>57</v>
       </c>
@@ -16286,7 +16460,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="267" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B267" s="6">
         <v>60</v>
       </c>
@@ -16347,7 +16521,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="268" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B268" s="6">
         <v>63</v>
       </c>
@@ -16408,7 +16582,7 @@
         <v>0F</v>
       </c>
     </row>
-    <row r="269" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A269" s="14" t="s">
         <v>321</v>
       </c>
@@ -16472,7 +16646,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="270" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A270" s="6"/>
       <c r="B270" s="6">
         <v>69</v>
@@ -16540,7 +16714,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="271" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B271" s="6">
         <v>72</v>
       </c>
@@ -16607,7 +16781,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="272" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B272" s="6">
         <v>75</v>
       </c>
@@ -16669,7 +16843,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="273" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="273" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B273" s="6">
         <v>78</v>
       </c>
@@ -16731,25 +16905,25 @@
         <v>03</v>
       </c>
     </row>
-    <row r="274" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="274" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E274" s="6"/>
       <c r="O274" s="19"/>
       <c r="P274" s="19"/>
       <c r="Q274" s="19"/>
       <c r="R274" s="19"/>
     </row>
-    <row r="276" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="276" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O276" s="19"/>
       <c r="P276" s="19"/>
       <c r="Q276" s="19"/>
       <c r="R276" s="19"/>
     </row>
-    <row r="277" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="277" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D277" s="15" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="278" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="278" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B278" s="6">
         <v>0</v>
       </c>
@@ -16810,7 +16984,7 @@
         <v>05</v>
       </c>
     </row>
-    <row r="279" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="279" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B279" s="6">
         <v>3</v>
       </c>
@@ -16868,7 +17042,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="280" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="280" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B280" s="6">
         <v>6</v>
       </c>
@@ -16926,10 +17100,10 @@
         <v>00</v>
       </c>
     </row>
-    <row r="281" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="281" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D281" s="10"/>
     </row>
-    <row r="282" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="282" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B282" s="6">
         <v>48</v>
       </c>
@@ -16987,7 +17161,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="283" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="283" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B283" s="6">
         <v>51</v>
       </c>
@@ -17042,12 +17216,12 @@
         <v>00</v>
       </c>
     </row>
-    <row r="287" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="287" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D287" s="15" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="288" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="288" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B288" s="6">
         <v>0</v>
       </c>
@@ -17108,7 +17282,7 @@
         <v>05</v>
       </c>
     </row>
-    <row r="289" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="289" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B289" s="6">
         <v>3</v>
       </c>
@@ -17166,7 +17340,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="290" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="290" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B290" s="6">
         <v>6</v>
       </c>
@@ -17224,7 +17398,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="291" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="291" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B291" s="6">
         <v>9</v>
       </c>
@@ -17283,10 +17457,10 @@
         <v>03</v>
       </c>
     </row>
-    <row r="292" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="292" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D292" s="10"/>
     </row>
-    <row r="293" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="293" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B293" s="6">
         <v>48</v>
       </c>
@@ -17347,7 +17521,7 @@
         <v>05</v>
       </c>
     </row>
-    <row r="294" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="294" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B294" s="6">
         <v>51</v>
       </c>
@@ -17402,12 +17576,12 @@
         <v>00</v>
       </c>
     </row>
-    <row r="298" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="298" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D298" s="2" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="299" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="299" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B299" s="6">
         <v>0</v>
       </c>
@@ -17468,7 +17642,7 @@
         <v>05</v>
       </c>
     </row>
-    <row r="300" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="300" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B300" s="6">
         <v>3</v>
       </c>
@@ -17529,7 +17703,7 @@
         <v>06</v>
       </c>
     </row>
-    <row r="301" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="301" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B301" s="6">
         <v>6</v>
       </c>
@@ -17587,7 +17761,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="302" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="302" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B302" s="6">
         <v>9</v>
       </c>
@@ -17645,12 +17819,12 @@
         <v>00</v>
       </c>
     </row>
-    <row r="306" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:22" x14ac:dyDescent="0.3">
       <c r="D306" s="2" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="307" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B307" s="6">
         <v>0</v>
       </c>
@@ -17714,7 +17888,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="308" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B308" s="6">
         <v>3</v>
       </c>
@@ -17778,7 +17952,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="309" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B309" s="6">
         <v>6</v>
       </c>
@@ -17839,7 +18013,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="310" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B310" s="6">
         <v>9</v>
       </c>
@@ -17900,7 +18074,7 @@
         <v>05</v>
       </c>
     </row>
-    <row r="311" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A311" s="14" t="s">
         <v>272</v>
       </c>
@@ -17964,7 +18138,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="312" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B312" s="6">
         <v>15</v>
       </c>
@@ -18028,7 +18202,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="313" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B313" s="6">
         <v>18</v>
       </c>
@@ -18089,7 +18263,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="314" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B314" s="6">
         <v>21</v>
       </c>
@@ -18150,7 +18324,7 @@
         <v>1E</v>
       </c>
     </row>
-    <row r="315" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B315" s="6">
         <v>24</v>
       </c>
@@ -18214,7 +18388,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="316" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B316" s="6">
         <v>27</v>
       </c>
@@ -18272,7 +18446,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="317" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A317" s="14" t="s">
         <v>356</v>
       </c>
@@ -18339,7 +18513,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="318" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A318" s="14" t="s">
         <v>357</v>
       </c>
@@ -18400,7 +18574,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="319" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B319" s="6">
         <v>36</v>
       </c>
@@ -18458,22 +18632,22 @@
         <v>0C</v>
       </c>
     </row>
-    <row r="320" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:22" x14ac:dyDescent="0.3">
       <c r="F320" s="2" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="321" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:22" x14ac:dyDescent="0.3">
       <c r="F321" s="2" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="324" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:22" x14ac:dyDescent="0.3">
       <c r="D324" s="2" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="325" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B325" s="6">
         <v>0</v>
       </c>
@@ -18537,7 +18711,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="326" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B326" s="6">
         <v>3</v>
       </c>
@@ -18601,7 +18775,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="327" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B327" s="6">
         <v>6</v>
       </c>
@@ -18662,7 +18836,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="328" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B328" s="6">
         <v>9</v>
       </c>
@@ -18723,7 +18897,7 @@
         <v>05</v>
       </c>
     </row>
-    <row r="329" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A329" s="14" t="s">
         <v>272</v>
       </c>
@@ -18787,7 +18961,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="330" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B330" s="6">
         <v>15</v>
       </c>
@@ -18851,7 +19025,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="331" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B331" s="6">
         <v>18</v>
       </c>
@@ -18912,7 +19086,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="332" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B332" s="6">
         <v>21</v>
       </c>
@@ -18973,7 +19147,7 @@
         <v>1E</v>
       </c>
     </row>
-    <row r="333" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B333" s="6">
         <v>24</v>
       </c>
@@ -19037,7 +19211,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="334" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B334" s="6">
         <v>27</v>
       </c>
@@ -19095,7 +19269,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="335" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A335" s="14" t="s">
         <v>356</v>
       </c>
@@ -19162,7 +19336,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="336" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A336" s="14" t="s">
         <v>357</v>
       </c>
@@ -19223,7 +19397,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="337" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B337" s="6">
         <v>36</v>
       </c>
@@ -19281,22 +19455,22 @@
         <v>0C</v>
       </c>
     </row>
-    <row r="338" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:22" x14ac:dyDescent="0.3">
       <c r="F338" s="2" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="339" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:22" x14ac:dyDescent="0.3">
       <c r="F339" s="2" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="342" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:22" x14ac:dyDescent="0.3">
       <c r="D342" s="2" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="343" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B343" s="6">
         <v>0</v>
       </c>
@@ -19358,7 +19532,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="344" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B344" s="6">
         <v>3</v>
       </c>
@@ -19420,7 +19594,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="345" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A345" s="63"/>
       <c r="B345" s="6">
         <v>6</v>
@@ -19479,7 +19653,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="346" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:22" x14ac:dyDescent="0.3">
       <c r="D346" s="27"/>
       <c r="H346" s="28"/>
       <c r="O346" s="19"/>
@@ -19487,7 +19661,7 @@
       <c r="Q346" s="19"/>
       <c r="R346" s="19"/>
     </row>
-    <row r="347" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:22" x14ac:dyDescent="0.3">
       <c r="D347" s="27"/>
       <c r="H347" s="28"/>
       <c r="O347" s="19"/>
@@ -19495,7 +19669,7 @@
       <c r="Q347" s="19"/>
       <c r="R347" s="19"/>
     </row>
-    <row r="348" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:22" x14ac:dyDescent="0.3">
       <c r="D348" s="27"/>
       <c r="F348" s="2"/>
       <c r="H348" s="28"/>
@@ -19504,66 +19678,539 @@
       <c r="Q348" s="19"/>
       <c r="R348" s="19"/>
     </row>
-    <row r="349" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="D349" s="27"/>
-      <c r="H349" s="28"/>
-      <c r="O349" s="19"/>
-      <c r="P349" s="19"/>
-      <c r="Q349" s="19"/>
-      <c r="R349" s="19"/>
-    </row>
-    <row r="350" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="D350" s="27"/>
+    <row r="349" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="D349" s="2" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="350" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B350" s="6">
+        <v>0</v>
+      </c>
+      <c r="C350" s="6" t="str">
+        <f t="shared" ref="C350:C357" si="524">"0x" &amp; DEC2HEX(B350,3)</f>
+        <v>0x000</v>
+      </c>
+      <c r="D350" s="27" t="s">
+        <v>392</v>
+      </c>
       <c r="F350" s="2"/>
-      <c r="O350" s="19"/>
-      <c r="P350" s="19"/>
-      <c r="Q350" s="19"/>
-      <c r="R350" s="19"/>
-    </row>
-    <row r="351" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="D351" s="27"/>
+      <c r="G350" s="16">
+        <v>1</v>
+      </c>
+      <c r="H350" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="I350" s="6">
+        <f t="shared" ref="I350:I357" si="525">IF(H350="", "", VLOOKUP(H350, $X$3:$Y$10, 2))</f>
+        <v>0</v>
+      </c>
+      <c r="M350" s="6">
+        <v>1</v>
+      </c>
+      <c r="N350" s="18" t="str">
+        <f t="shared" ref="N350:N357" si="526">IF(G350="", "", TEXT(DEC2BIN(G350), "000000"))</f>
+        <v>000001</v>
+      </c>
+      <c r="O350" s="19" t="str">
+        <f t="shared" ref="O350" si="527">IF(I350="", "", TEXT(DEC2BIN(I350), "000"))</f>
+        <v>000</v>
+      </c>
+      <c r="P350" s="19" t="str">
+        <f t="shared" ref="P350:P357" si="528">IF(J350="", "", TEXT(DEC2BIN(J350), "000"))</f>
+        <v/>
+      </c>
+      <c r="Q350" s="19" t="str">
+        <f t="shared" ref="Q350:Q357" si="529">IF(K350="", "", TEXT(DEC2BIN(K350), "000"))</f>
+        <v/>
+      </c>
+      <c r="R350" s="19" t="str">
+        <f t="shared" ref="R350:R357" si="530">IF(L350="", "", TEXT(DEC2BIN(L350), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="S350" s="20" t="str">
+        <f t="shared" ref="S350:S357" si="531">IF(M350="", "", TEXT(DEC2BIN(M350), "00000000"))</f>
+        <v>00000001</v>
+      </c>
+      <c r="T350" s="6" t="str">
+        <f t="shared" ref="T350:T357" si="532">BIN2HEX(LEFT(CONCATENATE(N350,IF(O350="", "000", O350)), 8), 2)</f>
+        <v>04</v>
+      </c>
+      <c r="U350" s="6" t="str">
+        <f t="shared" ref="U350:U357" si="533">BIN2HEX(CONCATENATE(RIGHT(O350, 1), IF(P350 = "", "000", P350), IF(Q350 = "", "000", Q350), "0"), 2)</f>
+        <v>00</v>
+      </c>
+      <c r="V350" s="21" t="str">
+        <f t="shared" ref="V350:V357" si="534">IF(R350="", BIN2HEX(S350, 2), BIN2HEX(R350,2))</f>
+        <v>01</v>
+      </c>
+    </row>
+    <row r="351" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B351" s="6">
+        <v>3</v>
+      </c>
+      <c r="C351" s="6" t="str">
+        <f t="shared" ref="C351:C353" si="535">"0x" &amp; DEC2HEX(B351,3)</f>
+        <v>0x003</v>
+      </c>
+      <c r="D351" s="27" t="s">
+        <v>393</v>
+      </c>
       <c r="F351" s="2"/>
-      <c r="H351" s="59"/>
-      <c r="O351" s="19"/>
-      <c r="P351" s="19"/>
-      <c r="Q351" s="19"/>
-      <c r="R351" s="19"/>
-    </row>
-    <row r="352" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="D352" s="27"/>
-      <c r="O352" s="19"/>
-      <c r="P352" s="19"/>
-      <c r="Q352" s="19"/>
-      <c r="R352" s="19"/>
-    </row>
-    <row r="353" spans="4:18" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="D353" s="27"/>
-      <c r="F353" s="2"/>
-      <c r="H353" s="59"/>
-      <c r="O353" s="19"/>
-      <c r="P353" s="19"/>
-      <c r="Q353" s="19"/>
-      <c r="R353" s="19"/>
-    </row>
-    <row r="354" spans="4:18" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="D354" s="27"/>
-      <c r="O354" s="19"/>
-      <c r="P354" s="19"/>
-      <c r="Q354" s="19"/>
-      <c r="R354" s="19"/>
-    </row>
-    <row r="355" spans="4:18" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="D355" s="27"/>
-      <c r="O355" s="19"/>
-      <c r="P355" s="19"/>
-      <c r="Q355" s="19"/>
-      <c r="R355" s="19"/>
-    </row>
-    <row r="356" spans="4:18" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="F356" s="2"/>
-    </row>
-    <row r="357" spans="4:18" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="F357" s="2"/>
+      <c r="G351" s="16">
+        <v>1</v>
+      </c>
+      <c r="H351" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="I351" s="6">
+        <f t="shared" ref="I351:I353" si="536">IF(H351="", "", VLOOKUP(H351, $X$3:$Y$10, 2))</f>
+        <v>4</v>
+      </c>
+      <c r="M351" s="6">
+        <v>0</v>
+      </c>
+      <c r="N351" s="18" t="str">
+        <f t="shared" ref="N351:N353" si="537">IF(G351="", "", TEXT(DEC2BIN(G351), "000000"))</f>
+        <v>000001</v>
+      </c>
+      <c r="O351" s="19" t="str">
+        <f t="shared" ref="O351:O353" si="538">IF(I351="", "", TEXT(DEC2BIN(I351), "000"))</f>
+        <v>100</v>
+      </c>
+      <c r="P351" s="19" t="str">
+        <f t="shared" ref="P351:P353" si="539">IF(J351="", "", TEXT(DEC2BIN(J351), "000"))</f>
+        <v/>
+      </c>
+      <c r="Q351" s="19" t="str">
+        <f t="shared" ref="Q351:Q353" si="540">IF(K351="", "", TEXT(DEC2BIN(K351), "000"))</f>
+        <v/>
+      </c>
+      <c r="R351" s="19" t="str">
+        <f t="shared" ref="R351:R353" si="541">IF(L351="", "", TEXT(DEC2BIN(L351), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="S351" s="20" t="str">
+        <f t="shared" ref="S351:S353" si="542">IF(M351="", "", TEXT(DEC2BIN(M351), "00000000"))</f>
+        <v>00000000</v>
+      </c>
+      <c r="T351" s="6" t="str">
+        <f t="shared" ref="T351:T353" si="543">BIN2HEX(LEFT(CONCATENATE(N351,IF(O351="", "000", O351)), 8), 2)</f>
+        <v>06</v>
+      </c>
+      <c r="U351" s="6" t="str">
+        <f t="shared" ref="U351:U353" si="544">BIN2HEX(CONCATENATE(RIGHT(O351, 1), IF(P351 = "", "000", P351), IF(Q351 = "", "000", Q351), "0"), 2)</f>
+        <v>00</v>
+      </c>
+      <c r="V351" s="21" t="str">
+        <f t="shared" ref="V351:V353" si="545">IF(R351="", BIN2HEX(S351, 2), BIN2HEX(R351,2))</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="352" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B352" s="6">
+        <v>6</v>
+      </c>
+      <c r="C352" s="6" t="str">
+        <f t="shared" ref="C352" si="546">"0x" &amp; DEC2HEX(B352,3)</f>
+        <v>0x006</v>
+      </c>
+      <c r="D352" s="27" t="s">
+        <v>394</v>
+      </c>
+      <c r="F352" s="2"/>
+      <c r="G352" s="16">
+        <v>1</v>
+      </c>
+      <c r="H352" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="I352" s="6">
+        <f t="shared" ref="I352" si="547">IF(H352="", "", VLOOKUP(H352, $X$3:$Y$10, 2))</f>
+        <v>5</v>
+      </c>
+      <c r="M352" s="6">
+        <v>8</v>
+      </c>
+      <c r="N352" s="18" t="str">
+        <f t="shared" ref="N352" si="548">IF(G352="", "", TEXT(DEC2BIN(G352), "000000"))</f>
+        <v>000001</v>
+      </c>
+      <c r="O352" s="19" t="str">
+        <f t="shared" ref="O352" si="549">IF(I352="", "", TEXT(DEC2BIN(I352), "000"))</f>
+        <v>101</v>
+      </c>
+      <c r="P352" s="19" t="str">
+        <f t="shared" ref="P352" si="550">IF(J352="", "", TEXT(DEC2BIN(J352), "000"))</f>
+        <v/>
+      </c>
+      <c r="Q352" s="19" t="str">
+        <f t="shared" ref="Q352" si="551">IF(K352="", "", TEXT(DEC2BIN(K352), "000"))</f>
+        <v/>
+      </c>
+      <c r="R352" s="19" t="str">
+        <f t="shared" ref="R352" si="552">IF(L352="", "", TEXT(DEC2BIN(L352), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="S352" s="20" t="str">
+        <f t="shared" ref="S352" si="553">IF(M352="", "", TEXT(DEC2BIN(M352), "00000000"))</f>
+        <v>00001000</v>
+      </c>
+      <c r="T352" s="6" t="str">
+        <f t="shared" ref="T352" si="554">BIN2HEX(LEFT(CONCATENATE(N352,IF(O352="", "000", O352)), 8), 2)</f>
+        <v>06</v>
+      </c>
+      <c r="U352" s="6" t="str">
+        <f t="shared" ref="U352" si="555">BIN2HEX(CONCATENATE(RIGHT(O352, 1), IF(P352 = "", "000", P352), IF(Q352 = "", "000", Q352), "0"), 2)</f>
+        <v>80</v>
+      </c>
+      <c r="V352" s="21" t="str">
+        <f t="shared" ref="V352" si="556">IF(R352="", BIN2HEX(S352, 2), BIN2HEX(R352,2))</f>
+        <v>08</v>
+      </c>
+    </row>
+    <row r="353" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A353" s="6"/>
+      <c r="B353" s="6">
+        <v>9</v>
+      </c>
+      <c r="C353" s="6" t="str">
+        <f t="shared" si="535"/>
+        <v>0x009</v>
+      </c>
+      <c r="D353" s="27" t="s">
+        <v>291</v>
+      </c>
+      <c r="G353" s="16">
+        <v>17</v>
+      </c>
+      <c r="H353" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="I353" s="6">
+        <f t="shared" si="536"/>
+        <v>0</v>
+      </c>
+      <c r="J353" s="6">
+        <v>4</v>
+      </c>
+      <c r="K353" s="6">
+        <v>1</v>
+      </c>
+      <c r="N353" s="18" t="str">
+        <f t="shared" si="537"/>
+        <v>010001</v>
+      </c>
+      <c r="O353" s="19" t="str">
+        <f t="shared" si="538"/>
+        <v>000</v>
+      </c>
+      <c r="P353" s="19" t="str">
+        <f t="shared" si="539"/>
+        <v>100</v>
+      </c>
+      <c r="Q353" s="19" t="str">
+        <f t="shared" si="540"/>
+        <v>001</v>
+      </c>
+      <c r="R353" s="19" t="str">
+        <f t="shared" si="541"/>
+        <v/>
+      </c>
+      <c r="S353" s="20" t="str">
+        <f t="shared" si="542"/>
+        <v/>
+      </c>
+      <c r="T353" s="6" t="str">
+        <f t="shared" si="543"/>
+        <v>44</v>
+      </c>
+      <c r="U353" s="6" t="str">
+        <f t="shared" si="544"/>
+        <v>42</v>
+      </c>
+      <c r="V353" s="21" t="str">
+        <f t="shared" si="545"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="354" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A354" s="6"/>
+      <c r="B354" s="6">
+        <v>12</v>
+      </c>
+      <c r="C354" s="6" t="str">
+        <f t="shared" ref="C354:C356" si="557">"0x" &amp; DEC2HEX(B354,3)</f>
+        <v>0x00C</v>
+      </c>
+      <c r="D354" s="27" t="s">
+        <v>395</v>
+      </c>
+      <c r="F354" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="G354" s="16">
+        <v>17</v>
+      </c>
+      <c r="H354" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="I354" s="6">
+        <f t="shared" ref="I354:I356" si="558">IF(H354="", "", VLOOKUP(H354, $X$3:$Y$10, 2))</f>
+        <v>0</v>
+      </c>
+      <c r="J354" s="6">
+        <v>5</v>
+      </c>
+      <c r="K354" s="6">
+        <v>1</v>
+      </c>
+      <c r="N354" s="18" t="str">
+        <f t="shared" ref="N354:N356" si="559">IF(G354="", "", TEXT(DEC2BIN(G354), "000000"))</f>
+        <v>010001</v>
+      </c>
+      <c r="O354" s="19" t="str">
+        <f t="shared" ref="O354:O356" si="560">IF(I354="", "", TEXT(DEC2BIN(I354), "000"))</f>
+        <v>000</v>
+      </c>
+      <c r="P354" s="19" t="str">
+        <f t="shared" ref="P354:P356" si="561">IF(J354="", "", TEXT(DEC2BIN(J354), "000"))</f>
+        <v>101</v>
+      </c>
+      <c r="Q354" s="19" t="str">
+        <f t="shared" ref="Q354:Q356" si="562">IF(K354="", "", TEXT(DEC2BIN(K354), "000"))</f>
+        <v>001</v>
+      </c>
+      <c r="R354" s="19" t="str">
+        <f t="shared" ref="R354:R356" si="563">IF(L354="", "", TEXT(DEC2BIN(L354), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="S354" s="20" t="str">
+        <f t="shared" ref="S354:S356" si="564">IF(M354="", "", TEXT(DEC2BIN(M354), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="T354" s="6" t="str">
+        <f t="shared" ref="T354:T356" si="565">BIN2HEX(LEFT(CONCATENATE(N354,IF(O354="", "000", O354)), 8), 2)</f>
+        <v>44</v>
+      </c>
+      <c r="U354" s="6" t="str">
+        <f t="shared" ref="U354:U356" si="566">BIN2HEX(CONCATENATE(RIGHT(O354, 1), IF(P354 = "", "000", P354), IF(Q354 = "", "000", Q354), "0"), 2)</f>
+        <v>52</v>
+      </c>
+      <c r="V354" s="21" t="str">
+        <f t="shared" ref="V354:V356" si="567">IF(R354="", BIN2HEX(S354, 2), BIN2HEX(R354,2))</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="355" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B355" s="6">
+        <v>15</v>
+      </c>
+      <c r="C355" s="6" t="str">
+        <f t="shared" si="557"/>
+        <v>0x00F</v>
+      </c>
+      <c r="D355" s="27" t="s">
+        <v>396</v>
+      </c>
+      <c r="F355" s="2"/>
+      <c r="G355" s="16">
+        <v>44</v>
+      </c>
+      <c r="H355" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="I355" s="6">
+        <f t="shared" si="558"/>
+        <v>0</v>
+      </c>
+      <c r="J355" s="6">
+        <v>0</v>
+      </c>
+      <c r="N355" s="18" t="str">
+        <f t="shared" si="559"/>
+        <v>101100</v>
+      </c>
+      <c r="O355" s="19" t="str">
+        <f t="shared" si="560"/>
+        <v>000</v>
+      </c>
+      <c r="P355" s="19" t="str">
+        <f t="shared" si="561"/>
+        <v>000</v>
+      </c>
+      <c r="Q355" s="19" t="str">
+        <f t="shared" si="562"/>
+        <v/>
+      </c>
+      <c r="R355" s="19" t="str">
+        <f t="shared" si="563"/>
+        <v/>
+      </c>
+      <c r="S355" s="20" t="str">
+        <f t="shared" si="564"/>
+        <v/>
+      </c>
+      <c r="T355" s="6" t="str">
+        <f t="shared" si="565"/>
+        <v>B0</v>
+      </c>
+      <c r="U355" s="6" t="str">
+        <f t="shared" si="566"/>
+        <v>00</v>
+      </c>
+      <c r="V355" s="21" t="str">
+        <f t="shared" si="567"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="356" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B356" s="6">
+        <v>18</v>
+      </c>
+      <c r="C356" s="6" t="str">
+        <f t="shared" si="557"/>
+        <v>0x012</v>
+      </c>
+      <c r="D356" s="27" t="s">
+        <v>397</v>
+      </c>
+      <c r="G356" s="16">
+        <v>6</v>
+      </c>
+      <c r="I356" s="6" t="str">
+        <f t="shared" si="558"/>
+        <v/>
+      </c>
+      <c r="L356" s="6">
+        <v>0</v>
+      </c>
+      <c r="N356" s="18" t="str">
+        <f t="shared" si="559"/>
+        <v>000110</v>
+      </c>
+      <c r="O356" s="19" t="str">
+        <f t="shared" si="560"/>
+        <v/>
+      </c>
+      <c r="P356" s="19" t="str">
+        <f t="shared" si="561"/>
+        <v/>
+      </c>
+      <c r="Q356" s="19" t="str">
+        <f t="shared" si="562"/>
+        <v/>
+      </c>
+      <c r="R356" s="19" t="str">
+        <f t="shared" si="563"/>
+        <v>00000000</v>
+      </c>
+      <c r="S356" s="20" t="str">
+        <f t="shared" si="564"/>
+        <v/>
+      </c>
+      <c r="T356" s="6" t="str">
+        <f t="shared" si="565"/>
+        <v>18</v>
+      </c>
+      <c r="U356" s="6" t="str">
+        <f t="shared" si="566"/>
+        <v>00</v>
+      </c>
+      <c r="V356" s="21" t="str">
+        <f t="shared" si="567"/>
+        <v>00</v>
+      </c>
+      <c r="Y356" s="21"/>
+    </row>
+    <row r="357" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A357" s="63"/>
+      <c r="B357" s="6">
+        <v>21</v>
+      </c>
+      <c r="C357" s="6" t="str">
+        <f t="shared" si="524"/>
+        <v>0x015</v>
+      </c>
+      <c r="D357" s="27" t="s">
+        <v>381</v>
+      </c>
+      <c r="G357" s="16">
+        <v>5</v>
+      </c>
+      <c r="I357" s="6" t="str">
+        <f t="shared" si="525"/>
+        <v/>
+      </c>
+      <c r="L357" s="6">
+        <v>9</v>
+      </c>
+      <c r="N357" s="18" t="str">
+        <f t="shared" si="526"/>
+        <v>000101</v>
+      </c>
+      <c r="O357" s="19" t="str">
+        <f>IF(I357="", "", TEXT(DEC2BIN(I357), "000"))</f>
+        <v/>
+      </c>
+      <c r="P357" s="19" t="str">
+        <f t="shared" si="528"/>
+        <v/>
+      </c>
+      <c r="Q357" s="19" t="str">
+        <f t="shared" si="529"/>
+        <v/>
+      </c>
+      <c r="R357" s="19" t="str">
+        <f t="shared" si="530"/>
+        <v>00001001</v>
+      </c>
+      <c r="S357" s="20" t="str">
+        <f t="shared" si="531"/>
+        <v/>
+      </c>
+      <c r="T357" s="6" t="str">
+        <f t="shared" si="532"/>
+        <v>14</v>
+      </c>
+      <c r="U357" s="6" t="str">
+        <f t="shared" si="533"/>
+        <v>00</v>
+      </c>
+      <c r="V357" s="21" t="str">
+        <f t="shared" si="534"/>
+        <v>09</v>
+      </c>
+    </row>
+    <row r="358" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="D358" s="27"/>
+      <c r="F358" s="2"/>
+      <c r="H358" s="59"/>
+      <c r="L358" s="10"/>
+      <c r="O358" s="19"/>
+      <c r="P358" s="19"/>
+      <c r="Q358" s="19"/>
+      <c r="R358" s="19"/>
+    </row>
+    <row r="359" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="D359" s="27"/>
+      <c r="O359" s="19"/>
+      <c r="P359" s="19"/>
+      <c r="Q359" s="19"/>
+      <c r="R359" s="19"/>
+    </row>
+    <row r="360" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="D360" s="27"/>
+      <c r="O360" s="19"/>
+      <c r="P360" s="19"/>
+      <c r="Q360" s="19"/>
+      <c r="R360" s="19"/>
+    </row>
+    <row r="361" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="F361" s="2"/>
+    </row>
+    <row r="362" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="F362" s="2"/>
     </row>
   </sheetData>
   <sortState ref="X16:Y18">
@@ -19576,7 +20223,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z17">
       <formula1>$X$16:$X$18</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H6 H9:H11 H201:H224 H141:H149 H102:H112 H117:H132 H83:H93 H49 H41:H42 H31:H33 H17:H26 H229:H242 H154:H174 H276 H247:H273 H282:H283 H278:H280 H293:H294 H288:H291 H299:H302 H307:H319 H325:H337 H343:H355">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H6 H9:H11 H201:H224 H141:H149 H102:H112 H117:H132 H83:H93 H49 H41:H42 H31:H33 H17:H26 H229:H242 H154:H174 H276 H247:H273 H282:H283 H278:H280 H293:H294 H288:H291 H299:H302 H307:H319 H325:H337 H343:H348 H350:H360">
       <formula1>$X$3:$X$10</formula1>
     </dataValidation>
   </dataValidations>
@@ -19594,9 +20241,9 @@
       <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="22.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -20287,11 +20934,11 @@
       <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Test program for the JP C instruction (not working)
</commit_message>
<xml_diff>
--- a/2nd gen - 8 bit cpu/Instruction control lines.xlsx
+++ b/2nd gen - 8 bit cpu/Instruction control lines.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21901"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E7EDEB3-67FA-4262-8D2F-A7B5074C6F84}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8E02CF1-188E-4607-B765-4F06DE1A1F8E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Control Lines" sheetId="1" r:id="rId1"/>
@@ -160,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1084" uniqueCount="446">
   <si>
     <t>LD R1, data</t>
   </si>
@@ -1489,6 +1489,15 @@
   </si>
   <si>
     <t>Active Low/High</t>
+  </si>
+  <si>
+    <t>// 25 - Test JP C instruction</t>
+  </si>
+  <si>
+    <t>LD A, 0xFF</t>
+  </si>
+  <si>
+    <t>JP C, 0x000</t>
   </si>
 </sst>
 </file>
@@ -2032,6 +2041,13 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2040,15 +2056,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2062,11 +2069,14 @@
     <xf numFmtId="0" fontId="10" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2077,7 +2087,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2465,9 +2474,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AY61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AK9" sqref="AK9"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2488,10 +2497,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="D1" s="101" t="s">
+      <c r="D1" s="92" t="s">
         <v>441</v>
       </c>
-      <c r="E1" s="102"/>
+      <c r="E1" s="93"/>
       <c r="F1" s="97" t="s">
         <v>438</v>
       </c>
@@ -2522,40 +2531,40 @@
       <c r="AA1" s="98"/>
       <c r="AB1" s="98"/>
       <c r="AC1" s="98"/>
-      <c r="AD1" s="91" t="s">
+      <c r="AD1" s="94" t="s">
         <v>441</v>
       </c>
-      <c r="AE1" s="91" t="s">
+      <c r="AE1" s="94" t="s">
         <v>438</v>
       </c>
-      <c r="AF1" s="91" t="s">
+      <c r="AF1" s="94" t="s">
         <v>440</v>
       </c>
-      <c r="AG1" s="91" t="s">
+      <c r="AG1" s="94" t="s">
         <v>439</v>
       </c>
-      <c r="AI1" s="91" t="s">
+      <c r="AI1" s="94" t="s">
         <v>441</v>
       </c>
-      <c r="AJ1" s="91" t="s">
+      <c r="AJ1" s="94" t="s">
         <v>438</v>
       </c>
-      <c r="AK1" s="91" t="s">
+      <c r="AK1" s="94" t="s">
         <v>440</v>
       </c>
-      <c r="AL1" s="91" t="s">
+      <c r="AL1" s="94" t="s">
         <v>439</v>
       </c>
-      <c r="AM1" s="91" t="s">
+      <c r="AM1" s="94" t="s">
         <v>441</v>
       </c>
-      <c r="AN1" s="91" t="s">
+      <c r="AN1" s="94" t="s">
         <v>438</v>
       </c>
-      <c r="AO1" s="91" t="s">
+      <c r="AO1" s="94" t="s">
         <v>440</v>
       </c>
-      <c r="AP1" s="91" t="s">
+      <c r="AP1" s="94" t="s">
         <v>439</v>
       </c>
     </row>
@@ -2639,34 +2648,34 @@
       <c r="AC2" s="71">
         <v>0</v>
       </c>
-      <c r="AD2" s="92"/>
-      <c r="AE2" s="92">
+      <c r="AD2" s="95"/>
+      <c r="AE2" s="95">
         <v>2</v>
       </c>
-      <c r="AF2" s="92">
+      <c r="AF2" s="95">
         <v>2</v>
       </c>
-      <c r="AG2" s="92">
+      <c r="AG2" s="95">
         <v>2</v>
       </c>
-      <c r="AI2" s="92"/>
-      <c r="AJ2" s="92">
+      <c r="AI2" s="95"/>
+      <c r="AJ2" s="95">
         <v>2</v>
       </c>
-      <c r="AK2" s="92">
+      <c r="AK2" s="95">
         <v>2</v>
       </c>
-      <c r="AL2" s="92">
+      <c r="AL2" s="95">
         <v>2</v>
       </c>
-      <c r="AM2" s="92"/>
-      <c r="AN2" s="92">
+      <c r="AM2" s="95"/>
+      <c r="AN2" s="95">
         <v>2</v>
       </c>
-      <c r="AO2" s="92">
+      <c r="AO2" s="95">
         <v>2</v>
       </c>
-      <c r="AP2" s="92">
+      <c r="AP2" s="95">
         <v>2</v>
       </c>
     </row>
@@ -2714,18 +2723,18 @@
       <c r="AA3" s="70"/>
       <c r="AB3" s="70"/>
       <c r="AC3" s="71"/>
-      <c r="AD3" s="93"/>
-      <c r="AE3" s="93"/>
-      <c r="AF3" s="93"/>
-      <c r="AG3" s="93"/>
-      <c r="AI3" s="93"/>
-      <c r="AJ3" s="93"/>
-      <c r="AK3" s="93"/>
-      <c r="AL3" s="93"/>
-      <c r="AM3" s="93"/>
-      <c r="AN3" s="93"/>
-      <c r="AO3" s="93"/>
-      <c r="AP3" s="93"/>
+      <c r="AD3" s="96"/>
+      <c r="AE3" s="96"/>
+      <c r="AF3" s="96"/>
+      <c r="AG3" s="96"/>
+      <c r="AI3" s="96"/>
+      <c r="AJ3" s="96"/>
+      <c r="AK3" s="96"/>
+      <c r="AL3" s="96"/>
+      <c r="AM3" s="96"/>
+      <c r="AN3" s="96"/>
+      <c r="AO3" s="96"/>
+      <c r="AP3" s="96"/>
     </row>
     <row r="4" spans="1:50" s="30" customFormat="1" ht="130.80000000000001" x14ac:dyDescent="0.3">
       <c r="A4" s="54" t="s">
@@ -2815,19 +2824,19 @@
       <c r="AC4" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="AD4" s="94" t="s">
+      <c r="AD4" s="101" t="s">
         <v>429</v>
       </c>
-      <c r="AE4" s="95"/>
-      <c r="AF4" s="95"/>
-      <c r="AG4" s="96"/>
+      <c r="AE4" s="102"/>
+      <c r="AF4" s="102"/>
+      <c r="AG4" s="103"/>
       <c r="AH4" s="56"/>
-      <c r="AI4" s="94" t="s">
+      <c r="AI4" s="101" t="s">
         <v>430</v>
       </c>
-      <c r="AJ4" s="95"/>
-      <c r="AK4" s="95"/>
-      <c r="AL4" s="96"/>
+      <c r="AJ4" s="102"/>
+      <c r="AK4" s="102"/>
+      <c r="AL4" s="103"/>
       <c r="AM4" s="56"/>
       <c r="AN4" s="56"/>
       <c r="AO4" s="56"/>
@@ -3541,7 +3550,7 @@
         <f t="shared" si="7"/>
         <v>10000000</v>
       </c>
-      <c r="AR9" s="106" t="s">
+      <c r="AR9" s="91" t="s">
         <v>432</v>
       </c>
       <c r="AX9" s="33"/>
@@ -8148,6 +8157,16 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="AP1:AP3"/>
+    <mergeCell ref="AD4:AG4"/>
+    <mergeCell ref="AI4:AL4"/>
+    <mergeCell ref="AK1:AK3"/>
+    <mergeCell ref="AL1:AL3"/>
+    <mergeCell ref="AI1:AI3"/>
+    <mergeCell ref="AJ1:AJ3"/>
+    <mergeCell ref="AM1:AM3"/>
+    <mergeCell ref="AN1:AN3"/>
+    <mergeCell ref="AO1:AO3"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="AD1:AD3"/>
     <mergeCell ref="AE1:AE3"/>
@@ -8156,16 +8175,6 @@
     <mergeCell ref="F1:M1"/>
     <mergeCell ref="V1:AC1"/>
     <mergeCell ref="N1:U1"/>
-    <mergeCell ref="AI1:AI3"/>
-    <mergeCell ref="AJ1:AJ3"/>
-    <mergeCell ref="AM1:AM3"/>
-    <mergeCell ref="AN1:AN3"/>
-    <mergeCell ref="AO1:AO3"/>
-    <mergeCell ref="AP1:AP3"/>
-    <mergeCell ref="AD4:AG4"/>
-    <mergeCell ref="AI4:AL4"/>
-    <mergeCell ref="AK1:AK3"/>
-    <mergeCell ref="AL1:AL3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8175,11 +8184,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AA410"/>
+  <dimension ref="A1:AA417"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A389" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T415" sqref="T415:V417"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8257,11 +8266,11 @@
       <c r="S1" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="T1" s="103" t="s">
+      <c r="T1" s="104" t="s">
         <v>140</v>
       </c>
-      <c r="U1" s="104"/>
-      <c r="V1" s="105"/>
+      <c r="U1" s="105"/>
+      <c r="V1" s="106"/>
     </row>
     <row r="2" spans="1:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="10"/>
@@ -24850,6 +24859,191 @@
       <c r="V410" s="21" t="str">
         <f t="shared" si="611"/>
         <v>2A</v>
+      </c>
+    </row>
+    <row r="414" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="D414" s="2" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="415" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B415" s="6">
+        <v>0</v>
+      </c>
+      <c r="C415" s="6" t="str">
+        <f t="shared" ref="C415:C417" si="631">"0x" &amp; DEC2HEX(B415,3)</f>
+        <v>0x000</v>
+      </c>
+      <c r="D415" s="27" t="s">
+        <v>444</v>
+      </c>
+      <c r="F415" s="2"/>
+      <c r="G415" s="16">
+        <v>1</v>
+      </c>
+      <c r="H415" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="I415" s="6">
+        <f t="shared" ref="I415:I417" si="632">IF(H415="", "", VLOOKUP(H415, $X$3:$Y$10, 2))</f>
+        <v>0</v>
+      </c>
+      <c r="M415" s="6">
+        <v>255</v>
+      </c>
+      <c r="N415" s="18" t="str">
+        <f t="shared" ref="N415:N417" si="633">IF(G415="", "", TEXT(DEC2BIN(G415), "000000"))</f>
+        <v>000001</v>
+      </c>
+      <c r="O415" s="19" t="str">
+        <f t="shared" ref="O415:O416" si="634">IF(I415="", "", TEXT(DEC2BIN(I415), "000"))</f>
+        <v>000</v>
+      </c>
+      <c r="P415" s="19" t="str">
+        <f t="shared" ref="P415:P417" si="635">IF(J415="", "", TEXT(DEC2BIN(J415), "000"))</f>
+        <v/>
+      </c>
+      <c r="Q415" s="19" t="str">
+        <f t="shared" ref="Q415:Q417" si="636">IF(K415="", "", TEXT(DEC2BIN(K415), "000"))</f>
+        <v/>
+      </c>
+      <c r="R415" s="19" t="str">
+        <f t="shared" ref="R415:R417" si="637">IF(L415="", "", TEXT(DEC2BIN(L415), "00000000"))</f>
+        <v/>
+      </c>
+      <c r="S415" s="20" t="str">
+        <f t="shared" ref="S415:S417" si="638">IF(M415="", "", TEXT(DEC2BIN(M415), "00000000"))</f>
+        <v>11111111</v>
+      </c>
+      <c r="T415" s="6" t="str">
+        <f t="shared" ref="T415:T417" si="639">BIN2HEX(LEFT(CONCATENATE(N415,IF(O415="", "000", O415)), 8), 2)</f>
+        <v>04</v>
+      </c>
+      <c r="U415" s="6" t="str">
+        <f t="shared" ref="U415:U417" si="640">BIN2HEX(CONCATENATE(RIGHT(O415, 1), IF(P415 = "", "000", P415), IF(Q415 = "", "000", Q415), "0"), 2)</f>
+        <v>00</v>
+      </c>
+      <c r="V415" s="21" t="str">
+        <f t="shared" ref="V415:V417" si="641">IF(R415="", BIN2HEX(S415, 2), BIN2HEX(R415,2))</f>
+        <v>FF</v>
+      </c>
+    </row>
+    <row r="416" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B416" s="6">
+        <v>3</v>
+      </c>
+      <c r="C416" s="6" t="str">
+        <f t="shared" si="631"/>
+        <v>0x003</v>
+      </c>
+      <c r="D416" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="F416" s="2"/>
+      <c r="G416" s="16">
+        <v>40</v>
+      </c>
+      <c r="H416" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="I416" s="6">
+        <f t="shared" si="632"/>
+        <v>0</v>
+      </c>
+      <c r="N416" s="18" t="str">
+        <f t="shared" si="633"/>
+        <v>101000</v>
+      </c>
+      <c r="O416" s="19" t="str">
+        <f t="shared" si="634"/>
+        <v>000</v>
+      </c>
+      <c r="P416" s="19" t="str">
+        <f t="shared" si="635"/>
+        <v/>
+      </c>
+      <c r="Q416" s="19" t="str">
+        <f t="shared" si="636"/>
+        <v/>
+      </c>
+      <c r="R416" s="19" t="str">
+        <f t="shared" si="637"/>
+        <v/>
+      </c>
+      <c r="S416" s="20" t="str">
+        <f t="shared" si="638"/>
+        <v/>
+      </c>
+      <c r="T416" s="6" t="str">
+        <f t="shared" si="639"/>
+        <v>A0</v>
+      </c>
+      <c r="U416" s="6" t="str">
+        <f t="shared" si="640"/>
+        <v>00</v>
+      </c>
+      <c r="V416" s="21" t="str">
+        <f t="shared" si="641"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="417" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A417" s="51"/>
+      <c r="B417" s="6">
+        <v>6</v>
+      </c>
+      <c r="C417" s="6" t="str">
+        <f t="shared" si="631"/>
+        <v>0x006</v>
+      </c>
+      <c r="D417" s="27" t="s">
+        <v>445</v>
+      </c>
+      <c r="G417" s="16">
+        <v>12</v>
+      </c>
+      <c r="I417" s="6" t="str">
+        <f t="shared" si="632"/>
+        <v/>
+      </c>
+      <c r="L417" s="6">
+        <v>0</v>
+      </c>
+      <c r="N417" s="18" t="str">
+        <f t="shared" si="633"/>
+        <v>001100</v>
+      </c>
+      <c r="O417" s="19" t="str">
+        <f>IF(I417="", "", TEXT(DEC2BIN(I417), "000"))</f>
+        <v/>
+      </c>
+      <c r="P417" s="19" t="str">
+        <f t="shared" si="635"/>
+        <v/>
+      </c>
+      <c r="Q417" s="19" t="str">
+        <f t="shared" si="636"/>
+        <v/>
+      </c>
+      <c r="R417" s="19" t="str">
+        <f t="shared" si="637"/>
+        <v>00000000</v>
+      </c>
+      <c r="S417" s="20" t="str">
+        <f t="shared" si="638"/>
+        <v/>
+      </c>
+      <c r="T417" s="6" t="str">
+        <f t="shared" si="639"/>
+        <v>30</v>
+      </c>
+      <c r="U417" s="6" t="str">
+        <f t="shared" si="640"/>
+        <v>00</v>
+      </c>
+      <c r="V417" s="21" t="str">
+        <f t="shared" si="641"/>
+        <v>00</v>
       </c>
     </row>
   </sheetData>
@@ -24863,7 +25057,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z17" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>$X$16:$X$18</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H6 H9:H11 H201:H224 H141:H149 H102:H112 H117:H132 H83:H93 H49 H41:H42 H31:H33 H17:H26 H229:H242 H154:H174 H276 H247:H273 H282:H283 H278:H280 H293:H294 H288:H291 H299:H302 H307:H319 H325:H337 H343:H348 H374:H387 H350:H360 H362:H372 H392:H410" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H6 H9:H11 H201:H224 H141:H149 H102:H112 H117:H132 H83:H93 H49 H41:H42 H31:H33 H17:H26 H229:H242 H154:H174 H276 H247:H273 H282:H283 H278:H280 H293:H294 H288:H291 H299:H302 H307:H319 H325:H337 H343:H348 H374:H387 H350:H360 H362:H372 H392:H410 H415:H417" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>$X$3:$X$10</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>